<commit_message>
cambios actualizando el excel,(Post withdraw new) y cambios en withdraw service para que se muestre Withdraw made sucessfully
</commit_message>
<xml_diff>
--- a/.readmeFiles/Endpoints.xlsx
+++ b/.readmeFiles/Endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/dceballr_emeal_nttdata_com/Documents/Escritorio/Backend/Repositorio/back-end-framework/.readmeFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/anfrodri_emeal_nttdata_com/Documents/Escritorio/Git backend/back-end-framework/.readmeFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="391" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1228B490-CAF6-4317-BEE9-DC448C568E6B}"/>
+  <xr:revisionPtr revIDLastSave="402" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05E72A7F-B62A-4117-8EC3-154EB610D5C6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="203">
   <si>
     <t>HTTP Method</t>
   </si>
@@ -636,6 +636,15 @@
   </si>
   <si>
     <t>Delete withdraws by its cardId</t>
+  </si>
+  <si>
+    <t>"Forbidden: card does not belong to the authenticated customer"</t>
+  </si>
+  <si>
+    <t>Card not found</t>
+  </si>
+  <si>
+    <t>"Withdraw made successfully"</t>
   </si>
 </sst>
 </file>
@@ -1300,15 +1309,78 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1318,6 +1390,57 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1327,29 +1450,107 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1357,216 +1558,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="2" fillId="8" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1919,23 +1930,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA3F6E-09E5-46A7-9DF8-4B95ED8D48E7}">
   <dimension ref="B2:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" topLeftCell="C61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="41.1796875" customWidth="1"/>
+    <col min="5" max="5" width="30.453125" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" customWidth="1"/>
-    <col min="8" max="8" width="67.140625" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="7" max="7" width="32.453125" customWidth="1"/>
+    <col min="8" max="8" width="67.1796875" customWidth="1"/>
+    <col min="9" max="9" width="26.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:9" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1958,7 +1969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1979,7 +1990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="5"/>
       <c r="D5" s="34" t="s">
         <v>13</v>
@@ -1998,7 +2009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="5"/>
       <c r="D6" s="34" t="s">
         <v>16</v>
@@ -2017,7 +2028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -2039,7 +2050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="5"/>
       <c r="D8" s="34" t="s">
         <v>23</v>
@@ -2058,15 +2069,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="5"/>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="66" t="s">
+      <c r="E9" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="127" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -2075,45 +2086,45 @@
       <c r="H9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="133" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="5"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="66"/>
+      <c r="D10" s="127"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="127"/>
       <c r="G10" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="64"/>
-    </row>
-    <row r="11" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="133"/>
+    </row>
+    <row r="11" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="5"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="66"/>
+      <c r="D11" s="127"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="127"/>
       <c r="G11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="64"/>
-    </row>
-    <row r="12" spans="2:9" ht="28.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="133"/>
+    </row>
+    <row r="12" spans="2:9" ht="28.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="5"/>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="66" t="s">
+      <c r="E12" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="127" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="38" t="s">
@@ -2122,37 +2133,37 @@
       <c r="H12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="64" t="s">
+      <c r="I12" s="133" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="5"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="66"/>
+      <c r="D13" s="127"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="127"/>
       <c r="G13" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="64"/>
-    </row>
-    <row r="14" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="133"/>
+    </row>
+    <row r="14" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="5"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="66"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="127"/>
       <c r="G14" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="64"/>
-    </row>
-    <row r="15" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="133"/>
+    </row>
+    <row r="15" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="5"/>
       <c r="D15" s="34" t="s">
         <v>36</v>
@@ -2171,7 +2182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="5"/>
       <c r="D16" s="34" t="s">
         <v>38</v>
@@ -2190,7 +2201,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="5"/>
       <c r="D17" s="34" t="s">
         <v>41</v>
@@ -2209,7 +2220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C18" s="5"/>
       <c r="D18" s="34" t="s">
         <v>44</v>
@@ -2228,7 +2239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="5"/>
       <c r="D19" s="34" t="s">
         <v>46</v>
@@ -2247,15 +2258,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="3:9" ht="40.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
-      <c r="D20" s="66" t="s">
+      <c r="D20" s="127" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="66" t="s">
+      <c r="E20" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="127" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="39" t="s">
@@ -2264,58 +2275,58 @@
       <c r="H20" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="64" t="s">
+      <c r="I20" s="133" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="3:9" ht="40.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="66"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="128"/>
+      <c r="F21" s="127"/>
       <c r="G21" s="39" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="64"/>
-    </row>
-    <row r="22" spans="3:9" ht="40.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I21" s="133"/>
+    </row>
+    <row r="22" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="66"/>
+      <c r="D22" s="127"/>
+      <c r="E22" s="128"/>
+      <c r="F22" s="127"/>
       <c r="G22" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="64"/>
-    </row>
-    <row r="23" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="133"/>
+    </row>
+    <row r="23" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C23" s="5"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="66"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="127"/>
       <c r="G23" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H23" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="64"/>
-    </row>
-    <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="133"/>
+    </row>
+    <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="5"/>
-      <c r="D24" s="66" t="s">
+      <c r="D24" s="127" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="66" t="s">
+      <c r="E24" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="127" t="s">
         <v>57</v>
       </c>
       <c r="G24" s="38" t="s">
@@ -2324,45 +2335,45 @@
       <c r="H24" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="64" t="s">
+      <c r="I24" s="133" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="5"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="66"/>
+      <c r="D25" s="127"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="127"/>
       <c r="G25" s="42" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="I25" s="64"/>
-    </row>
-    <row r="26" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="133"/>
+    </row>
+    <row r="26" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C26" s="5"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="66"/>
+      <c r="D26" s="127"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="127"/>
       <c r="G26" s="42" t="s">
         <v>53</v>
       </c>
       <c r="H26" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="64"/>
-    </row>
-    <row r="27" spans="3:9" ht="58.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="133"/>
+    </row>
+    <row r="27" spans="3:9" ht="58.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C27" s="5"/>
-      <c r="D27" s="66" t="s">
+      <c r="D27" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="68" t="s">
+      <c r="E27" s="105" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="132" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="38" t="s">
@@ -2371,84 +2382,84 @@
       <c r="H27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="64" t="s">
+      <c r="I27" s="133" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="5"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="68"/>
+      <c r="D28" s="127"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="132"/>
       <c r="G28" s="42" t="s">
         <v>63</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="64"/>
-    </row>
-    <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="133"/>
+    </row>
+    <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="5"/>
-      <c r="D29" s="91" t="s">
+      <c r="D29" s="129" t="s">
         <v>181</v>
       </c>
-      <c r="E29" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="69" t="s">
+      <c r="E29" s="105" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="72" t="s">
+      <c r="G29" s="136" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="144" t="s">
+      <c r="H29" s="138" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="78" t="s">
+      <c r="I29" s="111" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="5"/>
-      <c r="D30" s="92"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="144"/>
-      <c r="I30" s="79"/>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="130"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="109"/>
+      <c r="G30" s="137"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="112"/>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C31" s="5"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="75" t="s">
+      <c r="D31" s="130"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="109"/>
+      <c r="G31" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="74" t="s">
+      <c r="H31" s="141" t="s">
         <v>66</v>
       </c>
-      <c r="I31" s="79"/>
-    </row>
-    <row r="32" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I31" s="112"/>
+    </row>
+    <row r="32" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="5"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="96"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="76"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="80"/>
-    </row>
-    <row r="33" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="131"/>
+      <c r="E32" s="107"/>
+      <c r="F32" s="110"/>
+      <c r="G32" s="140"/>
+      <c r="H32" s="142"/>
+      <c r="I32" s="113"/>
+    </row>
+    <row r="33" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="5"/>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="68" t="s">
+      <c r="E33" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="132" t="s">
         <v>68</v>
       </c>
       <c r="G33" s="54" t="s">
@@ -2457,181 +2468,181 @@
       <c r="H33" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="64" t="s">
+      <c r="I33" s="133" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C34" s="5"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="90"/>
-      <c r="F34" s="68"/>
+      <c r="D34" s="132"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="132"/>
       <c r="G34" s="47" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I34" s="64"/>
-    </row>
-    <row r="35" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="123"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="90"/>
-      <c r="F35" s="68"/>
+      <c r="I34" s="133"/>
+    </row>
+    <row r="35" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C35" s="5"/>
+      <c r="D35" s="132"/>
+      <c r="E35" s="128"/>
+      <c r="F35" s="132"/>
       <c r="G35" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H35" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="64"/>
-    </row>
-    <row r="36" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="123"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="90"/>
-      <c r="F36" s="68"/>
+      <c r="I35" s="133"/>
+    </row>
+    <row r="36" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C36" s="5"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="128"/>
+      <c r="F36" s="132"/>
       <c r="G36" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H36" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I36" s="64"/>
-    </row>
-    <row r="37" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="123"/>
-      <c r="D37" s="124" t="s">
+      <c r="I36" s="133"/>
+    </row>
+    <row r="37" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C37" s="5"/>
+      <c r="D37" s="102" t="s">
         <v>182</v>
       </c>
-      <c r="E37" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="69" t="s">
+      <c r="E37" s="105" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="108" t="s">
         <v>183</v>
       </c>
-      <c r="G37" s="141" t="s">
+      <c r="G37" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H37" s="141" t="s">
+      <c r="H37" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="I37" s="78" t="s">
+      <c r="I37" s="111" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="123"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="95"/>
-      <c r="F38" s="70"/>
+    <row r="38" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C38" s="5"/>
+      <c r="D38" s="103"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="109"/>
       <c r="G38" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="H38" s="120"/>
-      <c r="I38" s="79"/>
-    </row>
-    <row r="39" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="122"/>
-      <c r="D39" s="126"/>
-      <c r="E39" s="96"/>
-      <c r="F39" s="71"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="112"/>
+    </row>
+    <row r="39" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C39" s="114"/>
+      <c r="D39" s="104"/>
+      <c r="E39" s="107"/>
+      <c r="F39" s="110"/>
       <c r="G39" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="H39" s="120"/>
-      <c r="I39" s="80"/>
-    </row>
-    <row r="40" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="122"/>
-      <c r="D40" s="124" t="s">
+      <c r="H39" s="55"/>
+      <c r="I39" s="113"/>
+    </row>
+    <row r="40" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C40" s="114"/>
+      <c r="D40" s="102" t="s">
         <v>186</v>
       </c>
-      <c r="E40" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="69" t="s">
+      <c r="E40" s="105" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="108" t="s">
         <v>187</v>
       </c>
-      <c r="G40" s="141" t="s">
+      <c r="G40" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H40" s="141" t="s">
+      <c r="H40" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="I40" s="78" t="s">
+      <c r="I40" s="111" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="41" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="122"/>
-      <c r="D41" s="125"/>
-      <c r="E41" s="95"/>
-      <c r="F41" s="70"/>
+    <row r="41" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C41" s="114"/>
+      <c r="D41" s="103"/>
+      <c r="E41" s="106"/>
+      <c r="F41" s="109"/>
       <c r="G41" s="42"/>
-      <c r="H41" s="120"/>
-      <c r="I41" s="79"/>
-    </row>
-    <row r="42" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="122"/>
-      <c r="D42" s="126"/>
-      <c r="E42" s="96"/>
-      <c r="F42" s="71"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="112"/>
+    </row>
+    <row r="42" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C42" s="114"/>
+      <c r="D42" s="104"/>
+      <c r="E42" s="107"/>
+      <c r="F42" s="110"/>
       <c r="G42" s="42"/>
-      <c r="H42" s="120"/>
-      <c r="I42" s="80"/>
-    </row>
-    <row r="43" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="122"/>
-      <c r="D43" s="124" t="s">
+      <c r="H42" s="55"/>
+      <c r="I42" s="113"/>
+    </row>
+    <row r="43" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C43" s="114"/>
+      <c r="D43" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="69" t="s">
+      <c r="E43" s="105" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="108" t="s">
         <v>189</v>
       </c>
-      <c r="G43" s="141" t="s">
+      <c r="G43" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H43" s="141" t="s">
+      <c r="H43" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="I43" s="78" t="s">
+      <c r="I43" s="111" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="44" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="122"/>
-      <c r="D44" s="125"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="70"/>
+    <row r="44" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C44" s="114"/>
+      <c r="D44" s="103"/>
+      <c r="E44" s="106"/>
+      <c r="F44" s="109"/>
       <c r="G44" s="42"/>
-      <c r="H44" s="120"/>
-      <c r="I44" s="79"/>
-    </row>
-    <row r="45" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="121"/>
-      <c r="D45" s="126"/>
-      <c r="E45" s="96"/>
-      <c r="F45" s="71"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="112"/>
+    </row>
+    <row r="45" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C45" s="115"/>
+      <c r="D45" s="104"/>
+      <c r="E45" s="107"/>
+      <c r="F45" s="110"/>
       <c r="G45" s="42"/>
-      <c r="H45" s="120"/>
-      <c r="I45" s="80"/>
-    </row>
-    <row r="46" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H45" s="55"/>
+      <c r="I45" s="113"/>
+    </row>
+    <row r="46" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="115" t="s">
+      <c r="D46" s="116" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="116" t="s">
+      <c r="E46" s="117" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="67" t="s">
+      <c r="F46" s="135" t="s">
         <v>78</v>
       </c>
       <c r="G46" s="30" t="s">
@@ -2640,45 +2651,45 @@
       <c r="H46" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="65" t="s">
+      <c r="I46" s="134" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C47" s="16"/>
-      <c r="D47" s="115"/>
-      <c r="E47" s="116"/>
-      <c r="F47" s="67"/>
+      <c r="D47" s="116"/>
+      <c r="E47" s="117"/>
+      <c r="F47" s="135"/>
       <c r="G47" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="I47" s="65"/>
-    </row>
-    <row r="48" spans="3:9" ht="31.35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I47" s="134"/>
+    </row>
+    <row r="48" spans="3:9" ht="31.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C48" s="7"/>
-      <c r="D48" s="115"/>
-      <c r="E48" s="116"/>
-      <c r="F48" s="67"/>
+      <c r="D48" s="116"/>
+      <c r="E48" s="117"/>
+      <c r="F48" s="135"/>
       <c r="G48" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H48" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="65"/>
-    </row>
-    <row r="49" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I48" s="134"/>
+    </row>
+    <row r="49" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C49" s="7"/>
-      <c r="D49" s="100" t="s">
+      <c r="D49" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="97" t="s">
+      <c r="E49" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="112" t="s">
+      <c r="F49" s="96" t="s">
         <v>85</v>
       </c>
       <c r="G49" s="30" t="s">
@@ -2687,45 +2698,45 @@
       <c r="H49" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I49" s="61" t="s">
+      <c r="I49" s="99" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="7"/>
-      <c r="D50" s="101"/>
-      <c r="E50" s="98"/>
-      <c r="F50" s="113"/>
+      <c r="D50" s="119"/>
+      <c r="E50" s="94"/>
+      <c r="F50" s="97"/>
       <c r="G50" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H50" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="I50" s="62"/>
-    </row>
-    <row r="51" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I50" s="100"/>
+    </row>
+    <row r="51" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C51" s="7"/>
-      <c r="D51" s="102"/>
-      <c r="E51" s="99"/>
-      <c r="F51" s="114"/>
+      <c r="D51" s="120"/>
+      <c r="E51" s="95"/>
+      <c r="F51" s="98"/>
       <c r="G51" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H51" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I51" s="63"/>
-    </row>
-    <row r="52" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I51" s="101"/>
+    </row>
+    <row r="52" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C52" s="7"/>
-      <c r="D52" s="100" t="s">
+      <c r="D52" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="112" t="s">
+      <c r="E52" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="96" t="s">
         <v>91</v>
       </c>
       <c r="G52" s="30" t="s">
@@ -2734,24 +2745,24 @@
       <c r="H52" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="61" t="s">
+      <c r="I52" s="99" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C53" s="7"/>
-      <c r="D53" s="102"/>
-      <c r="E53" s="99"/>
-      <c r="F53" s="114"/>
+      <c r="D53" s="120"/>
+      <c r="E53" s="95"/>
+      <c r="F53" s="98"/>
       <c r="G53" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H53" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="I53" s="63"/>
-    </row>
-    <row r="54" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I53" s="101"/>
+    </row>
+    <row r="54" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C54" s="7"/>
       <c r="D54" s="50"/>
       <c r="E54" s="49"/>
@@ -2764,7 +2775,7 @@
       </c>
       <c r="I54" s="51"/>
     </row>
-    <row r="55" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C55" s="7"/>
       <c r="D55" s="50" t="s">
         <v>179</v>
@@ -2783,7 +2794,7 @@
       </c>
       <c r="I55" s="51"/>
     </row>
-    <row r="56" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C56" s="7"/>
       <c r="D56" s="50"/>
       <c r="E56" s="49"/>
@@ -2794,15 +2805,15 @@
       <c r="H56" s="52"/>
       <c r="I56" s="51"/>
     </row>
-    <row r="57" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C57" s="7"/>
-      <c r="D57" s="100" t="s">
+      <c r="D57" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="97" t="s">
+      <c r="E57" s="93" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="112" t="s">
+      <c r="F57" s="96" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="30" t="s">
@@ -2811,58 +2822,58 @@
       <c r="H57" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="I57" s="61" t="s">
+      <c r="I57" s="99" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C58" s="7"/>
-      <c r="D58" s="101"/>
-      <c r="E58" s="98"/>
-      <c r="F58" s="113"/>
+      <c r="D58" s="119"/>
+      <c r="E58" s="94"/>
+      <c r="F58" s="97"/>
       <c r="G58" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H58" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="I58" s="62"/>
-    </row>
-    <row r="59" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I58" s="100"/>
+    </row>
+    <row r="59" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C59" s="7"/>
-      <c r="D59" s="101"/>
-      <c r="E59" s="98"/>
-      <c r="F59" s="113"/>
+      <c r="D59" s="119"/>
+      <c r="E59" s="94"/>
+      <c r="F59" s="97"/>
       <c r="G59" s="32" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I59" s="62"/>
-    </row>
-    <row r="60" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I59" s="100"/>
+    </row>
+    <row r="60" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C60" s="7"/>
-      <c r="D60" s="102"/>
-      <c r="E60" s="99"/>
-      <c r="F60" s="114"/>
+      <c r="D60" s="120"/>
+      <c r="E60" s="95"/>
+      <c r="F60" s="98"/>
       <c r="G60" s="32" t="s">
         <v>100</v>
       </c>
       <c r="H60" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I60" s="63"/>
-    </row>
-    <row r="61" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I60" s="101"/>
+    </row>
+    <row r="61" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C61" s="7"/>
-      <c r="D61" s="100" t="s">
+      <c r="D61" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="97" t="s">
+      <c r="E61" s="93" t="s">
         <v>103</v>
       </c>
-      <c r="F61" s="112" t="s">
+      <c r="F61" s="96" t="s">
         <v>104</v>
       </c>
       <c r="G61" s="30" t="s">
@@ -2871,58 +2882,58 @@
       <c r="H61" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="I61" s="61" t="s">
+      <c r="I61" s="99" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C62" s="7"/>
-      <c r="D62" s="101"/>
-      <c r="E62" s="98"/>
-      <c r="F62" s="113"/>
+      <c r="D62" s="119"/>
+      <c r="E62" s="94"/>
+      <c r="F62" s="97"/>
       <c r="G62" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H62" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I62" s="62"/>
-    </row>
-    <row r="63" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I62" s="100"/>
+    </row>
+    <row r="63" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C63" s="7"/>
-      <c r="D63" s="101"/>
-      <c r="E63" s="98"/>
-      <c r="F63" s="113"/>
+      <c r="D63" s="119"/>
+      <c r="E63" s="94"/>
+      <c r="F63" s="97"/>
       <c r="G63" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H63" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="I63" s="62"/>
-    </row>
-    <row r="64" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I63" s="100"/>
+    </row>
+    <row r="64" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C64" s="7"/>
-      <c r="D64" s="102"/>
-      <c r="E64" s="99"/>
-      <c r="F64" s="114"/>
+      <c r="D64" s="120"/>
+      <c r="E64" s="95"/>
+      <c r="F64" s="98"/>
       <c r="G64" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H64" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I64" s="63"/>
-    </row>
-    <row r="65" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I64" s="101"/>
+    </row>
+    <row r="65" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C65" s="7"/>
-      <c r="D65" s="100" t="s">
+      <c r="D65" s="118" t="s">
         <v>109</v>
       </c>
-      <c r="E65" s="97" t="s">
+      <c r="E65" s="93" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="112" t="s">
+      <c r="F65" s="96" t="s">
         <v>111</v>
       </c>
       <c r="G65" s="30" t="s">
@@ -2931,132 +2942,146 @@
       <c r="H65" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="I65" s="61" t="s">
+      <c r="I65" s="99" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C66" s="7"/>
-      <c r="D66" s="101"/>
-      <c r="E66" s="98"/>
-      <c r="F66" s="113"/>
+      <c r="D66" s="119"/>
+      <c r="E66" s="94"/>
+      <c r="F66" s="97"/>
       <c r="G66" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H66" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I66" s="62"/>
-    </row>
-    <row r="67" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I66" s="100"/>
+    </row>
+    <row r="67" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C67" s="7"/>
-      <c r="D67" s="101"/>
-      <c r="E67" s="98"/>
-      <c r="F67" s="113"/>
+      <c r="D67" s="119"/>
+      <c r="E67" s="94"/>
+      <c r="F67" s="97"/>
       <c r="G67" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H67" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="I67" s="62"/>
-    </row>
-    <row r="68" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I67" s="100"/>
+    </row>
+    <row r="68" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C68" s="7"/>
-      <c r="D68" s="101"/>
-      <c r="E68" s="98"/>
-      <c r="F68" s="113"/>
+      <c r="D68" s="119"/>
+      <c r="E68" s="94"/>
+      <c r="F68" s="97"/>
       <c r="G68" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H68" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="I68" s="62"/>
-    </row>
-    <row r="69" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I68" s="100"/>
+    </row>
+    <row r="69" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C69" s="7"/>
-      <c r="D69" s="101"/>
-      <c r="E69" s="98"/>
-      <c r="F69" s="113"/>
+      <c r="D69" s="119"/>
+      <c r="E69" s="94"/>
+      <c r="F69" s="97"/>
       <c r="G69" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H69" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I69" s="62"/>
-    </row>
-    <row r="70" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C70" s="128"/>
-      <c r="D70" s="102"/>
-      <c r="E70" s="99"/>
-      <c r="F70" s="114"/>
+      <c r="I69" s="100"/>
+    </row>
+    <row r="70" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C70" s="88"/>
+      <c r="D70" s="120"/>
+      <c r="E70" s="95"/>
+      <c r="F70" s="98"/>
       <c r="G70" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H70" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="I70" s="63"/>
-    </row>
-    <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C71" s="128"/>
-      <c r="D71" s="129" t="s">
+      <c r="I70" s="101"/>
+    </row>
+    <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C71" s="88"/>
+      <c r="D71" s="90" t="s">
         <v>190</v>
       </c>
-      <c r="E71" s="97" t="s">
+      <c r="E71" s="93" t="s">
         <v>191</v>
       </c>
-      <c r="F71" s="112" t="s">
+      <c r="F71" s="96" t="s">
         <v>192</v>
       </c>
       <c r="G71" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H71" s="142"/>
-      <c r="I71" s="61" t="s">
+      <c r="H71" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="I71" s="99" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="72" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="128"/>
-      <c r="D72" s="130"/>
-      <c r="E72" s="98"/>
-      <c r="F72" s="113"/>
-      <c r="G72" s="32"/>
-      <c r="H72" s="52"/>
-      <c r="I72" s="62"/>
-    </row>
-    <row r="73" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C73" s="128"/>
-      <c r="D73" s="130"/>
-      <c r="E73" s="98"/>
-      <c r="F73" s="113"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="62"/>
-    </row>
-    <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C74" s="127"/>
-      <c r="D74" s="131"/>
-      <c r="E74" s="99"/>
-      <c r="F74" s="114"/>
-      <c r="G74" s="32"/>
-      <c r="H74" s="52"/>
-      <c r="I74" s="63"/>
-    </row>
-    <row r="75" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C72" s="88"/>
+      <c r="D72" s="91"/>
+      <c r="E72" s="94"/>
+      <c r="F72" s="97"/>
+      <c r="G72" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H72" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="I72" s="100"/>
+    </row>
+    <row r="73" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C73" s="88"/>
+      <c r="D73" s="91"/>
+      <c r="E73" s="94"/>
+      <c r="F73" s="97"/>
+      <c r="G73" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H73" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="I73" s="100"/>
+    </row>
+    <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C74" s="89"/>
+      <c r="D74" s="92"/>
+      <c r="E74" s="95"/>
+      <c r="F74" s="98"/>
+      <c r="G74" s="144" t="s">
+        <v>31</v>
+      </c>
+      <c r="H74" s="52" t="s">
+        <v>201</v>
+      </c>
+      <c r="I74" s="101"/>
+    </row>
+    <row r="75" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D75" s="106" t="s">
+      <c r="D75" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="103" t="s">
+      <c r="E75" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="F75" s="117" t="s">
+      <c r="F75" s="121" t="s">
         <v>121</v>
       </c>
       <c r="G75" s="26" t="s">
@@ -3065,58 +3090,58 @@
       <c r="H75" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="I75" s="58" t="s">
+      <c r="I75" s="79" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C76" s="9"/>
-      <c r="D76" s="107"/>
-      <c r="E76" s="104"/>
-      <c r="F76" s="118"/>
+      <c r="D76" s="83"/>
+      <c r="E76" s="72"/>
+      <c r="F76" s="122"/>
       <c r="G76" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="I76" s="59"/>
-    </row>
-    <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I76" s="80"/>
+    </row>
+    <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C77" s="10"/>
-      <c r="D77" s="107"/>
-      <c r="E77" s="104"/>
-      <c r="F77" s="118"/>
+      <c r="D77" s="83"/>
+      <c r="E77" s="72"/>
+      <c r="F77" s="122"/>
       <c r="G77" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H77" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I77" s="59"/>
-    </row>
-    <row r="78" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I77" s="80"/>
+    </row>
+    <row r="78" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C78" s="10"/>
-      <c r="D78" s="108"/>
-      <c r="E78" s="105"/>
-      <c r="F78" s="119"/>
+      <c r="D78" s="84"/>
+      <c r="E78" s="73"/>
+      <c r="F78" s="123"/>
       <c r="G78" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H78" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="I78" s="60"/>
-    </row>
-    <row r="79" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I78" s="81"/>
+    </row>
+    <row r="79" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C79" s="10"/>
-      <c r="D79" s="106" t="s">
+      <c r="D79" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="E79" s="103" t="s">
+      <c r="E79" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="109" t="s">
+      <c r="F79" s="85" t="s">
         <v>127</v>
       </c>
       <c r="G79" s="26" t="s">
@@ -3125,45 +3150,45 @@
       <c r="H79" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="I79" s="58" t="s">
+      <c r="I79" s="79" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C80" s="10"/>
-      <c r="D80" s="107"/>
-      <c r="E80" s="104"/>
-      <c r="F80" s="110"/>
+      <c r="D80" s="83"/>
+      <c r="E80" s="72"/>
+      <c r="F80" s="86"/>
       <c r="G80" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H80" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="I80" s="59"/>
-    </row>
-    <row r="81" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I80" s="80"/>
+    </row>
+    <row r="81" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C81" s="10"/>
-      <c r="D81" s="108"/>
-      <c r="E81" s="105"/>
-      <c r="F81" s="111"/>
+      <c r="D81" s="84"/>
+      <c r="E81" s="73"/>
+      <c r="F81" s="87"/>
       <c r="G81" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H81" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I81" s="60"/>
-    </row>
-    <row r="82" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I81" s="81"/>
+    </row>
+    <row r="82" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C82" s="10"/>
-      <c r="D82" s="106" t="s">
+      <c r="D82" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="E82" s="103" t="s">
+      <c r="E82" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="F82" s="109" t="s">
+      <c r="F82" s="85" t="s">
         <v>132</v>
       </c>
       <c r="G82" s="26" t="s">
@@ -3172,45 +3197,45 @@
       <c r="H82" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="I82" s="58" t="s">
+      <c r="I82" s="79" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C83" s="10"/>
-      <c r="D83" s="107"/>
-      <c r="E83" s="104"/>
-      <c r="F83" s="110"/>
+      <c r="D83" s="83"/>
+      <c r="E83" s="72"/>
+      <c r="F83" s="86"/>
       <c r="G83" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H83" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="I83" s="59"/>
-    </row>
-    <row r="84" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I83" s="80"/>
+    </row>
+    <row r="84" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C84" s="10"/>
-      <c r="D84" s="108"/>
-      <c r="E84" s="105"/>
-      <c r="F84" s="111"/>
+      <c r="D84" s="84"/>
+      <c r="E84" s="73"/>
+      <c r="F84" s="87"/>
       <c r="G84" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H84" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I84" s="60"/>
-    </row>
-    <row r="85" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I84" s="81"/>
+    </row>
+    <row r="85" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C85" s="10"/>
-      <c r="D85" s="106" t="s">
+      <c r="D85" s="82" t="s">
         <v>135</v>
       </c>
-      <c r="E85" s="103" t="s">
+      <c r="E85" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="F85" s="109" t="s">
+      <c r="F85" s="85" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="26" t="s">
@@ -3219,152 +3244,152 @@
       <c r="H85" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="I85" s="58" t="s">
+      <c r="I85" s="79" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C86" s="133"/>
-      <c r="D86" s="107"/>
-      <c r="E86" s="104"/>
-      <c r="F86" s="110"/>
+    <row r="86" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C86" s="77"/>
+      <c r="D86" s="83"/>
+      <c r="E86" s="72"/>
+      <c r="F86" s="86"/>
       <c r="G86" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H86" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="I86" s="59"/>
-    </row>
-    <row r="87" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C87" s="133"/>
-      <c r="D87" s="108"/>
-      <c r="E87" s="105"/>
-      <c r="F87" s="111"/>
+      <c r="I86" s="80"/>
+    </row>
+    <row r="87" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C87" s="77"/>
+      <c r="D87" s="84"/>
+      <c r="E87" s="73"/>
+      <c r="F87" s="87"/>
       <c r="G87" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H87" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I87" s="60"/>
-    </row>
-    <row r="88" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C88" s="133"/>
-      <c r="D88" s="135" t="s">
+      <c r="I87" s="81"/>
+    </row>
+    <row r="88" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C88" s="77"/>
+      <c r="D88" s="68" t="s">
         <v>193</v>
       </c>
-      <c r="E88" s="103" t="s">
+      <c r="E88" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="F88" s="138" t="s">
+      <c r="F88" s="74" t="s">
         <v>196</v>
       </c>
       <c r="G88" s="26"/>
-      <c r="H88" s="143"/>
-      <c r="I88" s="58" t="s">
+      <c r="H88" s="59"/>
+      <c r="I88" s="79" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C89" s="133"/>
-      <c r="D89" s="136"/>
-      <c r="E89" s="104"/>
-      <c r="F89" s="139"/>
+    <row r="89" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C89" s="77"/>
+      <c r="D89" s="69"/>
+      <c r="E89" s="72"/>
+      <c r="F89" s="75"/>
       <c r="G89" s="28"/>
-      <c r="H89" s="132"/>
-      <c r="I89" s="59"/>
-    </row>
-    <row r="90" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C90" s="133"/>
-      <c r="D90" s="137"/>
-      <c r="E90" s="105"/>
-      <c r="F90" s="140"/>
+      <c r="H89" s="56"/>
+      <c r="I89" s="80"/>
+    </row>
+    <row r="90" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C90" s="77"/>
+      <c r="D90" s="70"/>
+      <c r="E90" s="73"/>
+      <c r="F90" s="76"/>
       <c r="G90" s="28"/>
-      <c r="H90" s="132"/>
-      <c r="I90" s="60"/>
-    </row>
-    <row r="91" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C91" s="133"/>
-      <c r="D91" s="135" t="s">
+      <c r="H90" s="56"/>
+      <c r="I90" s="81"/>
+    </row>
+    <row r="91" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C91" s="77"/>
+      <c r="D91" s="68" t="s">
         <v>194</v>
       </c>
-      <c r="E91" s="103" t="s">
+      <c r="E91" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="F91" s="138" t="s">
+      <c r="F91" s="74" t="s">
         <v>197</v>
       </c>
       <c r="G91" s="26"/>
-      <c r="H91" s="143"/>
-      <c r="I91" s="58" t="s">
+      <c r="H91" s="59"/>
+      <c r="I91" s="79" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C92" s="133"/>
-      <c r="D92" s="136"/>
-      <c r="E92" s="104"/>
-      <c r="F92" s="139"/>
+    <row r="92" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C92" s="77"/>
+      <c r="D92" s="69"/>
+      <c r="E92" s="72"/>
+      <c r="F92" s="75"/>
       <c r="G92" s="28"/>
-      <c r="H92" s="132"/>
-      <c r="I92" s="59"/>
-    </row>
-    <row r="93" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C93" s="133"/>
-      <c r="D93" s="137"/>
-      <c r="E93" s="105"/>
-      <c r="F93" s="140"/>
+      <c r="H92" s="56"/>
+      <c r="I92" s="80"/>
+    </row>
+    <row r="93" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C93" s="77"/>
+      <c r="D93" s="70"/>
+      <c r="E93" s="73"/>
+      <c r="F93" s="76"/>
       <c r="G93" s="28"/>
-      <c r="H93" s="132"/>
-      <c r="I93" s="60"/>
-    </row>
-    <row r="94" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C94" s="133"/>
-      <c r="D94" s="135" t="s">
+      <c r="H93" s="56"/>
+      <c r="I93" s="81"/>
+    </row>
+    <row r="94" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C94" s="77"/>
+      <c r="D94" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="E94" s="103" t="s">
+      <c r="E94" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="F94" s="138" t="s">
+      <c r="F94" s="74" t="s">
         <v>197</v>
       </c>
       <c r="G94" s="26"/>
-      <c r="H94" s="143"/>
-      <c r="I94" s="58" t="s">
+      <c r="H94" s="59"/>
+      <c r="I94" s="79" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C95" s="133"/>
-      <c r="D95" s="136"/>
-      <c r="E95" s="104"/>
-      <c r="F95" s="139"/>
+    <row r="95" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C95" s="77"/>
+      <c r="D95" s="69"/>
+      <c r="E95" s="72"/>
+      <c r="F95" s="75"/>
       <c r="G95" s="28"/>
-      <c r="H95" s="132"/>
-      <c r="I95" s="59"/>
-    </row>
-    <row r="96" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C96" s="134"/>
-      <c r="D96" s="137"/>
-      <c r="E96" s="105"/>
-      <c r="F96" s="140"/>
+      <c r="H95" s="56"/>
+      <c r="I95" s="80"/>
+    </row>
+    <row r="96" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C96" s="78"/>
+      <c r="D96" s="70"/>
+      <c r="E96" s="73"/>
+      <c r="F96" s="76"/>
       <c r="G96" s="28"/>
-      <c r="H96" s="132"/>
-      <c r="I96" s="60"/>
-    </row>
-    <row r="97" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H96" s="56"/>
+      <c r="I96" s="81"/>
+    </row>
+    <row r="97" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C97" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D97" s="84" t="s">
+      <c r="D97" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="E97" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F97" s="81" t="s">
+      <c r="E97" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="64" t="s">
         <v>141</v>
       </c>
       <c r="G97" s="18" t="s">
@@ -3373,45 +3398,45 @@
       <c r="H97" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="I97" s="55" t="s">
+      <c r="I97" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C98" s="12"/>
-      <c r="D98" s="89"/>
-      <c r="E98" s="87"/>
-      <c r="F98" s="82"/>
+      <c r="D98" s="126"/>
+      <c r="E98" s="124"/>
+      <c r="F98" s="125"/>
       <c r="G98" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H98" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="I98" s="56"/>
-    </row>
-    <row r="99" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I98" s="143"/>
+    </row>
+    <row r="99" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C99" s="13"/>
-      <c r="D99" s="85"/>
-      <c r="E99" s="88"/>
-      <c r="F99" s="83"/>
+      <c r="D99" s="61"/>
+      <c r="E99" s="63"/>
+      <c r="F99" s="65"/>
       <c r="G99" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H99" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="I99" s="57"/>
-    </row>
-    <row r="100" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I99" s="67"/>
+    </row>
+    <row r="100" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C100" s="13"/>
-      <c r="D100" s="84" t="s">
+      <c r="D100" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="E100" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="81" t="s">
+      <c r="E100" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="64" t="s">
         <v>147</v>
       </c>
       <c r="G100" s="18" t="s">
@@ -3420,58 +3445,58 @@
       <c r="H100" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="I100" s="55" t="s">
+      <c r="I100" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C101" s="13"/>
-      <c r="D101" s="89"/>
-      <c r="E101" s="87"/>
-      <c r="F101" s="82"/>
+      <c r="D101" s="126"/>
+      <c r="E101" s="124"/>
+      <c r="F101" s="125"/>
       <c r="G101" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H101" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I101" s="56"/>
-    </row>
-    <row r="102" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I101" s="143"/>
+    </row>
+    <row r="102" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C102" s="13"/>
-      <c r="D102" s="89"/>
-      <c r="E102" s="87"/>
-      <c r="F102" s="82"/>
+      <c r="D102" s="126"/>
+      <c r="E102" s="124"/>
+      <c r="F102" s="125"/>
       <c r="G102" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H102" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I102" s="56"/>
-    </row>
-    <row r="103" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I102" s="143"/>
+    </row>
+    <row r="103" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C103" s="13"/>
-      <c r="D103" s="85"/>
-      <c r="E103" s="88"/>
-      <c r="F103" s="83"/>
+      <c r="D103" s="61"/>
+      <c r="E103" s="63"/>
+      <c r="F103" s="65"/>
       <c r="G103" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H103" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="I103" s="57"/>
-    </row>
-    <row r="104" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I103" s="67"/>
+    </row>
+    <row r="104" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C104" s="13"/>
-      <c r="D104" s="84" t="s">
+      <c r="D104" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="E104" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F104" s="81" t="s">
+      <c r="E104" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" s="64" t="s">
         <v>153</v>
       </c>
       <c r="G104" s="18" t="s">
@@ -3480,58 +3505,58 @@
       <c r="H104" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="I104" s="55" t="s">
+      <c r="I104" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C105" s="13"/>
-      <c r="D105" s="89"/>
-      <c r="E105" s="87"/>
-      <c r="F105" s="82"/>
+      <c r="D105" s="126"/>
+      <c r="E105" s="124"/>
+      <c r="F105" s="125"/>
       <c r="G105" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H105" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="I105" s="56"/>
-    </row>
-    <row r="106" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I105" s="143"/>
+    </row>
+    <row r="106" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C106" s="13"/>
-      <c r="D106" s="89"/>
-      <c r="E106" s="87"/>
-      <c r="F106" s="82"/>
+      <c r="D106" s="126"/>
+      <c r="E106" s="124"/>
+      <c r="F106" s="125"/>
       <c r="G106" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H106" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="I106" s="56"/>
-    </row>
-    <row r="107" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I106" s="143"/>
+    </row>
+    <row r="107" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C107" s="13"/>
-      <c r="D107" s="85"/>
-      <c r="E107" s="88"/>
-      <c r="F107" s="83"/>
+      <c r="D107" s="61"/>
+      <c r="E107" s="63"/>
+      <c r="F107" s="65"/>
       <c r="G107" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H107" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="I107" s="57"/>
-    </row>
-    <row r="108" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I107" s="67"/>
+    </row>
+    <row r="108" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C108" s="13"/>
-      <c r="D108" s="84" t="s">
+      <c r="D108" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="E108" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F108" s="81" t="s">
+      <c r="E108" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108" s="64" t="s">
         <v>159</v>
       </c>
       <c r="G108" s="18" t="s">
@@ -3540,58 +3565,58 @@
       <c r="H108" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="I108" s="55" t="s">
+      <c r="I108" s="66" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C109" s="13"/>
-      <c r="D109" s="89"/>
-      <c r="E109" s="87"/>
-      <c r="F109" s="82"/>
+      <c r="D109" s="126"/>
+      <c r="E109" s="124"/>
+      <c r="F109" s="125"/>
       <c r="G109" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H109" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I109" s="56"/>
-    </row>
-    <row r="110" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I109" s="143"/>
+    </row>
+    <row r="110" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C110" s="13"/>
-      <c r="D110" s="89"/>
-      <c r="E110" s="87"/>
-      <c r="F110" s="82"/>
+      <c r="D110" s="126"/>
+      <c r="E110" s="124"/>
+      <c r="F110" s="125"/>
       <c r="G110" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H110" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I110" s="56"/>
-    </row>
-    <row r="111" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I110" s="143"/>
+    </row>
+    <row r="111" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C111" s="13"/>
-      <c r="D111" s="85"/>
-      <c r="E111" s="88"/>
-      <c r="F111" s="83"/>
+      <c r="D111" s="61"/>
+      <c r="E111" s="63"/>
+      <c r="F111" s="65"/>
       <c r="G111" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H111" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="I111" s="57"/>
-    </row>
-    <row r="112" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I111" s="67"/>
+    </row>
+    <row r="112" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C112" s="13"/>
-      <c r="D112" s="84" t="s">
+      <c r="D112" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="E112" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F112" s="81" t="s">
+      <c r="E112" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F112" s="64" t="s">
         <v>162</v>
       </c>
       <c r="G112" s="18" t="s">
@@ -3600,45 +3625,45 @@
       <c r="H112" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="I112" s="55" t="s">
+      <c r="I112" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C113" s="13"/>
-      <c r="D113" s="89"/>
-      <c r="E113" s="87"/>
-      <c r="F113" s="82"/>
+      <c r="D113" s="126"/>
+      <c r="E113" s="124"/>
+      <c r="F113" s="125"/>
       <c r="G113" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H113" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="I113" s="56"/>
-    </row>
-    <row r="114" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I113" s="143"/>
+    </row>
+    <row r="114" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C114" s="14"/>
-      <c r="D114" s="85"/>
-      <c r="E114" s="88"/>
-      <c r="F114" s="83"/>
+      <c r="D114" s="61"/>
+      <c r="E114" s="63"/>
+      <c r="F114" s="65"/>
       <c r="G114" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H114" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I114" s="57"/>
-    </row>
-    <row r="115" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I114" s="67"/>
+    </row>
+    <row r="115" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C115" s="14"/>
-      <c r="D115" s="84" t="s">
+      <c r="D115" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="E115" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F115" s="81" t="s">
+      <c r="E115" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F115" s="64" t="s">
         <v>166</v>
       </c>
       <c r="G115" s="18" t="s">
@@ -3647,32 +3672,32 @@
       <c r="H115" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="I115" s="55" t="s">
+      <c r="I115" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C116" s="13"/>
-      <c r="D116" s="85"/>
-      <c r="E116" s="88"/>
-      <c r="F116" s="83"/>
+      <c r="D116" s="61"/>
+      <c r="E116" s="63"/>
+      <c r="F116" s="65"/>
       <c r="G116" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H116" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="I116" s="57"/>
-    </row>
-    <row r="117" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I116" s="67"/>
+    </row>
+    <row r="117" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C117" s="13"/>
-      <c r="D117" s="84" t="s">
+      <c r="D117" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="E117" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F117" s="81" t="s">
+      <c r="E117" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F117" s="64" t="s">
         <v>170</v>
       </c>
       <c r="G117" s="18" t="s">
@@ -3681,32 +3706,32 @@
       <c r="H117" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="I117" s="55" t="s">
+      <c r="I117" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C118" s="13"/>
-      <c r="D118" s="85"/>
-      <c r="E118" s="88"/>
-      <c r="F118" s="83"/>
+      <c r="D118" s="61"/>
+      <c r="E118" s="63"/>
+      <c r="F118" s="65"/>
       <c r="G118" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H118" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="I118" s="57"/>
-    </row>
-    <row r="119" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I118" s="67"/>
+    </row>
+    <row r="119" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C119" s="13"/>
-      <c r="D119" s="84" t="s">
+      <c r="D119" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="E119" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F119" s="81" t="s">
+      <c r="E119" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F119" s="64" t="s">
         <v>174</v>
       </c>
       <c r="G119" s="18" t="s">
@@ -3715,58 +3740,58 @@
       <c r="H119" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="I119" s="55" t="s">
+      <c r="I119" s="66" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C120" s="13"/>
-      <c r="D120" s="89"/>
-      <c r="E120" s="87"/>
-      <c r="F120" s="82"/>
+      <c r="D120" s="126"/>
+      <c r="E120" s="124"/>
+      <c r="F120" s="125"/>
       <c r="G120" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H120" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="I120" s="56"/>
-    </row>
-    <row r="121" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I120" s="143"/>
+    </row>
+    <row r="121" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C121" s="13"/>
-      <c r="D121" s="89"/>
-      <c r="E121" s="87"/>
-      <c r="F121" s="82"/>
+      <c r="D121" s="126"/>
+      <c r="E121" s="124"/>
+      <c r="F121" s="125"/>
       <c r="G121" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H121" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I121" s="56"/>
-    </row>
-    <row r="122" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I121" s="143"/>
+    </row>
+    <row r="122" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C122" s="13"/>
-      <c r="D122" s="85"/>
-      <c r="E122" s="88"/>
-      <c r="F122" s="83"/>
+      <c r="D122" s="61"/>
+      <c r="E122" s="63"/>
+      <c r="F122" s="65"/>
       <c r="G122" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H122" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I122" s="57"/>
-    </row>
-    <row r="123" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I122" s="67"/>
+    </row>
+    <row r="123" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C123" s="13"/>
-      <c r="D123" s="84" t="s">
+      <c r="D123" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="E123" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F123" s="81" t="s">
+      <c r="E123" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F123" s="64" t="s">
         <v>177</v>
       </c>
       <c r="G123" s="18" t="s">
@@ -3775,32 +3800,32 @@
       <c r="H123" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I123" s="55" t="s">
+      <c r="I123" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C124" s="15"/>
-      <c r="D124" s="85"/>
-      <c r="E124" s="88"/>
-      <c r="F124" s="83"/>
+      <c r="D124" s="61"/>
+      <c r="E124" s="63"/>
+      <c r="F124" s="65"/>
       <c r="G124" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H124" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I124" s="57"/>
-    </row>
-    <row r="125" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I124" s="67"/>
+    </row>
+    <row r="125" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C125" s="13"/>
-      <c r="D125" s="84" t="s">
+      <c r="D125" s="60" t="s">
         <v>198</v>
       </c>
-      <c r="E125" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F125" s="81" t="s">
+      <c r="E125" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F125" s="64" t="s">
         <v>199</v>
       </c>
       <c r="G125" s="18" t="s">
@@ -3809,48 +3834,109 @@
       <c r="H125" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I125" s="55" t="s">
+      <c r="I125" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C126" s="15"/>
-      <c r="D126" s="85"/>
-      <c r="E126" s="88"/>
-      <c r="F126" s="83"/>
+      <c r="D126" s="61"/>
+      <c r="E126" s="63"/>
+      <c r="F126" s="65"/>
       <c r="G126" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H126" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I126" s="57"/>
+      <c r="I126" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="143">
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="E125:E126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="I125:I126"/>
-    <mergeCell ref="D88:D90"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="E91:E93"/>
-    <mergeCell ref="F91:F93"/>
-    <mergeCell ref="C86:C96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="I82:I84"/>
-    <mergeCell ref="I79:I81"/>
-    <mergeCell ref="E82:E84"/>
-    <mergeCell ref="D85:D87"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="E79:E81"/>
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="D82:D84"/>
-    <mergeCell ref="I91:I93"/>
+    <mergeCell ref="I123:I124"/>
+    <mergeCell ref="I85:I87"/>
+    <mergeCell ref="I97:I99"/>
+    <mergeCell ref="I100:I103"/>
+    <mergeCell ref="I104:I107"/>
+    <mergeCell ref="I108:I111"/>
+    <mergeCell ref="I88:I90"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="I75:I78"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="I112:I114"/>
+    <mergeCell ref="I115:I116"/>
+    <mergeCell ref="I117:I118"/>
+    <mergeCell ref="I119:I122"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="F119:F122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="E119:E122"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="E117:E118"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="F108:F111"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="F112:F114"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="F115:F116"/>
+    <mergeCell ref="E108:E111"/>
+    <mergeCell ref="E112:E114"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="F117:F118"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="D119:D122"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="D61:D64"/>
     <mergeCell ref="C70:C74"/>
     <mergeCell ref="D71:D74"/>
     <mergeCell ref="E71:E74"/>
@@ -3874,18 +3960,31 @@
     <mergeCell ref="E46:E48"/>
     <mergeCell ref="D49:D51"/>
     <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="F65:F70"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="I65:I70"/>
+    <mergeCell ref="I82:I84"/>
+    <mergeCell ref="I79:I81"/>
+    <mergeCell ref="E82:E84"/>
+    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="E79:E81"/>
+    <mergeCell ref="F79:F81"/>
+    <mergeCell ref="F82:F84"/>
+    <mergeCell ref="D82:D84"/>
     <mergeCell ref="F85:F87"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="I125:I126"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="E91:E93"/>
+    <mergeCell ref="F91:F93"/>
+    <mergeCell ref="C86:C96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="I91:I93"/>
     <mergeCell ref="E104:E107"/>
     <mergeCell ref="E100:E103"/>
     <mergeCell ref="E97:E99"/>
@@ -3897,80 +3996,6 @@
     <mergeCell ref="D97:D99"/>
     <mergeCell ref="F88:F90"/>
     <mergeCell ref="E88:E90"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="D61:D64"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="F119:F122"/>
-    <mergeCell ref="D123:D124"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="E119:E122"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="E117:E118"/>
-    <mergeCell ref="D108:D111"/>
-    <mergeCell ref="F108:F111"/>
-    <mergeCell ref="D112:D114"/>
-    <mergeCell ref="F112:F114"/>
-    <mergeCell ref="D115:D116"/>
-    <mergeCell ref="F115:F116"/>
-    <mergeCell ref="E108:E111"/>
-    <mergeCell ref="E112:E114"/>
-    <mergeCell ref="E115:E116"/>
-    <mergeCell ref="F117:F118"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="D119:D122"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="I65:I70"/>
-    <mergeCell ref="I75:I78"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I60"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="I112:I114"/>
-    <mergeCell ref="I115:I116"/>
-    <mergeCell ref="I117:I118"/>
-    <mergeCell ref="I119:I122"/>
-    <mergeCell ref="I123:I124"/>
-    <mergeCell ref="I85:I87"/>
-    <mergeCell ref="I97:I99"/>
-    <mergeCell ref="I100:I103"/>
-    <mergeCell ref="I104:I107"/>
-    <mergeCell ref="I108:I111"/>
-    <mergeCell ref="I88:I90"/>
-    <mergeCell ref="I94:I96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Añadido y terminados gets de withdraws en el excel
</commit_message>
<xml_diff>
--- a/.readmeFiles/Endpoints.xlsx
+++ b/.readmeFiles/Endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/anfrodri_emeal_nttdata_com/Documents/Escritorio/Git backend/back-end-framework/.readmeFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/dceballr_emeal_nttdata_com/Documents/Escritorio/Backend/Repositorio/back-end-framework/.readmeFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05E72A7F-B62A-4117-8EC3-154EB610D5C6}"/>
+  <xr:revisionPtr revIDLastSave="415" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB7AC51B-3141-4470-B534-CE7958E2996E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="206">
   <si>
     <t>HTTP Method</t>
   </si>
@@ -645,6 +645,15 @@
   </si>
   <si>
     <t>"Withdraw made successfully"</t>
+  </si>
+  <si>
+    <t>"Card not found"</t>
+  </si>
+  <si>
+    <t>"Forbidden: Account does not belong to the authenticated customer"</t>
+  </si>
+  <si>
+    <t>"Account not found"</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1170,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1324,6 +1333,99 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="46" fontId="2" fillId="8" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -1333,20 +1435,134 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1357,15 +1573,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1381,203 +1588,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="2" fillId="8" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1930,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA3F6E-09E5-46A7-9DF8-4B95ED8D48E7}">
   <dimension ref="B2:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2071,13 +2083,13 @@
     </row>
     <row r="9" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="5"/>
-      <c r="D9" s="127" t="s">
+      <c r="D9" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="128" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="127" t="s">
+      <c r="E9" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="72" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -2086,45 +2098,45 @@
       <c r="H9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="133" t="s">
+      <c r="I9" s="70" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="5"/>
-      <c r="D10" s="127"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="127"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="72"/>
       <c r="G10" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="133"/>
+      <c r="I10" s="70"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="5"/>
-      <c r="D11" s="127"/>
-      <c r="E11" s="128"/>
-      <c r="F11" s="127"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="72"/>
       <c r="G11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="133"/>
+      <c r="I11" s="70"/>
     </row>
     <row r="12" spans="2:9" ht="28.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="5"/>
-      <c r="D12" s="127" t="s">
+      <c r="D12" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="128" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="127" t="s">
+      <c r="E12" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="72" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="38" t="s">
@@ -2133,35 +2145,35 @@
       <c r="H12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="133" t="s">
+      <c r="I12" s="70" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="5"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="127"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="72"/>
       <c r="G13" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="133"/>
+      <c r="I13" s="70"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="5"/>
-      <c r="D14" s="127"/>
-      <c r="E14" s="128"/>
-      <c r="F14" s="127"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="72"/>
       <c r="G14" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="133"/>
+      <c r="I14" s="70"/>
     </row>
     <row r="15" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="5"/>
@@ -2260,13 +2272,13 @@
     </row>
     <row r="20" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
-      <c r="D20" s="127" t="s">
+      <c r="D20" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="128" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="127" t="s">
+      <c r="E20" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="72" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="39" t="s">
@@ -2275,58 +2287,58 @@
       <c r="H20" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="133" t="s">
+      <c r="I20" s="70" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="128"/>
-      <c r="F21" s="127"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="97"/>
+      <c r="F21" s="72"/>
       <c r="G21" s="39" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="133"/>
+      <c r="I21" s="70"/>
     </row>
     <row r="22" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
-      <c r="D22" s="127"/>
-      <c r="E22" s="128"/>
-      <c r="F22" s="127"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="72"/>
       <c r="G22" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="133"/>
+      <c r="I22" s="70"/>
     </row>
     <row r="23" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C23" s="5"/>
-      <c r="D23" s="127"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="127"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="72"/>
       <c r="G23" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H23" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="133"/>
+      <c r="I23" s="70"/>
     </row>
     <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="5"/>
-      <c r="D24" s="127" t="s">
+      <c r="D24" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="128" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="127" t="s">
+      <c r="E24" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="72" t="s">
         <v>57</v>
       </c>
       <c r="G24" s="38" t="s">
@@ -2335,45 +2347,45 @@
       <c r="H24" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="133" t="s">
+      <c r="I24" s="70" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="5"/>
-      <c r="D25" s="127"/>
-      <c r="E25" s="128"/>
-      <c r="F25" s="127"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="72"/>
       <c r="G25" s="42" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="I25" s="133"/>
+      <c r="I25" s="70"/>
     </row>
     <row r="26" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C26" s="5"/>
-      <c r="D26" s="127"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="127"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="72"/>
       <c r="G26" s="42" t="s">
         <v>53</v>
       </c>
       <c r="H26" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="133"/>
+      <c r="I26" s="70"/>
     </row>
     <row r="27" spans="3:9" ht="58.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C27" s="5"/>
-      <c r="D27" s="127" t="s">
+      <c r="D27" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="105" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="132" t="s">
+      <c r="E27" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="74" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="38" t="s">
@@ -2382,84 +2394,84 @@
       <c r="H27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="133" t="s">
+      <c r="I27" s="70" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="5"/>
-      <c r="D28" s="127"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="132"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="74"/>
       <c r="G28" s="42" t="s">
         <v>63</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="133"/>
+      <c r="I28" s="70"/>
     </row>
     <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="5"/>
-      <c r="D29" s="129" t="s">
+      <c r="D29" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="E29" s="105" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="108" t="s">
+      <c r="E29" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="136" t="s">
+      <c r="G29" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="138" t="s">
+      <c r="H29" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="111" t="s">
+      <c r="I29" s="85" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="3:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="5"/>
-      <c r="D30" s="130"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="109"/>
-      <c r="G30" s="137"/>
-      <c r="H30" s="138"/>
-      <c r="I30" s="112"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="102"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="86"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C31" s="5"/>
-      <c r="D31" s="130"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="109"/>
-      <c r="G31" s="139" t="s">
+      <c r="D31" s="99"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="141" t="s">
+      <c r="H31" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="I31" s="112"/>
+      <c r="I31" s="86"/>
     </row>
     <row r="32" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="5"/>
-      <c r="D32" s="131"/>
-      <c r="E32" s="107"/>
-      <c r="F32" s="110"/>
-      <c r="G32" s="140"/>
-      <c r="H32" s="142"/>
-      <c r="I32" s="113"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="87"/>
     </row>
     <row r="33" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="5"/>
-      <c r="D33" s="132" t="s">
+      <c r="D33" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="128" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="132" t="s">
+      <c r="E33" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="74" t="s">
         <v>68</v>
       </c>
       <c r="G33" s="54" t="s">
@@ -2468,181 +2480,201 @@
       <c r="H33" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="133" t="s">
+      <c r="I33" s="70" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C34" s="5"/>
-      <c r="D34" s="132"/>
-      <c r="E34" s="128"/>
-      <c r="F34" s="132"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="74"/>
       <c r="G34" s="47" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I34" s="133"/>
+      <c r="I34" s="70"/>
     </row>
     <row r="35" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C35" s="5"/>
-      <c r="D35" s="132"/>
-      <c r="E35" s="128"/>
-      <c r="F35" s="132"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="97"/>
+      <c r="F35" s="74"/>
       <c r="G35" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H35" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="133"/>
+      <c r="I35" s="70"/>
     </row>
     <row r="36" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C36" s="5"/>
-      <c r="D36" s="132"/>
-      <c r="E36" s="128"/>
-      <c r="F36" s="132"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="97"/>
+      <c r="F36" s="74"/>
       <c r="G36" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H36" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I36" s="133"/>
+      <c r="I36" s="70"/>
     </row>
     <row r="37" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C37" s="5"/>
-      <c r="D37" s="102" t="s">
+      <c r="D37" s="127" t="s">
         <v>182</v>
       </c>
-      <c r="E37" s="105" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="108" t="s">
+      <c r="E37" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="75" t="s">
         <v>183</v>
       </c>
       <c r="G37" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H37" s="57" t="s">
+      <c r="H37" s="145" t="s">
         <v>185</v>
       </c>
-      <c r="I37" s="111" t="s">
+      <c r="I37" s="85" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C38" s="5"/>
-      <c r="D38" s="103"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="109"/>
+      <c r="D38" s="128"/>
+      <c r="E38" s="102"/>
+      <c r="F38" s="76"/>
       <c r="G38" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="H38" s="55"/>
-      <c r="I38" s="112"/>
+      <c r="H38" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="I38" s="86"/>
     </row>
     <row r="39" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="114"/>
-      <c r="D39" s="104"/>
-      <c r="E39" s="107"/>
-      <c r="F39" s="110"/>
+      <c r="C39" s="130"/>
+      <c r="D39" s="129"/>
+      <c r="E39" s="103"/>
+      <c r="F39" s="77"/>
       <c r="G39" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="H39" s="55"/>
-      <c r="I39" s="113"/>
+      <c r="H39" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39" s="87"/>
     </row>
     <row r="40" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="114"/>
-      <c r="D40" s="102" t="s">
+      <c r="C40" s="130"/>
+      <c r="D40" s="127" t="s">
         <v>186</v>
       </c>
-      <c r="E40" s="105" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="108" t="s">
+      <c r="E40" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="75" t="s">
         <v>187</v>
       </c>
       <c r="G40" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H40" s="57" t="s">
+      <c r="H40" s="145" t="s">
         <v>185</v>
       </c>
-      <c r="I40" s="111" t="s">
+      <c r="I40" s="85" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="41" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C41" s="114"/>
-      <c r="D41" s="103"/>
-      <c r="E41" s="106"/>
-      <c r="F41" s="109"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="112"/>
+      <c r="C41" s="130"/>
+      <c r="D41" s="128"/>
+      <c r="E41" s="102"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="H41" s="55" t="s">
+        <v>200</v>
+      </c>
+      <c r="I41" s="86"/>
     </row>
     <row r="42" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C42" s="114"/>
-      <c r="D42" s="104"/>
-      <c r="E42" s="107"/>
-      <c r="F42" s="110"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="113"/>
+      <c r="C42" s="130"/>
+      <c r="D42" s="129"/>
+      <c r="E42" s="103"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="H42" s="55" t="s">
+        <v>203</v>
+      </c>
+      <c r="I42" s="87"/>
     </row>
     <row r="43" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C43" s="114"/>
-      <c r="D43" s="102" t="s">
+      <c r="C43" s="130"/>
+      <c r="D43" s="127" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="105" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="108" t="s">
+      <c r="E43" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="75" t="s">
         <v>189</v>
       </c>
       <c r="G43" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H43" s="57" t="s">
+      <c r="H43" s="145" t="s">
         <v>185</v>
       </c>
-      <c r="I43" s="111" t="s">
+      <c r="I43" s="85" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="44" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C44" s="114"/>
-      <c r="D44" s="103"/>
-      <c r="E44" s="106"/>
-      <c r="F44" s="109"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="112"/>
+      <c r="C44" s="130"/>
+      <c r="D44" s="128"/>
+      <c r="E44" s="102"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="H44" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="I44" s="86"/>
     </row>
     <row r="45" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C45" s="115"/>
-      <c r="D45" s="104"/>
-      <c r="E45" s="107"/>
-      <c r="F45" s="110"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="113"/>
+      <c r="C45" s="131"/>
+      <c r="D45" s="129"/>
+      <c r="E45" s="103"/>
+      <c r="F45" s="77"/>
+      <c r="G45" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="H45" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="I45" s="87"/>
     </row>
     <row r="46" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="116" t="s">
+      <c r="D46" s="132" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="117" t="s">
+      <c r="E46" s="133" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="135" t="s">
+      <c r="F46" s="73" t="s">
         <v>78</v>
       </c>
       <c r="G46" s="30" t="s">
@@ -2651,45 +2683,45 @@
       <c r="H46" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="134" t="s">
+      <c r="I46" s="71" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C47" s="16"/>
-      <c r="D47" s="116"/>
-      <c r="E47" s="117"/>
-      <c r="F47" s="135"/>
+      <c r="D47" s="132"/>
+      <c r="E47" s="133"/>
+      <c r="F47" s="73"/>
       <c r="G47" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="I47" s="134"/>
+      <c r="I47" s="71"/>
     </row>
     <row r="48" spans="3:9" ht="31.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C48" s="7"/>
-      <c r="D48" s="116"/>
-      <c r="E48" s="117"/>
-      <c r="F48" s="135"/>
+      <c r="D48" s="132"/>
+      <c r="E48" s="133"/>
+      <c r="F48" s="73"/>
       <c r="G48" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H48" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="134"/>
+      <c r="I48" s="71"/>
     </row>
     <row r="49" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C49" s="7"/>
-      <c r="D49" s="118" t="s">
+      <c r="D49" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="93" t="s">
+      <c r="E49" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="96" t="s">
+      <c r="F49" s="110" t="s">
         <v>85</v>
       </c>
       <c r="G49" s="30" t="s">
@@ -2698,45 +2730,45 @@
       <c r="H49" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I49" s="99" t="s">
+      <c r="I49" s="67" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="50" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="7"/>
-      <c r="D50" s="119"/>
-      <c r="E50" s="94"/>
-      <c r="F50" s="97"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="105"/>
+      <c r="F50" s="111"/>
       <c r="G50" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H50" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="I50" s="100"/>
+      <c r="I50" s="68"/>
     </row>
     <row r="51" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C51" s="7"/>
       <c r="D51" s="120"/>
-      <c r="E51" s="95"/>
-      <c r="F51" s="98"/>
+      <c r="E51" s="106"/>
+      <c r="F51" s="112"/>
       <c r="G51" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H51" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I51" s="101"/>
+      <c r="I51" s="69"/>
     </row>
     <row r="52" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C52" s="7"/>
-      <c r="D52" s="118" t="s">
+      <c r="D52" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="96" t="s">
+      <c r="E52" s="104" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="110" t="s">
         <v>91</v>
       </c>
       <c r="G52" s="30" t="s">
@@ -2745,22 +2777,22 @@
       <c r="H52" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="99" t="s">
+      <c r="I52" s="67" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C53" s="7"/>
       <c r="D53" s="120"/>
-      <c r="E53" s="95"/>
-      <c r="F53" s="98"/>
+      <c r="E53" s="106"/>
+      <c r="F53" s="112"/>
       <c r="G53" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H53" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="I53" s="101"/>
+      <c r="I53" s="69"/>
     </row>
     <row r="54" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C54" s="7"/>
@@ -2807,13 +2839,13 @@
     </row>
     <row r="57" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C57" s="7"/>
-      <c r="D57" s="118" t="s">
+      <c r="D57" s="119" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="93" t="s">
+      <c r="E57" s="104" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="96" t="s">
+      <c r="F57" s="110" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="30" t="s">
@@ -2822,58 +2854,58 @@
       <c r="H57" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="I57" s="99" t="s">
+      <c r="I57" s="67" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="58" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C58" s="7"/>
-      <c r="D58" s="119"/>
-      <c r="E58" s="94"/>
-      <c r="F58" s="97"/>
+      <c r="D58" s="121"/>
+      <c r="E58" s="105"/>
+      <c r="F58" s="111"/>
       <c r="G58" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H58" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="I58" s="100"/>
+      <c r="I58" s="68"/>
     </row>
     <row r="59" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C59" s="7"/>
-      <c r="D59" s="119"/>
-      <c r="E59" s="94"/>
-      <c r="F59" s="97"/>
+      <c r="D59" s="121"/>
+      <c r="E59" s="105"/>
+      <c r="F59" s="111"/>
       <c r="G59" s="32" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I59" s="100"/>
+      <c r="I59" s="68"/>
     </row>
     <row r="60" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C60" s="7"/>
       <c r="D60" s="120"/>
-      <c r="E60" s="95"/>
-      <c r="F60" s="98"/>
+      <c r="E60" s="106"/>
+      <c r="F60" s="112"/>
       <c r="G60" s="32" t="s">
         <v>100</v>
       </c>
       <c r="H60" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I60" s="101"/>
+      <c r="I60" s="69"/>
     </row>
     <row r="61" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C61" s="7"/>
-      <c r="D61" s="118" t="s">
+      <c r="D61" s="119" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="93" t="s">
+      <c r="E61" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="F61" s="96" t="s">
+      <c r="F61" s="110" t="s">
         <v>104</v>
       </c>
       <c r="G61" s="30" t="s">
@@ -2882,58 +2914,58 @@
       <c r="H61" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="I61" s="99" t="s">
+      <c r="I61" s="67" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C62" s="7"/>
-      <c r="D62" s="119"/>
-      <c r="E62" s="94"/>
-      <c r="F62" s="97"/>
+      <c r="D62" s="121"/>
+      <c r="E62" s="105"/>
+      <c r="F62" s="111"/>
       <c r="G62" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H62" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I62" s="100"/>
+      <c r="I62" s="68"/>
     </row>
     <row r="63" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C63" s="7"/>
-      <c r="D63" s="119"/>
-      <c r="E63" s="94"/>
-      <c r="F63" s="97"/>
+      <c r="D63" s="121"/>
+      <c r="E63" s="105"/>
+      <c r="F63" s="111"/>
       <c r="G63" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H63" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="I63" s="100"/>
+      <c r="I63" s="68"/>
     </row>
     <row r="64" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C64" s="7"/>
       <c r="D64" s="120"/>
-      <c r="E64" s="95"/>
-      <c r="F64" s="98"/>
+      <c r="E64" s="106"/>
+      <c r="F64" s="112"/>
       <c r="G64" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H64" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I64" s="101"/>
+      <c r="I64" s="69"/>
     </row>
     <row r="65" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C65" s="7"/>
-      <c r="D65" s="118" t="s">
+      <c r="D65" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="E65" s="93" t="s">
+      <c r="E65" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="96" t="s">
+      <c r="F65" s="110" t="s">
         <v>111</v>
       </c>
       <c r="G65" s="30" t="s">
@@ -2942,84 +2974,84 @@
       <c r="H65" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="I65" s="99" t="s">
+      <c r="I65" s="67" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C66" s="7"/>
-      <c r="D66" s="119"/>
-      <c r="E66" s="94"/>
-      <c r="F66" s="97"/>
+      <c r="D66" s="121"/>
+      <c r="E66" s="105"/>
+      <c r="F66" s="111"/>
       <c r="G66" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H66" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I66" s="100"/>
+      <c r="I66" s="68"/>
     </row>
     <row r="67" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C67" s="7"/>
-      <c r="D67" s="119"/>
-      <c r="E67" s="94"/>
-      <c r="F67" s="97"/>
+      <c r="D67" s="121"/>
+      <c r="E67" s="105"/>
+      <c r="F67" s="111"/>
       <c r="G67" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H67" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="I67" s="100"/>
+      <c r="I67" s="68"/>
     </row>
     <row r="68" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C68" s="7"/>
-      <c r="D68" s="119"/>
-      <c r="E68" s="94"/>
-      <c r="F68" s="97"/>
+      <c r="D68" s="121"/>
+      <c r="E68" s="105"/>
+      <c r="F68" s="111"/>
       <c r="G68" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H68" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="I68" s="100"/>
+      <c r="I68" s="68"/>
     </row>
     <row r="69" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C69" s="7"/>
-      <c r="D69" s="119"/>
-      <c r="E69" s="94"/>
-      <c r="F69" s="97"/>
+      <c r="D69" s="121"/>
+      <c r="E69" s="105"/>
+      <c r="F69" s="111"/>
       <c r="G69" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H69" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I69" s="100"/>
+      <c r="I69" s="68"/>
     </row>
     <row r="70" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C70" s="88"/>
+      <c r="C70" s="122"/>
       <c r="D70" s="120"/>
-      <c r="E70" s="95"/>
-      <c r="F70" s="98"/>
+      <c r="E70" s="106"/>
+      <c r="F70" s="112"/>
       <c r="G70" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H70" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="I70" s="101"/>
+      <c r="I70" s="69"/>
     </row>
     <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C71" s="88"/>
-      <c r="D71" s="90" t="s">
+      <c r="C71" s="122"/>
+      <c r="D71" s="124" t="s">
         <v>190</v>
       </c>
-      <c r="E71" s="93" t="s">
+      <c r="E71" s="104" t="s">
         <v>191</v>
       </c>
-      <c r="F71" s="96" t="s">
+      <c r="F71" s="110" t="s">
         <v>192</v>
       </c>
       <c r="G71" s="30" t="s">
@@ -3028,60 +3060,60 @@
       <c r="H71" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="I71" s="99" t="s">
+      <c r="I71" s="67" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="72" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C72" s="88"/>
-      <c r="D72" s="91"/>
-      <c r="E72" s="94"/>
-      <c r="F72" s="97"/>
+      <c r="C72" s="122"/>
+      <c r="D72" s="125"/>
+      <c r="E72" s="105"/>
+      <c r="F72" s="111"/>
       <c r="G72" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H72" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="I72" s="100"/>
+      <c r="I72" s="68"/>
     </row>
     <row r="73" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C73" s="88"/>
-      <c r="D73" s="91"/>
-      <c r="E73" s="94"/>
-      <c r="F73" s="97"/>
+      <c r="C73" s="122"/>
+      <c r="D73" s="125"/>
+      <c r="E73" s="105"/>
+      <c r="F73" s="111"/>
       <c r="G73" s="32" t="s">
         <v>72</v>
       </c>
       <c r="H73" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="I73" s="100"/>
+      <c r="I73" s="68"/>
     </row>
     <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C74" s="89"/>
-      <c r="D74" s="92"/>
-      <c r="E74" s="95"/>
-      <c r="F74" s="98"/>
-      <c r="G74" s="144" t="s">
+      <c r="C74" s="123"/>
+      <c r="D74" s="126"/>
+      <c r="E74" s="106"/>
+      <c r="F74" s="112"/>
+      <c r="G74" s="60" t="s">
         <v>31</v>
       </c>
       <c r="H74" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="I74" s="101"/>
+      <c r="I74" s="69"/>
     </row>
     <row r="75" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D75" s="82" t="s">
+      <c r="D75" s="116" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="71" t="s">
+      <c r="E75" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="F75" s="121" t="s">
+      <c r="F75" s="107" t="s">
         <v>121</v>
       </c>
       <c r="G75" s="26" t="s">
@@ -3090,58 +3122,58 @@
       <c r="H75" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="I75" s="79" t="s">
+      <c r="I75" s="63" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="76" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C76" s="9"/>
-      <c r="D76" s="83"/>
-      <c r="E76" s="72"/>
-      <c r="F76" s="122"/>
+      <c r="D76" s="117"/>
+      <c r="E76" s="114"/>
+      <c r="F76" s="108"/>
       <c r="G76" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="I76" s="80"/>
+      <c r="I76" s="64"/>
     </row>
     <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C77" s="10"/>
-      <c r="D77" s="83"/>
-      <c r="E77" s="72"/>
-      <c r="F77" s="122"/>
+      <c r="D77" s="117"/>
+      <c r="E77" s="114"/>
+      <c r="F77" s="108"/>
       <c r="G77" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H77" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I77" s="80"/>
+      <c r="I77" s="64"/>
     </row>
     <row r="78" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C78" s="10"/>
-      <c r="D78" s="84"/>
-      <c r="E78" s="73"/>
-      <c r="F78" s="123"/>
+      <c r="D78" s="118"/>
+      <c r="E78" s="115"/>
+      <c r="F78" s="109"/>
       <c r="G78" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H78" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="I78" s="81"/>
+      <c r="I78" s="65"/>
     </row>
     <row r="79" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C79" s="10"/>
-      <c r="D79" s="82" t="s">
+      <c r="D79" s="116" t="s">
         <v>126</v>
       </c>
-      <c r="E79" s="71" t="s">
+      <c r="E79" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="85" t="s">
+      <c r="F79" s="134" t="s">
         <v>127</v>
       </c>
       <c r="G79" s="26" t="s">
@@ -3150,45 +3182,45 @@
       <c r="H79" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="I79" s="79" t="s">
+      <c r="I79" s="63" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="80" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C80" s="10"/>
-      <c r="D80" s="83"/>
-      <c r="E80" s="72"/>
-      <c r="F80" s="86"/>
+      <c r="D80" s="117"/>
+      <c r="E80" s="114"/>
+      <c r="F80" s="135"/>
       <c r="G80" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H80" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="I80" s="80"/>
+      <c r="I80" s="64"/>
     </row>
     <row r="81" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C81" s="10"/>
-      <c r="D81" s="84"/>
-      <c r="E81" s="73"/>
-      <c r="F81" s="87"/>
+      <c r="D81" s="118"/>
+      <c r="E81" s="115"/>
+      <c r="F81" s="136"/>
       <c r="G81" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H81" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I81" s="81"/>
+      <c r="I81" s="65"/>
     </row>
     <row r="82" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C82" s="10"/>
-      <c r="D82" s="82" t="s">
+      <c r="D82" s="116" t="s">
         <v>131</v>
       </c>
-      <c r="E82" s="71" t="s">
+      <c r="E82" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="F82" s="85" t="s">
+      <c r="F82" s="134" t="s">
         <v>132</v>
       </c>
       <c r="G82" s="26" t="s">
@@ -3197,45 +3229,45 @@
       <c r="H82" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="I82" s="79" t="s">
+      <c r="I82" s="63" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="83" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C83" s="10"/>
-      <c r="D83" s="83"/>
-      <c r="E83" s="72"/>
-      <c r="F83" s="86"/>
+      <c r="D83" s="117"/>
+      <c r="E83" s="114"/>
+      <c r="F83" s="135"/>
       <c r="G83" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H83" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="I83" s="80"/>
+      <c r="I83" s="64"/>
     </row>
     <row r="84" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C84" s="10"/>
-      <c r="D84" s="84"/>
-      <c r="E84" s="73"/>
-      <c r="F84" s="87"/>
+      <c r="D84" s="118"/>
+      <c r="E84" s="115"/>
+      <c r="F84" s="136"/>
       <c r="G84" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H84" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I84" s="81"/>
+      <c r="I84" s="65"/>
     </row>
     <row r="85" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C85" s="10"/>
-      <c r="D85" s="82" t="s">
+      <c r="D85" s="116" t="s">
         <v>135</v>
       </c>
-      <c r="E85" s="71" t="s">
+      <c r="E85" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="F85" s="85" t="s">
+      <c r="F85" s="134" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="26" t="s">
@@ -3244,152 +3276,152 @@
       <c r="H85" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="I85" s="79" t="s">
+      <c r="I85" s="63" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="86" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C86" s="77"/>
-      <c r="D86" s="83"/>
-      <c r="E86" s="72"/>
-      <c r="F86" s="86"/>
+      <c r="C86" s="143"/>
+      <c r="D86" s="117"/>
+      <c r="E86" s="114"/>
+      <c r="F86" s="135"/>
       <c r="G86" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H86" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="I86" s="80"/>
+      <c r="I86" s="64"/>
     </row>
     <row r="87" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C87" s="77"/>
-      <c r="D87" s="84"/>
-      <c r="E87" s="73"/>
-      <c r="F87" s="87"/>
+      <c r="C87" s="143"/>
+      <c r="D87" s="118"/>
+      <c r="E87" s="115"/>
+      <c r="F87" s="136"/>
       <c r="G87" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H87" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I87" s="81"/>
+      <c r="I87" s="65"/>
     </row>
     <row r="88" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C88" s="77"/>
-      <c r="D88" s="68" t="s">
+      <c r="C88" s="143"/>
+      <c r="D88" s="137" t="s">
         <v>193</v>
       </c>
-      <c r="E88" s="71" t="s">
+      <c r="E88" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="F88" s="74" t="s">
+      <c r="F88" s="140" t="s">
         <v>196</v>
       </c>
       <c r="G88" s="26"/>
       <c r="H88" s="59"/>
-      <c r="I88" s="79" t="s">
+      <c r="I88" s="63" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="89" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C89" s="77"/>
-      <c r="D89" s="69"/>
-      <c r="E89" s="72"/>
-      <c r="F89" s="75"/>
+      <c r="C89" s="143"/>
+      <c r="D89" s="138"/>
+      <c r="E89" s="114"/>
+      <c r="F89" s="141"/>
       <c r="G89" s="28"/>
       <c r="H89" s="56"/>
-      <c r="I89" s="80"/>
+      <c r="I89" s="64"/>
     </row>
     <row r="90" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C90" s="77"/>
-      <c r="D90" s="70"/>
-      <c r="E90" s="73"/>
-      <c r="F90" s="76"/>
+      <c r="C90" s="143"/>
+      <c r="D90" s="139"/>
+      <c r="E90" s="115"/>
+      <c r="F90" s="142"/>
       <c r="G90" s="28"/>
       <c r="H90" s="56"/>
-      <c r="I90" s="81"/>
+      <c r="I90" s="65"/>
     </row>
     <row r="91" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C91" s="77"/>
-      <c r="D91" s="68" t="s">
+      <c r="C91" s="143"/>
+      <c r="D91" s="137" t="s">
         <v>194</v>
       </c>
-      <c r="E91" s="71" t="s">
+      <c r="E91" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="F91" s="74" t="s">
+      <c r="F91" s="140" t="s">
         <v>197</v>
       </c>
       <c r="G91" s="26"/>
       <c r="H91" s="59"/>
-      <c r="I91" s="79" t="s">
+      <c r="I91" s="63" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="92" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C92" s="77"/>
-      <c r="D92" s="69"/>
-      <c r="E92" s="72"/>
-      <c r="F92" s="75"/>
+      <c r="C92" s="143"/>
+      <c r="D92" s="138"/>
+      <c r="E92" s="114"/>
+      <c r="F92" s="141"/>
       <c r="G92" s="28"/>
       <c r="H92" s="56"/>
-      <c r="I92" s="80"/>
+      <c r="I92" s="64"/>
     </row>
     <row r="93" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C93" s="77"/>
-      <c r="D93" s="70"/>
-      <c r="E93" s="73"/>
-      <c r="F93" s="76"/>
+      <c r="C93" s="143"/>
+      <c r="D93" s="139"/>
+      <c r="E93" s="115"/>
+      <c r="F93" s="142"/>
       <c r="G93" s="28"/>
       <c r="H93" s="56"/>
-      <c r="I93" s="81"/>
+      <c r="I93" s="65"/>
     </row>
     <row r="94" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C94" s="77"/>
-      <c r="D94" s="68" t="s">
+      <c r="C94" s="143"/>
+      <c r="D94" s="137" t="s">
         <v>195</v>
       </c>
-      <c r="E94" s="71" t="s">
+      <c r="E94" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="F94" s="74" t="s">
+      <c r="F94" s="140" t="s">
         <v>197</v>
       </c>
       <c r="G94" s="26"/>
       <c r="H94" s="59"/>
-      <c r="I94" s="79" t="s">
+      <c r="I94" s="63" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="95" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C95" s="77"/>
-      <c r="D95" s="69"/>
-      <c r="E95" s="72"/>
-      <c r="F95" s="75"/>
+      <c r="C95" s="143"/>
+      <c r="D95" s="138"/>
+      <c r="E95" s="114"/>
+      <c r="F95" s="141"/>
       <c r="G95" s="28"/>
       <c r="H95" s="56"/>
-      <c r="I95" s="80"/>
+      <c r="I95" s="64"/>
     </row>
     <row r="96" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C96" s="78"/>
-      <c r="D96" s="70"/>
-      <c r="E96" s="73"/>
-      <c r="F96" s="76"/>
+      <c r="C96" s="144"/>
+      <c r="D96" s="139"/>
+      <c r="E96" s="115"/>
+      <c r="F96" s="142"/>
       <c r="G96" s="28"/>
       <c r="H96" s="56"/>
-      <c r="I96" s="81"/>
+      <c r="I96" s="65"/>
     </row>
     <row r="97" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C97" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D97" s="60" t="s">
+      <c r="D97" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="E97" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F97" s="64" t="s">
+      <c r="E97" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="88" t="s">
         <v>141</v>
       </c>
       <c r="G97" s="18" t="s">
@@ -3398,45 +3430,45 @@
       <c r="H97" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="I97" s="66" t="s">
+      <c r="I97" s="61" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="98" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C98" s="12"/>
-      <c r="D98" s="126"/>
-      <c r="E98" s="124"/>
-      <c r="F98" s="125"/>
+      <c r="D98" s="96"/>
+      <c r="E98" s="94"/>
+      <c r="F98" s="89"/>
       <c r="G98" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H98" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="I98" s="143"/>
+      <c r="I98" s="66"/>
     </row>
     <row r="99" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C99" s="13"/>
-      <c r="D99" s="61"/>
-      <c r="E99" s="63"/>
-      <c r="F99" s="65"/>
+      <c r="D99" s="92"/>
+      <c r="E99" s="95"/>
+      <c r="F99" s="90"/>
       <c r="G99" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H99" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="I99" s="67"/>
+      <c r="I99" s="62"/>
     </row>
     <row r="100" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C100" s="13"/>
-      <c r="D100" s="60" t="s">
+      <c r="D100" s="91" t="s">
         <v>146</v>
       </c>
-      <c r="E100" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="64" t="s">
+      <c r="E100" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="88" t="s">
         <v>147</v>
       </c>
       <c r="G100" s="18" t="s">
@@ -3445,58 +3477,58 @@
       <c r="H100" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="I100" s="66" t="s">
+      <c r="I100" s="61" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="101" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C101" s="13"/>
-      <c r="D101" s="126"/>
-      <c r="E101" s="124"/>
-      <c r="F101" s="125"/>
+      <c r="D101" s="96"/>
+      <c r="E101" s="94"/>
+      <c r="F101" s="89"/>
       <c r="G101" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H101" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I101" s="143"/>
+      <c r="I101" s="66"/>
     </row>
     <row r="102" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C102" s="13"/>
-      <c r="D102" s="126"/>
-      <c r="E102" s="124"/>
-      <c r="F102" s="125"/>
+      <c r="D102" s="96"/>
+      <c r="E102" s="94"/>
+      <c r="F102" s="89"/>
       <c r="G102" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H102" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I102" s="143"/>
+      <c r="I102" s="66"/>
     </row>
     <row r="103" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C103" s="13"/>
-      <c r="D103" s="61"/>
-      <c r="E103" s="63"/>
-      <c r="F103" s="65"/>
+      <c r="D103" s="92"/>
+      <c r="E103" s="95"/>
+      <c r="F103" s="90"/>
       <c r="G103" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H103" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="I103" s="67"/>
+      <c r="I103" s="62"/>
     </row>
     <row r="104" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C104" s="13"/>
-      <c r="D104" s="60" t="s">
+      <c r="D104" s="91" t="s">
         <v>152</v>
       </c>
-      <c r="E104" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F104" s="64" t="s">
+      <c r="E104" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" s="88" t="s">
         <v>153</v>
       </c>
       <c r="G104" s="18" t="s">
@@ -3505,58 +3537,58 @@
       <c r="H104" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="I104" s="66" t="s">
+      <c r="I104" s="61" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="105" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C105" s="13"/>
-      <c r="D105" s="126"/>
-      <c r="E105" s="124"/>
-      <c r="F105" s="125"/>
+      <c r="D105" s="96"/>
+      <c r="E105" s="94"/>
+      <c r="F105" s="89"/>
       <c r="G105" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H105" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="I105" s="143"/>
+      <c r="I105" s="66"/>
     </row>
     <row r="106" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C106" s="13"/>
-      <c r="D106" s="126"/>
-      <c r="E106" s="124"/>
-      <c r="F106" s="125"/>
+      <c r="D106" s="96"/>
+      <c r="E106" s="94"/>
+      <c r="F106" s="89"/>
       <c r="G106" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H106" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="I106" s="143"/>
+      <c r="I106" s="66"/>
     </row>
     <row r="107" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C107" s="13"/>
-      <c r="D107" s="61"/>
-      <c r="E107" s="63"/>
-      <c r="F107" s="65"/>
+      <c r="D107" s="92"/>
+      <c r="E107" s="95"/>
+      <c r="F107" s="90"/>
       <c r="G107" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H107" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="I107" s="67"/>
+      <c r="I107" s="62"/>
     </row>
     <row r="108" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C108" s="13"/>
-      <c r="D108" s="60" t="s">
+      <c r="D108" s="91" t="s">
         <v>158</v>
       </c>
-      <c r="E108" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F108" s="64" t="s">
+      <c r="E108" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108" s="88" t="s">
         <v>159</v>
       </c>
       <c r="G108" s="18" t="s">
@@ -3565,58 +3597,58 @@
       <c r="H108" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="I108" s="66" t="s">
+      <c r="I108" s="61" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="109" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C109" s="13"/>
-      <c r="D109" s="126"/>
-      <c r="E109" s="124"/>
-      <c r="F109" s="125"/>
+      <c r="D109" s="96"/>
+      <c r="E109" s="94"/>
+      <c r="F109" s="89"/>
       <c r="G109" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H109" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I109" s="143"/>
+      <c r="I109" s="66"/>
     </row>
     <row r="110" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C110" s="13"/>
-      <c r="D110" s="126"/>
-      <c r="E110" s="124"/>
-      <c r="F110" s="125"/>
+      <c r="D110" s="96"/>
+      <c r="E110" s="94"/>
+      <c r="F110" s="89"/>
       <c r="G110" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H110" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I110" s="143"/>
+      <c r="I110" s="66"/>
     </row>
     <row r="111" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C111" s="13"/>
-      <c r="D111" s="61"/>
-      <c r="E111" s="63"/>
-      <c r="F111" s="65"/>
+      <c r="D111" s="92"/>
+      <c r="E111" s="95"/>
+      <c r="F111" s="90"/>
       <c r="G111" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H111" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="I111" s="67"/>
+      <c r="I111" s="62"/>
     </row>
     <row r="112" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C112" s="13"/>
-      <c r="D112" s="60" t="s">
+      <c r="D112" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="E112" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F112" s="64" t="s">
+      <c r="E112" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F112" s="88" t="s">
         <v>162</v>
       </c>
       <c r="G112" s="18" t="s">
@@ -3625,45 +3657,45 @@
       <c r="H112" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="I112" s="66" t="s">
+      <c r="I112" s="61" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="113" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C113" s="13"/>
-      <c r="D113" s="126"/>
-      <c r="E113" s="124"/>
-      <c r="F113" s="125"/>
+      <c r="D113" s="96"/>
+      <c r="E113" s="94"/>
+      <c r="F113" s="89"/>
       <c r="G113" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H113" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="I113" s="143"/>
+      <c r="I113" s="66"/>
     </row>
     <row r="114" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C114" s="14"/>
-      <c r="D114" s="61"/>
-      <c r="E114" s="63"/>
-      <c r="F114" s="65"/>
+      <c r="D114" s="92"/>
+      <c r="E114" s="95"/>
+      <c r="F114" s="90"/>
       <c r="G114" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H114" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I114" s="67"/>
+      <c r="I114" s="62"/>
     </row>
     <row r="115" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C115" s="14"/>
-      <c r="D115" s="60" t="s">
+      <c r="D115" s="91" t="s">
         <v>165</v>
       </c>
-      <c r="E115" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F115" s="64" t="s">
+      <c r="E115" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F115" s="88" t="s">
         <v>166</v>
       </c>
       <c r="G115" s="18" t="s">
@@ -3672,32 +3704,32 @@
       <c r="H115" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="I115" s="66" t="s">
+      <c r="I115" s="61" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="116" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C116" s="13"/>
-      <c r="D116" s="61"/>
-      <c r="E116" s="63"/>
-      <c r="F116" s="65"/>
+      <c r="D116" s="92"/>
+      <c r="E116" s="95"/>
+      <c r="F116" s="90"/>
       <c r="G116" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H116" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="I116" s="67"/>
+      <c r="I116" s="62"/>
     </row>
     <row r="117" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C117" s="13"/>
-      <c r="D117" s="60" t="s">
+      <c r="D117" s="91" t="s">
         <v>169</v>
       </c>
-      <c r="E117" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F117" s="64" t="s">
+      <c r="E117" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F117" s="88" t="s">
         <v>170</v>
       </c>
       <c r="G117" s="18" t="s">
@@ -3706,32 +3738,32 @@
       <c r="H117" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="I117" s="66" t="s">
+      <c r="I117" s="61" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="118" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C118" s="13"/>
-      <c r="D118" s="61"/>
-      <c r="E118" s="63"/>
-      <c r="F118" s="65"/>
+      <c r="D118" s="92"/>
+      <c r="E118" s="95"/>
+      <c r="F118" s="90"/>
       <c r="G118" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H118" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="I118" s="67"/>
+      <c r="I118" s="62"/>
     </row>
     <row r="119" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C119" s="13"/>
-      <c r="D119" s="60" t="s">
+      <c r="D119" s="91" t="s">
         <v>173</v>
       </c>
-      <c r="E119" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F119" s="64" t="s">
+      <c r="E119" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F119" s="88" t="s">
         <v>174</v>
       </c>
       <c r="G119" s="18" t="s">
@@ -3740,58 +3772,58 @@
       <c r="H119" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="I119" s="66" t="s">
+      <c r="I119" s="61" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="120" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C120" s="13"/>
-      <c r="D120" s="126"/>
-      <c r="E120" s="124"/>
-      <c r="F120" s="125"/>
+      <c r="D120" s="96"/>
+      <c r="E120" s="94"/>
+      <c r="F120" s="89"/>
       <c r="G120" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H120" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="I120" s="143"/>
+      <c r="I120" s="66"/>
     </row>
     <row r="121" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C121" s="13"/>
-      <c r="D121" s="126"/>
-      <c r="E121" s="124"/>
-      <c r="F121" s="125"/>
+      <c r="D121" s="96"/>
+      <c r="E121" s="94"/>
+      <c r="F121" s="89"/>
       <c r="G121" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H121" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I121" s="143"/>
+      <c r="I121" s="66"/>
     </row>
     <row r="122" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C122" s="13"/>
-      <c r="D122" s="61"/>
-      <c r="E122" s="63"/>
-      <c r="F122" s="65"/>
+      <c r="D122" s="92"/>
+      <c r="E122" s="95"/>
+      <c r="F122" s="90"/>
       <c r="G122" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H122" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I122" s="67"/>
+      <c r="I122" s="62"/>
     </row>
     <row r="123" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C123" s="13"/>
-      <c r="D123" s="60" t="s">
+      <c r="D123" s="91" t="s">
         <v>176</v>
       </c>
-      <c r="E123" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F123" s="64" t="s">
+      <c r="E123" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F123" s="88" t="s">
         <v>177</v>
       </c>
       <c r="G123" s="18" t="s">
@@ -3800,32 +3832,32 @@
       <c r="H123" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I123" s="66" t="s">
+      <c r="I123" s="61" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="124" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C124" s="15"/>
-      <c r="D124" s="61"/>
-      <c r="E124" s="63"/>
-      <c r="F124" s="65"/>
+      <c r="D124" s="92"/>
+      <c r="E124" s="95"/>
+      <c r="F124" s="90"/>
       <c r="G124" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H124" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I124" s="67"/>
+      <c r="I124" s="62"/>
     </row>
     <row r="125" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C125" s="13"/>
-      <c r="D125" s="60" t="s">
+      <c r="D125" s="91" t="s">
         <v>198</v>
       </c>
-      <c r="E125" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F125" s="64" t="s">
+      <c r="E125" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F125" s="88" t="s">
         <v>199</v>
       </c>
       <c r="G125" s="18" t="s">
@@ -3834,109 +3866,58 @@
       <c r="H125" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I125" s="66" t="s">
+      <c r="I125" s="61" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="126" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C126" s="15"/>
-      <c r="D126" s="61"/>
-      <c r="E126" s="63"/>
-      <c r="F126" s="65"/>
+      <c r="D126" s="92"/>
+      <c r="E126" s="95"/>
+      <c r="F126" s="90"/>
       <c r="G126" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H126" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I126" s="67"/>
+      <c r="I126" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="143">
-    <mergeCell ref="I123:I124"/>
-    <mergeCell ref="I85:I87"/>
-    <mergeCell ref="I97:I99"/>
-    <mergeCell ref="I100:I103"/>
-    <mergeCell ref="I104:I107"/>
-    <mergeCell ref="I108:I111"/>
-    <mergeCell ref="I88:I90"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="I75:I78"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I60"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="I112:I114"/>
-    <mergeCell ref="I115:I116"/>
-    <mergeCell ref="I117:I118"/>
-    <mergeCell ref="I119:I122"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="F119:F122"/>
-    <mergeCell ref="D123:D124"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="E119:E122"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="E117:E118"/>
-    <mergeCell ref="D108:D111"/>
-    <mergeCell ref="F108:F111"/>
-    <mergeCell ref="D112:D114"/>
-    <mergeCell ref="F112:F114"/>
-    <mergeCell ref="D115:D116"/>
-    <mergeCell ref="F115:F116"/>
-    <mergeCell ref="E108:E111"/>
-    <mergeCell ref="E112:E114"/>
-    <mergeCell ref="E115:E116"/>
-    <mergeCell ref="F117:F118"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="D119:D122"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="F65:F70"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="I125:I126"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="E91:E93"/>
+    <mergeCell ref="F91:F93"/>
+    <mergeCell ref="C86:C96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="I91:I93"/>
+    <mergeCell ref="E104:E107"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="E97:E99"/>
+    <mergeCell ref="F104:F107"/>
+    <mergeCell ref="D104:D107"/>
+    <mergeCell ref="F100:F103"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="F97:F99"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E82:E84"/>
+    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="E79:E81"/>
+    <mergeCell ref="F79:F81"/>
+    <mergeCell ref="F82:F84"/>
+    <mergeCell ref="D82:D84"/>
+    <mergeCell ref="F85:F87"/>
     <mergeCell ref="C70:C74"/>
     <mergeCell ref="D71:D74"/>
     <mergeCell ref="E71:E74"/>
@@ -3961,41 +3942,92 @@
     <mergeCell ref="D49:D51"/>
     <mergeCell ref="E49:E51"/>
     <mergeCell ref="I65:I70"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="F119:F122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="E119:E122"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="E117:E118"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="F108:F111"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="F112:F114"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="F115:F116"/>
+    <mergeCell ref="E108:E111"/>
+    <mergeCell ref="E112:E114"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="F117:F118"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="D119:D122"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="I112:I114"/>
+    <mergeCell ref="I115:I116"/>
+    <mergeCell ref="I117:I118"/>
+    <mergeCell ref="I119:I122"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="I46:I48"/>
     <mergeCell ref="I82:I84"/>
     <mergeCell ref="I79:I81"/>
-    <mergeCell ref="E82:E84"/>
-    <mergeCell ref="D85:D87"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="E79:E81"/>
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="D82:D84"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="E125:E126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="I125:I126"/>
-    <mergeCell ref="D88:D90"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="E91:E93"/>
-    <mergeCell ref="F91:F93"/>
-    <mergeCell ref="C86:C96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="I91:I93"/>
-    <mergeCell ref="E104:E107"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="E97:E99"/>
-    <mergeCell ref="F104:F107"/>
-    <mergeCell ref="D104:D107"/>
-    <mergeCell ref="F100:F103"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="F97:F99"/>
-    <mergeCell ref="D97:D99"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="I123:I124"/>
+    <mergeCell ref="I85:I87"/>
+    <mergeCell ref="I97:I99"/>
+    <mergeCell ref="I100:I103"/>
+    <mergeCell ref="I104:I107"/>
+    <mergeCell ref="I108:I111"/>
+    <mergeCell ref="I88:I90"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="I75:I78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
actualizacion en el excel de endpoints de los updates y cambios en el cardcontroller los tipos de status para que sea mas descriptivo el error
</commit_message>
<xml_diff>
--- a/.readmeFiles/Endpoints.xlsx
+++ b/.readmeFiles/Endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/dceballr_emeal_nttdata_com/Documents/Escritorio/Backend/Repositorio/back-end-framework/.readmeFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/anfrodri_emeal_nttdata_com/Documents/Escritorio/Git backend/back-end-framework/.readmeFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="415" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB7AC51B-3141-4470-B534-CE7958E2996E}"/>
+  <xr:revisionPtr revIDLastSave="436" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04A5F564-3AC0-4A37-A784-E5D06C4565C8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="217">
   <si>
     <t>HTTP Method</t>
   </si>
@@ -654,6 +654,39 @@
   </si>
   <si>
     <t>"Account not found"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">403: Forbidden </t>
+  </si>
+  <si>
+    <t>404: Bad Request</t>
+  </si>
+  <si>
+    <t>"Card does not belong to the user"</t>
+  </si>
+  <si>
+    <t>"There is no card with ID:" + cardId</t>
+  </si>
+  <si>
+    <t>"The block state has been updated successfully"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200: OK </t>
+  </si>
+  <si>
+    <t>400: Bad request</t>
+  </si>
+  <si>
+    <t>"The new daily limit has been updated successfully"</t>
+  </si>
+  <si>
+    <t>"The new daily limit must be greater than 0"</t>
+  </si>
+  <si>
+    <t>"The new monthly limit has been updated successfully"</t>
+  </si>
+  <si>
+    <t>"The new monthly limit must be greater than 0"</t>
   </si>
 </sst>
 </file>
@@ -1336,12 +1369,66 @@
     <xf numFmtId="46" fontId="2" fillId="8" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1351,7 +1438,64 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1363,29 +1507,95 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1408,187 +1618,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1621,6 +1654,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1942,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA3F6E-09E5-46A7-9DF8-4B95ED8D48E7}">
   <dimension ref="B2:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="C81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2083,13 +2120,13 @@
     </row>
     <row r="9" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="5"/>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="72" t="s">
+      <c r="E9" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="129" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -2098,45 +2135,45 @@
       <c r="H9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="70" t="s">
+      <c r="I9" s="135" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="5"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="72"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="129"/>
       <c r="G10" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="70"/>
+      <c r="I10" s="135"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="5"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="97"/>
-      <c r="F11" s="72"/>
+      <c r="D11" s="129"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="129"/>
       <c r="G11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="70"/>
+      <c r="I11" s="135"/>
     </row>
     <row r="12" spans="2:9" ht="28.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="5"/>
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="129" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="72" t="s">
+      <c r="E12" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="129" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="38" t="s">
@@ -2145,35 +2182,35 @@
       <c r="H12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="70" t="s">
+      <c r="I12" s="135" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="5"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="72"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="129"/>
       <c r="G13" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="70"/>
+      <c r="I13" s="135"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="5"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="72"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="129"/>
       <c r="G14" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="70"/>
+      <c r="I14" s="135"/>
     </row>
     <row r="15" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="5"/>
@@ -2272,13 +2309,13 @@
     </row>
     <row r="20" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
-      <c r="D20" s="72" t="s">
+      <c r="D20" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="72" t="s">
+      <c r="E20" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="129" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="39" t="s">
@@ -2287,58 +2324,58 @@
       <c r="H20" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="70" t="s">
+      <c r="I20" s="135" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="72"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="129"/>
       <c r="G21" s="39" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="70"/>
+      <c r="I21" s="135"/>
     </row>
     <row r="22" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="72"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="129"/>
       <c r="G22" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="70"/>
+      <c r="I22" s="135"/>
     </row>
     <row r="23" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C23" s="5"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="72"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="129"/>
       <c r="G23" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H23" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="70"/>
+      <c r="I23" s="135"/>
     </row>
     <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="5"/>
-      <c r="D24" s="72" t="s">
+      <c r="D24" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="72" t="s">
+      <c r="E24" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="129" t="s">
         <v>57</v>
       </c>
       <c r="G24" s="38" t="s">
@@ -2347,45 +2384,45 @@
       <c r="H24" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="70" t="s">
+      <c r="I24" s="135" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="5"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="72"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="129"/>
       <c r="G25" s="42" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="I25" s="70"/>
+      <c r="I25" s="135"/>
     </row>
     <row r="26" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C26" s="5"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="72"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="129"/>
       <c r="G26" s="42" t="s">
         <v>53</v>
       </c>
       <c r="H26" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="70"/>
+      <c r="I26" s="135"/>
     </row>
     <row r="27" spans="3:9" ht="58.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C27" s="5"/>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="74" t="s">
+      <c r="E27" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="134" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="38" t="s">
@@ -2394,84 +2431,84 @@
       <c r="H27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="70" t="s">
+      <c r="I27" s="135" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="5"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="103"/>
-      <c r="F28" s="74"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="134"/>
       <c r="G28" s="42" t="s">
         <v>63</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="70"/>
+      <c r="I28" s="135"/>
     </row>
     <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="5"/>
-      <c r="D29" s="98" t="s">
+      <c r="D29" s="131" t="s">
         <v>181</v>
       </c>
-      <c r="E29" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="75" t="s">
+      <c r="E29" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="78" t="s">
+      <c r="G29" s="137" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="80" t="s">
+      <c r="H29" s="139" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="85" t="s">
+      <c r="I29" s="116" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="3:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="5"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="102"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="86"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="111"/>
+      <c r="F30" s="114"/>
+      <c r="G30" s="138"/>
+      <c r="H30" s="139"/>
+      <c r="I30" s="117"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C31" s="5"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="102"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="81" t="s">
+      <c r="D31" s="132"/>
+      <c r="E31" s="111"/>
+      <c r="F31" s="114"/>
+      <c r="G31" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="83" t="s">
+      <c r="H31" s="142" t="s">
         <v>66</v>
       </c>
-      <c r="I31" s="86"/>
+      <c r="I31" s="117"/>
     </row>
     <row r="32" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="5"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="82"/>
-      <c r="H32" s="84"/>
-      <c r="I32" s="87"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="141"/>
+      <c r="H32" s="143"/>
+      <c r="I32" s="118"/>
     </row>
     <row r="33" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="5"/>
-      <c r="D33" s="74" t="s">
+      <c r="D33" s="134" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="74" t="s">
+      <c r="E33" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="134" t="s">
         <v>68</v>
       </c>
       <c r="G33" s="54" t="s">
@@ -2480,201 +2517,201 @@
       <c r="H33" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="70" t="s">
+      <c r="I33" s="135" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C34" s="5"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="97"/>
-      <c r="F34" s="74"/>
+      <c r="D34" s="134"/>
+      <c r="E34" s="130"/>
+      <c r="F34" s="134"/>
       <c r="G34" s="47" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I34" s="70"/>
+      <c r="I34" s="135"/>
     </row>
     <row r="35" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C35" s="5"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="74"/>
+      <c r="D35" s="134"/>
+      <c r="E35" s="130"/>
+      <c r="F35" s="134"/>
       <c r="G35" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H35" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="70"/>
+      <c r="I35" s="135"/>
     </row>
     <row r="36" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C36" s="5"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="97"/>
-      <c r="F36" s="74"/>
+      <c r="D36" s="134"/>
+      <c r="E36" s="130"/>
+      <c r="F36" s="134"/>
       <c r="G36" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H36" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I36" s="70"/>
+      <c r="I36" s="135"/>
     </row>
     <row r="37" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C37" s="5"/>
-      <c r="D37" s="127" t="s">
+      <c r="D37" s="107" t="s">
         <v>182</v>
       </c>
-      <c r="E37" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="75" t="s">
+      <c r="E37" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="113" t="s">
         <v>183</v>
       </c>
       <c r="G37" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H37" s="145" t="s">
+      <c r="H37" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="I37" s="85" t="s">
+      <c r="I37" s="116" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C38" s="5"/>
-      <c r="D38" s="128"/>
-      <c r="E38" s="102"/>
-      <c r="F38" s="76"/>
+      <c r="D38" s="108"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="114"/>
       <c r="G38" s="42" t="s">
         <v>70</v>
       </c>
       <c r="H38" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="86"/>
+      <c r="I38" s="117"/>
     </row>
     <row r="39" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="130"/>
-      <c r="D39" s="129"/>
-      <c r="E39" s="103"/>
-      <c r="F39" s="77"/>
+      <c r="C39" s="119"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="115"/>
       <c r="G39" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H39" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="I39" s="87"/>
+      <c r="I39" s="118"/>
     </row>
     <row r="40" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="130"/>
-      <c r="D40" s="127" t="s">
+      <c r="C40" s="119"/>
+      <c r="D40" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="E40" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="75" t="s">
+      <c r="E40" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="113" t="s">
         <v>187</v>
       </c>
       <c r="G40" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H40" s="145" t="s">
+      <c r="H40" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="I40" s="85" t="s">
+      <c r="I40" s="116" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="41" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C41" s="130"/>
-      <c r="D41" s="128"/>
-      <c r="E41" s="102"/>
-      <c r="F41" s="76"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="108"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="114"/>
       <c r="G41" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H41" s="55" t="s">
         <v>200</v>
       </c>
-      <c r="I41" s="86"/>
+      <c r="I41" s="117"/>
     </row>
     <row r="42" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C42" s="130"/>
-      <c r="D42" s="129"/>
-      <c r="E42" s="103"/>
-      <c r="F42" s="77"/>
+      <c r="C42" s="119"/>
+      <c r="D42" s="109"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="115"/>
       <c r="G42" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H42" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="I42" s="87"/>
+      <c r="I42" s="118"/>
     </row>
     <row r="43" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C43" s="130"/>
-      <c r="D43" s="127" t="s">
+      <c r="C43" s="119"/>
+      <c r="D43" s="107" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="75" t="s">
+      <c r="E43" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="113" t="s">
         <v>189</v>
       </c>
       <c r="G43" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="H43" s="145" t="s">
+      <c r="H43" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="I43" s="85" t="s">
+      <c r="I43" s="116" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="44" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C44" s="130"/>
-      <c r="D44" s="128"/>
-      <c r="E44" s="102"/>
-      <c r="F44" s="76"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="108"/>
+      <c r="E44" s="111"/>
+      <c r="F44" s="114"/>
       <c r="G44" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H44" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="I44" s="86"/>
+      <c r="I44" s="117"/>
     </row>
     <row r="45" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C45" s="131"/>
-      <c r="D45" s="129"/>
-      <c r="E45" s="103"/>
-      <c r="F45" s="77"/>
+      <c r="C45" s="120"/>
+      <c r="D45" s="109"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="115"/>
       <c r="G45" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H45" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="I45" s="87"/>
+      <c r="I45" s="118"/>
     </row>
     <row r="46" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="132" t="s">
+      <c r="D46" s="121" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="133" t="s">
+      <c r="E46" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="73" t="s">
+      <c r="F46" s="136" t="s">
         <v>78</v>
       </c>
       <c r="G46" s="30" t="s">
@@ -2683,45 +2720,45 @@
       <c r="H46" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="71" t="s">
+      <c r="I46" s="145" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C47" s="16"/>
-      <c r="D47" s="132"/>
-      <c r="E47" s="133"/>
-      <c r="F47" s="73"/>
+      <c r="D47" s="121"/>
+      <c r="E47" s="122"/>
+      <c r="F47" s="136"/>
       <c r="G47" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="I47" s="71"/>
+      <c r="I47" s="145"/>
     </row>
     <row r="48" spans="3:9" ht="31.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C48" s="7"/>
-      <c r="D48" s="132"/>
-      <c r="E48" s="133"/>
-      <c r="F48" s="73"/>
+      <c r="D48" s="121"/>
+      <c r="E48" s="122"/>
+      <c r="F48" s="136"/>
       <c r="G48" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H48" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="71"/>
+      <c r="I48" s="145"/>
     </row>
     <row r="49" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C49" s="7"/>
-      <c r="D49" s="119" t="s">
+      <c r="D49" s="123" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="104" t="s">
+      <c r="E49" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="110" t="s">
+      <c r="F49" s="101" t="s">
         <v>85</v>
       </c>
       <c r="G49" s="30" t="s">
@@ -2730,45 +2767,45 @@
       <c r="H49" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I49" s="67" t="s">
+      <c r="I49" s="104" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="50" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="7"/>
-      <c r="D50" s="121"/>
-      <c r="E50" s="105"/>
-      <c r="F50" s="111"/>
+      <c r="D50" s="124"/>
+      <c r="E50" s="99"/>
+      <c r="F50" s="102"/>
       <c r="G50" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H50" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="I50" s="68"/>
+      <c r="I50" s="105"/>
     </row>
     <row r="51" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C51" s="7"/>
-      <c r="D51" s="120"/>
-      <c r="E51" s="106"/>
-      <c r="F51" s="112"/>
+      <c r="D51" s="125"/>
+      <c r="E51" s="100"/>
+      <c r="F51" s="103"/>
       <c r="G51" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H51" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I51" s="69"/>
+      <c r="I51" s="106"/>
     </row>
     <row r="52" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C52" s="7"/>
-      <c r="D52" s="119" t="s">
+      <c r="D52" s="123" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="104" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="110" t="s">
+      <c r="E52" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="101" t="s">
         <v>91</v>
       </c>
       <c r="G52" s="30" t="s">
@@ -2777,22 +2814,22 @@
       <c r="H52" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="67" t="s">
+      <c r="I52" s="104" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C53" s="7"/>
-      <c r="D53" s="120"/>
-      <c r="E53" s="106"/>
-      <c r="F53" s="112"/>
+      <c r="D53" s="125"/>
+      <c r="E53" s="100"/>
+      <c r="F53" s="103"/>
       <c r="G53" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H53" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="I53" s="69"/>
+      <c r="I53" s="106"/>
     </row>
     <row r="54" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C54" s="7"/>
@@ -2839,13 +2876,13 @@
     </row>
     <row r="57" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C57" s="7"/>
-      <c r="D57" s="119" t="s">
+      <c r="D57" s="123" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="104" t="s">
+      <c r="E57" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="110" t="s">
+      <c r="F57" s="101" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="30" t="s">
@@ -2854,58 +2891,58 @@
       <c r="H57" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="I57" s="67" t="s">
+      <c r="I57" s="104" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="58" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C58" s="7"/>
-      <c r="D58" s="121"/>
-      <c r="E58" s="105"/>
-      <c r="F58" s="111"/>
+      <c r="D58" s="124"/>
+      <c r="E58" s="99"/>
+      <c r="F58" s="102"/>
       <c r="G58" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H58" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="I58" s="68"/>
+      <c r="I58" s="105"/>
     </row>
     <row r="59" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C59" s="7"/>
-      <c r="D59" s="121"/>
-      <c r="E59" s="105"/>
-      <c r="F59" s="111"/>
+      <c r="D59" s="124"/>
+      <c r="E59" s="99"/>
+      <c r="F59" s="102"/>
       <c r="G59" s="32" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I59" s="68"/>
+      <c r="I59" s="105"/>
     </row>
     <row r="60" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C60" s="7"/>
-      <c r="D60" s="120"/>
-      <c r="E60" s="106"/>
-      <c r="F60" s="112"/>
+      <c r="D60" s="125"/>
+      <c r="E60" s="100"/>
+      <c r="F60" s="103"/>
       <c r="G60" s="32" t="s">
         <v>100</v>
       </c>
       <c r="H60" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I60" s="69"/>
+      <c r="I60" s="106"/>
     </row>
     <row r="61" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C61" s="7"/>
-      <c r="D61" s="119" t="s">
+      <c r="D61" s="123" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="104" t="s">
+      <c r="E61" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="F61" s="110" t="s">
+      <c r="F61" s="101" t="s">
         <v>104</v>
       </c>
       <c r="G61" s="30" t="s">
@@ -2914,58 +2951,58 @@
       <c r="H61" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="I61" s="67" t="s">
+      <c r="I61" s="104" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C62" s="7"/>
-      <c r="D62" s="121"/>
-      <c r="E62" s="105"/>
-      <c r="F62" s="111"/>
+      <c r="D62" s="124"/>
+      <c r="E62" s="99"/>
+      <c r="F62" s="102"/>
       <c r="G62" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H62" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I62" s="68"/>
+      <c r="I62" s="105"/>
     </row>
     <row r="63" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C63" s="7"/>
-      <c r="D63" s="121"/>
-      <c r="E63" s="105"/>
-      <c r="F63" s="111"/>
+      <c r="D63" s="124"/>
+      <c r="E63" s="99"/>
+      <c r="F63" s="102"/>
       <c r="G63" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H63" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="I63" s="68"/>
+      <c r="I63" s="105"/>
     </row>
     <row r="64" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C64" s="7"/>
-      <c r="D64" s="120"/>
-      <c r="E64" s="106"/>
-      <c r="F64" s="112"/>
+      <c r="D64" s="125"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="103"/>
       <c r="G64" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H64" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I64" s="69"/>
+      <c r="I64" s="106"/>
     </row>
     <row r="65" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C65" s="7"/>
-      <c r="D65" s="119" t="s">
+      <c r="D65" s="123" t="s">
         <v>109</v>
       </c>
-      <c r="E65" s="104" t="s">
+      <c r="E65" s="98" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="110" t="s">
+      <c r="F65" s="101" t="s">
         <v>111</v>
       </c>
       <c r="G65" s="30" t="s">
@@ -2974,84 +3011,84 @@
       <c r="H65" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="I65" s="67" t="s">
+      <c r="I65" s="104" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C66" s="7"/>
-      <c r="D66" s="121"/>
-      <c r="E66" s="105"/>
-      <c r="F66" s="111"/>
+      <c r="D66" s="124"/>
+      <c r="E66" s="99"/>
+      <c r="F66" s="102"/>
       <c r="G66" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H66" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I66" s="68"/>
+      <c r="I66" s="105"/>
     </row>
     <row r="67" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C67" s="7"/>
-      <c r="D67" s="121"/>
-      <c r="E67" s="105"/>
-      <c r="F67" s="111"/>
+      <c r="D67" s="124"/>
+      <c r="E67" s="99"/>
+      <c r="F67" s="102"/>
       <c r="G67" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H67" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="I67" s="68"/>
+      <c r="I67" s="105"/>
     </row>
     <row r="68" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C68" s="7"/>
-      <c r="D68" s="121"/>
-      <c r="E68" s="105"/>
-      <c r="F68" s="111"/>
+      <c r="D68" s="124"/>
+      <c r="E68" s="99"/>
+      <c r="F68" s="102"/>
       <c r="G68" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H68" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="I68" s="68"/>
+      <c r="I68" s="105"/>
     </row>
     <row r="69" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C69" s="7"/>
-      <c r="D69" s="121"/>
-      <c r="E69" s="105"/>
-      <c r="F69" s="111"/>
+      <c r="D69" s="124"/>
+      <c r="E69" s="99"/>
+      <c r="F69" s="102"/>
       <c r="G69" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H69" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I69" s="68"/>
+      <c r="I69" s="105"/>
     </row>
     <row r="70" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C70" s="122"/>
-      <c r="D70" s="120"/>
-      <c r="E70" s="106"/>
-      <c r="F70" s="112"/>
+      <c r="C70" s="93"/>
+      <c r="D70" s="125"/>
+      <c r="E70" s="100"/>
+      <c r="F70" s="103"/>
       <c r="G70" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H70" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="I70" s="69"/>
+      <c r="I70" s="106"/>
     </row>
     <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C71" s="122"/>
-      <c r="D71" s="124" t="s">
+      <c r="C71" s="93"/>
+      <c r="D71" s="95" t="s">
         <v>190</v>
       </c>
-      <c r="E71" s="104" t="s">
+      <c r="E71" s="98" t="s">
         <v>191</v>
       </c>
-      <c r="F71" s="110" t="s">
+      <c r="F71" s="101" t="s">
         <v>192</v>
       </c>
       <c r="G71" s="30" t="s">
@@ -3060,60 +3097,60 @@
       <c r="H71" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="I71" s="67" t="s">
+      <c r="I71" s="104" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="72" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C72" s="122"/>
-      <c r="D72" s="125"/>
-      <c r="E72" s="105"/>
-      <c r="F72" s="111"/>
+      <c r="C72" s="93"/>
+      <c r="D72" s="96"/>
+      <c r="E72" s="99"/>
+      <c r="F72" s="102"/>
       <c r="G72" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H72" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="I72" s="68"/>
+      <c r="I72" s="105"/>
     </row>
     <row r="73" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C73" s="122"/>
-      <c r="D73" s="125"/>
-      <c r="E73" s="105"/>
-      <c r="F73" s="111"/>
+      <c r="C73" s="93"/>
+      <c r="D73" s="96"/>
+      <c r="E73" s="99"/>
+      <c r="F73" s="102"/>
       <c r="G73" s="32" t="s">
         <v>72</v>
       </c>
       <c r="H73" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="I73" s="68"/>
+      <c r="I73" s="105"/>
     </row>
     <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C74" s="123"/>
-      <c r="D74" s="126"/>
-      <c r="E74" s="106"/>
-      <c r="F74" s="112"/>
+      <c r="C74" s="94"/>
+      <c r="D74" s="97"/>
+      <c r="E74" s="100"/>
+      <c r="F74" s="103"/>
       <c r="G74" s="60" t="s">
         <v>31</v>
       </c>
       <c r="H74" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="I74" s="69"/>
+      <c r="I74" s="106"/>
     </row>
     <row r="75" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D75" s="116" t="s">
+      <c r="D75" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="113" t="s">
+      <c r="E75" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F75" s="107" t="s">
+      <c r="F75" s="126" t="s">
         <v>121</v>
       </c>
       <c r="G75" s="26" t="s">
@@ -3122,58 +3159,58 @@
       <c r="H75" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="I75" s="63" t="s">
+      <c r="I75" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="76" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C76" s="9"/>
-      <c r="D76" s="117"/>
-      <c r="E76" s="114"/>
-      <c r="F76" s="108"/>
+      <c r="D76" s="88"/>
+      <c r="E76" s="74"/>
+      <c r="F76" s="127"/>
       <c r="G76" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="I76" s="64"/>
+      <c r="I76" s="82"/>
     </row>
     <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C77" s="10"/>
-      <c r="D77" s="117"/>
-      <c r="E77" s="114"/>
-      <c r="F77" s="108"/>
+      <c r="D77" s="88"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="127"/>
       <c r="G77" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H77" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I77" s="64"/>
+      <c r="I77" s="82"/>
     </row>
     <row r="78" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C78" s="10"/>
-      <c r="D78" s="118"/>
-      <c r="E78" s="115"/>
-      <c r="F78" s="109"/>
+      <c r="D78" s="89"/>
+      <c r="E78" s="75"/>
+      <c r="F78" s="128"/>
       <c r="G78" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H78" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="I78" s="65"/>
+      <c r="I78" s="83"/>
     </row>
     <row r="79" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C79" s="10"/>
-      <c r="D79" s="116" t="s">
+      <c r="D79" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="E79" s="113" t="s">
+      <c r="E79" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="134" t="s">
+      <c r="F79" s="90" t="s">
         <v>127</v>
       </c>
       <c r="G79" s="26" t="s">
@@ -3182,45 +3219,45 @@
       <c r="H79" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="I79" s="63" t="s">
+      <c r="I79" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="80" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C80" s="10"/>
-      <c r="D80" s="117"/>
-      <c r="E80" s="114"/>
-      <c r="F80" s="135"/>
+      <c r="D80" s="88"/>
+      <c r="E80" s="74"/>
+      <c r="F80" s="91"/>
       <c r="G80" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H80" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="I80" s="64"/>
+      <c r="I80" s="82"/>
     </row>
     <row r="81" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C81" s="10"/>
-      <c r="D81" s="118"/>
-      <c r="E81" s="115"/>
-      <c r="F81" s="136"/>
+      <c r="D81" s="89"/>
+      <c r="E81" s="75"/>
+      <c r="F81" s="92"/>
       <c r="G81" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H81" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I81" s="65"/>
+      <c r="I81" s="83"/>
     </row>
     <row r="82" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C82" s="10"/>
-      <c r="D82" s="116" t="s">
+      <c r="D82" s="87" t="s">
         <v>131</v>
       </c>
-      <c r="E82" s="113" t="s">
+      <c r="E82" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F82" s="134" t="s">
+      <c r="F82" s="90" t="s">
         <v>132</v>
       </c>
       <c r="G82" s="26" t="s">
@@ -3229,45 +3266,45 @@
       <c r="H82" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="I82" s="63" t="s">
+      <c r="I82" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="83" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C83" s="10"/>
-      <c r="D83" s="117"/>
-      <c r="E83" s="114"/>
-      <c r="F83" s="135"/>
+      <c r="D83" s="88"/>
+      <c r="E83" s="74"/>
+      <c r="F83" s="91"/>
       <c r="G83" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H83" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="I83" s="64"/>
+      <c r="I83" s="82"/>
     </row>
     <row r="84" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C84" s="10"/>
-      <c r="D84" s="118"/>
-      <c r="E84" s="115"/>
-      <c r="F84" s="136"/>
+      <c r="D84" s="89"/>
+      <c r="E84" s="75"/>
+      <c r="F84" s="92"/>
       <c r="G84" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H84" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I84" s="65"/>
+      <c r="I84" s="83"/>
     </row>
     <row r="85" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C85" s="10"/>
-      <c r="D85" s="116" t="s">
+      <c r="D85" s="87" t="s">
         <v>135</v>
       </c>
-      <c r="E85" s="113" t="s">
+      <c r="E85" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F85" s="134" t="s">
+      <c r="F85" s="90" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="26" t="s">
@@ -3276,152 +3313,188 @@
       <c r="H85" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="I85" s="63" t="s">
+      <c r="I85" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="86" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C86" s="143"/>
-      <c r="D86" s="117"/>
-      <c r="E86" s="114"/>
-      <c r="F86" s="135"/>
+      <c r="C86" s="79"/>
+      <c r="D86" s="88"/>
+      <c r="E86" s="74"/>
+      <c r="F86" s="91"/>
       <c r="G86" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H86" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="I86" s="64"/>
+      <c r="I86" s="82"/>
     </row>
     <row r="87" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C87" s="143"/>
-      <c r="D87" s="118"/>
-      <c r="E87" s="115"/>
-      <c r="F87" s="136"/>
+      <c r="C87" s="79"/>
+      <c r="D87" s="89"/>
+      <c r="E87" s="75"/>
+      <c r="F87" s="92"/>
       <c r="G87" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H87" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I87" s="65"/>
+      <c r="I87" s="83"/>
     </row>
     <row r="88" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C88" s="143"/>
-      <c r="D88" s="137" t="s">
+      <c r="C88" s="79"/>
+      <c r="D88" s="70" t="s">
         <v>193</v>
       </c>
-      <c r="E88" s="113" t="s">
+      <c r="E88" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F88" s="140" t="s">
+      <c r="F88" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="G88" s="26"/>
-      <c r="H88" s="59"/>
-      <c r="I88" s="63" t="s">
+      <c r="G88" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H88" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="I88" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="89" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C89" s="143"/>
-      <c r="D89" s="138"/>
-      <c r="E89" s="114"/>
-      <c r="F89" s="141"/>
-      <c r="G89" s="28"/>
-      <c r="H89" s="56"/>
-      <c r="I89" s="64"/>
+      <c r="C89" s="79"/>
+      <c r="D89" s="71"/>
+      <c r="E89" s="74"/>
+      <c r="F89" s="77"/>
+      <c r="G89" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="H89" s="56" t="s">
+        <v>208</v>
+      </c>
+      <c r="I89" s="82"/>
     </row>
     <row r="90" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C90" s="143"/>
-      <c r="D90" s="139"/>
-      <c r="E90" s="115"/>
-      <c r="F90" s="142"/>
-      <c r="G90" s="28"/>
-      <c r="H90" s="56"/>
-      <c r="I90" s="65"/>
+      <c r="C90" s="79"/>
+      <c r="D90" s="72"/>
+      <c r="E90" s="75"/>
+      <c r="F90" s="78"/>
+      <c r="G90" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H90" s="56" t="s">
+        <v>209</v>
+      </c>
+      <c r="I90" s="83"/>
     </row>
     <row r="91" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C91" s="143"/>
-      <c r="D91" s="137" t="s">
+      <c r="C91" s="79"/>
+      <c r="D91" s="70" t="s">
         <v>194</v>
       </c>
-      <c r="E91" s="113" t="s">
+      <c r="E91" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F91" s="140" t="s">
+      <c r="F91" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="G91" s="26"/>
-      <c r="H91" s="59"/>
-      <c r="I91" s="63" t="s">
+      <c r="G91" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="H91" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="I91" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="92" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C92" s="143"/>
-      <c r="D92" s="138"/>
-      <c r="E92" s="114"/>
-      <c r="F92" s="141"/>
-      <c r="G92" s="28"/>
-      <c r="H92" s="56"/>
-      <c r="I92" s="64"/>
+      <c r="C92" s="79"/>
+      <c r="D92" s="71"/>
+      <c r="E92" s="74"/>
+      <c r="F92" s="77"/>
+      <c r="G92" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="H92" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="I92" s="82"/>
     </row>
     <row r="93" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C93" s="143"/>
-      <c r="D93" s="139"/>
-      <c r="E93" s="115"/>
-      <c r="F93" s="142"/>
-      <c r="G93" s="28"/>
-      <c r="H93" s="56"/>
-      <c r="I93" s="65"/>
+      <c r="C93" s="79"/>
+      <c r="D93" s="72"/>
+      <c r="E93" s="75"/>
+      <c r="F93" s="78"/>
+      <c r="G93" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H93" s="56" t="s">
+        <v>208</v>
+      </c>
+      <c r="I93" s="83"/>
     </row>
     <row r="94" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C94" s="143"/>
-      <c r="D94" s="137" t="s">
+      <c r="C94" s="79"/>
+      <c r="D94" s="70" t="s">
         <v>195</v>
       </c>
-      <c r="E94" s="113" t="s">
+      <c r="E94" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F94" s="140" t="s">
+      <c r="F94" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="G94" s="26"/>
-      <c r="H94" s="59"/>
-      <c r="I94" s="63" t="s">
+      <c r="G94" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="H94" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="I94" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="95" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C95" s="143"/>
-      <c r="D95" s="138"/>
-      <c r="E95" s="114"/>
-      <c r="F95" s="141"/>
-      <c r="G95" s="28"/>
-      <c r="H95" s="56"/>
-      <c r="I95" s="64"/>
+      <c r="C95" s="79"/>
+      <c r="D95" s="71"/>
+      <c r="E95" s="74"/>
+      <c r="F95" s="77"/>
+      <c r="G95" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="H95" s="56" t="s">
+        <v>216</v>
+      </c>
+      <c r="I95" s="82"/>
     </row>
     <row r="96" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C96" s="144"/>
-      <c r="D96" s="139"/>
-      <c r="E96" s="115"/>
-      <c r="F96" s="142"/>
-      <c r="G96" s="28"/>
-      <c r="H96" s="56"/>
-      <c r="I96" s="65"/>
+      <c r="C96" s="80"/>
+      <c r="D96" s="72"/>
+      <c r="E96" s="75"/>
+      <c r="F96" s="78"/>
+      <c r="G96" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H96" s="56" t="s">
+        <v>208</v>
+      </c>
+      <c r="I96" s="83"/>
     </row>
     <row r="97" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C97" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D97" s="91" t="s">
+      <c r="D97" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="E97" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F97" s="88" t="s">
+      <c r="E97" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="66" t="s">
         <v>141</v>
       </c>
       <c r="G97" s="18" t="s">
@@ -3430,45 +3503,45 @@
       <c r="H97" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="I97" s="61" t="s">
+      <c r="I97" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="98" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C98" s="12"/>
-      <c r="D98" s="96"/>
-      <c r="E98" s="94"/>
-      <c r="F98" s="89"/>
+      <c r="D98" s="86"/>
+      <c r="E98" s="84"/>
+      <c r="F98" s="85"/>
       <c r="G98" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H98" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="I98" s="66"/>
+      <c r="I98" s="144"/>
     </row>
     <row r="99" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C99" s="13"/>
-      <c r="D99" s="92"/>
-      <c r="E99" s="95"/>
-      <c r="F99" s="90"/>
+      <c r="D99" s="63"/>
+      <c r="E99" s="65"/>
+      <c r="F99" s="67"/>
       <c r="G99" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H99" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="I99" s="62"/>
+      <c r="I99" s="69"/>
     </row>
     <row r="100" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C100" s="13"/>
-      <c r="D100" s="91" t="s">
+      <c r="D100" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="E100" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="88" t="s">
+      <c r="E100" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="66" t="s">
         <v>147</v>
       </c>
       <c r="G100" s="18" t="s">
@@ -3477,58 +3550,58 @@
       <c r="H100" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="I100" s="61" t="s">
+      <c r="I100" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="101" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C101" s="13"/>
-      <c r="D101" s="96"/>
-      <c r="E101" s="94"/>
-      <c r="F101" s="89"/>
+      <c r="D101" s="86"/>
+      <c r="E101" s="84"/>
+      <c r="F101" s="85"/>
       <c r="G101" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H101" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I101" s="66"/>
+      <c r="I101" s="144"/>
     </row>
     <row r="102" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C102" s="13"/>
-      <c r="D102" s="96"/>
-      <c r="E102" s="94"/>
-      <c r="F102" s="89"/>
+      <c r="D102" s="86"/>
+      <c r="E102" s="84"/>
+      <c r="F102" s="85"/>
       <c r="G102" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H102" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I102" s="66"/>
+      <c r="I102" s="144"/>
     </row>
     <row r="103" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C103" s="13"/>
-      <c r="D103" s="92"/>
-      <c r="E103" s="95"/>
-      <c r="F103" s="90"/>
+      <c r="D103" s="63"/>
+      <c r="E103" s="65"/>
+      <c r="F103" s="67"/>
       <c r="G103" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H103" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="I103" s="62"/>
+      <c r="I103" s="69"/>
     </row>
     <row r="104" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C104" s="13"/>
-      <c r="D104" s="91" t="s">
+      <c r="D104" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="E104" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F104" s="88" t="s">
+      <c r="E104" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" s="66" t="s">
         <v>153</v>
       </c>
       <c r="G104" s="18" t="s">
@@ -3537,58 +3610,58 @@
       <c r="H104" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="I104" s="61" t="s">
+      <c r="I104" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="105" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C105" s="13"/>
-      <c r="D105" s="96"/>
-      <c r="E105" s="94"/>
-      <c r="F105" s="89"/>
+      <c r="D105" s="86"/>
+      <c r="E105" s="84"/>
+      <c r="F105" s="85"/>
       <c r="G105" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H105" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="I105" s="66"/>
+      <c r="I105" s="144"/>
     </row>
     <row r="106" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C106" s="13"/>
-      <c r="D106" s="96"/>
-      <c r="E106" s="94"/>
-      <c r="F106" s="89"/>
+      <c r="D106" s="86"/>
+      <c r="E106" s="84"/>
+      <c r="F106" s="85"/>
       <c r="G106" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H106" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="I106" s="66"/>
+      <c r="I106" s="144"/>
     </row>
     <row r="107" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C107" s="13"/>
-      <c r="D107" s="92"/>
-      <c r="E107" s="95"/>
-      <c r="F107" s="90"/>
+      <c r="D107" s="63"/>
+      <c r="E107" s="65"/>
+      <c r="F107" s="67"/>
       <c r="G107" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H107" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="I107" s="62"/>
+      <c r="I107" s="69"/>
     </row>
     <row r="108" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C108" s="13"/>
-      <c r="D108" s="91" t="s">
+      <c r="D108" s="62" t="s">
         <v>158</v>
       </c>
-      <c r="E108" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F108" s="88" t="s">
+      <c r="E108" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108" s="66" t="s">
         <v>159</v>
       </c>
       <c r="G108" s="18" t="s">
@@ -3597,58 +3670,58 @@
       <c r="H108" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="I108" s="61" t="s">
+      <c r="I108" s="68" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="109" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C109" s="13"/>
-      <c r="D109" s="96"/>
-      <c r="E109" s="94"/>
-      <c r="F109" s="89"/>
+      <c r="D109" s="86"/>
+      <c r="E109" s="84"/>
+      <c r="F109" s="85"/>
       <c r="G109" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H109" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I109" s="66"/>
+      <c r="I109" s="144"/>
     </row>
     <row r="110" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C110" s="13"/>
-      <c r="D110" s="96"/>
-      <c r="E110" s="94"/>
-      <c r="F110" s="89"/>
+      <c r="D110" s="86"/>
+      <c r="E110" s="84"/>
+      <c r="F110" s="85"/>
       <c r="G110" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H110" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I110" s="66"/>
+      <c r="I110" s="144"/>
     </row>
     <row r="111" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C111" s="13"/>
-      <c r="D111" s="92"/>
-      <c r="E111" s="95"/>
-      <c r="F111" s="90"/>
+      <c r="D111" s="63"/>
+      <c r="E111" s="65"/>
+      <c r="F111" s="67"/>
       <c r="G111" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H111" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="I111" s="62"/>
+      <c r="I111" s="69"/>
     </row>
     <row r="112" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C112" s="13"/>
-      <c r="D112" s="91" t="s">
+      <c r="D112" s="62" t="s">
         <v>161</v>
       </c>
-      <c r="E112" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F112" s="88" t="s">
+      <c r="E112" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F112" s="66" t="s">
         <v>162</v>
       </c>
       <c r="G112" s="18" t="s">
@@ -3657,45 +3730,45 @@
       <c r="H112" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="I112" s="61" t="s">
+      <c r="I112" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="113" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C113" s="13"/>
-      <c r="D113" s="96"/>
-      <c r="E113" s="94"/>
-      <c r="F113" s="89"/>
+      <c r="D113" s="86"/>
+      <c r="E113" s="84"/>
+      <c r="F113" s="85"/>
       <c r="G113" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H113" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="I113" s="66"/>
+      <c r="I113" s="144"/>
     </row>
     <row r="114" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C114" s="14"/>
-      <c r="D114" s="92"/>
-      <c r="E114" s="95"/>
-      <c r="F114" s="90"/>
+      <c r="D114" s="63"/>
+      <c r="E114" s="65"/>
+      <c r="F114" s="67"/>
       <c r="G114" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H114" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I114" s="62"/>
+      <c r="I114" s="69"/>
     </row>
     <row r="115" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C115" s="14"/>
-      <c r="D115" s="91" t="s">
+      <c r="D115" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="E115" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F115" s="88" t="s">
+      <c r="E115" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F115" s="66" t="s">
         <v>166</v>
       </c>
       <c r="G115" s="18" t="s">
@@ -3704,32 +3777,32 @@
       <c r="H115" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="I115" s="61" t="s">
+      <c r="I115" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="116" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C116" s="13"/>
-      <c r="D116" s="92"/>
-      <c r="E116" s="95"/>
-      <c r="F116" s="90"/>
+      <c r="D116" s="63"/>
+      <c r="E116" s="65"/>
+      <c r="F116" s="67"/>
       <c r="G116" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H116" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="I116" s="62"/>
+      <c r="I116" s="69"/>
     </row>
     <row r="117" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C117" s="13"/>
-      <c r="D117" s="91" t="s">
+      <c r="D117" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="E117" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F117" s="88" t="s">
+      <c r="E117" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F117" s="66" t="s">
         <v>170</v>
       </c>
       <c r="G117" s="18" t="s">
@@ -3738,32 +3811,32 @@
       <c r="H117" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="I117" s="61" t="s">
+      <c r="I117" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="118" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C118" s="13"/>
-      <c r="D118" s="92"/>
-      <c r="E118" s="95"/>
-      <c r="F118" s="90"/>
+      <c r="D118" s="63"/>
+      <c r="E118" s="65"/>
+      <c r="F118" s="67"/>
       <c r="G118" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H118" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="I118" s="62"/>
+      <c r="I118" s="69"/>
     </row>
     <row r="119" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C119" s="13"/>
-      <c r="D119" s="91" t="s">
+      <c r="D119" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="E119" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F119" s="88" t="s">
+      <c r="E119" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F119" s="66" t="s">
         <v>174</v>
       </c>
       <c r="G119" s="18" t="s">
@@ -3772,58 +3845,58 @@
       <c r="H119" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="I119" s="61" t="s">
+      <c r="I119" s="68" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="120" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C120" s="13"/>
-      <c r="D120" s="96"/>
-      <c r="E120" s="94"/>
-      <c r="F120" s="89"/>
+      <c r="D120" s="86"/>
+      <c r="E120" s="84"/>
+      <c r="F120" s="85"/>
       <c r="G120" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H120" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="I120" s="66"/>
+      <c r="I120" s="144"/>
     </row>
     <row r="121" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C121" s="13"/>
-      <c r="D121" s="96"/>
-      <c r="E121" s="94"/>
-      <c r="F121" s="89"/>
+      <c r="D121" s="86"/>
+      <c r="E121" s="84"/>
+      <c r="F121" s="85"/>
       <c r="G121" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H121" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I121" s="66"/>
+      <c r="I121" s="144"/>
     </row>
     <row r="122" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C122" s="13"/>
-      <c r="D122" s="92"/>
-      <c r="E122" s="95"/>
-      <c r="F122" s="90"/>
+      <c r="D122" s="63"/>
+      <c r="E122" s="65"/>
+      <c r="F122" s="67"/>
       <c r="G122" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H122" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I122" s="62"/>
+      <c r="I122" s="69"/>
     </row>
     <row r="123" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C123" s="13"/>
-      <c r="D123" s="91" t="s">
+      <c r="D123" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="E123" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F123" s="88" t="s">
+      <c r="E123" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F123" s="66" t="s">
         <v>177</v>
       </c>
       <c r="G123" s="18" t="s">
@@ -3832,32 +3905,32 @@
       <c r="H123" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I123" s="61" t="s">
+      <c r="I123" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="124" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C124" s="15"/>
-      <c r="D124" s="92"/>
-      <c r="E124" s="95"/>
-      <c r="F124" s="90"/>
+      <c r="D124" s="63"/>
+      <c r="E124" s="65"/>
+      <c r="F124" s="67"/>
       <c r="G124" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H124" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I124" s="62"/>
+      <c r="I124" s="69"/>
     </row>
     <row r="125" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C125" s="13"/>
-      <c r="D125" s="91" t="s">
+      <c r="D125" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="E125" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F125" s="88" t="s">
+      <c r="E125" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F125" s="66" t="s">
         <v>199</v>
       </c>
       <c r="G125" s="18" t="s">
@@ -3866,25 +3939,144 @@
       <c r="H125" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I125" s="61" t="s">
+      <c r="I125" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="126" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C126" s="15"/>
-      <c r="D126" s="92"/>
-      <c r="E126" s="95"/>
-      <c r="F126" s="90"/>
+      <c r="D126" s="63"/>
+      <c r="E126" s="65"/>
+      <c r="F126" s="67"/>
       <c r="G126" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H126" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I126" s="62"/>
+      <c r="I126" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="143">
+    <mergeCell ref="I123:I124"/>
+    <mergeCell ref="I85:I87"/>
+    <mergeCell ref="I97:I99"/>
+    <mergeCell ref="I100:I103"/>
+    <mergeCell ref="I104:I107"/>
+    <mergeCell ref="I108:I111"/>
+    <mergeCell ref="I88:I90"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="I75:I78"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="I112:I114"/>
+    <mergeCell ref="I115:I116"/>
+    <mergeCell ref="I117:I118"/>
+    <mergeCell ref="I119:I122"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="I82:I84"/>
+    <mergeCell ref="I79:I81"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="F119:F122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="E119:E122"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="E117:E118"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="F108:F111"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="F112:F114"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="F115:F116"/>
+    <mergeCell ref="E108:E111"/>
+    <mergeCell ref="E112:E114"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="F117:F118"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="D119:D122"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="I71:I74"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="C39:C45"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="I43:I45"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="I65:I70"/>
+    <mergeCell ref="E82:E84"/>
+    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="E79:E81"/>
+    <mergeCell ref="F79:F81"/>
+    <mergeCell ref="F82:F84"/>
+    <mergeCell ref="D82:D84"/>
+    <mergeCell ref="F85:F87"/>
     <mergeCell ref="D125:D126"/>
     <mergeCell ref="E125:E126"/>
     <mergeCell ref="F125:F126"/>
@@ -3909,125 +4101,6 @@
     <mergeCell ref="D97:D99"/>
     <mergeCell ref="F88:F90"/>
     <mergeCell ref="E88:E90"/>
-    <mergeCell ref="E82:E84"/>
-    <mergeCell ref="D85:D87"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="E79:E81"/>
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="D82:D84"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="C70:C74"/>
-    <mergeCell ref="D71:D74"/>
-    <mergeCell ref="E71:E74"/>
-    <mergeCell ref="F71:F74"/>
-    <mergeCell ref="I71:I74"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="C39:C45"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="I43:I45"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="I65:I70"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="F65:F70"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="D61:D64"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="F119:F122"/>
-    <mergeCell ref="D123:D124"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="E119:E122"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="E117:E118"/>
-    <mergeCell ref="D108:D111"/>
-    <mergeCell ref="F108:F111"/>
-    <mergeCell ref="D112:D114"/>
-    <mergeCell ref="F112:F114"/>
-    <mergeCell ref="D115:D116"/>
-    <mergeCell ref="F115:F116"/>
-    <mergeCell ref="E108:E111"/>
-    <mergeCell ref="E112:E114"/>
-    <mergeCell ref="E115:E116"/>
-    <mergeCell ref="F117:F118"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="D119:D122"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I60"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="I112:I114"/>
-    <mergeCell ref="I115:I116"/>
-    <mergeCell ref="I117:I118"/>
-    <mergeCell ref="I119:I122"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="I82:I84"/>
-    <mergeCell ref="I79:I81"/>
-    <mergeCell ref="I123:I124"/>
-    <mergeCell ref="I85:I87"/>
-    <mergeCell ref="I97:I99"/>
-    <mergeCell ref="I100:I103"/>
-    <mergeCell ref="I104:I107"/>
-    <mergeCell ref="I108:I111"/>
-    <mergeCell ref="I88:I90"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="I75:I78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Añadido endpoint delete para withdraws y tipo de status.
</commit_message>
<xml_diff>
--- a/.readmeFiles/Endpoints.xlsx
+++ b/.readmeFiles/Endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/anfrodri_emeal_nttdata_com/Documents/Escritorio/Git backend/back-end-framework/.readmeFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/dceballr_emeal_nttdata_com/Documents/Escritorio/Backend/Repositorio/back-end-framework/.readmeFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="436" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04A5F564-3AC0-4A37-A784-E5D06C4565C8}"/>
+  <xr:revisionPtr revIDLastSave="438" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8282590D-4C2D-461C-99A0-8C9B6200F954}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1372,6 +1372,96 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -1381,20 +1471,134 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1405,15 +1609,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1428,201 +1623,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1654,10 +1654,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1979,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA3F6E-09E5-46A7-9DF8-4B95ED8D48E7}">
   <dimension ref="B2:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView tabSelected="1" topLeftCell="C101" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2120,13 +2116,13 @@
     </row>
     <row r="9" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="5"/>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="130" t="s">
+      <c r="E9" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="129" t="s">
+      <c r="F9" s="73" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -2135,45 +2131,45 @@
       <c r="H9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="135" t="s">
+      <c r="I9" s="71" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="5"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="129"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="135"/>
+      <c r="I10" s="71"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="5"/>
-      <c r="D11" s="129"/>
-      <c r="E11" s="130"/>
-      <c r="F11" s="129"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="135"/>
+      <c r="I11" s="71"/>
     </row>
     <row r="12" spans="2:9" ht="28.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="5"/>
-      <c r="D12" s="129" t="s">
+      <c r="D12" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="130" t="s">
+      <c r="E12" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="129" t="s">
+      <c r="F12" s="73" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="38" t="s">
@@ -2182,35 +2178,35 @@
       <c r="H12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="135" t="s">
+      <c r="I12" s="71" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="5"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="130"/>
-      <c r="F13" s="129"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="73"/>
       <c r="G13" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="135"/>
+      <c r="I13" s="71"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="5"/>
-      <c r="D14" s="129"/>
-      <c r="E14" s="130"/>
-      <c r="F14" s="129"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="73"/>
       <c r="G14" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="135"/>
+      <c r="I14" s="71"/>
     </row>
     <row r="15" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="5"/>
@@ -2309,13 +2305,13 @@
     </row>
     <row r="20" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
-      <c r="D20" s="129" t="s">
+      <c r="D20" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="130" t="s">
+      <c r="E20" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="129" t="s">
+      <c r="F20" s="73" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="39" t="s">
@@ -2324,58 +2320,58 @@
       <c r="H20" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="135" t="s">
+      <c r="I20" s="71" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="129"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="73"/>
       <c r="G21" s="39" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="135"/>
+      <c r="I21" s="71"/>
     </row>
     <row r="22" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="129"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="73"/>
       <c r="G22" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="135"/>
+      <c r="I22" s="71"/>
     </row>
     <row r="23" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C23" s="5"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="129"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="73"/>
       <c r="G23" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H23" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="135"/>
+      <c r="I23" s="71"/>
     </row>
     <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="5"/>
-      <c r="D24" s="129" t="s">
+      <c r="D24" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="130" t="s">
+      <c r="E24" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="129" t="s">
+      <c r="F24" s="73" t="s">
         <v>57</v>
       </c>
       <c r="G24" s="38" t="s">
@@ -2384,45 +2380,45 @@
       <c r="H24" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="135" t="s">
+      <c r="I24" s="71" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="5"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="129"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="73"/>
       <c r="G25" s="42" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="I25" s="135"/>
+      <c r="I25" s="71"/>
     </row>
     <row r="26" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C26" s="5"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="129"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="73"/>
       <c r="G26" s="42" t="s">
         <v>53</v>
       </c>
       <c r="H26" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="135"/>
+      <c r="I26" s="71"/>
     </row>
     <row r="27" spans="3:9" ht="58.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C27" s="5"/>
-      <c r="D27" s="129" t="s">
+      <c r="D27" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="110" t="s">
+      <c r="E27" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="134" t="s">
+      <c r="F27" s="75" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="38" t="s">
@@ -2431,84 +2427,84 @@
       <c r="H27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="135" t="s">
+      <c r="I27" s="71" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="5"/>
-      <c r="D28" s="129"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="134"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="75"/>
       <c r="G28" s="42" t="s">
         <v>63</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="135"/>
+      <c r="I28" s="71"/>
     </row>
     <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="5"/>
-      <c r="D29" s="131" t="s">
+      <c r="D29" s="99" t="s">
         <v>181</v>
       </c>
-      <c r="E29" s="110" t="s">
+      <c r="E29" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="113" t="s">
+      <c r="F29" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="137" t="s">
+      <c r="G29" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="139" t="s">
+      <c r="H29" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="116" t="s">
+      <c r="I29" s="86" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="3:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="5"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="111"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="139"/>
-      <c r="I30" s="117"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="87"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C31" s="5"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="140" t="s">
+      <c r="D31" s="100"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="142" t="s">
+      <c r="H31" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="I31" s="117"/>
+      <c r="I31" s="87"/>
     </row>
     <row r="32" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="5"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="112"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="143"/>
-      <c r="I32" s="118"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="104"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="85"/>
+      <c r="I32" s="88"/>
     </row>
     <row r="33" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="5"/>
-      <c r="D33" s="134" t="s">
+      <c r="D33" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="130" t="s">
+      <c r="E33" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="134" t="s">
+      <c r="F33" s="75" t="s">
         <v>68</v>
       </c>
       <c r="G33" s="54" t="s">
@@ -2517,58 +2513,58 @@
       <c r="H33" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="135" t="s">
+      <c r="I33" s="71" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C34" s="5"/>
-      <c r="D34" s="134"/>
-      <c r="E34" s="130"/>
-      <c r="F34" s="134"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="75"/>
       <c r="G34" s="47" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I34" s="135"/>
+      <c r="I34" s="71"/>
     </row>
     <row r="35" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C35" s="5"/>
-      <c r="D35" s="134"/>
-      <c r="E35" s="130"/>
-      <c r="F35" s="134"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="75"/>
       <c r="G35" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H35" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="135"/>
+      <c r="I35" s="71"/>
     </row>
     <row r="36" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C36" s="5"/>
-      <c r="D36" s="134"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="134"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="75"/>
       <c r="G36" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H36" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I36" s="135"/>
+      <c r="I36" s="71"/>
     </row>
     <row r="37" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C37" s="5"/>
-      <c r="D37" s="107" t="s">
+      <c r="D37" s="128" t="s">
         <v>182</v>
       </c>
-      <c r="E37" s="110" t="s">
+      <c r="E37" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="113" t="s">
+      <c r="F37" s="76" t="s">
         <v>183</v>
       </c>
       <c r="G37" s="57" t="s">
@@ -2577,45 +2573,45 @@
       <c r="H37" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="I37" s="116" t="s">
+      <c r="I37" s="86" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C38" s="5"/>
-      <c r="D38" s="108"/>
-      <c r="E38" s="111"/>
-      <c r="F38" s="114"/>
+      <c r="D38" s="129"/>
+      <c r="E38" s="103"/>
+      <c r="F38" s="77"/>
       <c r="G38" s="42" t="s">
         <v>70</v>
       </c>
       <c r="H38" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="117"/>
+      <c r="I38" s="87"/>
     </row>
     <row r="39" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="119"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="112"/>
-      <c r="F39" s="115"/>
+      <c r="C39" s="131"/>
+      <c r="D39" s="130"/>
+      <c r="E39" s="104"/>
+      <c r="F39" s="78"/>
       <c r="G39" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H39" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="I39" s="118"/>
+      <c r="I39" s="88"/>
     </row>
     <row r="40" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="119"/>
-      <c r="D40" s="107" t="s">
+      <c r="C40" s="131"/>
+      <c r="D40" s="128" t="s">
         <v>186</v>
       </c>
-      <c r="E40" s="110" t="s">
+      <c r="E40" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="113" t="s">
+      <c r="F40" s="76" t="s">
         <v>187</v>
       </c>
       <c r="G40" s="57" t="s">
@@ -2624,45 +2620,45 @@
       <c r="H40" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="I40" s="116" t="s">
+      <c r="I40" s="86" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="41" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C41" s="119"/>
-      <c r="D41" s="108"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="114"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="103"/>
+      <c r="F41" s="77"/>
       <c r="G41" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H41" s="55" t="s">
         <v>200</v>
       </c>
-      <c r="I41" s="117"/>
+      <c r="I41" s="87"/>
     </row>
     <row r="42" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C42" s="119"/>
-      <c r="D42" s="109"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="115"/>
+      <c r="C42" s="131"/>
+      <c r="D42" s="130"/>
+      <c r="E42" s="104"/>
+      <c r="F42" s="78"/>
       <c r="G42" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H42" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="I42" s="118"/>
+      <c r="I42" s="88"/>
     </row>
     <row r="43" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C43" s="119"/>
-      <c r="D43" s="107" t="s">
+      <c r="C43" s="131"/>
+      <c r="D43" s="128" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="110" t="s">
+      <c r="E43" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="113" t="s">
+      <c r="F43" s="76" t="s">
         <v>189</v>
       </c>
       <c r="G43" s="57" t="s">
@@ -2671,47 +2667,47 @@
       <c r="H43" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="I43" s="116" t="s">
+      <c r="I43" s="86" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="44" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C44" s="119"/>
-      <c r="D44" s="108"/>
-      <c r="E44" s="111"/>
-      <c r="F44" s="114"/>
+      <c r="C44" s="131"/>
+      <c r="D44" s="129"/>
+      <c r="E44" s="103"/>
+      <c r="F44" s="77"/>
       <c r="G44" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H44" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="I44" s="117"/>
+      <c r="I44" s="87"/>
     </row>
     <row r="45" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C45" s="120"/>
-      <c r="D45" s="109"/>
-      <c r="E45" s="112"/>
-      <c r="F45" s="115"/>
+      <c r="C45" s="132"/>
+      <c r="D45" s="130"/>
+      <c r="E45" s="104"/>
+      <c r="F45" s="78"/>
       <c r="G45" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H45" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="I45" s="118"/>
+      <c r="I45" s="88"/>
     </row>
     <row r="46" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="121" t="s">
+      <c r="D46" s="133" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="122" t="s">
+      <c r="E46" s="134" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="136" t="s">
+      <c r="F46" s="74" t="s">
         <v>78</v>
       </c>
       <c r="G46" s="30" t="s">
@@ -2720,45 +2716,45 @@
       <c r="H46" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="145" t="s">
+      <c r="I46" s="72" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C47" s="16"/>
-      <c r="D47" s="121"/>
-      <c r="E47" s="122"/>
-      <c r="F47" s="136"/>
+      <c r="D47" s="133"/>
+      <c r="E47" s="134"/>
+      <c r="F47" s="74"/>
       <c r="G47" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="I47" s="145"/>
+      <c r="I47" s="72"/>
     </row>
     <row r="48" spans="3:9" ht="31.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C48" s="7"/>
-      <c r="D48" s="121"/>
-      <c r="E48" s="122"/>
-      <c r="F48" s="136"/>
+      <c r="D48" s="133"/>
+      <c r="E48" s="134"/>
+      <c r="F48" s="74"/>
       <c r="G48" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H48" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="145"/>
+      <c r="I48" s="72"/>
     </row>
     <row r="49" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C49" s="7"/>
-      <c r="D49" s="123" t="s">
+      <c r="D49" s="120" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="98" t="s">
+      <c r="E49" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="101" t="s">
+      <c r="F49" s="111" t="s">
         <v>85</v>
       </c>
       <c r="G49" s="30" t="s">
@@ -2767,45 +2763,45 @@
       <c r="H49" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I49" s="104" t="s">
+      <c r="I49" s="68" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="50" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="7"/>
-      <c r="D50" s="124"/>
-      <c r="E50" s="99"/>
-      <c r="F50" s="102"/>
+      <c r="D50" s="122"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="112"/>
       <c r="G50" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H50" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="I50" s="105"/>
+      <c r="I50" s="69"/>
     </row>
     <row r="51" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C51" s="7"/>
-      <c r="D51" s="125"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="103"/>
+      <c r="D51" s="121"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="113"/>
       <c r="G51" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H51" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I51" s="106"/>
+      <c r="I51" s="70"/>
     </row>
     <row r="52" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C52" s="7"/>
-      <c r="D52" s="123" t="s">
+      <c r="D52" s="120" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="98" t="s">
+      <c r="E52" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="F52" s="101" t="s">
+      <c r="F52" s="111" t="s">
         <v>91</v>
       </c>
       <c r="G52" s="30" t="s">
@@ -2814,22 +2810,22 @@
       <c r="H52" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="104" t="s">
+      <c r="I52" s="68" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C53" s="7"/>
-      <c r="D53" s="125"/>
-      <c r="E53" s="100"/>
-      <c r="F53" s="103"/>
+      <c r="D53" s="121"/>
+      <c r="E53" s="107"/>
+      <c r="F53" s="113"/>
       <c r="G53" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H53" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="I53" s="106"/>
+      <c r="I53" s="70"/>
     </row>
     <row r="54" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C54" s="7"/>
@@ -2876,13 +2872,13 @@
     </row>
     <row r="57" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C57" s="7"/>
-      <c r="D57" s="123" t="s">
+      <c r="D57" s="120" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="98" t="s">
+      <c r="E57" s="105" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="101" t="s">
+      <c r="F57" s="111" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="30" t="s">
@@ -2891,58 +2887,58 @@
       <c r="H57" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="I57" s="104" t="s">
+      <c r="I57" s="68" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="58" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C58" s="7"/>
-      <c r="D58" s="124"/>
-      <c r="E58" s="99"/>
-      <c r="F58" s="102"/>
+      <c r="D58" s="122"/>
+      <c r="E58" s="106"/>
+      <c r="F58" s="112"/>
       <c r="G58" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H58" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="I58" s="105"/>
+      <c r="I58" s="69"/>
     </row>
     <row r="59" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C59" s="7"/>
-      <c r="D59" s="124"/>
-      <c r="E59" s="99"/>
-      <c r="F59" s="102"/>
+      <c r="D59" s="122"/>
+      <c r="E59" s="106"/>
+      <c r="F59" s="112"/>
       <c r="G59" s="32" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I59" s="105"/>
+      <c r="I59" s="69"/>
     </row>
     <row r="60" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C60" s="7"/>
-      <c r="D60" s="125"/>
-      <c r="E60" s="100"/>
-      <c r="F60" s="103"/>
+      <c r="D60" s="121"/>
+      <c r="E60" s="107"/>
+      <c r="F60" s="113"/>
       <c r="G60" s="32" t="s">
         <v>100</v>
       </c>
       <c r="H60" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I60" s="106"/>
+      <c r="I60" s="70"/>
     </row>
     <row r="61" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C61" s="7"/>
-      <c r="D61" s="123" t="s">
+      <c r="D61" s="120" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="98" t="s">
+      <c r="E61" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="F61" s="101" t="s">
+      <c r="F61" s="111" t="s">
         <v>104</v>
       </c>
       <c r="G61" s="30" t="s">
@@ -2951,58 +2947,58 @@
       <c r="H61" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="I61" s="104" t="s">
+      <c r="I61" s="68" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C62" s="7"/>
-      <c r="D62" s="124"/>
-      <c r="E62" s="99"/>
-      <c r="F62" s="102"/>
+      <c r="D62" s="122"/>
+      <c r="E62" s="106"/>
+      <c r="F62" s="112"/>
       <c r="G62" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H62" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I62" s="105"/>
+      <c r="I62" s="69"/>
     </row>
     <row r="63" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C63" s="7"/>
-      <c r="D63" s="124"/>
-      <c r="E63" s="99"/>
-      <c r="F63" s="102"/>
+      <c r="D63" s="122"/>
+      <c r="E63" s="106"/>
+      <c r="F63" s="112"/>
       <c r="G63" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H63" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="I63" s="105"/>
+      <c r="I63" s="69"/>
     </row>
     <row r="64" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C64" s="7"/>
-      <c r="D64" s="125"/>
-      <c r="E64" s="100"/>
-      <c r="F64" s="103"/>
+      <c r="D64" s="121"/>
+      <c r="E64" s="107"/>
+      <c r="F64" s="113"/>
       <c r="G64" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H64" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I64" s="106"/>
+      <c r="I64" s="70"/>
     </row>
     <row r="65" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C65" s="7"/>
-      <c r="D65" s="123" t="s">
+      <c r="D65" s="120" t="s">
         <v>109</v>
       </c>
-      <c r="E65" s="98" t="s">
+      <c r="E65" s="105" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="101" t="s">
+      <c r="F65" s="111" t="s">
         <v>111</v>
       </c>
       <c r="G65" s="30" t="s">
@@ -3011,84 +3007,84 @@
       <c r="H65" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="I65" s="104" t="s">
+      <c r="I65" s="68" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C66" s="7"/>
-      <c r="D66" s="124"/>
-      <c r="E66" s="99"/>
-      <c r="F66" s="102"/>
+      <c r="D66" s="122"/>
+      <c r="E66" s="106"/>
+      <c r="F66" s="112"/>
       <c r="G66" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H66" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I66" s="105"/>
+      <c r="I66" s="69"/>
     </row>
     <row r="67" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C67" s="7"/>
-      <c r="D67" s="124"/>
-      <c r="E67" s="99"/>
-      <c r="F67" s="102"/>
+      <c r="D67" s="122"/>
+      <c r="E67" s="106"/>
+      <c r="F67" s="112"/>
       <c r="G67" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H67" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="I67" s="105"/>
+      <c r="I67" s="69"/>
     </row>
     <row r="68" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C68" s="7"/>
-      <c r="D68" s="124"/>
-      <c r="E68" s="99"/>
-      <c r="F68" s="102"/>
+      <c r="D68" s="122"/>
+      <c r="E68" s="106"/>
+      <c r="F68" s="112"/>
       <c r="G68" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H68" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="I68" s="105"/>
+      <c r="I68" s="69"/>
     </row>
     <row r="69" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C69" s="7"/>
-      <c r="D69" s="124"/>
-      <c r="E69" s="99"/>
-      <c r="F69" s="102"/>
+      <c r="D69" s="122"/>
+      <c r="E69" s="106"/>
+      <c r="F69" s="112"/>
       <c r="G69" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H69" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I69" s="105"/>
+      <c r="I69" s="69"/>
     </row>
     <row r="70" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C70" s="93"/>
-      <c r="D70" s="125"/>
-      <c r="E70" s="100"/>
-      <c r="F70" s="103"/>
+      <c r="C70" s="123"/>
+      <c r="D70" s="121"/>
+      <c r="E70" s="107"/>
+      <c r="F70" s="113"/>
       <c r="G70" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H70" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="I70" s="106"/>
+      <c r="I70" s="70"/>
     </row>
     <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C71" s="93"/>
-      <c r="D71" s="95" t="s">
+      <c r="C71" s="123"/>
+      <c r="D71" s="125" t="s">
         <v>190</v>
       </c>
-      <c r="E71" s="98" t="s">
+      <c r="E71" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="F71" s="101" t="s">
+      <c r="F71" s="111" t="s">
         <v>192</v>
       </c>
       <c r="G71" s="30" t="s">
@@ -3097,60 +3093,60 @@
       <c r="H71" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="I71" s="104" t="s">
+      <c r="I71" s="68" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="72" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C72" s="93"/>
-      <c r="D72" s="96"/>
-      <c r="E72" s="99"/>
-      <c r="F72" s="102"/>
+      <c r="C72" s="123"/>
+      <c r="D72" s="126"/>
+      <c r="E72" s="106"/>
+      <c r="F72" s="112"/>
       <c r="G72" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H72" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="I72" s="105"/>
+      <c r="I72" s="69"/>
     </row>
     <row r="73" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C73" s="93"/>
-      <c r="D73" s="96"/>
-      <c r="E73" s="99"/>
-      <c r="F73" s="102"/>
+      <c r="C73" s="123"/>
+      <c r="D73" s="126"/>
+      <c r="E73" s="106"/>
+      <c r="F73" s="112"/>
       <c r="G73" s="32" t="s">
         <v>72</v>
       </c>
       <c r="H73" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="I73" s="105"/>
+      <c r="I73" s="69"/>
     </row>
     <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C74" s="94"/>
-      <c r="D74" s="97"/>
-      <c r="E74" s="100"/>
-      <c r="F74" s="103"/>
+      <c r="C74" s="124"/>
+      <c r="D74" s="127"/>
+      <c r="E74" s="107"/>
+      <c r="F74" s="113"/>
       <c r="G74" s="60" t="s">
         <v>31</v>
       </c>
       <c r="H74" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="I74" s="106"/>
+      <c r="I74" s="70"/>
     </row>
     <row r="75" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D75" s="87" t="s">
+      <c r="D75" s="117" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="73" t="s">
+      <c r="E75" s="114" t="s">
         <v>120</v>
       </c>
-      <c r="F75" s="126" t="s">
+      <c r="F75" s="108" t="s">
         <v>121</v>
       </c>
       <c r="G75" s="26" t="s">
@@ -3159,58 +3155,58 @@
       <c r="H75" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="I75" s="81" t="s">
+      <c r="I75" s="64" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="76" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C76" s="9"/>
-      <c r="D76" s="88"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="127"/>
+      <c r="D76" s="118"/>
+      <c r="E76" s="115"/>
+      <c r="F76" s="109"/>
       <c r="G76" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="I76" s="82"/>
+      <c r="I76" s="65"/>
     </row>
     <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C77" s="10"/>
-      <c r="D77" s="88"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="127"/>
+      <c r="D77" s="118"/>
+      <c r="E77" s="115"/>
+      <c r="F77" s="109"/>
       <c r="G77" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H77" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I77" s="82"/>
+      <c r="I77" s="65"/>
     </row>
     <row r="78" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C78" s="10"/>
-      <c r="D78" s="89"/>
-      <c r="E78" s="75"/>
-      <c r="F78" s="128"/>
+      <c r="D78" s="119"/>
+      <c r="E78" s="116"/>
+      <c r="F78" s="110"/>
       <c r="G78" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H78" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="I78" s="83"/>
+      <c r="I78" s="66"/>
     </row>
     <row r="79" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C79" s="10"/>
-      <c r="D79" s="87" t="s">
+      <c r="D79" s="117" t="s">
         <v>126</v>
       </c>
-      <c r="E79" s="73" t="s">
+      <c r="E79" s="114" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="90" t="s">
+      <c r="F79" s="135" t="s">
         <v>127</v>
       </c>
       <c r="G79" s="26" t="s">
@@ -3219,45 +3215,45 @@
       <c r="H79" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="I79" s="81" t="s">
+      <c r="I79" s="64" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="80" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C80" s="10"/>
-      <c r="D80" s="88"/>
-      <c r="E80" s="74"/>
-      <c r="F80" s="91"/>
+      <c r="D80" s="118"/>
+      <c r="E80" s="115"/>
+      <c r="F80" s="136"/>
       <c r="G80" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H80" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="I80" s="82"/>
+      <c r="I80" s="65"/>
     </row>
     <row r="81" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C81" s="10"/>
-      <c r="D81" s="89"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="92"/>
+      <c r="D81" s="119"/>
+      <c r="E81" s="116"/>
+      <c r="F81" s="137"/>
       <c r="G81" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H81" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I81" s="83"/>
+      <c r="I81" s="66"/>
     </row>
     <row r="82" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C82" s="10"/>
-      <c r="D82" s="87" t="s">
+      <c r="D82" s="117" t="s">
         <v>131</v>
       </c>
-      <c r="E82" s="73" t="s">
+      <c r="E82" s="114" t="s">
         <v>120</v>
       </c>
-      <c r="F82" s="90" t="s">
+      <c r="F82" s="135" t="s">
         <v>132</v>
       </c>
       <c r="G82" s="26" t="s">
@@ -3266,45 +3262,45 @@
       <c r="H82" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="I82" s="81" t="s">
+      <c r="I82" s="64" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="83" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C83" s="10"/>
-      <c r="D83" s="88"/>
-      <c r="E83" s="74"/>
-      <c r="F83" s="91"/>
+      <c r="D83" s="118"/>
+      <c r="E83" s="115"/>
+      <c r="F83" s="136"/>
       <c r="G83" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H83" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="I83" s="82"/>
+      <c r="I83" s="65"/>
     </row>
     <row r="84" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C84" s="10"/>
-      <c r="D84" s="89"/>
-      <c r="E84" s="75"/>
-      <c r="F84" s="92"/>
+      <c r="D84" s="119"/>
+      <c r="E84" s="116"/>
+      <c r="F84" s="137"/>
       <c r="G84" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H84" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I84" s="83"/>
+      <c r="I84" s="66"/>
     </row>
     <row r="85" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C85" s="10"/>
-      <c r="D85" s="87" t="s">
+      <c r="D85" s="117" t="s">
         <v>135</v>
       </c>
-      <c r="E85" s="73" t="s">
+      <c r="E85" s="114" t="s">
         <v>120</v>
       </c>
-      <c r="F85" s="90" t="s">
+      <c r="F85" s="135" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="26" t="s">
@@ -3313,45 +3309,45 @@
       <c r="H85" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="I85" s="81" t="s">
+      <c r="I85" s="64" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="86" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C86" s="79"/>
-      <c r="D86" s="88"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="91"/>
+      <c r="C86" s="144"/>
+      <c r="D86" s="118"/>
+      <c r="E86" s="115"/>
+      <c r="F86" s="136"/>
       <c r="G86" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H86" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="I86" s="82"/>
+      <c r="I86" s="65"/>
     </row>
     <row r="87" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C87" s="79"/>
-      <c r="D87" s="89"/>
-      <c r="E87" s="75"/>
-      <c r="F87" s="92"/>
+      <c r="C87" s="144"/>
+      <c r="D87" s="119"/>
+      <c r="E87" s="116"/>
+      <c r="F87" s="137"/>
       <c r="G87" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H87" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I87" s="83"/>
+      <c r="I87" s="66"/>
     </row>
     <row r="88" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C88" s="79"/>
-      <c r="D88" s="70" t="s">
+      <c r="C88" s="144"/>
+      <c r="D88" s="138" t="s">
         <v>193</v>
       </c>
-      <c r="E88" s="73" t="s">
+      <c r="E88" s="114" t="s">
         <v>120</v>
       </c>
-      <c r="F88" s="76" t="s">
+      <c r="F88" s="141" t="s">
         <v>196</v>
       </c>
       <c r="G88" s="26" t="s">
@@ -3360,45 +3356,45 @@
       <c r="H88" s="59" t="s">
         <v>210</v>
       </c>
-      <c r="I88" s="81" t="s">
+      <c r="I88" s="64" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="89" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C89" s="79"/>
-      <c r="D89" s="71"/>
-      <c r="E89" s="74"/>
-      <c r="F89" s="77"/>
+      <c r="C89" s="144"/>
+      <c r="D89" s="139"/>
+      <c r="E89" s="115"/>
+      <c r="F89" s="142"/>
       <c r="G89" s="28" t="s">
         <v>206</v>
       </c>
       <c r="H89" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="I89" s="82"/>
+      <c r="I89" s="65"/>
     </row>
     <row r="90" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C90" s="79"/>
-      <c r="D90" s="72"/>
-      <c r="E90" s="75"/>
-      <c r="F90" s="78"/>
+      <c r="C90" s="144"/>
+      <c r="D90" s="140"/>
+      <c r="E90" s="116"/>
+      <c r="F90" s="143"/>
       <c r="G90" s="28" t="s">
         <v>207</v>
       </c>
       <c r="H90" s="56" t="s">
         <v>209</v>
       </c>
-      <c r="I90" s="83"/>
+      <c r="I90" s="66"/>
     </row>
     <row r="91" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C91" s="79"/>
-      <c r="D91" s="70" t="s">
+      <c r="C91" s="144"/>
+      <c r="D91" s="138" t="s">
         <v>194</v>
       </c>
-      <c r="E91" s="73" t="s">
+      <c r="E91" s="114" t="s">
         <v>120</v>
       </c>
-      <c r="F91" s="76" t="s">
+      <c r="F91" s="141" t="s">
         <v>197</v>
       </c>
       <c r="G91" s="26" t="s">
@@ -3407,45 +3403,45 @@
       <c r="H91" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="I91" s="81" t="s">
+      <c r="I91" s="64" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="92" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C92" s="79"/>
-      <c r="D92" s="71"/>
-      <c r="E92" s="74"/>
-      <c r="F92" s="77"/>
+      <c r="C92" s="144"/>
+      <c r="D92" s="139"/>
+      <c r="E92" s="115"/>
+      <c r="F92" s="142"/>
       <c r="G92" s="28" t="s">
         <v>212</v>
       </c>
       <c r="H92" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="I92" s="82"/>
+      <c r="I92" s="65"/>
     </row>
     <row r="93" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C93" s="79"/>
-      <c r="D93" s="72"/>
-      <c r="E93" s="75"/>
-      <c r="F93" s="78"/>
+      <c r="C93" s="144"/>
+      <c r="D93" s="140"/>
+      <c r="E93" s="116"/>
+      <c r="F93" s="143"/>
       <c r="G93" s="28" t="s">
         <v>72</v>
       </c>
       <c r="H93" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="I93" s="83"/>
+      <c r="I93" s="66"/>
     </row>
     <row r="94" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C94" s="79"/>
-      <c r="D94" s="70" t="s">
+      <c r="C94" s="144"/>
+      <c r="D94" s="138" t="s">
         <v>195</v>
       </c>
-      <c r="E94" s="73" t="s">
+      <c r="E94" s="114" t="s">
         <v>120</v>
       </c>
-      <c r="F94" s="76" t="s">
+      <c r="F94" s="141" t="s">
         <v>197</v>
       </c>
       <c r="G94" s="26" t="s">
@@ -3454,47 +3450,47 @@
       <c r="H94" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="I94" s="81" t="s">
+      <c r="I94" s="64" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="95" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C95" s="79"/>
-      <c r="D95" s="71"/>
-      <c r="E95" s="74"/>
-      <c r="F95" s="77"/>
+      <c r="C95" s="144"/>
+      <c r="D95" s="139"/>
+      <c r="E95" s="115"/>
+      <c r="F95" s="142"/>
       <c r="G95" s="28" t="s">
         <v>212</v>
       </c>
       <c r="H95" s="56" t="s">
         <v>216</v>
       </c>
-      <c r="I95" s="82"/>
+      <c r="I95" s="65"/>
     </row>
     <row r="96" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C96" s="80"/>
-      <c r="D96" s="72"/>
-      <c r="E96" s="75"/>
-      <c r="F96" s="78"/>
+      <c r="C96" s="145"/>
+      <c r="D96" s="140"/>
+      <c r="E96" s="116"/>
+      <c r="F96" s="143"/>
       <c r="G96" s="28" t="s">
         <v>72</v>
       </c>
       <c r="H96" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="I96" s="83"/>
+      <c r="I96" s="66"/>
     </row>
     <row r="97" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C97" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D97" s="62" t="s">
+      <c r="D97" s="92" t="s">
         <v>140</v>
       </c>
-      <c r="E97" s="64" t="s">
+      <c r="E97" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F97" s="66" t="s">
+      <c r="F97" s="89" t="s">
         <v>141</v>
       </c>
       <c r="G97" s="18" t="s">
@@ -3503,45 +3499,45 @@
       <c r="H97" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="I97" s="68" t="s">
+      <c r="I97" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="98" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C98" s="12"/>
-      <c r="D98" s="86"/>
-      <c r="E98" s="84"/>
-      <c r="F98" s="85"/>
+      <c r="D98" s="97"/>
+      <c r="E98" s="95"/>
+      <c r="F98" s="90"/>
       <c r="G98" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H98" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="I98" s="144"/>
+      <c r="I98" s="67"/>
     </row>
     <row r="99" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C99" s="13"/>
-      <c r="D99" s="63"/>
-      <c r="E99" s="65"/>
-      <c r="F99" s="67"/>
+      <c r="D99" s="93"/>
+      <c r="E99" s="96"/>
+      <c r="F99" s="91"/>
       <c r="G99" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H99" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="I99" s="69"/>
+      <c r="I99" s="63"/>
     </row>
     <row r="100" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C100" s="13"/>
-      <c r="D100" s="62" t="s">
+      <c r="D100" s="92" t="s">
         <v>146</v>
       </c>
-      <c r="E100" s="64" t="s">
+      <c r="E100" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F100" s="66" t="s">
+      <c r="F100" s="89" t="s">
         <v>147</v>
       </c>
       <c r="G100" s="18" t="s">
@@ -3550,58 +3546,58 @@
       <c r="H100" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="I100" s="68" t="s">
+      <c r="I100" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="101" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C101" s="13"/>
-      <c r="D101" s="86"/>
-      <c r="E101" s="84"/>
-      <c r="F101" s="85"/>
+      <c r="D101" s="97"/>
+      <c r="E101" s="95"/>
+      <c r="F101" s="90"/>
       <c r="G101" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H101" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I101" s="144"/>
+      <c r="I101" s="67"/>
     </row>
     <row r="102" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C102" s="13"/>
-      <c r="D102" s="86"/>
-      <c r="E102" s="84"/>
-      <c r="F102" s="85"/>
+      <c r="D102" s="97"/>
+      <c r="E102" s="95"/>
+      <c r="F102" s="90"/>
       <c r="G102" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H102" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I102" s="144"/>
+      <c r="I102" s="67"/>
     </row>
     <row r="103" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C103" s="13"/>
-      <c r="D103" s="63"/>
-      <c r="E103" s="65"/>
-      <c r="F103" s="67"/>
+      <c r="D103" s="93"/>
+      <c r="E103" s="96"/>
+      <c r="F103" s="91"/>
       <c r="G103" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H103" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="I103" s="69"/>
+      <c r="I103" s="63"/>
     </row>
     <row r="104" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C104" s="13"/>
-      <c r="D104" s="62" t="s">
+      <c r="D104" s="92" t="s">
         <v>152</v>
       </c>
-      <c r="E104" s="64" t="s">
+      <c r="E104" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F104" s="66" t="s">
+      <c r="F104" s="89" t="s">
         <v>153</v>
       </c>
       <c r="G104" s="18" t="s">
@@ -3610,58 +3606,58 @@
       <c r="H104" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="I104" s="68" t="s">
+      <c r="I104" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="105" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C105" s="13"/>
-      <c r="D105" s="86"/>
-      <c r="E105" s="84"/>
-      <c r="F105" s="85"/>
+      <c r="D105" s="97"/>
+      <c r="E105" s="95"/>
+      <c r="F105" s="90"/>
       <c r="G105" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H105" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="I105" s="144"/>
+      <c r="I105" s="67"/>
     </row>
     <row r="106" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C106" s="13"/>
-      <c r="D106" s="86"/>
-      <c r="E106" s="84"/>
-      <c r="F106" s="85"/>
+      <c r="D106" s="97"/>
+      <c r="E106" s="95"/>
+      <c r="F106" s="90"/>
       <c r="G106" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H106" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="I106" s="144"/>
+      <c r="I106" s="67"/>
     </row>
     <row r="107" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C107" s="13"/>
-      <c r="D107" s="63"/>
-      <c r="E107" s="65"/>
-      <c r="F107" s="67"/>
+      <c r="D107" s="93"/>
+      <c r="E107" s="96"/>
+      <c r="F107" s="91"/>
       <c r="G107" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H107" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="I107" s="69"/>
+      <c r="I107" s="63"/>
     </row>
     <row r="108" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C108" s="13"/>
-      <c r="D108" s="62" t="s">
+      <c r="D108" s="92" t="s">
         <v>158</v>
       </c>
-      <c r="E108" s="64" t="s">
+      <c r="E108" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F108" s="66" t="s">
+      <c r="F108" s="89" t="s">
         <v>159</v>
       </c>
       <c r="G108" s="18" t="s">
@@ -3670,58 +3666,58 @@
       <c r="H108" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="I108" s="68" t="s">
+      <c r="I108" s="62" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="109" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C109" s="13"/>
-      <c r="D109" s="86"/>
-      <c r="E109" s="84"/>
-      <c r="F109" s="85"/>
+      <c r="D109" s="97"/>
+      <c r="E109" s="95"/>
+      <c r="F109" s="90"/>
       <c r="G109" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H109" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I109" s="144"/>
+      <c r="I109" s="67"/>
     </row>
     <row r="110" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C110" s="13"/>
-      <c r="D110" s="86"/>
-      <c r="E110" s="84"/>
-      <c r="F110" s="85"/>
+      <c r="D110" s="97"/>
+      <c r="E110" s="95"/>
+      <c r="F110" s="90"/>
       <c r="G110" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H110" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I110" s="144"/>
+      <c r="I110" s="67"/>
     </row>
     <row r="111" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C111" s="13"/>
-      <c r="D111" s="63"/>
-      <c r="E111" s="65"/>
-      <c r="F111" s="67"/>
+      <c r="D111" s="93"/>
+      <c r="E111" s="96"/>
+      <c r="F111" s="91"/>
       <c r="G111" s="20" t="s">
         <v>144</v>
       </c>
       <c r="H111" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="I111" s="69"/>
+      <c r="I111" s="63"/>
     </row>
     <row r="112" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C112" s="13"/>
-      <c r="D112" s="62" t="s">
+      <c r="D112" s="92" t="s">
         <v>161</v>
       </c>
-      <c r="E112" s="64" t="s">
+      <c r="E112" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F112" s="66" t="s">
+      <c r="F112" s="89" t="s">
         <v>162</v>
       </c>
       <c r="G112" s="18" t="s">
@@ -3730,45 +3726,45 @@
       <c r="H112" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="I112" s="68" t="s">
+      <c r="I112" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="113" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C113" s="13"/>
-      <c r="D113" s="86"/>
-      <c r="E113" s="84"/>
-      <c r="F113" s="85"/>
+      <c r="D113" s="97"/>
+      <c r="E113" s="95"/>
+      <c r="F113" s="90"/>
       <c r="G113" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H113" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="I113" s="144"/>
+      <c r="I113" s="67"/>
     </row>
     <row r="114" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C114" s="14"/>
-      <c r="D114" s="63"/>
-      <c r="E114" s="65"/>
-      <c r="F114" s="67"/>
+      <c r="D114" s="93"/>
+      <c r="E114" s="96"/>
+      <c r="F114" s="91"/>
       <c r="G114" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H114" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I114" s="69"/>
+      <c r="I114" s="63"/>
     </row>
     <row r="115" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C115" s="14"/>
-      <c r="D115" s="62" t="s">
+      <c r="D115" s="92" t="s">
         <v>165</v>
       </c>
-      <c r="E115" s="64" t="s">
+      <c r="E115" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F115" s="66" t="s">
+      <c r="F115" s="89" t="s">
         <v>166</v>
       </c>
       <c r="G115" s="18" t="s">
@@ -3777,32 +3773,32 @@
       <c r="H115" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="I115" s="68" t="s">
+      <c r="I115" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="116" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C116" s="13"/>
-      <c r="D116" s="63"/>
-      <c r="E116" s="65"/>
-      <c r="F116" s="67"/>
+      <c r="D116" s="93"/>
+      <c r="E116" s="96"/>
+      <c r="F116" s="91"/>
       <c r="G116" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H116" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="I116" s="69"/>
+      <c r="I116" s="63"/>
     </row>
     <row r="117" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C117" s="13"/>
-      <c r="D117" s="62" t="s">
+      <c r="D117" s="92" t="s">
         <v>169</v>
       </c>
-      <c r="E117" s="64" t="s">
+      <c r="E117" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F117" s="66" t="s">
+      <c r="F117" s="89" t="s">
         <v>170</v>
       </c>
       <c r="G117" s="18" t="s">
@@ -3811,32 +3807,32 @@
       <c r="H117" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="I117" s="68" t="s">
+      <c r="I117" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="118" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C118" s="13"/>
-      <c r="D118" s="63"/>
-      <c r="E118" s="65"/>
-      <c r="F118" s="67"/>
+      <c r="D118" s="93"/>
+      <c r="E118" s="96"/>
+      <c r="F118" s="91"/>
       <c r="G118" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H118" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="I118" s="69"/>
+      <c r="I118" s="63"/>
     </row>
     <row r="119" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C119" s="13"/>
-      <c r="D119" s="62" t="s">
+      <c r="D119" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="E119" s="64" t="s">
+      <c r="E119" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F119" s="66" t="s">
+      <c r="F119" s="89" t="s">
         <v>174</v>
       </c>
       <c r="G119" s="18" t="s">
@@ -3845,58 +3841,58 @@
       <c r="H119" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="I119" s="68" t="s">
+      <c r="I119" s="62" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="120" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C120" s="13"/>
-      <c r="D120" s="86"/>
-      <c r="E120" s="84"/>
-      <c r="F120" s="85"/>
+      <c r="D120" s="97"/>
+      <c r="E120" s="95"/>
+      <c r="F120" s="90"/>
       <c r="G120" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H120" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="I120" s="144"/>
+      <c r="I120" s="67"/>
     </row>
     <row r="121" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C121" s="13"/>
-      <c r="D121" s="86"/>
-      <c r="E121" s="84"/>
-      <c r="F121" s="85"/>
+      <c r="D121" s="97"/>
+      <c r="E121" s="95"/>
+      <c r="F121" s="90"/>
       <c r="G121" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H121" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I121" s="144"/>
+      <c r="I121" s="67"/>
     </row>
     <row r="122" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C122" s="13"/>
-      <c r="D122" s="63"/>
-      <c r="E122" s="65"/>
-      <c r="F122" s="67"/>
+      <c r="D122" s="93"/>
+      <c r="E122" s="96"/>
+      <c r="F122" s="91"/>
       <c r="G122" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H122" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I122" s="69"/>
+      <c r="I122" s="63"/>
     </row>
     <row r="123" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C123" s="13"/>
-      <c r="D123" s="62" t="s">
+      <c r="D123" s="92" t="s">
         <v>176</v>
       </c>
-      <c r="E123" s="64" t="s">
+      <c r="E123" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F123" s="66" t="s">
+      <c r="F123" s="89" t="s">
         <v>177</v>
       </c>
       <c r="G123" s="18" t="s">
@@ -3905,145 +3901,92 @@
       <c r="H123" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I123" s="68" t="s">
+      <c r="I123" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="124" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C124" s="15"/>
-      <c r="D124" s="63"/>
-      <c r="E124" s="65"/>
-      <c r="F124" s="67"/>
+      <c r="D124" s="93"/>
+      <c r="E124" s="96"/>
+      <c r="F124" s="91"/>
       <c r="G124" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H124" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I124" s="69"/>
+      <c r="I124" s="63"/>
     </row>
     <row r="125" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C125" s="13"/>
-      <c r="D125" s="62" t="s">
+      <c r="D125" s="92" t="s">
         <v>198</v>
       </c>
-      <c r="E125" s="64" t="s">
+      <c r="E125" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="F125" s="66" t="s">
+      <c r="F125" s="89" t="s">
         <v>199</v>
       </c>
       <c r="G125" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H125" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="I125" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="I125" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="126" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C126" s="15"/>
-      <c r="D126" s="63"/>
-      <c r="E126" s="65"/>
-      <c r="F126" s="67"/>
+      <c r="D126" s="93"/>
+      <c r="E126" s="96"/>
+      <c r="F126" s="91"/>
       <c r="G126" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H126" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I126" s="69"/>
+        <v>172</v>
+      </c>
+      <c r="I126" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="143">
-    <mergeCell ref="I123:I124"/>
-    <mergeCell ref="I85:I87"/>
-    <mergeCell ref="I97:I99"/>
-    <mergeCell ref="I100:I103"/>
-    <mergeCell ref="I104:I107"/>
-    <mergeCell ref="I108:I111"/>
-    <mergeCell ref="I88:I90"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="I75:I78"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I60"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="I112:I114"/>
-    <mergeCell ref="I115:I116"/>
-    <mergeCell ref="I117:I118"/>
-    <mergeCell ref="I119:I122"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="I82:I84"/>
-    <mergeCell ref="I79:I81"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="F119:F122"/>
-    <mergeCell ref="D123:D124"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="E119:E122"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="E117:E118"/>
-    <mergeCell ref="D108:D111"/>
-    <mergeCell ref="F108:F111"/>
-    <mergeCell ref="D112:D114"/>
-    <mergeCell ref="F112:F114"/>
-    <mergeCell ref="D115:D116"/>
-    <mergeCell ref="F115:F116"/>
-    <mergeCell ref="E108:E111"/>
-    <mergeCell ref="E112:E114"/>
-    <mergeCell ref="E115:E116"/>
-    <mergeCell ref="F117:F118"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="D119:D122"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="F65:F70"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="I125:I126"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="E91:E93"/>
+    <mergeCell ref="F91:F93"/>
+    <mergeCell ref="C86:C96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="I91:I93"/>
+    <mergeCell ref="E104:E107"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="E97:E99"/>
+    <mergeCell ref="F104:F107"/>
+    <mergeCell ref="D104:D107"/>
+    <mergeCell ref="F100:F103"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="F97:F99"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E82:E84"/>
+    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="E79:E81"/>
+    <mergeCell ref="F79:F81"/>
+    <mergeCell ref="F82:F84"/>
+    <mergeCell ref="D82:D84"/>
+    <mergeCell ref="F85:F87"/>
     <mergeCell ref="C70:C74"/>
     <mergeCell ref="D71:D74"/>
     <mergeCell ref="E71:E74"/>
@@ -4068,39 +4011,92 @@
     <mergeCell ref="D49:D51"/>
     <mergeCell ref="E49:E51"/>
     <mergeCell ref="I65:I70"/>
-    <mergeCell ref="E82:E84"/>
-    <mergeCell ref="D85:D87"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="E79:E81"/>
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="D82:D84"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="E125:E126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="I125:I126"/>
-    <mergeCell ref="D88:D90"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="E91:E93"/>
-    <mergeCell ref="F91:F93"/>
-    <mergeCell ref="C86:C96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="I91:I93"/>
-    <mergeCell ref="E104:E107"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="E97:E99"/>
-    <mergeCell ref="F104:F107"/>
-    <mergeCell ref="D104:D107"/>
-    <mergeCell ref="F100:F103"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="F97:F99"/>
-    <mergeCell ref="D97:D99"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="F119:F122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="F123:F124"/>
+    <mergeCell ref="E119:E122"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="E117:E118"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="F108:F111"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="F112:F114"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="F115:F116"/>
+    <mergeCell ref="E108:E111"/>
+    <mergeCell ref="E112:E114"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="F117:F118"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="D119:D122"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="I112:I114"/>
+    <mergeCell ref="I115:I116"/>
+    <mergeCell ref="I117:I118"/>
+    <mergeCell ref="I119:I122"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="I82:I84"/>
+    <mergeCell ref="I79:I81"/>
+    <mergeCell ref="I123:I124"/>
+    <mergeCell ref="I85:I87"/>
+    <mergeCell ref="I97:I99"/>
+    <mergeCell ref="I100:I103"/>
+    <mergeCell ref="I104:I107"/>
+    <mergeCell ref="I108:I111"/>
+    <mergeCell ref="I88:I90"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="I75:I78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion del Endpoint.xlsx añadiendo o el endpoint de eliminar un customer por el id
</commit_message>
<xml_diff>
--- a/.readmeFiles/Endpoints.xlsx
+++ b/.readmeFiles/Endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/dceballr_emeal_nttdata_com/Documents/Escritorio/Backend/Repositorio/back-end-framework/.readmeFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/pcalvenl_emeal_nttdata_com/Documents/Escritorio/gitTarjetitas/back-end-framework/.readmeFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="438" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8282590D-4C2D-461C-99A0-8C9B6200F954}"/>
+  <xr:revisionPtr revIDLastSave="495" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0F463AF-E117-4214-8C8E-A04638FE6420}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="221">
   <si>
     <t>HTTP Method</t>
   </si>
@@ -464,9 +464,6 @@
     <t>Deletes a user by their email</t>
   </si>
   <si>
-    <t>"Customer deleted successfully"</t>
-  </si>
-  <si>
     <t>"Customer not found"</t>
   </si>
   <si>
@@ -687,13 +684,28 @@
   </si>
   <si>
     <t>"The new monthly limit must be greater than 0"</t>
+  </si>
+  <si>
+    <t>/public/customer/delete/{customerId}</t>
+  </si>
+  <si>
+    <t>Deletes a user by their customer Id</t>
+  </si>
+  <si>
+    <t>"Customer deleted succesfully"</t>
+  </si>
+  <si>
+    <t>"Error ocurred during deletion"</t>
+  </si>
+  <si>
+    <t>"The customer has been deleted successfully."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -747,8 +759,27 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -797,8 +828,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDDDD"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1187,6 +1224,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1203,7 +1295,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1372,12 +1464,63 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1387,7 +1530,64 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1399,29 +1599,95 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1444,185 +1710,65 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="8" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1973,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA3F6E-09E5-46A7-9DF8-4B95ED8D48E7}">
-  <dimension ref="B2:I126"/>
+  <dimension ref="B2:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C101" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H133" sqref="H133"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2116,13 +2262,13 @@
     </row>
     <row r="9" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="5"/>
-      <c r="D9" s="73" t="s">
+      <c r="D9" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="73" t="s">
+      <c r="E9" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="129" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -2131,45 +2277,45 @@
       <c r="H9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="71" t="s">
+      <c r="I9" s="135" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="5"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="73"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="129"/>
       <c r="G10" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="71"/>
+      <c r="I10" s="135"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="5"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="73"/>
+      <c r="D11" s="129"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="129"/>
       <c r="G11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="71"/>
+      <c r="I11" s="135"/>
     </row>
     <row r="12" spans="2:9" ht="28.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="5"/>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="129" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="73" t="s">
+      <c r="E12" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="129" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="38" t="s">
@@ -2178,35 +2324,35 @@
       <c r="H12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="71" t="s">
+      <c r="I12" s="135" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="5"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="73"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="129"/>
       <c r="G13" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="71"/>
+      <c r="I13" s="135"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="5"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="73"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="129"/>
       <c r="G14" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="71"/>
+      <c r="I14" s="135"/>
     </row>
     <row r="15" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="5"/>
@@ -2305,13 +2451,13 @@
     </row>
     <row r="20" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
-      <c r="D20" s="73" t="s">
+      <c r="D20" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="73" t="s">
+      <c r="E20" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="129" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="39" t="s">
@@ -2320,58 +2466,58 @@
       <c r="H20" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="71" t="s">
+      <c r="I20" s="135" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="73"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="129"/>
       <c r="G21" s="39" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="71"/>
+      <c r="I21" s="135"/>
     </row>
     <row r="22" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="73"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="129"/>
       <c r="G22" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="71"/>
+      <c r="I22" s="135"/>
     </row>
     <row r="23" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C23" s="5"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="73"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="129"/>
       <c r="G23" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H23" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="71"/>
+      <c r="I23" s="135"/>
     </row>
     <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="5"/>
-      <c r="D24" s="73" t="s">
+      <c r="D24" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="73" t="s">
+      <c r="E24" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="129" t="s">
         <v>57</v>
       </c>
       <c r="G24" s="38" t="s">
@@ -2380,45 +2526,45 @@
       <c r="H24" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="71" t="s">
+      <c r="I24" s="135" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="5"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="73"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="129"/>
       <c r="G25" s="42" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="I25" s="71"/>
+      <c r="I25" s="135"/>
     </row>
     <row r="26" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C26" s="5"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="98"/>
-      <c r="F26" s="73"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="129"/>
       <c r="G26" s="42" t="s">
         <v>53</v>
       </c>
       <c r="H26" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="71"/>
+      <c r="I26" s="135"/>
     </row>
     <row r="27" spans="3:9" ht="58.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C27" s="5"/>
-      <c r="D27" s="73" t="s">
+      <c r="D27" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="75" t="s">
+      <c r="E27" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="134" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="38" t="s">
@@ -2427,84 +2573,84 @@
       <c r="H27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="71" t="s">
+      <c r="I27" s="135" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="5"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="75"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="134"/>
       <c r="G28" s="42" t="s">
         <v>63</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="71"/>
+      <c r="I28" s="135"/>
     </row>
     <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="5"/>
-      <c r="D29" s="99" t="s">
-        <v>181</v>
-      </c>
-      <c r="E29" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="76" t="s">
+      <c r="D29" s="131" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="79" t="s">
+      <c r="G29" s="137" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="81" t="s">
+      <c r="H29" s="139" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="86" t="s">
+      <c r="I29" s="116" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="3:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="5"/>
-      <c r="D30" s="100"/>
-      <c r="E30" s="103"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="80"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="87"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="111"/>
+      <c r="F30" s="114"/>
+      <c r="G30" s="138"/>
+      <c r="H30" s="139"/>
+      <c r="I30" s="117"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C31" s="5"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="82" t="s">
+      <c r="D31" s="132"/>
+      <c r="E31" s="111"/>
+      <c r="F31" s="114"/>
+      <c r="G31" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="84" t="s">
+      <c r="H31" s="142" t="s">
         <v>66</v>
       </c>
-      <c r="I31" s="87"/>
+      <c r="I31" s="117"/>
     </row>
     <row r="32" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="5"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="104"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="85"/>
-      <c r="I32" s="88"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="141"/>
+      <c r="H32" s="143"/>
+      <c r="I32" s="118"/>
     </row>
     <row r="33" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="5"/>
-      <c r="D33" s="75" t="s">
+      <c r="D33" s="134" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="75" t="s">
+      <c r="E33" s="130" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="134" t="s">
         <v>68</v>
       </c>
       <c r="G33" s="54" t="s">
@@ -2513,201 +2659,201 @@
       <c r="H33" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="71" t="s">
+      <c r="I33" s="135" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C34" s="5"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="75"/>
+      <c r="D34" s="134"/>
+      <c r="E34" s="130"/>
+      <c r="F34" s="134"/>
       <c r="G34" s="47" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I34" s="71"/>
+      <c r="I34" s="135"/>
     </row>
     <row r="35" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C35" s="5"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="98"/>
-      <c r="F35" s="75"/>
+      <c r="D35" s="134"/>
+      <c r="E35" s="130"/>
+      <c r="F35" s="134"/>
       <c r="G35" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H35" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="71"/>
+      <c r="I35" s="135"/>
     </row>
     <row r="36" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C36" s="5"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="75"/>
+      <c r="D36" s="134"/>
+      <c r="E36" s="130"/>
+      <c r="F36" s="134"/>
       <c r="G36" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H36" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I36" s="71"/>
+      <c r="I36" s="135"/>
     </row>
     <row r="37" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C37" s="5"/>
-      <c r="D37" s="128" t="s">
+      <c r="D37" s="107" t="s">
+        <v>181</v>
+      </c>
+      <c r="E37" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="113" t="s">
         <v>182</v>
-      </c>
-      <c r="E37" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="76" t="s">
-        <v>183</v>
       </c>
       <c r="G37" s="57" t="s">
         <v>28</v>
       </c>
       <c r="H37" s="61" t="s">
-        <v>185</v>
-      </c>
-      <c r="I37" s="86" t="s">
         <v>184</v>
+      </c>
+      <c r="I37" s="116" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C38" s="5"/>
-      <c r="D38" s="129"/>
-      <c r="E38" s="103"/>
-      <c r="F38" s="77"/>
+      <c r="D38" s="108"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="114"/>
       <c r="G38" s="42" t="s">
         <v>70</v>
       </c>
       <c r="H38" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="87"/>
+      <c r="I38" s="117"/>
     </row>
     <row r="39" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="131"/>
-      <c r="D39" s="130"/>
-      <c r="E39" s="104"/>
-      <c r="F39" s="78"/>
+      <c r="C39" s="119"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="115"/>
       <c r="G39" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H39" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="I39" s="88"/>
+      <c r="I39" s="118"/>
     </row>
     <row r="40" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="131"/>
-      <c r="D40" s="128" t="s">
+      <c r="C40" s="119"/>
+      <c r="D40" s="107" t="s">
+        <v>185</v>
+      </c>
+      <c r="E40" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="113" t="s">
         <v>186</v>
-      </c>
-      <c r="E40" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="76" t="s">
-        <v>187</v>
       </c>
       <c r="G40" s="57" t="s">
         <v>28</v>
       </c>
       <c r="H40" s="61" t="s">
-        <v>185</v>
-      </c>
-      <c r="I40" s="86" t="s">
         <v>184</v>
       </c>
+      <c r="I40" s="116" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="41" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C41" s="131"/>
-      <c r="D41" s="129"/>
-      <c r="E41" s="103"/>
-      <c r="F41" s="77"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="108"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="114"/>
       <c r="G41" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H41" s="55" t="s">
-        <v>200</v>
-      </c>
-      <c r="I41" s="87"/>
+        <v>199</v>
+      </c>
+      <c r="I41" s="117"/>
     </row>
     <row r="42" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C42" s="131"/>
-      <c r="D42" s="130"/>
-      <c r="E42" s="104"/>
-      <c r="F42" s="78"/>
+      <c r="C42" s="119"/>
+      <c r="D42" s="109"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="115"/>
       <c r="G42" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H42" s="55" t="s">
-        <v>203</v>
-      </c>
-      <c r="I42" s="88"/>
+        <v>202</v>
+      </c>
+      <c r="I42" s="118"/>
     </row>
     <row r="43" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C43" s="131"/>
-      <c r="D43" s="128" t="s">
+      <c r="C43" s="119"/>
+      <c r="D43" s="107" t="s">
+        <v>187</v>
+      </c>
+      <c r="E43" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="113" t="s">
         <v>188</v>
-      </c>
-      <c r="E43" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="76" t="s">
-        <v>189</v>
       </c>
       <c r="G43" s="57" t="s">
         <v>28</v>
       </c>
       <c r="H43" s="61" t="s">
-        <v>185</v>
-      </c>
-      <c r="I43" s="86" t="s">
         <v>184</v>
       </c>
+      <c r="I43" s="116" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="44" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C44" s="131"/>
-      <c r="D44" s="129"/>
-      <c r="E44" s="103"/>
-      <c r="F44" s="77"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="108"/>
+      <c r="E44" s="111"/>
+      <c r="F44" s="114"/>
       <c r="G44" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H44" s="55" t="s">
-        <v>204</v>
-      </c>
-      <c r="I44" s="87"/>
+        <v>203</v>
+      </c>
+      <c r="I44" s="117"/>
     </row>
     <row r="45" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C45" s="132"/>
-      <c r="D45" s="130"/>
-      <c r="E45" s="104"/>
-      <c r="F45" s="78"/>
+      <c r="C45" s="120"/>
+      <c r="D45" s="109"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="115"/>
       <c r="G45" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H45" s="55" t="s">
-        <v>205</v>
-      </c>
-      <c r="I45" s="88"/>
+        <v>204</v>
+      </c>
+      <c r="I45" s="118"/>
     </row>
     <row r="46" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="133" t="s">
+      <c r="D46" s="121" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="134" t="s">
+      <c r="E46" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="74" t="s">
+      <c r="F46" s="136" t="s">
         <v>78</v>
       </c>
       <c r="G46" s="30" t="s">
@@ -2716,45 +2862,45 @@
       <c r="H46" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="72" t="s">
+      <c r="I46" s="145" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C47" s="16"/>
-      <c r="D47" s="133"/>
-      <c r="E47" s="134"/>
-      <c r="F47" s="74"/>
+      <c r="D47" s="121"/>
+      <c r="E47" s="122"/>
+      <c r="F47" s="136"/>
       <c r="G47" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="I47" s="72"/>
+      <c r="I47" s="145"/>
     </row>
     <row r="48" spans="3:9" ht="31.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C48" s="7"/>
-      <c r="D48" s="133"/>
-      <c r="E48" s="134"/>
-      <c r="F48" s="74"/>
+      <c r="D48" s="121"/>
+      <c r="E48" s="122"/>
+      <c r="F48" s="136"/>
       <c r="G48" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H48" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="72"/>
+      <c r="I48" s="145"/>
     </row>
     <row r="49" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C49" s="7"/>
-      <c r="D49" s="120" t="s">
+      <c r="D49" s="123" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="105" t="s">
+      <c r="E49" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="111" t="s">
+      <c r="F49" s="101" t="s">
         <v>85</v>
       </c>
       <c r="G49" s="30" t="s">
@@ -2763,45 +2909,45 @@
       <c r="H49" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I49" s="68" t="s">
+      <c r="I49" s="104" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="50" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="7"/>
-      <c r="D50" s="122"/>
-      <c r="E50" s="106"/>
-      <c r="F50" s="112"/>
+      <c r="D50" s="124"/>
+      <c r="E50" s="99"/>
+      <c r="F50" s="102"/>
       <c r="G50" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H50" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="I50" s="69"/>
+      <c r="I50" s="105"/>
     </row>
     <row r="51" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C51" s="7"/>
-      <c r="D51" s="121"/>
-      <c r="E51" s="107"/>
-      <c r="F51" s="113"/>
+      <c r="D51" s="125"/>
+      <c r="E51" s="100"/>
+      <c r="F51" s="103"/>
       <c r="G51" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H51" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I51" s="70"/>
+      <c r="I51" s="106"/>
     </row>
     <row r="52" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C52" s="7"/>
-      <c r="D52" s="120" t="s">
+      <c r="D52" s="123" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="105" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="111" t="s">
+      <c r="E52" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="101" t="s">
         <v>91</v>
       </c>
       <c r="G52" s="30" t="s">
@@ -2810,22 +2956,22 @@
       <c r="H52" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="68" t="s">
+      <c r="I52" s="104" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C53" s="7"/>
-      <c r="D53" s="121"/>
-      <c r="E53" s="107"/>
-      <c r="F53" s="113"/>
+      <c r="D53" s="125"/>
+      <c r="E53" s="100"/>
+      <c r="F53" s="103"/>
       <c r="G53" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H53" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="I53" s="70"/>
+      <c r="I53" s="106"/>
     </row>
     <row r="54" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C54" s="7"/>
@@ -2833,7 +2979,7 @@
       <c r="E54" s="49"/>
       <c r="F54" s="48"/>
       <c r="G54" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H54" s="31" t="s">
         <v>80</v>
@@ -2843,13 +2989,13 @@
     <row r="55" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C55" s="7"/>
       <c r="D55" s="50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E55" s="49" t="s">
         <v>77</v>
       </c>
       <c r="F55" s="48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G55" s="32" t="s">
         <v>53</v>
@@ -2872,13 +3018,13 @@
     </row>
     <row r="57" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C57" s="7"/>
-      <c r="D57" s="120" t="s">
+      <c r="D57" s="123" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="105" t="s">
+      <c r="E57" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="111" t="s">
+      <c r="F57" s="101" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="30" t="s">
@@ -2887,58 +3033,58 @@
       <c r="H57" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="I57" s="68" t="s">
+      <c r="I57" s="104" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="58" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C58" s="7"/>
-      <c r="D58" s="122"/>
-      <c r="E58" s="106"/>
-      <c r="F58" s="112"/>
+      <c r="D58" s="124"/>
+      <c r="E58" s="99"/>
+      <c r="F58" s="102"/>
       <c r="G58" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H58" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="I58" s="69"/>
+      <c r="I58" s="105"/>
     </row>
     <row r="59" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C59" s="7"/>
-      <c r="D59" s="122"/>
-      <c r="E59" s="106"/>
-      <c r="F59" s="112"/>
+      <c r="D59" s="124"/>
+      <c r="E59" s="99"/>
+      <c r="F59" s="102"/>
       <c r="G59" s="32" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I59" s="69"/>
+      <c r="I59" s="105"/>
     </row>
     <row r="60" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C60" s="7"/>
-      <c r="D60" s="121"/>
-      <c r="E60" s="107"/>
-      <c r="F60" s="113"/>
+      <c r="D60" s="125"/>
+      <c r="E60" s="100"/>
+      <c r="F60" s="103"/>
       <c r="G60" s="32" t="s">
         <v>100</v>
       </c>
       <c r="H60" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I60" s="70"/>
+      <c r="I60" s="106"/>
     </row>
     <row r="61" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C61" s="7"/>
-      <c r="D61" s="120" t="s">
+      <c r="D61" s="123" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="105" t="s">
+      <c r="E61" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="F61" s="111" t="s">
+      <c r="F61" s="101" t="s">
         <v>104</v>
       </c>
       <c r="G61" s="30" t="s">
@@ -2947,58 +3093,58 @@
       <c r="H61" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="I61" s="68" t="s">
+      <c r="I61" s="104" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C62" s="7"/>
-      <c r="D62" s="122"/>
-      <c r="E62" s="106"/>
-      <c r="F62" s="112"/>
+      <c r="D62" s="124"/>
+      <c r="E62" s="99"/>
+      <c r="F62" s="102"/>
       <c r="G62" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H62" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I62" s="69"/>
+      <c r="I62" s="105"/>
     </row>
     <row r="63" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C63" s="7"/>
-      <c r="D63" s="122"/>
-      <c r="E63" s="106"/>
-      <c r="F63" s="112"/>
+      <c r="D63" s="124"/>
+      <c r="E63" s="99"/>
+      <c r="F63" s="102"/>
       <c r="G63" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H63" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="I63" s="69"/>
+      <c r="I63" s="105"/>
     </row>
     <row r="64" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C64" s="7"/>
-      <c r="D64" s="121"/>
-      <c r="E64" s="107"/>
-      <c r="F64" s="113"/>
+      <c r="D64" s="125"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="103"/>
       <c r="G64" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H64" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I64" s="70"/>
+      <c r="I64" s="106"/>
     </row>
     <row r="65" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C65" s="7"/>
-      <c r="D65" s="120" t="s">
+      <c r="D65" s="123" t="s">
         <v>109</v>
       </c>
-      <c r="E65" s="105" t="s">
+      <c r="E65" s="98" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="111" t="s">
+      <c r="F65" s="101" t="s">
         <v>111</v>
       </c>
       <c r="G65" s="30" t="s">
@@ -3007,146 +3153,146 @@
       <c r="H65" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="I65" s="68" t="s">
+      <c r="I65" s="104" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C66" s="7"/>
-      <c r="D66" s="122"/>
-      <c r="E66" s="106"/>
-      <c r="F66" s="112"/>
+      <c r="D66" s="124"/>
+      <c r="E66" s="99"/>
+      <c r="F66" s="102"/>
       <c r="G66" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H66" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I66" s="69"/>
+      <c r="I66" s="105"/>
     </row>
     <row r="67" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C67" s="7"/>
-      <c r="D67" s="122"/>
-      <c r="E67" s="106"/>
-      <c r="F67" s="112"/>
+      <c r="D67" s="124"/>
+      <c r="E67" s="99"/>
+      <c r="F67" s="102"/>
       <c r="G67" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H67" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="I67" s="69"/>
+      <c r="I67" s="105"/>
     </row>
     <row r="68" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C68" s="7"/>
-      <c r="D68" s="122"/>
-      <c r="E68" s="106"/>
-      <c r="F68" s="112"/>
+      <c r="D68" s="124"/>
+      <c r="E68" s="99"/>
+      <c r="F68" s="102"/>
       <c r="G68" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H68" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="I68" s="69"/>
+      <c r="I68" s="105"/>
     </row>
     <row r="69" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C69" s="7"/>
-      <c r="D69" s="122"/>
-      <c r="E69" s="106"/>
-      <c r="F69" s="112"/>
+      <c r="D69" s="124"/>
+      <c r="E69" s="99"/>
+      <c r="F69" s="102"/>
       <c r="G69" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H69" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I69" s="69"/>
+      <c r="I69" s="105"/>
     </row>
     <row r="70" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C70" s="123"/>
-      <c r="D70" s="121"/>
-      <c r="E70" s="107"/>
-      <c r="F70" s="113"/>
+      <c r="C70" s="93"/>
+      <c r="D70" s="125"/>
+      <c r="E70" s="100"/>
+      <c r="F70" s="103"/>
       <c r="G70" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H70" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="I70" s="70"/>
+      <c r="I70" s="106"/>
     </row>
     <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C71" s="123"/>
-      <c r="D71" s="125" t="s">
+      <c r="C71" s="93"/>
+      <c r="D71" s="95" t="s">
+        <v>189</v>
+      </c>
+      <c r="E71" s="98" t="s">
         <v>190</v>
       </c>
-      <c r="E71" s="105" t="s">
+      <c r="F71" s="101" t="s">
         <v>191</v>
-      </c>
-      <c r="F71" s="111" t="s">
-        <v>192</v>
       </c>
       <c r="G71" s="30" t="s">
         <v>28</v>
       </c>
       <c r="H71" s="58" t="s">
-        <v>202</v>
-      </c>
-      <c r="I71" s="68" t="s">
-        <v>184</v>
+        <v>201</v>
+      </c>
+      <c r="I71" s="104" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C72" s="123"/>
-      <c r="D72" s="126"/>
-      <c r="E72" s="106"/>
-      <c r="F72" s="112"/>
+      <c r="C72" s="93"/>
+      <c r="D72" s="96"/>
+      <c r="E72" s="99"/>
+      <c r="F72" s="102"/>
       <c r="G72" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H72" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="I72" s="69"/>
+      <c r="I72" s="105"/>
     </row>
     <row r="73" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C73" s="123"/>
-      <c r="D73" s="126"/>
-      <c r="E73" s="106"/>
-      <c r="F73" s="112"/>
+      <c r="C73" s="93"/>
+      <c r="D73" s="96"/>
+      <c r="E73" s="99"/>
+      <c r="F73" s="102"/>
       <c r="G73" s="32" t="s">
         <v>72</v>
       </c>
       <c r="H73" s="52" t="s">
-        <v>200</v>
-      </c>
-      <c r="I73" s="69"/>
+        <v>199</v>
+      </c>
+      <c r="I73" s="105"/>
     </row>
     <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C74" s="124"/>
-      <c r="D74" s="127"/>
-      <c r="E74" s="107"/>
-      <c r="F74" s="113"/>
+      <c r="C74" s="94"/>
+      <c r="D74" s="97"/>
+      <c r="E74" s="100"/>
+      <c r="F74" s="103"/>
       <c r="G74" s="60" t="s">
         <v>31</v>
       </c>
       <c r="H74" s="52" t="s">
-        <v>201</v>
-      </c>
-      <c r="I74" s="70"/>
+        <v>200</v>
+      </c>
+      <c r="I74" s="106"/>
     </row>
     <row r="75" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D75" s="117" t="s">
+      <c r="D75" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="114" t="s">
+      <c r="E75" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F75" s="108" t="s">
+      <c r="F75" s="126" t="s">
         <v>121</v>
       </c>
       <c r="G75" s="26" t="s">
@@ -3155,58 +3301,58 @@
       <c r="H75" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="I75" s="64" t="s">
+      <c r="I75" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="76" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C76" s="9"/>
-      <c r="D76" s="118"/>
-      <c r="E76" s="115"/>
-      <c r="F76" s="109"/>
+      <c r="D76" s="88"/>
+      <c r="E76" s="74"/>
+      <c r="F76" s="127"/>
       <c r="G76" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="I76" s="65"/>
+      <c r="I76" s="82"/>
     </row>
     <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C77" s="10"/>
-      <c r="D77" s="118"/>
-      <c r="E77" s="115"/>
-      <c r="F77" s="109"/>
+      <c r="D77" s="88"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="127"/>
       <c r="G77" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H77" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I77" s="65"/>
+      <c r="I77" s="82"/>
     </row>
     <row r="78" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C78" s="10"/>
-      <c r="D78" s="119"/>
-      <c r="E78" s="116"/>
-      <c r="F78" s="110"/>
+      <c r="D78" s="89"/>
+      <c r="E78" s="75"/>
+      <c r="F78" s="128"/>
       <c r="G78" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H78" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="I78" s="66"/>
+      <c r="I78" s="83"/>
     </row>
     <row r="79" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C79" s="10"/>
-      <c r="D79" s="117" t="s">
+      <c r="D79" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="E79" s="114" t="s">
+      <c r="E79" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="135" t="s">
+      <c r="F79" s="90" t="s">
         <v>127</v>
       </c>
       <c r="G79" s="26" t="s">
@@ -3215,45 +3361,45 @@
       <c r="H79" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="I79" s="64" t="s">
+      <c r="I79" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="80" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C80" s="10"/>
-      <c r="D80" s="118"/>
-      <c r="E80" s="115"/>
-      <c r="F80" s="136"/>
+      <c r="D80" s="88"/>
+      <c r="E80" s="74"/>
+      <c r="F80" s="91"/>
       <c r="G80" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H80" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="I80" s="65"/>
+      <c r="I80" s="82"/>
     </row>
     <row r="81" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C81" s="10"/>
-      <c r="D81" s="119"/>
-      <c r="E81" s="116"/>
-      <c r="F81" s="137"/>
+      <c r="D81" s="89"/>
+      <c r="E81" s="75"/>
+      <c r="F81" s="92"/>
       <c r="G81" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H81" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I81" s="66"/>
+      <c r="I81" s="83"/>
     </row>
     <row r="82" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C82" s="10"/>
-      <c r="D82" s="117" t="s">
+      <c r="D82" s="87" t="s">
         <v>131</v>
       </c>
-      <c r="E82" s="114" t="s">
+      <c r="E82" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F82" s="135" t="s">
+      <c r="F82" s="90" t="s">
         <v>132</v>
       </c>
       <c r="G82" s="26" t="s">
@@ -3262,45 +3408,45 @@
       <c r="H82" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="I82" s="64" t="s">
+      <c r="I82" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="83" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C83" s="10"/>
-      <c r="D83" s="118"/>
-      <c r="E83" s="115"/>
-      <c r="F83" s="136"/>
+      <c r="D83" s="88"/>
+      <c r="E83" s="74"/>
+      <c r="F83" s="91"/>
       <c r="G83" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H83" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="I83" s="65"/>
+      <c r="I83" s="82"/>
     </row>
     <row r="84" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C84" s="10"/>
-      <c r="D84" s="119"/>
-      <c r="E84" s="116"/>
-      <c r="F84" s="137"/>
+      <c r="D84" s="89"/>
+      <c r="E84" s="75"/>
+      <c r="F84" s="92"/>
       <c r="G84" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H84" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I84" s="66"/>
+      <c r="I84" s="83"/>
     </row>
     <row r="85" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C85" s="10"/>
-      <c r="D85" s="117" t="s">
+      <c r="D85" s="87" t="s">
         <v>135</v>
       </c>
-      <c r="E85" s="114" t="s">
+      <c r="E85" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F85" s="135" t="s">
+      <c r="F85" s="90" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="26" t="s">
@@ -3309,684 +3455,1245 @@
       <c r="H85" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="I85" s="64" t="s">
+      <c r="I85" s="81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="86" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C86" s="144"/>
-      <c r="D86" s="118"/>
-      <c r="E86" s="115"/>
-      <c r="F86" s="136"/>
+      <c r="C86" s="79"/>
+      <c r="D86" s="88"/>
+      <c r="E86" s="74"/>
+      <c r="F86" s="91"/>
       <c r="G86" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H86" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="I86" s="65"/>
+      <c r="I86" s="82"/>
     </row>
     <row r="87" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C87" s="144"/>
-      <c r="D87" s="119"/>
-      <c r="E87" s="116"/>
-      <c r="F87" s="137"/>
+      <c r="C87" s="79"/>
+      <c r="D87" s="89"/>
+      <c r="E87" s="75"/>
+      <c r="F87" s="92"/>
       <c r="G87" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H87" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I87" s="66"/>
+      <c r="I87" s="83"/>
     </row>
     <row r="88" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C88" s="144"/>
-      <c r="D88" s="138" t="s">
-        <v>193</v>
-      </c>
-      <c r="E88" s="114" t="s">
+      <c r="C88" s="79"/>
+      <c r="D88" s="70" t="s">
+        <v>192</v>
+      </c>
+      <c r="E88" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F88" s="141" t="s">
-        <v>196</v>
+      <c r="F88" s="76" t="s">
+        <v>195</v>
       </c>
       <c r="G88" s="26" t="s">
         <v>28</v>
       </c>
       <c r="H88" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="I88" s="81" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C89" s="79"/>
+      <c r="D89" s="71"/>
+      <c r="E89" s="74"/>
+      <c r="F89" s="77"/>
+      <c r="G89" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="H89" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="I89" s="82"/>
+    </row>
+    <row r="90" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C90" s="79"/>
+      <c r="D90" s="72"/>
+      <c r="E90" s="75"/>
+      <c r="F90" s="78"/>
+      <c r="G90" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="H90" s="56" t="s">
+        <v>208</v>
+      </c>
+      <c r="I90" s="83"/>
+    </row>
+    <row r="91" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C91" s="79"/>
+      <c r="D91" s="70" t="s">
+        <v>193</v>
+      </c>
+      <c r="E91" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="F91" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="G91" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I88" s="64" t="s">
+      <c r="H91" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="I91" s="81" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C89" s="144"/>
-      <c r="D89" s="139"/>
-      <c r="E89" s="115"/>
-      <c r="F89" s="142"/>
-      <c r="G89" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="H89" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="I89" s="65"/>
-    </row>
-    <row r="90" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C90" s="144"/>
-      <c r="D90" s="140"/>
-      <c r="E90" s="116"/>
-      <c r="F90" s="143"/>
-      <c r="G90" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="H90" s="56" t="s">
-        <v>209</v>
-      </c>
-      <c r="I90" s="66"/>
-    </row>
-    <row r="91" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C91" s="144"/>
-      <c r="D91" s="138" t="s">
-        <v>194</v>
-      </c>
-      <c r="E91" s="114" t="s">
-        <v>120</v>
-      </c>
-      <c r="F91" s="141" t="s">
-        <v>197</v>
-      </c>
-      <c r="G91" s="26" t="s">
+    <row r="92" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C92" s="79"/>
+      <c r="D92" s="71"/>
+      <c r="E92" s="74"/>
+      <c r="F92" s="77"/>
+      <c r="G92" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="H91" s="59" t="s">
+      <c r="H92" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="I91" s="64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="92" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C92" s="144"/>
-      <c r="D92" s="139"/>
-      <c r="E92" s="115"/>
-      <c r="F92" s="142"/>
-      <c r="G92" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="H92" s="56" t="s">
-        <v>214</v>
-      </c>
-      <c r="I92" s="65"/>
+      <c r="I92" s="82"/>
     </row>
     <row r="93" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C93" s="144"/>
-      <c r="D93" s="140"/>
-      <c r="E93" s="116"/>
-      <c r="F93" s="143"/>
+      <c r="C93" s="79"/>
+      <c r="D93" s="72"/>
+      <c r="E93" s="75"/>
+      <c r="F93" s="78"/>
       <c r="G93" s="28" t="s">
         <v>72</v>
       </c>
       <c r="H93" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="I93" s="66"/>
+        <v>207</v>
+      </c>
+      <c r="I93" s="83"/>
     </row>
     <row r="94" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C94" s="144"/>
-      <c r="D94" s="138" t="s">
-        <v>195</v>
-      </c>
-      <c r="E94" s="114" t="s">
+      <c r="C94" s="79"/>
+      <c r="D94" s="70" t="s">
+        <v>194</v>
+      </c>
+      <c r="E94" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="F94" s="141" t="s">
-        <v>197</v>
+      <c r="F94" s="76" t="s">
+        <v>196</v>
       </c>
       <c r="G94" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="H94" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="I94" s="81" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C95" s="79"/>
+      <c r="D95" s="71"/>
+      <c r="E95" s="74"/>
+      <c r="F95" s="77"/>
+      <c r="G95" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="H94" s="59" t="s">
+      <c r="H95" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="I94" s="64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="95" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C95" s="144"/>
-      <c r="D95" s="139"/>
-      <c r="E95" s="115"/>
-      <c r="F95" s="142"/>
-      <c r="G95" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="H95" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="I95" s="65"/>
+      <c r="I95" s="82"/>
     </row>
     <row r="96" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C96" s="145"/>
-      <c r="D96" s="140"/>
-      <c r="E96" s="116"/>
-      <c r="F96" s="143"/>
+      <c r="C96" s="80"/>
+      <c r="D96" s="72"/>
+      <c r="E96" s="75"/>
+      <c r="F96" s="78"/>
       <c r="G96" s="28" t="s">
         <v>72</v>
       </c>
       <c r="H96" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="I96" s="66"/>
+        <v>207</v>
+      </c>
+      <c r="I96" s="83"/>
     </row>
     <row r="97" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C97" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D97" s="92" t="s">
+      <c r="D97" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="E97" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F97" s="89" t="s">
+      <c r="E97" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="66" t="s">
         <v>141</v>
       </c>
       <c r="G97" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H97" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="I97" s="62" t="s">
+        <v>220</v>
+      </c>
+      <c r="I97" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="98" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C98" s="12"/>
-      <c r="D98" s="97"/>
-      <c r="E98" s="95"/>
-      <c r="F98" s="90"/>
+      <c r="D98" s="86"/>
+      <c r="E98" s="84"/>
+      <c r="F98" s="85"/>
       <c r="G98" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H98" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="I98" s="67"/>
+        <v>154</v>
+      </c>
+      <c r="I98" s="144"/>
     </row>
     <row r="99" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C99" s="13"/>
-      <c r="D99" s="93"/>
-      <c r="E99" s="96"/>
-      <c r="F99" s="91"/>
-      <c r="G99" s="20" t="s">
+      <c r="D99" s="63"/>
+      <c r="E99" s="65"/>
+      <c r="F99" s="67"/>
+      <c r="G99" s="160" t="s">
+        <v>143</v>
+      </c>
+      <c r="H99" s="161" t="s">
         <v>144</v>
       </c>
-      <c r="H99" s="21" t="s">
+      <c r="I99" s="69"/>
+    </row>
+    <row r="100" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C100" s="13"/>
+      <c r="D100" s="158"/>
+      <c r="E100" s="150" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="155" t="s">
+        <v>217</v>
+      </c>
+      <c r="G100" s="162" t="s">
+        <v>28</v>
+      </c>
+      <c r="H100" s="163" t="s">
+        <v>218</v>
+      </c>
+      <c r="I100" s="153"/>
+    </row>
+    <row r="101" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C101" s="13"/>
+      <c r="D101" s="158" t="s">
+        <v>216</v>
+      </c>
+      <c r="E101" s="151"/>
+      <c r="F101" s="156"/>
+      <c r="G101" s="154" t="s">
+        <v>53</v>
+      </c>
+      <c r="H101" s="149" t="s">
+        <v>142</v>
+      </c>
+      <c r="I101" s="153" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C102" s="13"/>
+      <c r="D102" s="159"/>
+      <c r="E102" s="152"/>
+      <c r="F102" s="157"/>
+      <c r="G102" s="148" t="s">
+        <v>143</v>
+      </c>
+      <c r="H102" s="149" t="s">
+        <v>219</v>
+      </c>
+      <c r="I102" s="153"/>
+    </row>
+    <row r="103" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C103" s="13"/>
+      <c r="D103" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="I99" s="63"/>
-    </row>
-    <row r="100" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C100" s="13"/>
-      <c r="D100" s="92" t="s">
+      <c r="E103" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F103" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="E100" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="89" t="s">
+      <c r="G103" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H103" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G100" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H100" s="19" t="s">
+      <c r="I103" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C104" s="13"/>
+      <c r="D104" s="86"/>
+      <c r="E104" s="84"/>
+      <c r="F104" s="85"/>
+      <c r="G104" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H104" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="I100" s="62" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="101" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C101" s="13"/>
-      <c r="D101" s="97"/>
-      <c r="E101" s="95"/>
-      <c r="F101" s="90"/>
-      <c r="G101" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H101" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="I101" s="67"/>
-    </row>
-    <row r="102" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C102" s="13"/>
-      <c r="D102" s="97"/>
-      <c r="E102" s="95"/>
-      <c r="F102" s="90"/>
-      <c r="G102" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H102" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I102" s="67"/>
-    </row>
-    <row r="103" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C103" s="13"/>
-      <c r="D103" s="93"/>
-      <c r="E103" s="96"/>
-      <c r="F103" s="91"/>
-      <c r="G103" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H103" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="I103" s="63"/>
-    </row>
-    <row r="104" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C104" s="13"/>
-      <c r="D104" s="92" t="s">
-        <v>152</v>
-      </c>
-      <c r="E104" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F104" s="89" t="s">
-        <v>153</v>
-      </c>
-      <c r="G104" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H104" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="I104" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="I104" s="144"/>
     </row>
     <row r="105" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C105" s="13"/>
-      <c r="D105" s="97"/>
-      <c r="E105" s="95"/>
-      <c r="F105" s="90"/>
+      <c r="D105" s="86"/>
+      <c r="E105" s="84"/>
+      <c r="F105" s="85"/>
       <c r="G105" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H105" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I105" s="67"/>
+        <v>149</v>
+      </c>
+      <c r="I105" s="144"/>
     </row>
     <row r="106" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C106" s="13"/>
-      <c r="D106" s="97"/>
-      <c r="E106" s="95"/>
-      <c r="F106" s="90"/>
+      <c r="D106" s="63"/>
+      <c r="E106" s="65"/>
+      <c r="F106" s="67"/>
       <c r="G106" s="20" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="H106" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I106" s="67"/>
-    </row>
-    <row r="107" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>150</v>
+      </c>
+      <c r="I106" s="69"/>
+    </row>
+    <row r="107" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C107" s="13"/>
-      <c r="D107" s="93"/>
-      <c r="E107" s="96"/>
-      <c r="F107" s="91"/>
-      <c r="G107" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="H107" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="I107" s="63"/>
-    </row>
-    <row r="108" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D107" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="E107" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="G107" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H107" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="I107" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C108" s="13"/>
-      <c r="D108" s="92" t="s">
-        <v>158</v>
-      </c>
-      <c r="E108" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F108" s="89" t="s">
-        <v>159</v>
-      </c>
-      <c r="G108" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H108" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="I108" s="62" t="s">
-        <v>29</v>
-      </c>
+      <c r="D108" s="86"/>
+      <c r="E108" s="84"/>
+      <c r="F108" s="85"/>
+      <c r="G108" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H108" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="I108" s="144"/>
     </row>
     <row r="109" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C109" s="13"/>
-      <c r="D109" s="97"/>
-      <c r="E109" s="95"/>
-      <c r="F109" s="90"/>
+      <c r="D109" s="86"/>
+      <c r="E109" s="84"/>
+      <c r="F109" s="85"/>
       <c r="G109" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H109" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="I109" s="144"/>
+    </row>
+    <row r="110" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C110" s="13"/>
+      <c r="D110" s="63"/>
+      <c r="E110" s="65"/>
+      <c r="F110" s="67"/>
+      <c r="G110" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H110" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="I110" s="69"/>
+    </row>
+    <row r="111" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C111" s="13"/>
+      <c r="D111" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="E111" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="G111" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H111" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="I111" s="68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="112" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C112" s="13"/>
+      <c r="D112" s="86"/>
+      <c r="E112" s="84"/>
+      <c r="F112" s="85"/>
+      <c r="G112" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H109" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I109" s="67"/>
-    </row>
-    <row r="110" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C110" s="13"/>
-      <c r="D110" s="97"/>
-      <c r="E110" s="95"/>
-      <c r="F110" s="90"/>
-      <c r="G110" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H110" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I110" s="67"/>
-    </row>
-    <row r="111" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C111" s="13"/>
-      <c r="D111" s="93"/>
-      <c r="E111" s="96"/>
-      <c r="F111" s="91"/>
-      <c r="G111" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="H111" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="I111" s="63"/>
-    </row>
-    <row r="112" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C112" s="13"/>
-      <c r="D112" s="92" t="s">
-        <v>161</v>
-      </c>
-      <c r="E112" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F112" s="89" t="s">
-        <v>162</v>
-      </c>
-      <c r="G112" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H112" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="I112" s="62" t="s">
-        <v>12</v>
-      </c>
+      <c r="H112" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I112" s="144"/>
     </row>
     <row r="113" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C113" s="13"/>
-      <c r="D113" s="97"/>
-      <c r="E113" s="95"/>
-      <c r="F113" s="90"/>
+      <c r="D113" s="86"/>
+      <c r="E113" s="84"/>
+      <c r="F113" s="85"/>
       <c r="G113" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H113" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="I113" s="67"/>
-    </row>
-    <row r="114" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C114" s="14"/>
-      <c r="D114" s="93"/>
-      <c r="E114" s="96"/>
-      <c r="F114" s="91"/>
+        <v>31</v>
+      </c>
+      <c r="H113" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I113" s="144"/>
+    </row>
+    <row r="114" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C114" s="13"/>
+      <c r="D114" s="63"/>
+      <c r="E114" s="65"/>
+      <c r="F114" s="67"/>
       <c r="G114" s="20" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
       <c r="H114" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="I114" s="63"/>
+        <v>156</v>
+      </c>
+      <c r="I114" s="69"/>
     </row>
     <row r="115" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C115" s="14"/>
-      <c r="D115" s="92" t="s">
-        <v>165</v>
-      </c>
-      <c r="E115" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F115" s="89" t="s">
-        <v>166</v>
+      <c r="C115" s="13"/>
+      <c r="D115" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="E115" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F115" s="66" t="s">
+        <v>161</v>
       </c>
       <c r="G115" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H115" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="I115" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="I115" s="68" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C116" s="13"/>
-      <c r="D116" s="93"/>
-      <c r="E116" s="96"/>
-      <c r="F116" s="91"/>
+      <c r="D116" s="86"/>
+      <c r="E116" s="84"/>
+      <c r="F116" s="85"/>
       <c r="G116" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H116" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="I116" s="144"/>
+    </row>
+    <row r="117" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C117" s="14"/>
+      <c r="D117" s="63"/>
+      <c r="E117" s="65"/>
+      <c r="F117" s="67"/>
+      <c r="G117" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H117" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="I117" s="69"/>
+    </row>
+    <row r="118" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C118" s="14"/>
+      <c r="D118" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="E118" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F118" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="G118" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H118" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="I118" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C119" s="13"/>
+      <c r="D119" s="63"/>
+      <c r="E119" s="65"/>
+      <c r="F119" s="67"/>
+      <c r="G119" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H119" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="I119" s="69"/>
+    </row>
+    <row r="120" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C120" s="13"/>
+      <c r="D120" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="I116" s="63"/>
-    </row>
-    <row r="117" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C117" s="13"/>
-      <c r="D117" s="92" t="s">
+      <c r="E120" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="E117" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F117" s="89" t="s">
+      <c r="G120" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H120" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="G117" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H117" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="I117" s="62" t="s">
+      <c r="I120" s="68" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="118" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C118" s="13"/>
-      <c r="D118" s="93"/>
-      <c r="E118" s="96"/>
-      <c r="F118" s="91"/>
-      <c r="G118" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H118" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="I118" s="63"/>
-    </row>
-    <row r="119" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C119" s="13"/>
-      <c r="D119" s="92" t="s">
-        <v>173</v>
-      </c>
-      <c r="E119" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F119" s="89" t="s">
-        <v>174</v>
-      </c>
-      <c r="G119" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H119" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="I119" s="62" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="120" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C120" s="13"/>
-      <c r="D120" s="97"/>
-      <c r="E120" s="95"/>
-      <c r="F120" s="90"/>
-      <c r="G120" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H120" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="I120" s="67"/>
     </row>
     <row r="121" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C121" s="13"/>
-      <c r="D121" s="97"/>
-      <c r="E121" s="95"/>
-      <c r="F121" s="90"/>
+      <c r="D121" s="63"/>
+      <c r="E121" s="65"/>
+      <c r="F121" s="67"/>
       <c r="G121" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H121" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I121" s="69"/>
+    </row>
+    <row r="122" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C122" s="13"/>
+      <c r="D122" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="E122" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F122" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="G122" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H122" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="I122" s="68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="123" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C123" s="13"/>
+      <c r="D123" s="86"/>
+      <c r="E123" s="84"/>
+      <c r="F123" s="85"/>
+      <c r="G123" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H123" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I123" s="144"/>
+    </row>
+    <row r="124" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C124" s="13"/>
+      <c r="D124" s="86"/>
+      <c r="E124" s="84"/>
+      <c r="F124" s="85"/>
+      <c r="G124" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H121" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I121" s="67"/>
-    </row>
-    <row r="122" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C122" s="13"/>
-      <c r="D122" s="93"/>
-      <c r="E122" s="96"/>
-      <c r="F122" s="91"/>
-      <c r="G122" s="20" t="s">
+      <c r="H124" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I124" s="144"/>
+    </row>
+    <row r="125" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C125" s="13"/>
+      <c r="D125" s="63"/>
+      <c r="E125" s="65"/>
+      <c r="F125" s="67"/>
+      <c r="G125" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H122" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I122" s="63"/>
-    </row>
-    <row r="123" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C123" s="13"/>
-      <c r="D123" s="92" t="s">
+      <c r="H125" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I125" s="69"/>
+    </row>
+    <row r="126" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C126" s="13"/>
+      <c r="D126" s="62" t="s">
+        <v>175</v>
+      </c>
+      <c r="E126" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F126" s="66" t="s">
         <v>176</v>
       </c>
-      <c r="E123" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F123" s="89" t="s">
-        <v>177</v>
-      </c>
-      <c r="G123" s="18" t="s">
+      <c r="G126" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H123" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="I123" s="62" t="s">
+      <c r="H126" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I126" s="68" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C124" s="15"/>
-      <c r="D124" s="93"/>
-      <c r="E124" s="96"/>
-      <c r="F124" s="91"/>
-      <c r="G124" s="24" t="s">
+    <row r="127" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C127" s="146"/>
+      <c r="D127" s="63"/>
+      <c r="E127" s="65"/>
+      <c r="F127" s="67"/>
+      <c r="G127" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H124" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I124" s="63"/>
-    </row>
-    <row r="125" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C125" s="13"/>
-      <c r="D125" s="92" t="s">
+      <c r="H127" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I127" s="69"/>
+    </row>
+    <row r="128" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C128" s="146"/>
+      <c r="D128" s="147" t="s">
+        <v>197</v>
+      </c>
+      <c r="E128" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F128" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="E125" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="F125" s="89" t="s">
-        <v>199</v>
-      </c>
-      <c r="G125" s="18" t="s">
+      <c r="G128" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H125" s="23" t="s">
+      <c r="H128" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="I128" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C129" s="13"/>
+      <c r="D129" s="63"/>
+      <c r="E129" s="65"/>
+      <c r="F129" s="67"/>
+      <c r="G129" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H129" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="I125" s="62" t="s">
+      <c r="I129" s="69"/>
+    </row>
+    <row r="130" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C130" s="13"/>
+      <c r="D130" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="E130" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F130" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="G130" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H130" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="I130" s="68" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C126" s="15"/>
-      <c r="D126" s="93"/>
-      <c r="E126" s="96"/>
-      <c r="F126" s="91"/>
-      <c r="G126" s="24" t="s">
+    <row r="131" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C131" s="13"/>
+      <c r="D131" s="86"/>
+      <c r="E131" s="84"/>
+      <c r="F131" s="85"/>
+      <c r="G131" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H131" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="I131" s="144"/>
+    </row>
+    <row r="132" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C132" s="13"/>
+      <c r="D132" s="86"/>
+      <c r="E132" s="84"/>
+      <c r="F132" s="85"/>
+      <c r="G132" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H132" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="I132" s="144"/>
+    </row>
+    <row r="133" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C133" s="13"/>
+      <c r="D133" s="63"/>
+      <c r="E133" s="65"/>
+      <c r="F133" s="67"/>
+      <c r="G133" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H133" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="I133" s="69"/>
+    </row>
+    <row r="134" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C134" s="13"/>
+      <c r="D134" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="E134" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F134" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="G134" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H134" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="I134" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C135" s="13"/>
+      <c r="D135" s="86"/>
+      <c r="E135" s="84"/>
+      <c r="F135" s="85"/>
+      <c r="G135" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H135" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="I135" s="144"/>
+    </row>
+    <row r="136" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C136" s="13"/>
+      <c r="D136" s="86"/>
+      <c r="E136" s="84"/>
+      <c r="F136" s="85"/>
+      <c r="G136" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H126" s="25" t="s">
+      <c r="H136" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="I136" s="144"/>
+    </row>
+    <row r="137" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C137" s="13"/>
+      <c r="D137" s="63"/>
+      <c r="E137" s="65"/>
+      <c r="F137" s="67"/>
+      <c r="G137" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H137" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="I137" s="69"/>
+    </row>
+    <row r="138" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C138" s="13"/>
+      <c r="D138" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="E138" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F138" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="G138" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H138" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="I138" s="68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="139" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C139" s="13"/>
+      <c r="D139" s="86"/>
+      <c r="E139" s="84"/>
+      <c r="F139" s="85"/>
+      <c r="G139" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H139" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I139" s="144"/>
+    </row>
+    <row r="140" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C140" s="13"/>
+      <c r="D140" s="86"/>
+      <c r="E140" s="84"/>
+      <c r="F140" s="85"/>
+      <c r="G140" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H140" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I140" s="144"/>
+    </row>
+    <row r="141" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C141" s="13"/>
+      <c r="D141" s="63"/>
+      <c r="E141" s="65"/>
+      <c r="F141" s="67"/>
+      <c r="G141" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H141" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="I141" s="69"/>
+    </row>
+    <row r="142" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C142" s="13"/>
+      <c r="D142" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="E142" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F142" s="66" t="s">
+        <v>161</v>
+      </c>
+      <c r="G142" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H142" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="I142" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C143" s="13"/>
+      <c r="D143" s="86"/>
+      <c r="E143" s="84"/>
+      <c r="F143" s="85"/>
+      <c r="G143" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H143" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="I143" s="144"/>
+    </row>
+    <row r="144" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C144" s="14"/>
+      <c r="D144" s="63"/>
+      <c r="E144" s="65"/>
+      <c r="F144" s="67"/>
+      <c r="G144" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H144" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="I144" s="69"/>
+    </row>
+    <row r="145" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C145" s="14"/>
+      <c r="D145" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="E145" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F145" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="G145" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H145" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="I145" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C146" s="13"/>
+      <c r="D146" s="63"/>
+      <c r="E146" s="65"/>
+      <c r="F146" s="67"/>
+      <c r="G146" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H146" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="I146" s="69"/>
+    </row>
+    <row r="147" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C147" s="13"/>
+      <c r="D147" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="E147" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F147" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="G147" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H147" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I147" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="148" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C148" s="13"/>
+      <c r="D148" s="63"/>
+      <c r="E148" s="65"/>
+      <c r="F148" s="67"/>
+      <c r="G148" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H148" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I148" s="69"/>
+    </row>
+    <row r="149" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C149" s="13"/>
+      <c r="D149" s="62" t="s">
         <v>172</v>
       </c>
-      <c r="I126" s="63"/>
+      <c r="E149" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F149" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="G149" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H149" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="I149" s="68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="150" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C150" s="13"/>
+      <c r="D150" s="86"/>
+      <c r="E150" s="84"/>
+      <c r="F150" s="85"/>
+      <c r="G150" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H150" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I150" s="144"/>
+    </row>
+    <row r="151" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C151" s="13"/>
+      <c r="D151" s="86"/>
+      <c r="E151" s="84"/>
+      <c r="F151" s="85"/>
+      <c r="G151" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H151" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I151" s="144"/>
+    </row>
+    <row r="152" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C152" s="13"/>
+      <c r="D152" s="63"/>
+      <c r="E152" s="65"/>
+      <c r="F152" s="67"/>
+      <c r="G152" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H152" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I152" s="69"/>
+    </row>
+    <row r="153" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C153" s="13"/>
+      <c r="D153" s="62" t="s">
+        <v>175</v>
+      </c>
+      <c r="E153" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F153" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="G153" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H153" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I153" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C154" s="146"/>
+      <c r="D154" s="63"/>
+      <c r="E154" s="65"/>
+      <c r="F154" s="67"/>
+      <c r="G154" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H154" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I154" s="69"/>
+    </row>
+    <row r="155" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C155" s="146"/>
+      <c r="D155" s="147" t="s">
+        <v>197</v>
+      </c>
+      <c r="E155" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F155" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="G155" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H155" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="I155" s="68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C156" s="15"/>
+      <c r="D156" s="63"/>
+      <c r="E156" s="65"/>
+      <c r="F156" s="67"/>
+      <c r="G156" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H156" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="I156" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="143">
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="E125:E126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="I125:I126"/>
-    <mergeCell ref="D88:D90"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="E91:E93"/>
-    <mergeCell ref="F91:F93"/>
-    <mergeCell ref="C86:C96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="I91:I93"/>
-    <mergeCell ref="E104:E107"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="E97:E99"/>
-    <mergeCell ref="F104:F107"/>
-    <mergeCell ref="D104:D107"/>
-    <mergeCell ref="F100:F103"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="F97:F99"/>
-    <mergeCell ref="D97:D99"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="E88:E90"/>
-    <mergeCell ref="E82:E84"/>
-    <mergeCell ref="D85:D87"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="E79:E81"/>
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="D82:D84"/>
-    <mergeCell ref="F85:F87"/>
+  <mergeCells count="181">
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="D149:D152"/>
+    <mergeCell ref="E149:E152"/>
+    <mergeCell ref="F149:F152"/>
+    <mergeCell ref="I149:I152"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="E153:E154"/>
+    <mergeCell ref="F153:F154"/>
+    <mergeCell ref="I153:I154"/>
+    <mergeCell ref="D155:D156"/>
+    <mergeCell ref="E155:E156"/>
+    <mergeCell ref="F155:F156"/>
+    <mergeCell ref="I155:I156"/>
+    <mergeCell ref="D142:D144"/>
+    <mergeCell ref="E142:E144"/>
+    <mergeCell ref="F142:F144"/>
+    <mergeCell ref="I142:I144"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="F145:F146"/>
+    <mergeCell ref="I145:I146"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="I147:I148"/>
+    <mergeCell ref="D130:D133"/>
+    <mergeCell ref="E130:E133"/>
+    <mergeCell ref="F130:F133"/>
+    <mergeCell ref="I130:I133"/>
+    <mergeCell ref="D134:D137"/>
+    <mergeCell ref="E134:E137"/>
+    <mergeCell ref="F134:F137"/>
+    <mergeCell ref="I134:I137"/>
+    <mergeCell ref="D138:D141"/>
+    <mergeCell ref="E138:E141"/>
+    <mergeCell ref="F138:F141"/>
+    <mergeCell ref="I138:I141"/>
+    <mergeCell ref="I126:I127"/>
+    <mergeCell ref="I85:I87"/>
+    <mergeCell ref="I97:I99"/>
+    <mergeCell ref="I103:I106"/>
+    <mergeCell ref="I107:I110"/>
+    <mergeCell ref="I111:I114"/>
+    <mergeCell ref="I88:I90"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="I75:I78"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="I115:I117"/>
+    <mergeCell ref="I118:I119"/>
+    <mergeCell ref="I120:I121"/>
+    <mergeCell ref="I122:I125"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="I82:I84"/>
+    <mergeCell ref="I79:I81"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="F122:F125"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="E122:E125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="D111:D114"/>
+    <mergeCell ref="F111:F114"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E111:E114"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="D61:D64"/>
     <mergeCell ref="C70:C74"/>
     <mergeCell ref="D71:D74"/>
     <mergeCell ref="E71:E74"/>
@@ -4011,92 +4718,39 @@
     <mergeCell ref="D49:D51"/>
     <mergeCell ref="E49:E51"/>
     <mergeCell ref="I65:I70"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="F65:F70"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="D61:D64"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="F119:F122"/>
-    <mergeCell ref="D123:D124"/>
-    <mergeCell ref="F123:F124"/>
-    <mergeCell ref="E119:E122"/>
-    <mergeCell ref="E123:E124"/>
-    <mergeCell ref="E117:E118"/>
-    <mergeCell ref="D108:D111"/>
-    <mergeCell ref="F108:F111"/>
-    <mergeCell ref="D112:D114"/>
-    <mergeCell ref="F112:F114"/>
-    <mergeCell ref="D115:D116"/>
-    <mergeCell ref="F115:F116"/>
-    <mergeCell ref="E108:E111"/>
-    <mergeCell ref="E112:E114"/>
-    <mergeCell ref="E115:E116"/>
-    <mergeCell ref="F117:F118"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="D119:D122"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I60"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="I112:I114"/>
-    <mergeCell ref="I115:I116"/>
-    <mergeCell ref="I117:I118"/>
-    <mergeCell ref="I119:I122"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="I82:I84"/>
-    <mergeCell ref="I79:I81"/>
-    <mergeCell ref="I123:I124"/>
-    <mergeCell ref="I85:I87"/>
-    <mergeCell ref="I97:I99"/>
-    <mergeCell ref="I100:I103"/>
-    <mergeCell ref="I104:I107"/>
-    <mergeCell ref="I108:I111"/>
-    <mergeCell ref="I88:I90"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="I75:I78"/>
+    <mergeCell ref="E82:E84"/>
+    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="E79:E81"/>
+    <mergeCell ref="F79:F81"/>
+    <mergeCell ref="F82:F84"/>
+    <mergeCell ref="D82:D84"/>
+    <mergeCell ref="F85:F87"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="E91:E93"/>
+    <mergeCell ref="F91:F93"/>
+    <mergeCell ref="C86:C96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="I91:I93"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="E103:E106"/>
+    <mergeCell ref="E97:E99"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="D107:D110"/>
+    <mergeCell ref="F103:F106"/>
+    <mergeCell ref="D103:D106"/>
+    <mergeCell ref="F97:F99"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="E88:E90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de la direccion del endpoint para que este mas ordenado
</commit_message>
<xml_diff>
--- a/.readmeFiles/Endpoints.xlsx
+++ b/.readmeFiles/Endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/pcalvenl_emeal_nttdata_com/Documents/Escritorio/gitTarjetitas/back-end-framework/.readmeFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="495" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0F463AF-E117-4214-8C8E-A04638FE6420}"/>
+  <xr:revisionPtr revIDLastSave="496" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D41E070B-248D-4606-A86A-6F83B854E7A8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
   </bookViews>
@@ -686,9 +686,6 @@
     <t>"The new monthly limit must be greater than 0"</t>
   </si>
   <si>
-    <t>/public/customer/delete/{customerId}</t>
-  </si>
-  <si>
     <t>Deletes a user by their customer Id</t>
   </si>
   <si>
@@ -699,6 +696,9 @@
   </si>
   <si>
     <t>"The customer has been deleted successfully."</t>
+  </si>
+  <si>
+    <t>/api/customer/delete/{customerId}</t>
   </si>
 </sst>
 </file>
@@ -1464,29 +1464,287 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="8" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1497,15 +1755,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1520,255 +1769,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="8" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1800,6 +1800,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2121,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA3F6E-09E5-46A7-9DF8-4B95ED8D48E7}">
   <dimension ref="B2:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="H98" sqref="H98"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2262,13 +2266,13 @@
     </row>
     <row r="9" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="5"/>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="129" t="s">
+      <c r="E9" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="100" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -2277,45 +2281,45 @@
       <c r="H9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="135" t="s">
+      <c r="I9" s="98" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="5"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="129"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="100"/>
       <c r="G10" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="135"/>
+      <c r="I10" s="98"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="5"/>
-      <c r="D11" s="129"/>
-      <c r="E11" s="130"/>
-      <c r="F11" s="129"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="100"/>
       <c r="G11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="135"/>
+      <c r="I11" s="98"/>
     </row>
     <row r="12" spans="2:9" ht="28.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="5"/>
-      <c r="D12" s="129" t="s">
+      <c r="D12" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="129" t="s">
+      <c r="E12" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="100" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="38" t="s">
@@ -2324,35 +2328,35 @@
       <c r="H12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="135" t="s">
+      <c r="I12" s="98" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="5"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="130"/>
-      <c r="F13" s="129"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="100"/>
       <c r="G13" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="135"/>
+      <c r="I13" s="98"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C14" s="5"/>
-      <c r="D14" s="129"/>
-      <c r="E14" s="130"/>
-      <c r="F14" s="129"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="100"/>
       <c r="G14" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="135"/>
+      <c r="I14" s="98"/>
     </row>
     <row r="15" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="5"/>
@@ -2451,13 +2455,13 @@
     </row>
     <row r="20" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
-      <c r="D20" s="129" t="s">
+      <c r="D20" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="129" t="s">
+      <c r="E20" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="100" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="39" t="s">
@@ -2466,58 +2470,58 @@
       <c r="H20" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="135" t="s">
+      <c r="I20" s="98" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="129"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="100"/>
       <c r="G21" s="39" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="135"/>
+      <c r="I21" s="98"/>
     </row>
     <row r="22" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="129"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="100"/>
       <c r="G22" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="135"/>
+      <c r="I22" s="98"/>
     </row>
     <row r="23" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C23" s="5"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="129"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="100"/>
       <c r="G23" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H23" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="135"/>
+      <c r="I23" s="98"/>
     </row>
     <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="5"/>
-      <c r="D24" s="129" t="s">
+      <c r="D24" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="129" t="s">
+      <c r="E24" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="100" t="s">
         <v>57</v>
       </c>
       <c r="G24" s="38" t="s">
@@ -2526,45 +2530,45 @@
       <c r="H24" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="135" t="s">
+      <c r="I24" s="98" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="5"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="129"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="100"/>
       <c r="G25" s="42" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="I25" s="135"/>
+      <c r="I25" s="98"/>
     </row>
     <row r="26" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C26" s="5"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="129"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="100"/>
       <c r="G26" s="42" t="s">
         <v>53</v>
       </c>
       <c r="H26" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="135"/>
+      <c r="I26" s="98"/>
     </row>
     <row r="27" spans="3:9" ht="58.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C27" s="5"/>
-      <c r="D27" s="129" t="s">
+      <c r="D27" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="134" t="s">
+      <c r="E27" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="102" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="38" t="s">
@@ -2573,84 +2577,84 @@
       <c r="H27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="135" t="s">
+      <c r="I27" s="98" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="5"/>
-      <c r="D28" s="129"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="134"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="122"/>
+      <c r="F28" s="102"/>
       <c r="G28" s="42" t="s">
         <v>63</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="135"/>
+      <c r="I28" s="98"/>
     </row>
     <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="5"/>
-      <c r="D29" s="131" t="s">
+      <c r="D29" s="117" t="s">
         <v>180</v>
       </c>
-      <c r="E29" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="113" t="s">
+      <c r="E29" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="137" t="s">
+      <c r="G29" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="139" t="s">
+      <c r="H29" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="116" t="s">
+      <c r="I29" s="113" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="3:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C30" s="5"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="111"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="139"/>
-      <c r="I30" s="117"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="104"/>
+      <c r="G30" s="107"/>
+      <c r="H30" s="108"/>
+      <c r="I30" s="114"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C31" s="5"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="140" t="s">
+      <c r="D31" s="118"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="142" t="s">
+      <c r="H31" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="I31" s="117"/>
+      <c r="I31" s="114"/>
     </row>
     <row r="32" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="5"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="112"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="143"/>
-      <c r="I32" s="118"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="105"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="115"/>
     </row>
     <row r="33" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="5"/>
-      <c r="D33" s="134" t="s">
+      <c r="D33" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="134" t="s">
+      <c r="E33" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="102" t="s">
         <v>68</v>
       </c>
       <c r="G33" s="54" t="s">
@@ -2659,58 +2663,58 @@
       <c r="H33" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="135" t="s">
+      <c r="I33" s="98" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C34" s="5"/>
-      <c r="D34" s="134"/>
-      <c r="E34" s="130"/>
-      <c r="F34" s="134"/>
+      <c r="D34" s="102"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="102"/>
       <c r="G34" s="47" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I34" s="135"/>
+      <c r="I34" s="98"/>
     </row>
     <row r="35" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C35" s="5"/>
-      <c r="D35" s="134"/>
-      <c r="E35" s="130"/>
-      <c r="F35" s="134"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="116"/>
+      <c r="F35" s="102"/>
       <c r="G35" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H35" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="135"/>
+      <c r="I35" s="98"/>
     </row>
     <row r="36" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C36" s="5"/>
-      <c r="D36" s="134"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="134"/>
+      <c r="D36" s="102"/>
+      <c r="E36" s="116"/>
+      <c r="F36" s="102"/>
       <c r="G36" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H36" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I36" s="135"/>
+      <c r="I36" s="98"/>
     </row>
     <row r="37" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C37" s="5"/>
-      <c r="D37" s="107" t="s">
+      <c r="D37" s="146" t="s">
         <v>181</v>
       </c>
-      <c r="E37" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="113" t="s">
+      <c r="E37" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="103" t="s">
         <v>182</v>
       </c>
       <c r="G37" s="57" t="s">
@@ -2719,45 +2723,45 @@
       <c r="H37" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="I37" s="116" t="s">
+      <c r="I37" s="113" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C38" s="5"/>
-      <c r="D38" s="108"/>
-      <c r="E38" s="111"/>
-      <c r="F38" s="114"/>
+      <c r="D38" s="147"/>
+      <c r="E38" s="121"/>
+      <c r="F38" s="104"/>
       <c r="G38" s="42" t="s">
         <v>70</v>
       </c>
       <c r="H38" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="117"/>
+      <c r="I38" s="114"/>
     </row>
     <row r="39" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="119"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="112"/>
-      <c r="F39" s="115"/>
+      <c r="C39" s="149"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="122"/>
+      <c r="F39" s="105"/>
       <c r="G39" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H39" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="I39" s="118"/>
+      <c r="I39" s="115"/>
     </row>
     <row r="40" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="119"/>
-      <c r="D40" s="107" t="s">
+      <c r="C40" s="149"/>
+      <c r="D40" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="E40" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="113" t="s">
+      <c r="E40" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="103" t="s">
         <v>186</v>
       </c>
       <c r="G40" s="57" t="s">
@@ -2766,45 +2770,45 @@
       <c r="H40" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="I40" s="116" t="s">
+      <c r="I40" s="113" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="41" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C41" s="119"/>
-      <c r="D41" s="108"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="114"/>
+      <c r="C41" s="149"/>
+      <c r="D41" s="147"/>
+      <c r="E41" s="121"/>
+      <c r="F41" s="104"/>
       <c r="G41" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H41" s="55" t="s">
         <v>199</v>
       </c>
-      <c r="I41" s="117"/>
+      <c r="I41" s="114"/>
     </row>
     <row r="42" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C42" s="119"/>
-      <c r="D42" s="109"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="115"/>
+      <c r="C42" s="149"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="122"/>
+      <c r="F42" s="105"/>
       <c r="G42" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H42" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="I42" s="118"/>
+      <c r="I42" s="115"/>
     </row>
     <row r="43" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C43" s="119"/>
-      <c r="D43" s="107" t="s">
+      <c r="C43" s="149"/>
+      <c r="D43" s="146" t="s">
         <v>187</v>
       </c>
-      <c r="E43" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="113" t="s">
+      <c r="E43" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="103" t="s">
         <v>188</v>
       </c>
       <c r="G43" s="57" t="s">
@@ -2813,47 +2817,47 @@
       <c r="H43" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="I43" s="116" t="s">
+      <c r="I43" s="113" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="44" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C44" s="119"/>
-      <c r="D44" s="108"/>
-      <c r="E44" s="111"/>
-      <c r="F44" s="114"/>
+      <c r="C44" s="149"/>
+      <c r="D44" s="147"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="104"/>
       <c r="G44" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H44" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="I44" s="117"/>
+      <c r="I44" s="114"/>
     </row>
     <row r="45" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C45" s="120"/>
-      <c r="D45" s="109"/>
-      <c r="E45" s="112"/>
-      <c r="F45" s="115"/>
+      <c r="C45" s="150"/>
+      <c r="D45" s="148"/>
+      <c r="E45" s="122"/>
+      <c r="F45" s="105"/>
       <c r="G45" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H45" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="I45" s="118"/>
+      <c r="I45" s="115"/>
     </row>
     <row r="46" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="121" t="s">
+      <c r="D46" s="151" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="122" t="s">
+      <c r="E46" s="152" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="136" t="s">
+      <c r="F46" s="101" t="s">
         <v>78</v>
       </c>
       <c r="G46" s="30" t="s">
@@ -2862,45 +2866,45 @@
       <c r="H46" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="145" t="s">
+      <c r="I46" s="99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C47" s="16"/>
-      <c r="D47" s="121"/>
-      <c r="E47" s="122"/>
-      <c r="F47" s="136"/>
+      <c r="D47" s="151"/>
+      <c r="E47" s="152"/>
+      <c r="F47" s="101"/>
       <c r="G47" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="I47" s="145"/>
+      <c r="I47" s="99"/>
     </row>
     <row r="48" spans="3:9" ht="31.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C48" s="7"/>
-      <c r="D48" s="121"/>
-      <c r="E48" s="122"/>
-      <c r="F48" s="136"/>
+      <c r="D48" s="151"/>
+      <c r="E48" s="152"/>
+      <c r="F48" s="101"/>
       <c r="G48" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H48" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="145"/>
+      <c r="I48" s="99"/>
     </row>
     <row r="49" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C49" s="7"/>
-      <c r="D49" s="123" t="s">
+      <c r="D49" s="138" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="98" t="s">
+      <c r="E49" s="123" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="101" t="s">
+      <c r="F49" s="129" t="s">
         <v>85</v>
       </c>
       <c r="G49" s="30" t="s">
@@ -2909,45 +2913,45 @@
       <c r="H49" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I49" s="104" t="s">
+      <c r="I49" s="95" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="50" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="7"/>
-      <c r="D50" s="124"/>
-      <c r="E50" s="99"/>
-      <c r="F50" s="102"/>
+      <c r="D50" s="140"/>
+      <c r="E50" s="124"/>
+      <c r="F50" s="130"/>
       <c r="G50" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H50" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="I50" s="105"/>
+      <c r="I50" s="96"/>
     </row>
     <row r="51" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C51" s="7"/>
-      <c r="D51" s="125"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="103"/>
+      <c r="D51" s="139"/>
+      <c r="E51" s="125"/>
+      <c r="F51" s="131"/>
       <c r="G51" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H51" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I51" s="106"/>
+      <c r="I51" s="97"/>
     </row>
     <row r="52" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C52" s="7"/>
-      <c r="D52" s="123" t="s">
+      <c r="D52" s="138" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="101" t="s">
+      <c r="E52" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="129" t="s">
         <v>91</v>
       </c>
       <c r="G52" s="30" t="s">
@@ -2956,22 +2960,22 @@
       <c r="H52" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="104" t="s">
+      <c r="I52" s="95" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C53" s="7"/>
-      <c r="D53" s="125"/>
-      <c r="E53" s="100"/>
-      <c r="F53" s="103"/>
+      <c r="D53" s="139"/>
+      <c r="E53" s="125"/>
+      <c r="F53" s="131"/>
       <c r="G53" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H53" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="I53" s="106"/>
+      <c r="I53" s="97"/>
     </row>
     <row r="54" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C54" s="7"/>
@@ -3018,13 +3022,13 @@
     </row>
     <row r="57" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C57" s="7"/>
-      <c r="D57" s="123" t="s">
+      <c r="D57" s="138" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="98" t="s">
+      <c r="E57" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="101" t="s">
+      <c r="F57" s="129" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="30" t="s">
@@ -3033,58 +3037,58 @@
       <c r="H57" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="I57" s="104" t="s">
+      <c r="I57" s="95" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="58" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C58" s="7"/>
-      <c r="D58" s="124"/>
-      <c r="E58" s="99"/>
-      <c r="F58" s="102"/>
+      <c r="D58" s="140"/>
+      <c r="E58" s="124"/>
+      <c r="F58" s="130"/>
       <c r="G58" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H58" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="I58" s="105"/>
+      <c r="I58" s="96"/>
     </row>
     <row r="59" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C59" s="7"/>
-      <c r="D59" s="124"/>
-      <c r="E59" s="99"/>
-      <c r="F59" s="102"/>
+      <c r="D59" s="140"/>
+      <c r="E59" s="124"/>
+      <c r="F59" s="130"/>
       <c r="G59" s="32" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I59" s="105"/>
+      <c r="I59" s="96"/>
     </row>
     <row r="60" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C60" s="7"/>
-      <c r="D60" s="125"/>
-      <c r="E60" s="100"/>
-      <c r="F60" s="103"/>
+      <c r="D60" s="139"/>
+      <c r="E60" s="125"/>
+      <c r="F60" s="131"/>
       <c r="G60" s="32" t="s">
         <v>100</v>
       </c>
       <c r="H60" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I60" s="106"/>
+      <c r="I60" s="97"/>
     </row>
     <row r="61" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C61" s="7"/>
-      <c r="D61" s="123" t="s">
+      <c r="D61" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="98" t="s">
+      <c r="E61" s="123" t="s">
         <v>103</v>
       </c>
-      <c r="F61" s="101" t="s">
+      <c r="F61" s="129" t="s">
         <v>104</v>
       </c>
       <c r="G61" s="30" t="s">
@@ -3093,58 +3097,58 @@
       <c r="H61" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="I61" s="104" t="s">
+      <c r="I61" s="95" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C62" s="7"/>
-      <c r="D62" s="124"/>
-      <c r="E62" s="99"/>
-      <c r="F62" s="102"/>
+      <c r="D62" s="140"/>
+      <c r="E62" s="124"/>
+      <c r="F62" s="130"/>
       <c r="G62" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H62" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I62" s="105"/>
+      <c r="I62" s="96"/>
     </row>
     <row r="63" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C63" s="7"/>
-      <c r="D63" s="124"/>
-      <c r="E63" s="99"/>
-      <c r="F63" s="102"/>
+      <c r="D63" s="140"/>
+      <c r="E63" s="124"/>
+      <c r="F63" s="130"/>
       <c r="G63" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H63" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="I63" s="105"/>
+      <c r="I63" s="96"/>
     </row>
     <row r="64" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C64" s="7"/>
-      <c r="D64" s="125"/>
-      <c r="E64" s="100"/>
-      <c r="F64" s="103"/>
+      <c r="D64" s="139"/>
+      <c r="E64" s="125"/>
+      <c r="F64" s="131"/>
       <c r="G64" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H64" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I64" s="106"/>
+      <c r="I64" s="97"/>
     </row>
     <row r="65" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C65" s="7"/>
-      <c r="D65" s="123" t="s">
+      <c r="D65" s="138" t="s">
         <v>109</v>
       </c>
-      <c r="E65" s="98" t="s">
+      <c r="E65" s="123" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="101" t="s">
+      <c r="F65" s="129" t="s">
         <v>111</v>
       </c>
       <c r="G65" s="30" t="s">
@@ -3153,84 +3157,84 @@
       <c r="H65" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="I65" s="104" t="s">
+      <c r="I65" s="95" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C66" s="7"/>
-      <c r="D66" s="124"/>
-      <c r="E66" s="99"/>
-      <c r="F66" s="102"/>
+      <c r="D66" s="140"/>
+      <c r="E66" s="124"/>
+      <c r="F66" s="130"/>
       <c r="G66" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H66" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I66" s="105"/>
+      <c r="I66" s="96"/>
     </row>
     <row r="67" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C67" s="7"/>
-      <c r="D67" s="124"/>
-      <c r="E67" s="99"/>
-      <c r="F67" s="102"/>
+      <c r="D67" s="140"/>
+      <c r="E67" s="124"/>
+      <c r="F67" s="130"/>
       <c r="G67" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H67" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="I67" s="105"/>
+      <c r="I67" s="96"/>
     </row>
     <row r="68" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C68" s="7"/>
-      <c r="D68" s="124"/>
-      <c r="E68" s="99"/>
-      <c r="F68" s="102"/>
+      <c r="D68" s="140"/>
+      <c r="E68" s="124"/>
+      <c r="F68" s="130"/>
       <c r="G68" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H68" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="I68" s="105"/>
+      <c r="I68" s="96"/>
     </row>
     <row r="69" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C69" s="7"/>
-      <c r="D69" s="124"/>
-      <c r="E69" s="99"/>
-      <c r="F69" s="102"/>
+      <c r="D69" s="140"/>
+      <c r="E69" s="124"/>
+      <c r="F69" s="130"/>
       <c r="G69" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H69" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I69" s="105"/>
+      <c r="I69" s="96"/>
     </row>
     <row r="70" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C70" s="93"/>
-      <c r="D70" s="125"/>
-      <c r="E70" s="100"/>
-      <c r="F70" s="103"/>
+      <c r="C70" s="141"/>
+      <c r="D70" s="139"/>
+      <c r="E70" s="125"/>
+      <c r="F70" s="131"/>
       <c r="G70" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H70" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="I70" s="106"/>
+      <c r="I70" s="97"/>
     </row>
     <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C71" s="93"/>
-      <c r="D71" s="95" t="s">
+      <c r="C71" s="141"/>
+      <c r="D71" s="143" t="s">
         <v>189</v>
       </c>
-      <c r="E71" s="98" t="s">
+      <c r="E71" s="123" t="s">
         <v>190</v>
       </c>
-      <c r="F71" s="101" t="s">
+      <c r="F71" s="129" t="s">
         <v>191</v>
       </c>
       <c r="G71" s="30" t="s">
@@ -3239,57 +3243,57 @@
       <c r="H71" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="I71" s="104" t="s">
+      <c r="I71" s="95" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="72" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C72" s="93"/>
-      <c r="D72" s="96"/>
-      <c r="E72" s="99"/>
-      <c r="F72" s="102"/>
+      <c r="C72" s="141"/>
+      <c r="D72" s="144"/>
+      <c r="E72" s="124"/>
+      <c r="F72" s="130"/>
       <c r="G72" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H72" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="I72" s="105"/>
+      <c r="I72" s="96"/>
     </row>
     <row r="73" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C73" s="93"/>
-      <c r="D73" s="96"/>
-      <c r="E73" s="99"/>
-      <c r="F73" s="102"/>
+      <c r="C73" s="141"/>
+      <c r="D73" s="144"/>
+      <c r="E73" s="124"/>
+      <c r="F73" s="130"/>
       <c r="G73" s="32" t="s">
         <v>72</v>
       </c>
       <c r="H73" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="I73" s="105"/>
+      <c r="I73" s="96"/>
     </row>
     <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C74" s="94"/>
-      <c r="D74" s="97"/>
-      <c r="E74" s="100"/>
-      <c r="F74" s="103"/>
+      <c r="C74" s="142"/>
+      <c r="D74" s="145"/>
+      <c r="E74" s="125"/>
+      <c r="F74" s="131"/>
       <c r="G74" s="60" t="s">
         <v>31</v>
       </c>
       <c r="H74" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="I74" s="106"/>
+      <c r="I74" s="97"/>
     </row>
     <row r="75" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D75" s="87" t="s">
+      <c r="D75" s="135" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="73" t="s">
+      <c r="E75" s="132" t="s">
         <v>120</v>
       </c>
       <c r="F75" s="126" t="s">
@@ -3301,14 +3305,14 @@
       <c r="H75" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="I75" s="81" t="s">
+      <c r="I75" s="92" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="76" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C76" s="9"/>
-      <c r="D76" s="88"/>
-      <c r="E76" s="74"/>
+      <c r="D76" s="136"/>
+      <c r="E76" s="133"/>
       <c r="F76" s="127"/>
       <c r="G76" s="28" t="s">
         <v>53</v>
@@ -3316,12 +3320,12 @@
       <c r="H76" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="I76" s="82"/>
+      <c r="I76" s="93"/>
     </row>
     <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C77" s="10"/>
-      <c r="D77" s="88"/>
-      <c r="E77" s="74"/>
+      <c r="D77" s="136"/>
+      <c r="E77" s="133"/>
       <c r="F77" s="127"/>
       <c r="G77" s="28" t="s">
         <v>53</v>
@@ -3329,12 +3333,12 @@
       <c r="H77" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I77" s="82"/>
+      <c r="I77" s="93"/>
     </row>
     <row r="78" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C78" s="10"/>
-      <c r="D78" s="89"/>
-      <c r="E78" s="75"/>
+      <c r="D78" s="137"/>
+      <c r="E78" s="134"/>
       <c r="F78" s="128"/>
       <c r="G78" s="28" t="s">
         <v>53</v>
@@ -3342,17 +3346,17 @@
       <c r="H78" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="I78" s="83"/>
+      <c r="I78" s="94"/>
     </row>
     <row r="79" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C79" s="10"/>
-      <c r="D79" s="87" t="s">
+      <c r="D79" s="135" t="s">
         <v>126</v>
       </c>
-      <c r="E79" s="73" t="s">
+      <c r="E79" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="90" t="s">
+      <c r="F79" s="153" t="s">
         <v>127</v>
       </c>
       <c r="G79" s="26" t="s">
@@ -3361,45 +3365,45 @@
       <c r="H79" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="I79" s="81" t="s">
+      <c r="I79" s="92" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="80" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C80" s="10"/>
-      <c r="D80" s="88"/>
-      <c r="E80" s="74"/>
-      <c r="F80" s="91"/>
+      <c r="D80" s="136"/>
+      <c r="E80" s="133"/>
+      <c r="F80" s="154"/>
       <c r="G80" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H80" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="I80" s="82"/>
+      <c r="I80" s="93"/>
     </row>
     <row r="81" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C81" s="10"/>
-      <c r="D81" s="89"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="92"/>
+      <c r="D81" s="137"/>
+      <c r="E81" s="134"/>
+      <c r="F81" s="155"/>
       <c r="G81" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H81" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I81" s="83"/>
+      <c r="I81" s="94"/>
     </row>
     <row r="82" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C82" s="10"/>
-      <c r="D82" s="87" t="s">
+      <c r="D82" s="135" t="s">
         <v>131</v>
       </c>
-      <c r="E82" s="73" t="s">
+      <c r="E82" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F82" s="90" t="s">
+      <c r="F82" s="153" t="s">
         <v>132</v>
       </c>
       <c r="G82" s="26" t="s">
@@ -3408,45 +3412,45 @@
       <c r="H82" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="I82" s="81" t="s">
+      <c r="I82" s="92" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="83" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C83" s="10"/>
-      <c r="D83" s="88"/>
-      <c r="E83" s="74"/>
-      <c r="F83" s="91"/>
+      <c r="D83" s="136"/>
+      <c r="E83" s="133"/>
+      <c r="F83" s="154"/>
       <c r="G83" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H83" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="I83" s="82"/>
+      <c r="I83" s="93"/>
     </row>
     <row r="84" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C84" s="10"/>
-      <c r="D84" s="89"/>
-      <c r="E84" s="75"/>
-      <c r="F84" s="92"/>
+      <c r="D84" s="137"/>
+      <c r="E84" s="134"/>
+      <c r="F84" s="155"/>
       <c r="G84" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H84" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I84" s="83"/>
+      <c r="I84" s="94"/>
     </row>
     <row r="85" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C85" s="10"/>
-      <c r="D85" s="87" t="s">
+      <c r="D85" s="135" t="s">
         <v>135</v>
       </c>
-      <c r="E85" s="73" t="s">
+      <c r="E85" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F85" s="90" t="s">
+      <c r="F85" s="153" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="26" t="s">
@@ -3455,45 +3459,45 @@
       <c r="H85" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="I85" s="81" t="s">
+      <c r="I85" s="92" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="86" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C86" s="79"/>
-      <c r="D86" s="88"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="91"/>
+      <c r="C86" s="162"/>
+      <c r="D86" s="136"/>
+      <c r="E86" s="133"/>
+      <c r="F86" s="154"/>
       <c r="G86" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H86" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="I86" s="82"/>
+      <c r="I86" s="93"/>
     </row>
     <row r="87" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C87" s="79"/>
-      <c r="D87" s="89"/>
-      <c r="E87" s="75"/>
-      <c r="F87" s="92"/>
+      <c r="C87" s="162"/>
+      <c r="D87" s="137"/>
+      <c r="E87" s="134"/>
+      <c r="F87" s="155"/>
       <c r="G87" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H87" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I87" s="83"/>
+      <c r="I87" s="94"/>
     </row>
     <row r="88" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C88" s="79"/>
-      <c r="D88" s="70" t="s">
+      <c r="C88" s="162"/>
+      <c r="D88" s="156" t="s">
         <v>192</v>
       </c>
-      <c r="E88" s="73" t="s">
+      <c r="E88" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F88" s="76" t="s">
+      <c r="F88" s="159" t="s">
         <v>195</v>
       </c>
       <c r="G88" s="26" t="s">
@@ -3502,45 +3506,45 @@
       <c r="H88" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="I88" s="81" t="s">
+      <c r="I88" s="92" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="89" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C89" s="79"/>
-      <c r="D89" s="71"/>
-      <c r="E89" s="74"/>
-      <c r="F89" s="77"/>
+      <c r="C89" s="162"/>
+      <c r="D89" s="157"/>
+      <c r="E89" s="133"/>
+      <c r="F89" s="160"/>
       <c r="G89" s="28" t="s">
         <v>205</v>
       </c>
       <c r="H89" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="I89" s="82"/>
+      <c r="I89" s="93"/>
     </row>
     <row r="90" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C90" s="79"/>
-      <c r="D90" s="72"/>
-      <c r="E90" s="75"/>
-      <c r="F90" s="78"/>
+      <c r="C90" s="162"/>
+      <c r="D90" s="158"/>
+      <c r="E90" s="134"/>
+      <c r="F90" s="161"/>
       <c r="G90" s="28" t="s">
         <v>206</v>
       </c>
       <c r="H90" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="I90" s="83"/>
+      <c r="I90" s="94"/>
     </row>
     <row r="91" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C91" s="79"/>
-      <c r="D91" s="70" t="s">
+      <c r="C91" s="162"/>
+      <c r="D91" s="156" t="s">
         <v>193</v>
       </c>
-      <c r="E91" s="73" t="s">
+      <c r="E91" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F91" s="76" t="s">
+      <c r="F91" s="159" t="s">
         <v>196</v>
       </c>
       <c r="G91" s="26" t="s">
@@ -3549,45 +3553,45 @@
       <c r="H91" s="59" t="s">
         <v>212</v>
       </c>
-      <c r="I91" s="81" t="s">
+      <c r="I91" s="92" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="92" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C92" s="79"/>
-      <c r="D92" s="71"/>
-      <c r="E92" s="74"/>
-      <c r="F92" s="77"/>
+      <c r="C92" s="162"/>
+      <c r="D92" s="157"/>
+      <c r="E92" s="133"/>
+      <c r="F92" s="160"/>
       <c r="G92" s="28" t="s">
         <v>211</v>
       </c>
       <c r="H92" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="I92" s="82"/>
+      <c r="I92" s="93"/>
     </row>
     <row r="93" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C93" s="79"/>
-      <c r="D93" s="72"/>
-      <c r="E93" s="75"/>
-      <c r="F93" s="78"/>
+      <c r="C93" s="162"/>
+      <c r="D93" s="158"/>
+      <c r="E93" s="134"/>
+      <c r="F93" s="161"/>
       <c r="G93" s="28" t="s">
         <v>72</v>
       </c>
       <c r="H93" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="I93" s="83"/>
+      <c r="I93" s="94"/>
     </row>
     <row r="94" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C94" s="79"/>
-      <c r="D94" s="70" t="s">
+      <c r="C94" s="162"/>
+      <c r="D94" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="E94" s="73" t="s">
+      <c r="E94" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F94" s="76" t="s">
+      <c r="F94" s="159" t="s">
         <v>196</v>
       </c>
       <c r="G94" s="26" t="s">
@@ -3596,141 +3600,141 @@
       <c r="H94" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="I94" s="81" t="s">
+      <c r="I94" s="92" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="95" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C95" s="79"/>
-      <c r="D95" s="71"/>
-      <c r="E95" s="74"/>
-      <c r="F95" s="77"/>
+      <c r="C95" s="162"/>
+      <c r="D95" s="157"/>
+      <c r="E95" s="133"/>
+      <c r="F95" s="160"/>
       <c r="G95" s="28" t="s">
         <v>211</v>
       </c>
       <c r="H95" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="I95" s="82"/>
+      <c r="I95" s="93"/>
     </row>
     <row r="96" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C96" s="80"/>
-      <c r="D96" s="72"/>
-      <c r="E96" s="75"/>
-      <c r="F96" s="78"/>
+      <c r="C96" s="163"/>
+      <c r="D96" s="158"/>
+      <c r="E96" s="134"/>
+      <c r="F96" s="161"/>
       <c r="G96" s="28" t="s">
         <v>72</v>
       </c>
       <c r="H96" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="I96" s="83"/>
+      <c r="I96" s="94"/>
     </row>
     <row r="97" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C97" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D97" s="62" t="s">
+      <c r="D97" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="E97" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F97" s="66" t="s">
+      <c r="E97" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="85" t="s">
         <v>141</v>
       </c>
       <c r="G97" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H97" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="I97" s="68" t="s">
+        <v>219</v>
+      </c>
+      <c r="I97" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="98" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C98" s="12"/>
-      <c r="D98" s="86"/>
-      <c r="E98" s="84"/>
-      <c r="F98" s="85"/>
+      <c r="D98" s="80"/>
+      <c r="E98" s="83"/>
+      <c r="F98" s="86"/>
       <c r="G98" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H98" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="I98" s="144"/>
+      <c r="I98" s="89"/>
     </row>
     <row r="99" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C99" s="13"/>
-      <c r="D99" s="63"/>
-      <c r="E99" s="65"/>
-      <c r="F99" s="67"/>
-      <c r="G99" s="160" t="s">
+      <c r="D99" s="81"/>
+      <c r="E99" s="84"/>
+      <c r="F99" s="87"/>
+      <c r="G99" s="69" t="s">
         <v>143</v>
       </c>
-      <c r="H99" s="161" t="s">
+      <c r="H99" s="70" t="s">
         <v>144</v>
       </c>
-      <c r="I99" s="69"/>
+      <c r="I99" s="90"/>
     </row>
     <row r="100" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C100" s="13"/>
-      <c r="D100" s="158"/>
-      <c r="E100" s="150" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="155" t="s">
+      <c r="D100" s="67"/>
+      <c r="E100" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="76" t="s">
+        <v>216</v>
+      </c>
+      <c r="G100" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="H100" s="72" t="s">
         <v>217</v>
       </c>
-      <c r="G100" s="162" t="s">
-        <v>28</v>
-      </c>
-      <c r="H100" s="163" t="s">
-        <v>218</v>
-      </c>
-      <c r="I100" s="153"/>
+      <c r="I100" s="65"/>
     </row>
     <row r="101" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C101" s="13"/>
-      <c r="D101" s="158" t="s">
-        <v>216</v>
-      </c>
-      <c r="E101" s="151"/>
-      <c r="F101" s="156"/>
-      <c r="G101" s="154" t="s">
+      <c r="D101" s="67" t="s">
+        <v>220</v>
+      </c>
+      <c r="E101" s="74"/>
+      <c r="F101" s="77"/>
+      <c r="G101" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="H101" s="149" t="s">
+      <c r="H101" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="I101" s="153" t="s">
+      <c r="I101" s="65" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="102" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C102" s="13"/>
-      <c r="D102" s="159"/>
-      <c r="E102" s="152"/>
-      <c r="F102" s="157"/>
-      <c r="G102" s="148" t="s">
+      <c r="D102" s="68"/>
+      <c r="E102" s="75"/>
+      <c r="F102" s="78"/>
+      <c r="G102" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="H102" s="149" t="s">
-        <v>219</v>
-      </c>
-      <c r="I102" s="153"/>
+      <c r="H102" s="64" t="s">
+        <v>218</v>
+      </c>
+      <c r="I102" s="65"/>
     </row>
     <row r="103" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C103" s="13"/>
-      <c r="D103" s="62" t="s">
+      <c r="D103" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="E103" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F103" s="66" t="s">
+      <c r="E103" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F103" s="85" t="s">
         <v>146</v>
       </c>
       <c r="G103" s="18" t="s">
@@ -3739,58 +3743,58 @@
       <c r="H103" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="I103" s="68" t="s">
+      <c r="I103" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="104" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C104" s="13"/>
-      <c r="D104" s="86"/>
-      <c r="E104" s="84"/>
-      <c r="F104" s="85"/>
+      <c r="D104" s="80"/>
+      <c r="E104" s="83"/>
+      <c r="F104" s="86"/>
       <c r="G104" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H104" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="I104" s="144"/>
+      <c r="I104" s="89"/>
     </row>
     <row r="105" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C105" s="13"/>
-      <c r="D105" s="86"/>
-      <c r="E105" s="84"/>
-      <c r="F105" s="85"/>
+      <c r="D105" s="80"/>
+      <c r="E105" s="83"/>
+      <c r="F105" s="86"/>
       <c r="G105" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H105" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I105" s="144"/>
+      <c r="I105" s="89"/>
     </row>
     <row r="106" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C106" s="13"/>
-      <c r="D106" s="63"/>
-      <c r="E106" s="65"/>
-      <c r="F106" s="67"/>
+      <c r="D106" s="81"/>
+      <c r="E106" s="84"/>
+      <c r="F106" s="87"/>
       <c r="G106" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H106" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I106" s="69"/>
+      <c r="I106" s="90"/>
     </row>
     <row r="107" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C107" s="13"/>
-      <c r="D107" s="62" t="s">
+      <c r="D107" s="79" t="s">
         <v>151</v>
       </c>
-      <c r="E107" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F107" s="66" t="s">
+      <c r="E107" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" s="85" t="s">
         <v>152</v>
       </c>
       <c r="G107" s="18" t="s">
@@ -3799,58 +3803,58 @@
       <c r="H107" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="I107" s="68" t="s">
+      <c r="I107" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="108" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C108" s="13"/>
-      <c r="D108" s="86"/>
-      <c r="E108" s="84"/>
-      <c r="F108" s="85"/>
+      <c r="D108" s="80"/>
+      <c r="E108" s="83"/>
+      <c r="F108" s="86"/>
       <c r="G108" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H108" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="I108" s="144"/>
+      <c r="I108" s="89"/>
     </row>
     <row r="109" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C109" s="13"/>
-      <c r="D109" s="86"/>
-      <c r="E109" s="84"/>
-      <c r="F109" s="85"/>
+      <c r="D109" s="80"/>
+      <c r="E109" s="83"/>
+      <c r="F109" s="86"/>
       <c r="G109" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H109" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="I109" s="144"/>
+      <c r="I109" s="89"/>
     </row>
     <row r="110" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C110" s="13"/>
-      <c r="D110" s="63"/>
-      <c r="E110" s="65"/>
-      <c r="F110" s="67"/>
+      <c r="D110" s="81"/>
+      <c r="E110" s="84"/>
+      <c r="F110" s="87"/>
       <c r="G110" s="20" t="s">
         <v>143</v>
       </c>
       <c r="H110" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="I110" s="69"/>
+      <c r="I110" s="90"/>
     </row>
     <row r="111" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C111" s="13"/>
-      <c r="D111" s="62" t="s">
+      <c r="D111" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="E111" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F111" s="66" t="s">
+      <c r="E111" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111" s="85" t="s">
         <v>158</v>
       </c>
       <c r="G111" s="18" t="s">
@@ -3859,58 +3863,58 @@
       <c r="H111" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="I111" s="68" t="s">
+      <c r="I111" s="88" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="112" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C112" s="13"/>
-      <c r="D112" s="86"/>
-      <c r="E112" s="84"/>
-      <c r="F112" s="85"/>
+      <c r="D112" s="80"/>
+      <c r="E112" s="83"/>
+      <c r="F112" s="86"/>
       <c r="G112" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H112" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I112" s="144"/>
+      <c r="I112" s="89"/>
     </row>
     <row r="113" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C113" s="13"/>
-      <c r="D113" s="86"/>
-      <c r="E113" s="84"/>
-      <c r="F113" s="85"/>
+      <c r="D113" s="80"/>
+      <c r="E113" s="83"/>
+      <c r="F113" s="86"/>
       <c r="G113" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H113" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I113" s="144"/>
+      <c r="I113" s="89"/>
     </row>
     <row r="114" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C114" s="13"/>
-      <c r="D114" s="63"/>
-      <c r="E114" s="65"/>
-      <c r="F114" s="67"/>
+      <c r="D114" s="81"/>
+      <c r="E114" s="84"/>
+      <c r="F114" s="87"/>
       <c r="G114" s="20" t="s">
         <v>143</v>
       </c>
       <c r="H114" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="I114" s="69"/>
+      <c r="I114" s="90"/>
     </row>
     <row r="115" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C115" s="13"/>
-      <c r="D115" s="62" t="s">
+      <c r="D115" s="79" t="s">
         <v>160</v>
       </c>
-      <c r="E115" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F115" s="66" t="s">
+      <c r="E115" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F115" s="85" t="s">
         <v>161</v>
       </c>
       <c r="G115" s="18" t="s">
@@ -3919,45 +3923,45 @@
       <c r="H115" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="I115" s="68" t="s">
+      <c r="I115" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="116" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C116" s="13"/>
-      <c r="D116" s="86"/>
-      <c r="E116" s="84"/>
-      <c r="F116" s="85"/>
+      <c r="D116" s="80"/>
+      <c r="E116" s="83"/>
+      <c r="F116" s="86"/>
       <c r="G116" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H116" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="I116" s="144"/>
+      <c r="I116" s="89"/>
     </row>
     <row r="117" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C117" s="14"/>
-      <c r="D117" s="63"/>
-      <c r="E117" s="65"/>
-      <c r="F117" s="67"/>
+      <c r="D117" s="81"/>
+      <c r="E117" s="84"/>
+      <c r="F117" s="87"/>
       <c r="G117" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H117" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="I117" s="69"/>
+      <c r="I117" s="90"/>
     </row>
     <row r="118" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C118" s="14"/>
-      <c r="D118" s="62" t="s">
+      <c r="D118" s="79" t="s">
         <v>164</v>
       </c>
-      <c r="E118" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F118" s="66" t="s">
+      <c r="E118" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F118" s="85" t="s">
         <v>165</v>
       </c>
       <c r="G118" s="18" t="s">
@@ -3966,32 +3970,32 @@
       <c r="H118" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="I118" s="68" t="s">
+      <c r="I118" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="119" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C119" s="13"/>
-      <c r="D119" s="63"/>
-      <c r="E119" s="65"/>
-      <c r="F119" s="67"/>
+      <c r="D119" s="81"/>
+      <c r="E119" s="84"/>
+      <c r="F119" s="87"/>
       <c r="G119" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H119" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="I119" s="69"/>
+      <c r="I119" s="90"/>
     </row>
     <row r="120" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C120" s="13"/>
-      <c r="D120" s="62" t="s">
+      <c r="D120" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="E120" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F120" s="66" t="s">
+      <c r="E120" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120" s="85" t="s">
         <v>169</v>
       </c>
       <c r="G120" s="18" t="s">
@@ -4000,32 +4004,32 @@
       <c r="H120" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="I120" s="68" t="s">
+      <c r="I120" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="121" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C121" s="13"/>
-      <c r="D121" s="63"/>
-      <c r="E121" s="65"/>
-      <c r="F121" s="67"/>
+      <c r="D121" s="81"/>
+      <c r="E121" s="84"/>
+      <c r="F121" s="87"/>
       <c r="G121" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H121" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="I121" s="69"/>
+      <c r="I121" s="90"/>
     </row>
     <row r="122" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C122" s="13"/>
-      <c r="D122" s="62" t="s">
+      <c r="D122" s="79" t="s">
         <v>172</v>
       </c>
-      <c r="E122" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F122" s="66" t="s">
+      <c r="E122" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F122" s="85" t="s">
         <v>173</v>
       </c>
       <c r="G122" s="18" t="s">
@@ -4034,58 +4038,58 @@
       <c r="H122" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="I122" s="68" t="s">
+      <c r="I122" s="88" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="123" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C123" s="13"/>
-      <c r="D123" s="86"/>
-      <c r="E123" s="84"/>
-      <c r="F123" s="85"/>
+      <c r="D123" s="80"/>
+      <c r="E123" s="83"/>
+      <c r="F123" s="86"/>
       <c r="G123" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H123" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="I123" s="144"/>
+      <c r="I123" s="89"/>
     </row>
     <row r="124" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C124" s="13"/>
-      <c r="D124" s="86"/>
-      <c r="E124" s="84"/>
-      <c r="F124" s="85"/>
+      <c r="D124" s="80"/>
+      <c r="E124" s="83"/>
+      <c r="F124" s="86"/>
       <c r="G124" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H124" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I124" s="144"/>
+      <c r="I124" s="89"/>
     </row>
     <row r="125" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C125" s="13"/>
-      <c r="D125" s="63"/>
-      <c r="E125" s="65"/>
-      <c r="F125" s="67"/>
+      <c r="D125" s="81"/>
+      <c r="E125" s="84"/>
+      <c r="F125" s="87"/>
       <c r="G125" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H125" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I125" s="69"/>
+      <c r="I125" s="90"/>
     </row>
     <row r="126" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C126" s="13"/>
-      <c r="D126" s="62" t="s">
+      <c r="D126" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="E126" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F126" s="66" t="s">
+      <c r="E126" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F126" s="85" t="s">
         <v>176</v>
       </c>
       <c r="G126" s="18" t="s">
@@ -4094,32 +4098,32 @@
       <c r="H126" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I126" s="68" t="s">
+      <c r="I126" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="127" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C127" s="146"/>
-      <c r="D127" s="63"/>
-      <c r="E127" s="65"/>
-      <c r="F127" s="67"/>
+      <c r="C127" s="62"/>
+      <c r="D127" s="81"/>
+      <c r="E127" s="84"/>
+      <c r="F127" s="87"/>
       <c r="G127" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H127" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I127" s="69"/>
+      <c r="I127" s="90"/>
     </row>
     <row r="128" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C128" s="146"/>
-      <c r="D128" s="147" t="s">
+      <c r="C128" s="62"/>
+      <c r="D128" s="91" t="s">
         <v>197</v>
       </c>
-      <c r="E128" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F128" s="66" t="s">
+      <c r="E128" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F128" s="85" t="s">
         <v>198</v>
       </c>
       <c r="G128" s="18" t="s">
@@ -4128,32 +4132,32 @@
       <c r="H128" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="I128" s="68" t="s">
+      <c r="I128" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="129" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C129" s="13"/>
-      <c r="D129" s="63"/>
-      <c r="E129" s="65"/>
-      <c r="F129" s="67"/>
+      <c r="D129" s="81"/>
+      <c r="E129" s="84"/>
+      <c r="F129" s="87"/>
       <c r="G129" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H129" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="I129" s="69"/>
+      <c r="I129" s="90"/>
     </row>
     <row r="130" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C130" s="13"/>
-      <c r="D130" s="62" t="s">
+      <c r="D130" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="E130" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F130" s="66" t="s">
+      <c r="E130" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F130" s="85" t="s">
         <v>146</v>
       </c>
       <c r="G130" s="18" t="s">
@@ -4162,58 +4166,58 @@
       <c r="H130" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="I130" s="68" t="s">
+      <c r="I130" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="131" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C131" s="13"/>
-      <c r="D131" s="86"/>
-      <c r="E131" s="84"/>
-      <c r="F131" s="85"/>
+      <c r="D131" s="80"/>
+      <c r="E131" s="83"/>
+      <c r="F131" s="86"/>
       <c r="G131" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H131" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="I131" s="144"/>
+      <c r="I131" s="89"/>
     </row>
     <row r="132" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C132" s="13"/>
-      <c r="D132" s="86"/>
-      <c r="E132" s="84"/>
-      <c r="F132" s="85"/>
+      <c r="D132" s="80"/>
+      <c r="E132" s="83"/>
+      <c r="F132" s="86"/>
       <c r="G132" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H132" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I132" s="144"/>
+      <c r="I132" s="89"/>
     </row>
     <row r="133" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C133" s="13"/>
-      <c r="D133" s="63"/>
-      <c r="E133" s="65"/>
-      <c r="F133" s="67"/>
+      <c r="D133" s="81"/>
+      <c r="E133" s="84"/>
+      <c r="F133" s="87"/>
       <c r="G133" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H133" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I133" s="69"/>
+      <c r="I133" s="90"/>
     </row>
     <row r="134" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C134" s="13"/>
-      <c r="D134" s="62" t="s">
+      <c r="D134" s="79" t="s">
         <v>151</v>
       </c>
-      <c r="E134" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F134" s="66" t="s">
+      <c r="E134" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F134" s="85" t="s">
         <v>152</v>
       </c>
       <c r="G134" s="18" t="s">
@@ -4222,58 +4226,58 @@
       <c r="H134" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="I134" s="68" t="s">
+      <c r="I134" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="135" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C135" s="13"/>
-      <c r="D135" s="86"/>
-      <c r="E135" s="84"/>
-      <c r="F135" s="85"/>
+      <c r="D135" s="80"/>
+      <c r="E135" s="83"/>
+      <c r="F135" s="86"/>
       <c r="G135" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H135" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="I135" s="144"/>
+      <c r="I135" s="89"/>
     </row>
     <row r="136" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C136" s="13"/>
-      <c r="D136" s="86"/>
-      <c r="E136" s="84"/>
-      <c r="F136" s="85"/>
+      <c r="D136" s="80"/>
+      <c r="E136" s="83"/>
+      <c r="F136" s="86"/>
       <c r="G136" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H136" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="I136" s="144"/>
+      <c r="I136" s="89"/>
     </row>
     <row r="137" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C137" s="13"/>
-      <c r="D137" s="63"/>
-      <c r="E137" s="65"/>
-      <c r="F137" s="67"/>
+      <c r="D137" s="81"/>
+      <c r="E137" s="84"/>
+      <c r="F137" s="87"/>
       <c r="G137" s="20" t="s">
         <v>143</v>
       </c>
       <c r="H137" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="I137" s="69"/>
+      <c r="I137" s="90"/>
     </row>
     <row r="138" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C138" s="13"/>
-      <c r="D138" s="62" t="s">
+      <c r="D138" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="E138" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F138" s="66" t="s">
+      <c r="E138" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F138" s="85" t="s">
         <v>158</v>
       </c>
       <c r="G138" s="18" t="s">
@@ -4282,58 +4286,58 @@
       <c r="H138" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="I138" s="68" t="s">
+      <c r="I138" s="88" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="139" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C139" s="13"/>
-      <c r="D139" s="86"/>
-      <c r="E139" s="84"/>
-      <c r="F139" s="85"/>
+      <c r="D139" s="80"/>
+      <c r="E139" s="83"/>
+      <c r="F139" s="86"/>
       <c r="G139" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H139" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I139" s="144"/>
+      <c r="I139" s="89"/>
     </row>
     <row r="140" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C140" s="13"/>
-      <c r="D140" s="86"/>
-      <c r="E140" s="84"/>
-      <c r="F140" s="85"/>
+      <c r="D140" s="80"/>
+      <c r="E140" s="83"/>
+      <c r="F140" s="86"/>
       <c r="G140" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H140" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I140" s="144"/>
+      <c r="I140" s="89"/>
     </row>
     <row r="141" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C141" s="13"/>
-      <c r="D141" s="63"/>
-      <c r="E141" s="65"/>
-      <c r="F141" s="67"/>
+      <c r="D141" s="81"/>
+      <c r="E141" s="84"/>
+      <c r="F141" s="87"/>
       <c r="G141" s="20" t="s">
         <v>143</v>
       </c>
       <c r="H141" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="I141" s="69"/>
+      <c r="I141" s="90"/>
     </row>
     <row r="142" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C142" s="13"/>
-      <c r="D142" s="62" t="s">
+      <c r="D142" s="79" t="s">
         <v>160</v>
       </c>
-      <c r="E142" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F142" s="66" t="s">
+      <c r="E142" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F142" s="85" t="s">
         <v>161</v>
       </c>
       <c r="G142" s="18" t="s">
@@ -4342,45 +4346,45 @@
       <c r="H142" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="I142" s="68" t="s">
+      <c r="I142" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="143" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C143" s="13"/>
-      <c r="D143" s="86"/>
-      <c r="E143" s="84"/>
-      <c r="F143" s="85"/>
+      <c r="D143" s="80"/>
+      <c r="E143" s="83"/>
+      <c r="F143" s="86"/>
       <c r="G143" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H143" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="I143" s="144"/>
+      <c r="I143" s="89"/>
     </row>
     <row r="144" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C144" s="14"/>
-      <c r="D144" s="63"/>
-      <c r="E144" s="65"/>
-      <c r="F144" s="67"/>
+      <c r="D144" s="81"/>
+      <c r="E144" s="84"/>
+      <c r="F144" s="87"/>
       <c r="G144" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H144" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="I144" s="69"/>
+      <c r="I144" s="90"/>
     </row>
     <row r="145" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C145" s="14"/>
-      <c r="D145" s="62" t="s">
+      <c r="D145" s="79" t="s">
         <v>164</v>
       </c>
-      <c r="E145" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F145" s="66" t="s">
+      <c r="E145" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F145" s="85" t="s">
         <v>165</v>
       </c>
       <c r="G145" s="18" t="s">
@@ -4389,32 +4393,32 @@
       <c r="H145" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="I145" s="68" t="s">
+      <c r="I145" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="146" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C146" s="13"/>
-      <c r="D146" s="63"/>
-      <c r="E146" s="65"/>
-      <c r="F146" s="67"/>
+      <c r="D146" s="81"/>
+      <c r="E146" s="84"/>
+      <c r="F146" s="87"/>
       <c r="G146" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H146" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="I146" s="69"/>
+      <c r="I146" s="90"/>
     </row>
     <row r="147" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C147" s="13"/>
-      <c r="D147" s="62" t="s">
+      <c r="D147" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="E147" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F147" s="66" t="s">
+      <c r="E147" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F147" s="85" t="s">
         <v>169</v>
       </c>
       <c r="G147" s="18" t="s">
@@ -4423,32 +4427,32 @@
       <c r="H147" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="I147" s="68" t="s">
+      <c r="I147" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="148" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C148" s="13"/>
-      <c r="D148" s="63"/>
-      <c r="E148" s="65"/>
-      <c r="F148" s="67"/>
+      <c r="D148" s="81"/>
+      <c r="E148" s="84"/>
+      <c r="F148" s="87"/>
       <c r="G148" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H148" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="I148" s="69"/>
+      <c r="I148" s="90"/>
     </row>
     <row r="149" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C149" s="13"/>
-      <c r="D149" s="62" t="s">
+      <c r="D149" s="79" t="s">
         <v>172</v>
       </c>
-      <c r="E149" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F149" s="66" t="s">
+      <c r="E149" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F149" s="85" t="s">
         <v>173</v>
       </c>
       <c r="G149" s="18" t="s">
@@ -4457,58 +4461,58 @@
       <c r="H149" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="I149" s="68" t="s">
+      <c r="I149" s="88" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="150" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C150" s="13"/>
-      <c r="D150" s="86"/>
-      <c r="E150" s="84"/>
-      <c r="F150" s="85"/>
+      <c r="D150" s="80"/>
+      <c r="E150" s="83"/>
+      <c r="F150" s="86"/>
       <c r="G150" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H150" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="I150" s="144"/>
+      <c r="I150" s="89"/>
     </row>
     <row r="151" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C151" s="13"/>
-      <c r="D151" s="86"/>
-      <c r="E151" s="84"/>
-      <c r="F151" s="85"/>
+      <c r="D151" s="80"/>
+      <c r="E151" s="83"/>
+      <c r="F151" s="86"/>
       <c r="G151" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H151" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I151" s="144"/>
+      <c r="I151" s="89"/>
     </row>
     <row r="152" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C152" s="13"/>
-      <c r="D152" s="63"/>
-      <c r="E152" s="65"/>
-      <c r="F152" s="67"/>
+      <c r="D152" s="81"/>
+      <c r="E152" s="84"/>
+      <c r="F152" s="87"/>
       <c r="G152" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H152" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I152" s="69"/>
+      <c r="I152" s="90"/>
     </row>
     <row r="153" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C153" s="13"/>
-      <c r="D153" s="62" t="s">
+      <c r="D153" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="E153" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F153" s="66" t="s">
+      <c r="E153" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F153" s="85" t="s">
         <v>176</v>
       </c>
       <c r="G153" s="18" t="s">
@@ -4517,32 +4521,32 @@
       <c r="H153" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I153" s="68" t="s">
+      <c r="I153" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="154" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C154" s="146"/>
-      <c r="D154" s="63"/>
-      <c r="E154" s="65"/>
-      <c r="F154" s="67"/>
+      <c r="C154" s="62"/>
+      <c r="D154" s="81"/>
+      <c r="E154" s="84"/>
+      <c r="F154" s="87"/>
       <c r="G154" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H154" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I154" s="69"/>
+      <c r="I154" s="90"/>
     </row>
     <row r="155" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C155" s="146"/>
-      <c r="D155" s="147" t="s">
+      <c r="C155" s="62"/>
+      <c r="D155" s="91" t="s">
         <v>197</v>
       </c>
-      <c r="E155" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F155" s="66" t="s">
+      <c r="E155" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F155" s="85" t="s">
         <v>198</v>
       </c>
       <c r="G155" s="18" t="s">
@@ -4551,149 +4555,58 @@
       <c r="H155" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="I155" s="68" t="s">
+      <c r="I155" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="156" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C156" s="15"/>
-      <c r="D156" s="63"/>
-      <c r="E156" s="65"/>
-      <c r="F156" s="67"/>
+      <c r="D156" s="81"/>
+      <c r="E156" s="84"/>
+      <c r="F156" s="87"/>
       <c r="G156" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H156" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="I156" s="69"/>
+      <c r="I156" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="181">
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="D149:D152"/>
-    <mergeCell ref="E149:E152"/>
-    <mergeCell ref="F149:F152"/>
-    <mergeCell ref="I149:I152"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="E153:E154"/>
-    <mergeCell ref="F153:F154"/>
-    <mergeCell ref="I153:I154"/>
-    <mergeCell ref="D155:D156"/>
-    <mergeCell ref="E155:E156"/>
-    <mergeCell ref="F155:F156"/>
-    <mergeCell ref="I155:I156"/>
-    <mergeCell ref="D142:D144"/>
-    <mergeCell ref="E142:E144"/>
-    <mergeCell ref="F142:F144"/>
-    <mergeCell ref="I142:I144"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="F145:F146"/>
-    <mergeCell ref="I145:I146"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="D130:D133"/>
-    <mergeCell ref="E130:E133"/>
-    <mergeCell ref="F130:F133"/>
-    <mergeCell ref="I130:I133"/>
-    <mergeCell ref="D134:D137"/>
-    <mergeCell ref="E134:E137"/>
-    <mergeCell ref="F134:F137"/>
-    <mergeCell ref="I134:I137"/>
-    <mergeCell ref="D138:D141"/>
-    <mergeCell ref="E138:E141"/>
-    <mergeCell ref="F138:F141"/>
-    <mergeCell ref="I138:I141"/>
-    <mergeCell ref="I126:I127"/>
-    <mergeCell ref="I85:I87"/>
-    <mergeCell ref="I97:I99"/>
-    <mergeCell ref="I103:I106"/>
-    <mergeCell ref="I107:I110"/>
-    <mergeCell ref="I111:I114"/>
-    <mergeCell ref="I88:I90"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="I75:I78"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I60"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="I115:I117"/>
-    <mergeCell ref="I118:I119"/>
-    <mergeCell ref="I120:I121"/>
-    <mergeCell ref="I122:I125"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="I82:I84"/>
-    <mergeCell ref="I79:I81"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="F122:F125"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="E122:E125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="D111:D114"/>
-    <mergeCell ref="F111:F114"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="F115:F117"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E111:E114"/>
-    <mergeCell ref="E115:E117"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="D122:D125"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="F65:F70"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="E91:E93"/>
+    <mergeCell ref="F91:F93"/>
+    <mergeCell ref="C86:C96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="I91:I93"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="E103:E106"/>
+    <mergeCell ref="E97:E99"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="D107:D110"/>
+    <mergeCell ref="F103:F106"/>
+    <mergeCell ref="D103:D106"/>
+    <mergeCell ref="F97:F99"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="F88:F90"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E82:E84"/>
+    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="E85:E87"/>
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="E79:E81"/>
+    <mergeCell ref="F79:F81"/>
+    <mergeCell ref="F82:F84"/>
+    <mergeCell ref="D82:D84"/>
+    <mergeCell ref="F85:F87"/>
     <mergeCell ref="C70:C74"/>
     <mergeCell ref="D71:D74"/>
     <mergeCell ref="E71:E74"/>
@@ -4718,39 +4631,130 @@
     <mergeCell ref="D49:D51"/>
     <mergeCell ref="E49:E51"/>
     <mergeCell ref="I65:I70"/>
-    <mergeCell ref="E82:E84"/>
-    <mergeCell ref="D85:D87"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="E79:E81"/>
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="D82:D84"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="D88:D90"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="E91:E93"/>
-    <mergeCell ref="F91:F93"/>
-    <mergeCell ref="C86:C96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="I91:I93"/>
-    <mergeCell ref="E107:E110"/>
-    <mergeCell ref="E103:E106"/>
-    <mergeCell ref="E97:E99"/>
-    <mergeCell ref="F107:F110"/>
-    <mergeCell ref="D107:D110"/>
-    <mergeCell ref="F103:F106"/>
-    <mergeCell ref="D103:D106"/>
-    <mergeCell ref="F97:F99"/>
-    <mergeCell ref="D97:D99"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="F122:F125"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="E122:E125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="D111:D114"/>
+    <mergeCell ref="F111:F114"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E111:E114"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="I118:I119"/>
+    <mergeCell ref="I120:I121"/>
+    <mergeCell ref="I122:I125"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="I82:I84"/>
+    <mergeCell ref="I79:I81"/>
+    <mergeCell ref="I85:I87"/>
+    <mergeCell ref="I97:I99"/>
+    <mergeCell ref="I103:I106"/>
+    <mergeCell ref="I107:I110"/>
+    <mergeCell ref="I111:I114"/>
+    <mergeCell ref="I88:I90"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="I75:I78"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="D155:D156"/>
+    <mergeCell ref="E155:E156"/>
+    <mergeCell ref="F155:F156"/>
+    <mergeCell ref="I155:I156"/>
+    <mergeCell ref="D142:D144"/>
+    <mergeCell ref="E142:E144"/>
+    <mergeCell ref="F142:F144"/>
+    <mergeCell ref="I142:I144"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="F145:F146"/>
+    <mergeCell ref="I145:I146"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="I147:I148"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="D149:D152"/>
+    <mergeCell ref="E149:E152"/>
+    <mergeCell ref="F149:F152"/>
+    <mergeCell ref="I149:I152"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="E153:E154"/>
+    <mergeCell ref="F153:F154"/>
+    <mergeCell ref="I153:I154"/>
+    <mergeCell ref="D130:D133"/>
+    <mergeCell ref="E130:E133"/>
+    <mergeCell ref="F130:F133"/>
+    <mergeCell ref="I130:I133"/>
+    <mergeCell ref="D134:D137"/>
+    <mergeCell ref="E134:E137"/>
+    <mergeCell ref="F134:F137"/>
+    <mergeCell ref="I134:I137"/>
+    <mergeCell ref="D138:D141"/>
+    <mergeCell ref="E138:E141"/>
+    <mergeCell ref="F138:F141"/>
+    <mergeCell ref="I138:I141"/>
+    <mergeCell ref="I126:I127"/>
+    <mergeCell ref="I115:I117"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
añadidos endpoints update accounts
</commit_message>
<xml_diff>
--- a/.readmeFiles/Endpoints.xlsx
+++ b/.readmeFiles/Endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/pcalvenl_emeal_nttdata_com/Documents/Escritorio/gitTarjetitas/back-end-framework/.readmeFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmanzanm\Git\back-end-framework\.readmeFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="495" documentId="13_ncr:1_{51D0DE2F-BFDE-4BAB-A0AE-18548CAA29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0F463AF-E117-4214-8C8E-A04638FE6420}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C36E7FD-A3C3-4604-A151-440F1B00E1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="237">
   <si>
     <t>HTTP Method</t>
   </si>
@@ -699,6 +699,54 @@
   </si>
   <si>
     <t>"The customer has been deleted successfully."</t>
+  </si>
+  <si>
+    <t>"/api/account/update/isblock/{accountId}"</t>
+  </si>
+  <si>
+    <t>Update the isBlocked account status.</t>
+  </si>
+  <si>
+    <t>"Your blocked status has been changed"</t>
+  </si>
+  <si>
+    <t>"You cannot change blocked status of an account that is not associated with you."</t>
+  </si>
+  <si>
+    <t>"/api/account/update/accountType/{accountId}"</t>
+  </si>
+  <si>
+    <t>Update the account Type.</t>
+  </si>
+  <si>
+    <t>"Your accountType has been changed"</t>
+  </si>
+  <si>
+    <t>"You cannot change accountType of an account that is not associated with you."</t>
+  </si>
+  <si>
+    <t>"/api/account/update/expirationDate/{accountId}"</t>
+  </si>
+  <si>
+    <t>Update the expiration date account.</t>
+  </si>
+  <si>
+    <t>"The expiration date has been updated to:"</t>
+  </si>
+  <si>
+    <t>"You can only extend the expiration date if it is within the next 3 months."</t>
+  </si>
+  <si>
+    <t>Blocked status cannot be null.</t>
+  </si>
+  <si>
+    <t>"The account already has the requested blocked status. No changes were made"</t>
+  </si>
+  <si>
+    <t>"Account type cannot be null."</t>
+  </si>
+  <si>
+    <t>"The account already has the requested account type. No changes were made"</t>
   </si>
 </sst>
 </file>
@@ -835,7 +883,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1279,6 +1327,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1295,7 +1382,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1464,29 +1551,287 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="8" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1497,15 +1842,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1521,253 +1857,37 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="4">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="8" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2119,25 +2239,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA3F6E-09E5-46A7-9DF8-4B95ED8D48E7}">
-  <dimension ref="B2:I156"/>
+  <dimension ref="B2:I169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="H98" sqref="H98"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="41.1796875" customWidth="1"/>
-    <col min="5" max="5" width="30.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="32.453125" customWidth="1"/>
-    <col min="8" max="8" width="67.1796875" customWidth="1"/>
-    <col min="9" max="9" width="26.54296875" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" customWidth="1"/>
+    <col min="8" max="8" width="83.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:9" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2160,7 +2280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -2181,7 +2301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:9" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="5"/>
       <c r="D5" s="34" t="s">
         <v>13</v>
@@ -2200,7 +2320,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="5"/>
       <c r="D6" s="34" t="s">
         <v>16</v>
@@ -2219,7 +2339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -2241,7 +2361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="5"/>
       <c r="D8" s="34" t="s">
         <v>23</v>
@@ -2260,15 +2380,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="5"/>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="129" t="s">
+      <c r="E9" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="100" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -2277,45 +2397,45 @@
       <c r="H9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="135" t="s">
+      <c r="I9" s="98" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="5"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="129"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="100"/>
       <c r="G10" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="135"/>
-    </row>
-    <row r="11" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I10" s="98"/>
+    </row>
+    <row r="11" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="5"/>
-      <c r="D11" s="129"/>
-      <c r="E11" s="130"/>
-      <c r="F11" s="129"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="100"/>
       <c r="G11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="135"/>
-    </row>
-    <row r="12" spans="2:9" ht="28.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I11" s="98"/>
+    </row>
+    <row r="12" spans="2:9" ht="28.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="5"/>
-      <c r="D12" s="129" t="s">
+      <c r="D12" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="129" t="s">
+      <c r="E12" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="100" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="38" t="s">
@@ -2324,37 +2444,37 @@
       <c r="H12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="135" t="s">
+      <c r="I12" s="98" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="5"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="130"/>
-      <c r="F13" s="129"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="100"/>
       <c r="G13" s="39" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="135"/>
-    </row>
-    <row r="14" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I13" s="98"/>
+    </row>
+    <row r="14" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="5"/>
-      <c r="D14" s="129"/>
-      <c r="E14" s="130"/>
-      <c r="F14" s="129"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="100"/>
       <c r="G14" s="39" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="135"/>
-    </row>
-    <row r="15" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I14" s="98"/>
+    </row>
+    <row r="15" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="5"/>
       <c r="D15" s="34" t="s">
         <v>36</v>
@@ -2373,7 +2493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="5"/>
       <c r="D16" s="34" t="s">
         <v>38</v>
@@ -2392,7 +2512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="5"/>
       <c r="D17" s="34" t="s">
         <v>41</v>
@@ -2411,7 +2531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="5"/>
       <c r="D18" s="34" t="s">
         <v>44</v>
@@ -2430,7 +2550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:9" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="5"/>
       <c r="D19" s="34" t="s">
         <v>46</v>
@@ -2449,15 +2569,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:9" ht="40.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="5"/>
-      <c r="D20" s="129" t="s">
+      <c r="D20" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="129" t="s">
+      <c r="E20" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="100" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="39" t="s">
@@ -2466,58 +2586,58 @@
       <c r="H20" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="135" t="s">
+      <c r="I20" s="98" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:9" ht="40.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="5"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="129"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="100"/>
       <c r="G21" s="39" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="135"/>
-    </row>
-    <row r="22" spans="3:9" ht="40.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I21" s="98"/>
+    </row>
+    <row r="22" spans="3:9" ht="40.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="5"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="129"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="100"/>
       <c r="G22" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="135"/>
-    </row>
-    <row r="23" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I22" s="98"/>
+    </row>
+    <row r="23" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="5"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="129"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="100"/>
       <c r="G23" s="39" t="s">
         <v>53</v>
       </c>
       <c r="H23" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="135"/>
-    </row>
-    <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I23" s="98"/>
+    </row>
+    <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="5"/>
-      <c r="D24" s="129" t="s">
+      <c r="D24" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="129" t="s">
+      <c r="E24" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="100" t="s">
         <v>57</v>
       </c>
       <c r="G24" s="38" t="s">
@@ -2526,45 +2646,45 @@
       <c r="H24" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="135" t="s">
+      <c r="I24" s="98" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="5"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="129"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="100"/>
       <c r="G25" s="42" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="I25" s="135"/>
-    </row>
-    <row r="26" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I25" s="98"/>
+    </row>
+    <row r="26" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="5"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="129"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="116"/>
+      <c r="F26" s="100"/>
       <c r="G26" s="42" t="s">
         <v>53</v>
       </c>
       <c r="H26" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="135"/>
-    </row>
-    <row r="27" spans="3:9" ht="58.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I26" s="98"/>
+    </row>
+    <row r="27" spans="3:9" ht="58.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
-      <c r="D27" s="129" t="s">
+      <c r="D27" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="134" t="s">
+      <c r="E27" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="102" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="38" t="s">
@@ -2573,84 +2693,84 @@
       <c r="H27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="135" t="s">
+      <c r="I27" s="98" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="5"/>
-      <c r="D28" s="129"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="134"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="122"/>
+      <c r="F28" s="102"/>
       <c r="G28" s="42" t="s">
         <v>63</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="135"/>
-    </row>
-    <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I28" s="98"/>
+    </row>
+    <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="5"/>
-      <c r="D29" s="131" t="s">
+      <c r="D29" s="117" t="s">
         <v>180</v>
       </c>
-      <c r="E29" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="113" t="s">
+      <c r="E29" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="137" t="s">
+      <c r="G29" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="139" t="s">
+      <c r="H29" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="116" t="s">
+      <c r="I29" s="113" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="3:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="5"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="111"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="139"/>
-      <c r="I30" s="117"/>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="D30" s="118"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="104"/>
+      <c r="G30" s="107"/>
+      <c r="H30" s="108"/>
+      <c r="I30" s="114"/>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="5"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="140" t="s">
+      <c r="D31" s="118"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="142" t="s">
+      <c r="H31" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="I31" s="117"/>
-    </row>
-    <row r="32" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I31" s="114"/>
+    </row>
+    <row r="32" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="5"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="112"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="143"/>
-      <c r="I32" s="118"/>
-    </row>
-    <row r="33" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D32" s="119"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="105"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="115"/>
+    </row>
+    <row r="33" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="5"/>
-      <c r="D33" s="134" t="s">
+      <c r="D33" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="134" t="s">
+      <c r="E33" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="102" t="s">
         <v>68</v>
       </c>
       <c r="G33" s="54" t="s">
@@ -2659,58 +2779,58 @@
       <c r="H33" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="135" t="s">
+      <c r="I33" s="98" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="5"/>
-      <c r="D34" s="134"/>
-      <c r="E34" s="130"/>
-      <c r="F34" s="134"/>
+      <c r="D34" s="102"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="102"/>
       <c r="G34" s="47" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I34" s="135"/>
-    </row>
-    <row r="35" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I34" s="98"/>
+    </row>
+    <row r="35" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="5"/>
-      <c r="D35" s="134"/>
-      <c r="E35" s="130"/>
-      <c r="F35" s="134"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="116"/>
+      <c r="F35" s="102"/>
       <c r="G35" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H35" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="135"/>
-    </row>
-    <row r="36" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I35" s="98"/>
+    </row>
+    <row r="36" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="5"/>
-      <c r="D36" s="134"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="134"/>
+      <c r="D36" s="102"/>
+      <c r="E36" s="116"/>
+      <c r="F36" s="102"/>
       <c r="G36" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H36" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I36" s="135"/>
-    </row>
-    <row r="37" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I36" s="98"/>
+    </row>
+    <row r="37" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="5"/>
-      <c r="D37" s="107" t="s">
+      <c r="D37" s="146" t="s">
         <v>181</v>
       </c>
-      <c r="E37" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="113" t="s">
+      <c r="E37" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="103" t="s">
         <v>182</v>
       </c>
       <c r="G37" s="57" t="s">
@@ -2719,45 +2839,45 @@
       <c r="H37" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="I37" s="116" t="s">
+      <c r="I37" s="113" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="5"/>
-      <c r="D38" s="108"/>
-      <c r="E38" s="111"/>
-      <c r="F38" s="114"/>
+      <c r="D38" s="147"/>
+      <c r="E38" s="121"/>
+      <c r="F38" s="104"/>
       <c r="G38" s="42" t="s">
         <v>70</v>
       </c>
       <c r="H38" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="117"/>
-    </row>
-    <row r="39" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="119"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="112"/>
-      <c r="F39" s="115"/>
+      <c r="I38" s="114"/>
+    </row>
+    <row r="39" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="149"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="122"/>
+      <c r="F39" s="105"/>
       <c r="G39" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H39" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="I39" s="118"/>
-    </row>
-    <row r="40" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="119"/>
-      <c r="D40" s="107" t="s">
+      <c r="I39" s="115"/>
+    </row>
+    <row r="40" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="149"/>
+      <c r="D40" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="E40" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="113" t="s">
+      <c r="E40" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="103" t="s">
         <v>186</v>
       </c>
       <c r="G40" s="57" t="s">
@@ -2766,45 +2886,45 @@
       <c r="H40" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="I40" s="116" t="s">
+      <c r="I40" s="113" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C41" s="119"/>
-      <c r="D41" s="108"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="114"/>
+    <row r="41" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="149"/>
+      <c r="D41" s="147"/>
+      <c r="E41" s="121"/>
+      <c r="F41" s="104"/>
       <c r="G41" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H41" s="55" t="s">
         <v>199</v>
       </c>
-      <c r="I41" s="117"/>
-    </row>
-    <row r="42" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C42" s="119"/>
-      <c r="D42" s="109"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="115"/>
+      <c r="I41" s="114"/>
+    </row>
+    <row r="42" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="149"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="122"/>
+      <c r="F42" s="105"/>
       <c r="G42" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H42" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="I42" s="118"/>
-    </row>
-    <row r="43" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C43" s="119"/>
-      <c r="D43" s="107" t="s">
+      <c r="I42" s="115"/>
+    </row>
+    <row r="43" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="149"/>
+      <c r="D43" s="146" t="s">
         <v>187</v>
       </c>
-      <c r="E43" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="113" t="s">
+      <c r="E43" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="103" t="s">
         <v>188</v>
       </c>
       <c r="G43" s="57" t="s">
@@ -2813,47 +2933,47 @@
       <c r="H43" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="I43" s="116" t="s">
+      <c r="I43" s="113" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C44" s="119"/>
-      <c r="D44" s="108"/>
-      <c r="E44" s="111"/>
-      <c r="F44" s="114"/>
+    <row r="44" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="149"/>
+      <c r="D44" s="147"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="104"/>
       <c r="G44" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H44" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="I44" s="117"/>
-    </row>
-    <row r="45" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C45" s="120"/>
-      <c r="D45" s="109"/>
-      <c r="E45" s="112"/>
-      <c r="F45" s="115"/>
+      <c r="I44" s="114"/>
+    </row>
+    <row r="45" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="150"/>
+      <c r="D45" s="148"/>
+      <c r="E45" s="122"/>
+      <c r="F45" s="105"/>
       <c r="G45" s="42" t="s">
         <v>31</v>
       </c>
       <c r="H45" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="I45" s="118"/>
-    </row>
-    <row r="46" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I45" s="115"/>
+    </row>
+    <row r="46" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="121" t="s">
+      <c r="D46" s="151" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="122" t="s">
+      <c r="E46" s="152" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="136" t="s">
+      <c r="F46" s="101" t="s">
         <v>78</v>
       </c>
       <c r="G46" s="30" t="s">
@@ -2862,45 +2982,45 @@
       <c r="H46" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="145" t="s">
+      <c r="I46" s="99" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="16"/>
-      <c r="D47" s="121"/>
-      <c r="E47" s="122"/>
-      <c r="F47" s="136"/>
+      <c r="D47" s="151"/>
+      <c r="E47" s="152"/>
+      <c r="F47" s="101"/>
       <c r="G47" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="I47" s="145"/>
-    </row>
-    <row r="48" spans="3:9" ht="31.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I47" s="99"/>
+    </row>
+    <row r="48" spans="3:9" ht="31.35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="7"/>
-      <c r="D48" s="121"/>
-      <c r="E48" s="122"/>
-      <c r="F48" s="136"/>
+      <c r="D48" s="151"/>
+      <c r="E48" s="152"/>
+      <c r="F48" s="101"/>
       <c r="G48" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H48" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="145"/>
-    </row>
-    <row r="49" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I48" s="99"/>
+    </row>
+    <row r="49" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="7"/>
-      <c r="D49" s="123" t="s">
+      <c r="D49" s="138" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="98" t="s">
+      <c r="E49" s="123" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="101" t="s">
+      <c r="F49" s="129" t="s">
         <v>85</v>
       </c>
       <c r="G49" s="30" t="s">
@@ -2909,45 +3029,45 @@
       <c r="H49" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I49" s="104" t="s">
+      <c r="I49" s="95" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="7"/>
-      <c r="D50" s="124"/>
-      <c r="E50" s="99"/>
-      <c r="F50" s="102"/>
+      <c r="D50" s="140"/>
+      <c r="E50" s="124"/>
+      <c r="F50" s="130"/>
       <c r="G50" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H50" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="I50" s="105"/>
-    </row>
-    <row r="51" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I50" s="96"/>
+    </row>
+    <row r="51" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="7"/>
-      <c r="D51" s="125"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="103"/>
+      <c r="D51" s="139"/>
+      <c r="E51" s="125"/>
+      <c r="F51" s="131"/>
       <c r="G51" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H51" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I51" s="106"/>
-    </row>
-    <row r="52" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I51" s="97"/>
+    </row>
+    <row r="52" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="7"/>
-      <c r="D52" s="123" t="s">
+      <c r="D52" s="138" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="101" t="s">
+      <c r="E52" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="129" t="s">
         <v>91</v>
       </c>
       <c r="G52" s="30" t="s">
@@ -2956,24 +3076,24 @@
       <c r="H52" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="104" t="s">
+      <c r="I52" s="95" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="7"/>
-      <c r="D53" s="125"/>
-      <c r="E53" s="100"/>
-      <c r="F53" s="103"/>
+      <c r="D53" s="139"/>
+      <c r="E53" s="125"/>
+      <c r="F53" s="131"/>
       <c r="G53" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H53" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="I53" s="106"/>
-    </row>
-    <row r="54" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I53" s="97"/>
+    </row>
+    <row r="54" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="7"/>
       <c r="D54" s="50"/>
       <c r="E54" s="49"/>
@@ -2986,7 +3106,7 @@
       </c>
       <c r="I54" s="51"/>
     </row>
-    <row r="55" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="7"/>
       <c r="D55" s="50" t="s">
         <v>178</v>
@@ -3005,7 +3125,7 @@
       </c>
       <c r="I55" s="51"/>
     </row>
-    <row r="56" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="7"/>
       <c r="D56" s="50"/>
       <c r="E56" s="49"/>
@@ -3016,15 +3136,15 @@
       <c r="H56" s="52"/>
       <c r="I56" s="51"/>
     </row>
-    <row r="57" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="7"/>
-      <c r="D57" s="123" t="s">
+      <c r="D57" s="138" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="98" t="s">
+      <c r="E57" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="101" t="s">
+      <c r="F57" s="129" t="s">
         <v>96</v>
       </c>
       <c r="G57" s="30" t="s">
@@ -3033,58 +3153,58 @@
       <c r="H57" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="I57" s="104" t="s">
+      <c r="I57" s="95" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="7"/>
-      <c r="D58" s="124"/>
-      <c r="E58" s="99"/>
-      <c r="F58" s="102"/>
+      <c r="D58" s="140"/>
+      <c r="E58" s="124"/>
+      <c r="F58" s="130"/>
       <c r="G58" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H58" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="I58" s="105"/>
-    </row>
-    <row r="59" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I58" s="96"/>
+    </row>
+    <row r="59" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="7"/>
-      <c r="D59" s="124"/>
-      <c r="E59" s="99"/>
-      <c r="F59" s="102"/>
+      <c r="D59" s="140"/>
+      <c r="E59" s="124"/>
+      <c r="F59" s="130"/>
       <c r="G59" s="32" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I59" s="105"/>
-    </row>
-    <row r="60" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I59" s="96"/>
+    </row>
+    <row r="60" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="7"/>
-      <c r="D60" s="125"/>
-      <c r="E60" s="100"/>
-      <c r="F60" s="103"/>
+      <c r="D60" s="139"/>
+      <c r="E60" s="125"/>
+      <c r="F60" s="131"/>
       <c r="G60" s="32" t="s">
         <v>100</v>
       </c>
       <c r="H60" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I60" s="106"/>
-    </row>
-    <row r="61" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I60" s="97"/>
+    </row>
+    <row r="61" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="7"/>
-      <c r="D61" s="123" t="s">
+      <c r="D61" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="98" t="s">
+      <c r="E61" s="123" t="s">
         <v>103</v>
       </c>
-      <c r="F61" s="101" t="s">
+      <c r="F61" s="129" t="s">
         <v>104</v>
       </c>
       <c r="G61" s="30" t="s">
@@ -3093,58 +3213,58 @@
       <c r="H61" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="I61" s="104" t="s">
+      <c r="I61" s="95" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="7"/>
-      <c r="D62" s="124"/>
-      <c r="E62" s="99"/>
-      <c r="F62" s="102"/>
+      <c r="D62" s="140"/>
+      <c r="E62" s="124"/>
+      <c r="F62" s="130"/>
       <c r="G62" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H62" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="I62" s="105"/>
-    </row>
-    <row r="63" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I62" s="96"/>
+    </row>
+    <row r="63" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C63" s="7"/>
-      <c r="D63" s="124"/>
-      <c r="E63" s="99"/>
-      <c r="F63" s="102"/>
+      <c r="D63" s="140"/>
+      <c r="E63" s="124"/>
+      <c r="F63" s="130"/>
       <c r="G63" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H63" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="I63" s="105"/>
-    </row>
-    <row r="64" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I63" s="96"/>
+    </row>
+    <row r="64" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="7"/>
-      <c r="D64" s="125"/>
-      <c r="E64" s="100"/>
-      <c r="F64" s="103"/>
+      <c r="D64" s="139"/>
+      <c r="E64" s="125"/>
+      <c r="F64" s="131"/>
       <c r="G64" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H64" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I64" s="106"/>
-    </row>
-    <row r="65" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I64" s="97"/>
+    </row>
+    <row r="65" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="7"/>
-      <c r="D65" s="123" t="s">
+      <c r="D65" s="138" t="s">
         <v>109</v>
       </c>
-      <c r="E65" s="98" t="s">
+      <c r="E65" s="123" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="101" t="s">
+      <c r="F65" s="129" t="s">
         <v>111</v>
       </c>
       <c r="G65" s="30" t="s">
@@ -3153,84 +3273,84 @@
       <c r="H65" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="I65" s="104" t="s">
+      <c r="I65" s="95" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="7"/>
-      <c r="D66" s="124"/>
-      <c r="E66" s="99"/>
-      <c r="F66" s="102"/>
+      <c r="D66" s="140"/>
+      <c r="E66" s="124"/>
+      <c r="F66" s="130"/>
       <c r="G66" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H66" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I66" s="105"/>
-    </row>
-    <row r="67" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I66" s="96"/>
+    </row>
+    <row r="67" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="7"/>
-      <c r="D67" s="124"/>
-      <c r="E67" s="99"/>
-      <c r="F67" s="102"/>
+      <c r="D67" s="140"/>
+      <c r="E67" s="124"/>
+      <c r="F67" s="130"/>
       <c r="G67" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H67" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="I67" s="105"/>
-    </row>
-    <row r="68" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I67" s="96"/>
+    </row>
+    <row r="68" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="7"/>
-      <c r="D68" s="124"/>
-      <c r="E68" s="99"/>
-      <c r="F68" s="102"/>
+      <c r="D68" s="140"/>
+      <c r="E68" s="124"/>
+      <c r="F68" s="130"/>
       <c r="G68" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H68" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="I68" s="105"/>
-    </row>
-    <row r="69" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I68" s="96"/>
+    </row>
+    <row r="69" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="7"/>
-      <c r="D69" s="124"/>
-      <c r="E69" s="99"/>
-      <c r="F69" s="102"/>
+      <c r="D69" s="140"/>
+      <c r="E69" s="124"/>
+      <c r="F69" s="130"/>
       <c r="G69" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H69" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I69" s="105"/>
-    </row>
-    <row r="70" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C70" s="93"/>
-      <c r="D70" s="125"/>
-      <c r="E70" s="100"/>
-      <c r="F70" s="103"/>
+      <c r="I69" s="96"/>
+    </row>
+    <row r="70" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="141"/>
+      <c r="D70" s="139"/>
+      <c r="E70" s="125"/>
+      <c r="F70" s="131"/>
       <c r="G70" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H70" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="I70" s="106"/>
-    </row>
-    <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C71" s="93"/>
-      <c r="D71" s="95" t="s">
+      <c r="I70" s="97"/>
+    </row>
+    <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="141"/>
+      <c r="D71" s="143" t="s">
         <v>189</v>
       </c>
-      <c r="E71" s="98" t="s">
+      <c r="E71" s="123" t="s">
         <v>190</v>
       </c>
-      <c r="F71" s="101" t="s">
+      <c r="F71" s="129" t="s">
         <v>191</v>
       </c>
       <c r="G71" s="30" t="s">
@@ -3239,57 +3359,57 @@
       <c r="H71" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="I71" s="104" t="s">
+      <c r="I71" s="95" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C72" s="93"/>
-      <c r="D72" s="96"/>
-      <c r="E72" s="99"/>
-      <c r="F72" s="102"/>
+    <row r="72" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="141"/>
+      <c r="D72" s="144"/>
+      <c r="E72" s="124"/>
+      <c r="F72" s="130"/>
       <c r="G72" s="32" t="s">
         <v>70</v>
       </c>
       <c r="H72" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="I72" s="105"/>
-    </row>
-    <row r="73" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C73" s="93"/>
-      <c r="D73" s="96"/>
-      <c r="E73" s="99"/>
-      <c r="F73" s="102"/>
+      <c r="I72" s="96"/>
+    </row>
+    <row r="73" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="141"/>
+      <c r="D73" s="144"/>
+      <c r="E73" s="124"/>
+      <c r="F73" s="130"/>
       <c r="G73" s="32" t="s">
         <v>72</v>
       </c>
       <c r="H73" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="I73" s="105"/>
-    </row>
-    <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C74" s="94"/>
-      <c r="D74" s="97"/>
-      <c r="E74" s="100"/>
-      <c r="F74" s="103"/>
+      <c r="I73" s="96"/>
+    </row>
+    <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="142"/>
+      <c r="D74" s="145"/>
+      <c r="E74" s="125"/>
+      <c r="F74" s="131"/>
       <c r="G74" s="60" t="s">
         <v>31</v>
       </c>
       <c r="H74" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="I74" s="106"/>
-    </row>
-    <row r="75" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I74" s="97"/>
+    </row>
+    <row r="75" spans="3:9" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D75" s="87" t="s">
+      <c r="D75" s="135" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="73" t="s">
+      <c r="E75" s="132" t="s">
         <v>120</v>
       </c>
       <c r="F75" s="126" t="s">
@@ -3301,14 +3421,14 @@
       <c r="H75" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="I75" s="81" t="s">
+      <c r="I75" s="92" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C76" s="9"/>
-      <c r="D76" s="88"/>
-      <c r="E76" s="74"/>
+      <c r="D76" s="136"/>
+      <c r="E76" s="133"/>
       <c r="F76" s="127"/>
       <c r="G76" s="28" t="s">
         <v>53</v>
@@ -3316,12 +3436,12 @@
       <c r="H76" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="I76" s="82"/>
-    </row>
-    <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I76" s="93"/>
+    </row>
+    <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C77" s="10"/>
-      <c r="D77" s="88"/>
-      <c r="E77" s="74"/>
+      <c r="D77" s="136"/>
+      <c r="E77" s="133"/>
       <c r="F77" s="127"/>
       <c r="G77" s="28" t="s">
         <v>53</v>
@@ -3329,12 +3449,12 @@
       <c r="H77" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I77" s="82"/>
-    </row>
-    <row r="78" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I77" s="93"/>
+    </row>
+    <row r="78" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C78" s="10"/>
-      <c r="D78" s="89"/>
-      <c r="E78" s="75"/>
+      <c r="D78" s="137"/>
+      <c r="E78" s="134"/>
       <c r="F78" s="128"/>
       <c r="G78" s="28" t="s">
         <v>53</v>
@@ -3342,1358 +3462,1471 @@
       <c r="H78" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="I78" s="83"/>
-    </row>
-    <row r="79" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I78" s="94"/>
+    </row>
+    <row r="79" spans="3:9" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="10"/>
-      <c r="D79" s="87" t="s">
+      <c r="D79" s="135" t="s">
+        <v>221</v>
+      </c>
+      <c r="E79" s="132" t="s">
+        <v>120</v>
+      </c>
+      <c r="F79" s="153" t="s">
+        <v>222</v>
+      </c>
+      <c r="G79" s="166" t="s">
+        <v>28</v>
+      </c>
+      <c r="H79" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="I79" s="92" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="10"/>
+      <c r="D80" s="136"/>
+      <c r="E80" s="133"/>
+      <c r="F80" s="154"/>
+      <c r="G80" s="167" t="s">
+        <v>65</v>
+      </c>
+      <c r="H80" s="164" t="s">
+        <v>234</v>
+      </c>
+      <c r="I80" s="93"/>
+    </row>
+    <row r="81" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="10"/>
+      <c r="D81" s="136"/>
+      <c r="E81" s="133"/>
+      <c r="F81" s="154"/>
+      <c r="G81" s="165" t="s">
+        <v>53</v>
+      </c>
+      <c r="H81" s="164" t="s">
+        <v>233</v>
+      </c>
+      <c r="I81" s="93"/>
+    </row>
+    <row r="82" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="10"/>
+      <c r="D82" s="136"/>
+      <c r="E82" s="133"/>
+      <c r="F82" s="154"/>
+      <c r="G82" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="H82" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="I82" s="93"/>
+    </row>
+    <row r="83" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C83" s="10"/>
+      <c r="D83" s="137"/>
+      <c r="E83" s="134"/>
+      <c r="F83" s="155"/>
+      <c r="G83" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H83" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="I83" s="94"/>
+    </row>
+    <row r="84" spans="3:9" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="10"/>
+      <c r="D84" s="135" t="s">
+        <v>225</v>
+      </c>
+      <c r="E84" s="132" t="s">
+        <v>120</v>
+      </c>
+      <c r="F84" s="153" t="s">
+        <v>226</v>
+      </c>
+      <c r="G84" s="168" t="s">
+        <v>28</v>
+      </c>
+      <c r="H84" s="170" t="s">
+        <v>227</v>
+      </c>
+      <c r="I84" s="92" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="3:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C85" s="10"/>
+      <c r="D85" s="136"/>
+      <c r="E85" s="133"/>
+      <c r="F85" s="154"/>
+      <c r="G85" s="169" t="s">
+        <v>28</v>
+      </c>
+      <c r="H85" s="171" t="s">
+        <v>236</v>
+      </c>
+      <c r="I85" s="93"/>
+    </row>
+    <row r="86" spans="3:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C86" s="10"/>
+      <c r="D86" s="136"/>
+      <c r="E86" s="133"/>
+      <c r="F86" s="154"/>
+      <c r="G86" s="169" t="s">
+        <v>53</v>
+      </c>
+      <c r="H86" s="171" t="s">
+        <v>235</v>
+      </c>
+      <c r="I86" s="93"/>
+    </row>
+    <row r="87" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C87" s="10"/>
+      <c r="D87" s="136"/>
+      <c r="E87" s="133"/>
+      <c r="F87" s="154"/>
+      <c r="G87" s="173" t="s">
+        <v>53</v>
+      </c>
+      <c r="H87" s="174" t="s">
+        <v>228</v>
+      </c>
+      <c r="I87" s="93"/>
+    </row>
+    <row r="88" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C88" s="10"/>
+      <c r="D88" s="137"/>
+      <c r="E88" s="134"/>
+      <c r="F88" s="155"/>
+      <c r="G88" s="172" t="s">
+        <v>70</v>
+      </c>
+      <c r="H88" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="I88" s="94"/>
+    </row>
+    <row r="89" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="10"/>
+      <c r="D89" s="135" t="s">
+        <v>229</v>
+      </c>
+      <c r="E89" s="132" t="s">
+        <v>120</v>
+      </c>
+      <c r="F89" s="153" t="s">
+        <v>230</v>
+      </c>
+      <c r="G89" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H89" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="I89" s="92" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="10"/>
+      <c r="D90" s="136"/>
+      <c r="E90" s="133"/>
+      <c r="F90" s="154"/>
+      <c r="G90" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="H90" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="I90" s="93"/>
+    </row>
+    <row r="91" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C91" s="10"/>
+      <c r="D91" s="137"/>
+      <c r="E91" s="134"/>
+      <c r="F91" s="155"/>
+      <c r="G91" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H91" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="I91" s="94"/>
+    </row>
+    <row r="92" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C92" s="10"/>
+      <c r="D92" s="135" t="s">
         <v>126</v>
       </c>
-      <c r="E79" s="73" t="s">
+      <c r="E92" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="90" t="s">
+      <c r="F92" s="153" t="s">
         <v>127</v>
       </c>
-      <c r="G79" s="26" t="s">
+      <c r="G92" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="H79" s="27" t="s">
+      <c r="H92" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="I79" s="81" t="s">
+      <c r="I92" s="92" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C80" s="10"/>
-      <c r="D80" s="88"/>
-      <c r="E80" s="74"/>
-      <c r="F80" s="91"/>
-      <c r="G80" s="28" t="s">
+    <row r="93" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C93" s="10"/>
+      <c r="D93" s="136"/>
+      <c r="E93" s="133"/>
+      <c r="F93" s="154"/>
+      <c r="G93" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H80" s="29" t="s">
+      <c r="H93" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="I80" s="82"/>
-    </row>
-    <row r="81" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C81" s="10"/>
-      <c r="D81" s="89"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="92"/>
-      <c r="G81" s="28" t="s">
+      <c r="I93" s="93"/>
+    </row>
+    <row r="94" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="10"/>
+      <c r="D94" s="137"/>
+      <c r="E94" s="134"/>
+      <c r="F94" s="155"/>
+      <c r="G94" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="H81" s="29" t="s">
+      <c r="H94" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I81" s="83"/>
-    </row>
-    <row r="82" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C82" s="10"/>
-      <c r="D82" s="87" t="s">
+      <c r="I94" s="94"/>
+    </row>
+    <row r="95" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="10"/>
+      <c r="D95" s="135" t="s">
         <v>131</v>
       </c>
-      <c r="E82" s="73" t="s">
+      <c r="E95" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F82" s="90" t="s">
+      <c r="F95" s="153" t="s">
         <v>132</v>
       </c>
-      <c r="G82" s="26" t="s">
+      <c r="G95" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="H82" s="27" t="s">
+      <c r="H95" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="I82" s="81" t="s">
+      <c r="I95" s="92" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C83" s="10"/>
-      <c r="D83" s="88"/>
-      <c r="E83" s="74"/>
-      <c r="F83" s="91"/>
-      <c r="G83" s="28" t="s">
+    <row r="96" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="10"/>
+      <c r="D96" s="136"/>
+      <c r="E96" s="133"/>
+      <c r="F96" s="154"/>
+      <c r="G96" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H83" s="29" t="s">
+      <c r="H96" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="I83" s="82"/>
-    </row>
-    <row r="84" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C84" s="10"/>
-      <c r="D84" s="89"/>
-      <c r="E84" s="75"/>
-      <c r="F84" s="92"/>
-      <c r="G84" s="28" t="s">
+      <c r="I96" s="93"/>
+    </row>
+    <row r="97" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C97" s="10"/>
+      <c r="D97" s="137"/>
+      <c r="E97" s="134"/>
+      <c r="F97" s="155"/>
+      <c r="G97" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="H84" s="29" t="s">
+      <c r="H97" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I84" s="83"/>
-    </row>
-    <row r="85" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C85" s="10"/>
-      <c r="D85" s="87" t="s">
+      <c r="I97" s="94"/>
+    </row>
+    <row r="98" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C98" s="10"/>
+      <c r="D98" s="135" t="s">
         <v>135</v>
       </c>
-      <c r="E85" s="73" t="s">
+      <c r="E98" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F85" s="90" t="s">
+      <c r="F98" s="153" t="s">
         <v>136</v>
       </c>
-      <c r="G85" s="26" t="s">
+      <c r="G98" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="H85" s="27" t="s">
+      <c r="H98" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="I85" s="81" t="s">
+      <c r="I98" s="92" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C86" s="79"/>
-      <c r="D86" s="88"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="91"/>
-      <c r="G86" s="28" t="s">
+    <row r="99" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C99" s="162"/>
+      <c r="D99" s="136"/>
+      <c r="E99" s="133"/>
+      <c r="F99" s="154"/>
+      <c r="G99" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H86" s="29" t="s">
+      <c r="H99" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="I86" s="82"/>
-    </row>
-    <row r="87" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C87" s="79"/>
-      <c r="D87" s="89"/>
-      <c r="E87" s="75"/>
-      <c r="F87" s="92"/>
-      <c r="G87" s="28" t="s">
+      <c r="I99" s="93"/>
+    </row>
+    <row r="100" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C100" s="162"/>
+      <c r="D100" s="137"/>
+      <c r="E100" s="134"/>
+      <c r="F100" s="155"/>
+      <c r="G100" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="H87" s="29" t="s">
+      <c r="H100" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="I87" s="83"/>
-    </row>
-    <row r="88" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C88" s="79"/>
-      <c r="D88" s="70" t="s">
+      <c r="I100" s="94"/>
+    </row>
+    <row r="101" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C101" s="162"/>
+      <c r="D101" s="156" t="s">
         <v>192</v>
       </c>
-      <c r="E88" s="73" t="s">
+      <c r="E101" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F88" s="76" t="s">
+      <c r="F101" s="159" t="s">
         <v>195</v>
       </c>
-      <c r="G88" s="26" t="s">
+      <c r="G101" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="H88" s="59" t="s">
+      <c r="H101" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="I88" s="81" t="s">
+      <c r="I101" s="92" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C89" s="79"/>
-      <c r="D89" s="71"/>
-      <c r="E89" s="74"/>
-      <c r="F89" s="77"/>
-      <c r="G89" s="28" t="s">
+    <row r="102" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="162"/>
+      <c r="D102" s="157"/>
+      <c r="E102" s="133"/>
+      <c r="F102" s="160"/>
+      <c r="G102" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="H89" s="56" t="s">
+      <c r="H102" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="I89" s="82"/>
-    </row>
-    <row r="90" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C90" s="79"/>
-      <c r="D90" s="72"/>
-      <c r="E90" s="75"/>
-      <c r="F90" s="78"/>
-      <c r="G90" s="28" t="s">
+      <c r="I102" s="93"/>
+    </row>
+    <row r="103" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C103" s="162"/>
+      <c r="D103" s="158"/>
+      <c r="E103" s="134"/>
+      <c r="F103" s="161"/>
+      <c r="G103" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="H90" s="56" t="s">
+      <c r="H103" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="I90" s="83"/>
-    </row>
-    <row r="91" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C91" s="79"/>
-      <c r="D91" s="70" t="s">
+      <c r="I103" s="94"/>
+    </row>
+    <row r="104" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C104" s="162"/>
+      <c r="D104" s="156" t="s">
         <v>193</v>
       </c>
-      <c r="E91" s="73" t="s">
+      <c r="E104" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F91" s="76" t="s">
+      <c r="F104" s="159" t="s">
         <v>196</v>
       </c>
-      <c r="G91" s="26" t="s">
+      <c r="G104" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="H91" s="59" t="s">
+      <c r="H104" s="59" t="s">
         <v>212</v>
       </c>
-      <c r="I91" s="81" t="s">
+      <c r="I104" s="92" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C92" s="79"/>
-      <c r="D92" s="71"/>
-      <c r="E92" s="74"/>
-      <c r="F92" s="77"/>
-      <c r="G92" s="28" t="s">
+    <row r="105" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C105" s="162"/>
+      <c r="D105" s="157"/>
+      <c r="E105" s="133"/>
+      <c r="F105" s="160"/>
+      <c r="G105" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="H92" s="56" t="s">
+      <c r="H105" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="I92" s="82"/>
-    </row>
-    <row r="93" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C93" s="79"/>
-      <c r="D93" s="72"/>
-      <c r="E93" s="75"/>
-      <c r="F93" s="78"/>
-      <c r="G93" s="28" t="s">
+      <c r="I105" s="93"/>
+    </row>
+    <row r="106" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C106" s="162"/>
+      <c r="D106" s="158"/>
+      <c r="E106" s="134"/>
+      <c r="F106" s="161"/>
+      <c r="G106" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H93" s="56" t="s">
+      <c r="H106" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="I93" s="83"/>
-    </row>
-    <row r="94" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C94" s="79"/>
-      <c r="D94" s="70" t="s">
+      <c r="I106" s="94"/>
+    </row>
+    <row r="107" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="162"/>
+      <c r="D107" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="E94" s="73" t="s">
+      <c r="E107" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="F94" s="76" t="s">
+      <c r="F107" s="159" t="s">
         <v>196</v>
       </c>
-      <c r="G94" s="26" t="s">
+      <c r="G107" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="H94" s="59" t="s">
+      <c r="H107" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="I94" s="81" t="s">
+      <c r="I107" s="92" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C95" s="79"/>
-      <c r="D95" s="71"/>
-      <c r="E95" s="74"/>
-      <c r="F95" s="77"/>
-      <c r="G95" s="28" t="s">
+    <row r="108" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C108" s="162"/>
+      <c r="D108" s="157"/>
+      <c r="E108" s="133"/>
+      <c r="F108" s="160"/>
+      <c r="G108" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="H95" s="56" t="s">
+      <c r="H108" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="I95" s="82"/>
-    </row>
-    <row r="96" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C96" s="80"/>
-      <c r="D96" s="72"/>
-      <c r="E96" s="75"/>
-      <c r="F96" s="78"/>
-      <c r="G96" s="28" t="s">
+      <c r="I108" s="93"/>
+    </row>
+    <row r="109" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C109" s="163"/>
+      <c r="D109" s="158"/>
+      <c r="E109" s="134"/>
+      <c r="F109" s="161"/>
+      <c r="G109" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H96" s="56" t="s">
+      <c r="H109" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="I96" s="83"/>
-    </row>
-    <row r="97" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C97" s="11" t="s">
+      <c r="I109" s="94"/>
+    </row>
+    <row r="110" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C110" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D97" s="62" t="s">
+      <c r="D110" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="E97" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F97" s="66" t="s">
+      <c r="E110" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="G97" s="18" t="s">
+      <c r="G110" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H97" s="19" t="s">
+      <c r="H110" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I97" s="68" t="s">
+      <c r="I110" s="88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C98" s="12"/>
-      <c r="D98" s="86"/>
-      <c r="E98" s="84"/>
-      <c r="F98" s="85"/>
-      <c r="G98" s="20" t="s">
+    <row r="111" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C111" s="12"/>
+      <c r="D111" s="80"/>
+      <c r="E111" s="83"/>
+      <c r="F111" s="86"/>
+      <c r="G111" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H98" s="21" t="s">
+      <c r="H111" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="I98" s="144"/>
-    </row>
-    <row r="99" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C99" s="13"/>
-      <c r="D99" s="63"/>
-      <c r="E99" s="65"/>
-      <c r="F99" s="67"/>
-      <c r="G99" s="160" t="s">
+      <c r="I111" s="89"/>
+    </row>
+    <row r="112" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C112" s="13"/>
+      <c r="D112" s="81"/>
+      <c r="E112" s="84"/>
+      <c r="F112" s="87"/>
+      <c r="G112" s="69" t="s">
         <v>143</v>
       </c>
-      <c r="H99" s="161" t="s">
+      <c r="H112" s="70" t="s">
         <v>144</v>
       </c>
-      <c r="I99" s="69"/>
-    </row>
-    <row r="100" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C100" s="13"/>
-      <c r="D100" s="158"/>
-      <c r="E100" s="150" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="155" t="s">
+      <c r="I112" s="90"/>
+    </row>
+    <row r="113" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C113" s="13"/>
+      <c r="D113" s="67"/>
+      <c r="E113" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F113" s="76" t="s">
         <v>217</v>
       </c>
-      <c r="G100" s="162" t="s">
+      <c r="G113" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="H100" s="163" t="s">
+      <c r="H113" s="72" t="s">
         <v>218</v>
       </c>
-      <c r="I100" s="153"/>
-    </row>
-    <row r="101" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C101" s="13"/>
-      <c r="D101" s="158" t="s">
+      <c r="I113" s="65"/>
+    </row>
+    <row r="114" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C114" s="13"/>
+      <c r="D114" s="67" t="s">
         <v>216</v>
       </c>
-      <c r="E101" s="151"/>
-      <c r="F101" s="156"/>
-      <c r="G101" s="154" t="s">
+      <c r="E114" s="74"/>
+      <c r="F114" s="77"/>
+      <c r="G114" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="H101" s="149" t="s">
+      <c r="H114" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="I101" s="153" t="s">
+      <c r="I114" s="65" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C102" s="13"/>
-      <c r="D102" s="159"/>
-      <c r="E102" s="152"/>
-      <c r="F102" s="157"/>
-      <c r="G102" s="148" t="s">
+    <row r="115" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C115" s="13"/>
+      <c r="D115" s="68"/>
+      <c r="E115" s="75"/>
+      <c r="F115" s="78"/>
+      <c r="G115" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="H102" s="149" t="s">
+      <c r="H115" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="I102" s="153"/>
-    </row>
-    <row r="103" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C103" s="13"/>
-      <c r="D103" s="62" t="s">
+      <c r="I115" s="65"/>
+    </row>
+    <row r="116" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C116" s="13"/>
+      <c r="D116" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="E103" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F103" s="66" t="s">
+      <c r="E116" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F116" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="G103" s="18" t="s">
+      <c r="G116" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H103" s="19" t="s">
+      <c r="H116" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="I103" s="68" t="s">
+      <c r="I116" s="88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C104" s="13"/>
-      <c r="D104" s="86"/>
-      <c r="E104" s="84"/>
-      <c r="F104" s="85"/>
-      <c r="G104" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H104" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="I104" s="144"/>
-    </row>
-    <row r="105" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C105" s="13"/>
-      <c r="D105" s="86"/>
-      <c r="E105" s="84"/>
-      <c r="F105" s="85"/>
-      <c r="G105" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H105" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="I105" s="144"/>
-    </row>
-    <row r="106" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C106" s="13"/>
-      <c r="D106" s="63"/>
-      <c r="E106" s="65"/>
-      <c r="F106" s="67"/>
-      <c r="G106" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H106" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I106" s="69"/>
-    </row>
-    <row r="107" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C107" s="13"/>
-      <c r="D107" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="E107" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F107" s="66" t="s">
-        <v>152</v>
-      </c>
-      <c r="G107" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H107" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="I107" s="68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="108" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C108" s="13"/>
-      <c r="D108" s="86"/>
-      <c r="E108" s="84"/>
-      <c r="F108" s="85"/>
-      <c r="G108" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H108" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="I108" s="144"/>
-    </row>
-    <row r="109" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C109" s="13"/>
-      <c r="D109" s="86"/>
-      <c r="E109" s="84"/>
-      <c r="F109" s="85"/>
-      <c r="G109" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H109" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I109" s="144"/>
-    </row>
-    <row r="110" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C110" s="13"/>
-      <c r="D110" s="63"/>
-      <c r="E110" s="65"/>
-      <c r="F110" s="67"/>
-      <c r="G110" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="H110" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I110" s="69"/>
-    </row>
-    <row r="111" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C111" s="13"/>
-      <c r="D111" s="62" t="s">
-        <v>157</v>
-      </c>
-      <c r="E111" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F111" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="G111" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H111" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="I111" s="68" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="112" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C112" s="13"/>
-      <c r="D112" s="86"/>
-      <c r="E112" s="84"/>
-      <c r="F112" s="85"/>
-      <c r="G112" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H112" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I112" s="144"/>
-    </row>
-    <row r="113" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C113" s="13"/>
-      <c r="D113" s="86"/>
-      <c r="E113" s="84"/>
-      <c r="F113" s="85"/>
-      <c r="G113" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H113" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I113" s="144"/>
-    </row>
-    <row r="114" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C114" s="13"/>
-      <c r="D114" s="63"/>
-      <c r="E114" s="65"/>
-      <c r="F114" s="67"/>
-      <c r="G114" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="H114" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I114" s="69"/>
-    </row>
-    <row r="115" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C115" s="13"/>
-      <c r="D115" s="62" t="s">
-        <v>160</v>
-      </c>
-      <c r="E115" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F115" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="G115" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H115" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="I115" s="68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="116" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C116" s="13"/>
-      <c r="D116" s="86"/>
-      <c r="E116" s="84"/>
-      <c r="F116" s="85"/>
-      <c r="G116" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H116" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="I116" s="144"/>
-    </row>
-    <row r="117" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C117" s="14"/>
-      <c r="D117" s="63"/>
-      <c r="E117" s="65"/>
-      <c r="F117" s="67"/>
+    <row r="117" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C117" s="13"/>
+      <c r="D117" s="80"/>
+      <c r="E117" s="83"/>
+      <c r="F117" s="86"/>
       <c r="G117" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H117" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="I117" s="69"/>
-    </row>
-    <row r="118" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C118" s="14"/>
-      <c r="D118" s="62" t="s">
-        <v>164</v>
-      </c>
-      <c r="E118" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F118" s="66" t="s">
-        <v>165</v>
-      </c>
-      <c r="G118" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H118" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="I118" s="68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="119" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I117" s="89"/>
+    </row>
+    <row r="118" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C118" s="13"/>
+      <c r="D118" s="80"/>
+      <c r="E118" s="83"/>
+      <c r="F118" s="86"/>
+      <c r="G118" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H118" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="I118" s="89"/>
+    </row>
+    <row r="119" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C119" s="13"/>
-      <c r="D119" s="63"/>
-      <c r="E119" s="65"/>
-      <c r="F119" s="67"/>
+      <c r="D119" s="81"/>
+      <c r="E119" s="84"/>
+      <c r="F119" s="87"/>
       <c r="G119" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H119" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="I119" s="69"/>
-    </row>
-    <row r="120" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>150</v>
+      </c>
+      <c r="I119" s="90"/>
+    </row>
+    <row r="120" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C120" s="13"/>
-      <c r="D120" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="E120" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F120" s="66" t="s">
-        <v>169</v>
+      <c r="D120" s="79" t="s">
+        <v>151</v>
+      </c>
+      <c r="E120" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120" s="85" t="s">
+        <v>152</v>
       </c>
       <c r="G120" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H120" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="I120" s="68" t="s">
+        <v>153</v>
+      </c>
+      <c r="I120" s="88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C121" s="13"/>
-      <c r="D121" s="63"/>
-      <c r="E121" s="65"/>
-      <c r="F121" s="67"/>
+      <c r="D121" s="80"/>
+      <c r="E121" s="83"/>
+      <c r="F121" s="86"/>
       <c r="G121" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H121" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I121" s="69"/>
-    </row>
-    <row r="122" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+      <c r="I121" s="89"/>
+    </row>
+    <row r="122" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C122" s="13"/>
-      <c r="D122" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="E122" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F122" s="66" t="s">
-        <v>173</v>
-      </c>
-      <c r="G122" s="18" t="s">
+      <c r="D122" s="80"/>
+      <c r="E122" s="83"/>
+      <c r="F122" s="86"/>
+      <c r="G122" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H122" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="I122" s="89"/>
+    </row>
+    <row r="123" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C123" s="13"/>
+      <c r="D123" s="81"/>
+      <c r="E123" s="84"/>
+      <c r="F123" s="87"/>
+      <c r="G123" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H123" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="I123" s="90"/>
+    </row>
+    <row r="124" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C124" s="13"/>
+      <c r="D124" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="E124" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F124" s="85" t="s">
+        <v>158</v>
+      </c>
+      <c r="G124" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H122" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="I122" s="68" t="s">
+      <c r="H124" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="I124" s="88" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C123" s="13"/>
-      <c r="D123" s="86"/>
-      <c r="E123" s="84"/>
-      <c r="F123" s="85"/>
-      <c r="G123" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H123" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I123" s="144"/>
-    </row>
-    <row r="124" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C124" s="13"/>
-      <c r="D124" s="86"/>
-      <c r="E124" s="84"/>
-      <c r="F124" s="85"/>
-      <c r="G124" s="20" t="s">
+    <row r="125" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C125" s="13"/>
+      <c r="D125" s="80"/>
+      <c r="E125" s="83"/>
+      <c r="F125" s="86"/>
+      <c r="G125" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H124" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I124" s="144"/>
-    </row>
-    <row r="125" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C125" s="13"/>
-      <c r="D125" s="63"/>
-      <c r="E125" s="65"/>
-      <c r="F125" s="67"/>
-      <c r="G125" s="20" t="s">
+      <c r="H125" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I125" s="89"/>
+    </row>
+    <row r="126" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C126" s="13"/>
+      <c r="D126" s="80"/>
+      <c r="E126" s="83"/>
+      <c r="F126" s="86"/>
+      <c r="G126" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H125" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I125" s="69"/>
-    </row>
-    <row r="126" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C126" s="13"/>
-      <c r="D126" s="62" t="s">
-        <v>175</v>
-      </c>
-      <c r="E126" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F126" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G126" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H126" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="I126" s="68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="127" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C127" s="146"/>
-      <c r="D127" s="63"/>
-      <c r="E127" s="65"/>
-      <c r="F127" s="67"/>
-      <c r="G127" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="H127" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I127" s="69"/>
-    </row>
-    <row r="128" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C128" s="146"/>
-      <c r="D128" s="147" t="s">
-        <v>197</v>
-      </c>
-      <c r="E128" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F128" s="66" t="s">
-        <v>198</v>
+      <c r="H126" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I126" s="89"/>
+    </row>
+    <row r="127" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C127" s="13"/>
+      <c r="D127" s="81"/>
+      <c r="E127" s="84"/>
+      <c r="F127" s="87"/>
+      <c r="G127" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H127" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="I127" s="90"/>
+    </row>
+    <row r="128" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C128" s="13"/>
+      <c r="D128" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="E128" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F128" s="85" t="s">
+        <v>161</v>
       </c>
       <c r="G128" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H128" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="I128" s="68" t="s">
+      <c r="H128" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="I128" s="88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C129" s="13"/>
-      <c r="D129" s="63"/>
-      <c r="E129" s="65"/>
-      <c r="F129" s="67"/>
-      <c r="G129" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="H129" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="I129" s="69"/>
-    </row>
-    <row r="130" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C130" s="13"/>
-      <c r="D130" s="62" t="s">
-        <v>145</v>
-      </c>
-      <c r="E130" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F130" s="66" t="s">
-        <v>146</v>
-      </c>
-      <c r="G130" s="18" t="s">
+      <c r="D129" s="80"/>
+      <c r="E129" s="83"/>
+      <c r="F129" s="86"/>
+      <c r="G129" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H129" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="I129" s="89"/>
+    </row>
+    <row r="130" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C130" s="14"/>
+      <c r="D130" s="81"/>
+      <c r="E130" s="84"/>
+      <c r="F130" s="87"/>
+      <c r="G130" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H130" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="I130" s="90"/>
+    </row>
+    <row r="131" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C131" s="14"/>
+      <c r="D131" s="79" t="s">
+        <v>164</v>
+      </c>
+      <c r="E131" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F131" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="G131" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H130" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I130" s="68" t="s">
+      <c r="H131" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="I131" s="88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C131" s="13"/>
-      <c r="D131" s="86"/>
-      <c r="E131" s="84"/>
-      <c r="F131" s="85"/>
-      <c r="G131" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H131" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="I131" s="144"/>
-    </row>
-    <row r="132" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="132" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C132" s="13"/>
-      <c r="D132" s="86"/>
+      <c r="D132" s="81"/>
       <c r="E132" s="84"/>
-      <c r="F132" s="85"/>
+      <c r="F132" s="87"/>
       <c r="G132" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H132" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="I132" s="144"/>
-    </row>
-    <row r="133" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+        <v>167</v>
+      </c>
+      <c r="I132" s="90"/>
+    </row>
+    <row r="133" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C133" s="13"/>
-      <c r="D133" s="63"/>
-      <c r="E133" s="65"/>
-      <c r="F133" s="67"/>
-      <c r="G133" s="20" t="s">
+      <c r="D133" s="79" t="s">
+        <v>168</v>
+      </c>
+      <c r="E133" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F133" s="85" t="s">
+        <v>169</v>
+      </c>
+      <c r="G133" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H133" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I133" s="88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C134" s="13"/>
+      <c r="D134" s="81"/>
+      <c r="E134" s="84"/>
+      <c r="F134" s="87"/>
+      <c r="G134" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H133" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I133" s="69"/>
-    </row>
-    <row r="134" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C134" s="13"/>
-      <c r="D134" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="E134" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F134" s="66" t="s">
-        <v>152</v>
-      </c>
-      <c r="G134" s="18" t="s">
+      <c r="H134" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I134" s="90"/>
+    </row>
+    <row r="135" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C135" s="13"/>
+      <c r="D135" s="79" t="s">
+        <v>172</v>
+      </c>
+      <c r="E135" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135" s="85" t="s">
+        <v>173</v>
+      </c>
+      <c r="G135" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H134" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="I134" s="68" t="s">
+      <c r="H135" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="I135" s="88" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="136" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C136" s="13"/>
+      <c r="D136" s="80"/>
+      <c r="E136" s="83"/>
+      <c r="F136" s="86"/>
+      <c r="G136" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H136" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I136" s="89"/>
+    </row>
+    <row r="137" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C137" s="13"/>
+      <c r="D137" s="80"/>
+      <c r="E137" s="83"/>
+      <c r="F137" s="86"/>
+      <c r="G137" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H137" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I137" s="89"/>
+    </row>
+    <row r="138" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C138" s="13"/>
+      <c r="D138" s="81"/>
+      <c r="E138" s="84"/>
+      <c r="F138" s="87"/>
+      <c r="G138" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H138" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I138" s="90"/>
+    </row>
+    <row r="139" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C139" s="13"/>
+      <c r="D139" s="79" t="s">
+        <v>175</v>
+      </c>
+      <c r="E139" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F139" s="85" t="s">
+        <v>176</v>
+      </c>
+      <c r="G139" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H139" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I139" s="88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C135" s="13"/>
-      <c r="D135" s="86"/>
-      <c r="E135" s="84"/>
-      <c r="F135" s="85"/>
-      <c r="G135" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H135" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="I135" s="144"/>
-    </row>
-    <row r="136" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C136" s="13"/>
-      <c r="D136" s="86"/>
-      <c r="E136" s="84"/>
-      <c r="F136" s="85"/>
-      <c r="G136" s="20" t="s">
+    <row r="140" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C140" s="62"/>
+      <c r="D140" s="81"/>
+      <c r="E140" s="84"/>
+      <c r="F140" s="87"/>
+      <c r="G140" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H136" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I136" s="144"/>
-    </row>
-    <row r="137" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C137" s="13"/>
-      <c r="D137" s="63"/>
-      <c r="E137" s="65"/>
-      <c r="F137" s="67"/>
-      <c r="G137" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="H137" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I137" s="69"/>
-    </row>
-    <row r="138" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C138" s="13"/>
-      <c r="D138" s="62" t="s">
-        <v>157</v>
-      </c>
-      <c r="E138" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F138" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="G138" s="18" t="s">
+      <c r="H140" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I140" s="90"/>
+    </row>
+    <row r="141" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C141" s="62"/>
+      <c r="D141" s="91" t="s">
+        <v>197</v>
+      </c>
+      <c r="E141" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F141" s="85" t="s">
+        <v>198</v>
+      </c>
+      <c r="G141" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H138" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="I138" s="68" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="139" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C139" s="13"/>
-      <c r="D139" s="86"/>
-      <c r="E139" s="84"/>
-      <c r="F139" s="85"/>
-      <c r="G139" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H139" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I139" s="144"/>
-    </row>
-    <row r="140" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C140" s="13"/>
-      <c r="D140" s="86"/>
-      <c r="E140" s="84"/>
-      <c r="F140" s="85"/>
-      <c r="G140" s="20" t="s">
+      <c r="H141" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="I141" s="88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="142" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C142" s="13"/>
+      <c r="D142" s="81"/>
+      <c r="E142" s="84"/>
+      <c r="F142" s="87"/>
+      <c r="G142" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H140" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I140" s="144"/>
-    </row>
-    <row r="141" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C141" s="13"/>
-      <c r="D141" s="63"/>
-      <c r="E141" s="65"/>
-      <c r="F141" s="67"/>
-      <c r="G141" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="H141" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I141" s="69"/>
-    </row>
-    <row r="142" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C142" s="13"/>
-      <c r="D142" s="62" t="s">
-        <v>160</v>
-      </c>
-      <c r="E142" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F142" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="G142" s="18" t="s">
+      <c r="H142" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="I142" s="90"/>
+    </row>
+    <row r="143" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C143" s="13"/>
+      <c r="D143" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="E143" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="85" t="s">
+        <v>146</v>
+      </c>
+      <c r="G143" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H142" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="I142" s="68" t="s">
+      <c r="H143" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="I143" s="88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C143" s="13"/>
-      <c r="D143" s="86"/>
-      <c r="E143" s="84"/>
-      <c r="F143" s="85"/>
-      <c r="G143" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H143" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="I143" s="144"/>
-    </row>
-    <row r="144" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C144" s="14"/>
-      <c r="D144" s="63"/>
-      <c r="E144" s="65"/>
-      <c r="F144" s="67"/>
+    <row r="144" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C144" s="13"/>
+      <c r="D144" s="80"/>
+      <c r="E144" s="83"/>
+      <c r="F144" s="86"/>
       <c r="G144" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H144" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="I144" s="69"/>
-    </row>
-    <row r="145" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C145" s="14"/>
-      <c r="D145" s="62" t="s">
-        <v>164</v>
-      </c>
-      <c r="E145" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F145" s="66" t="s">
-        <v>165</v>
-      </c>
-      <c r="G145" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H145" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="I145" s="68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="146" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I144" s="89"/>
+    </row>
+    <row r="145" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C145" s="13"/>
+      <c r="D145" s="80"/>
+      <c r="E145" s="83"/>
+      <c r="F145" s="86"/>
+      <c r="G145" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H145" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="I145" s="89"/>
+    </row>
+    <row r="146" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C146" s="13"/>
-      <c r="D146" s="63"/>
-      <c r="E146" s="65"/>
-      <c r="F146" s="67"/>
+      <c r="D146" s="81"/>
+      <c r="E146" s="84"/>
+      <c r="F146" s="87"/>
       <c r="G146" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H146" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="I146" s="69"/>
-    </row>
-    <row r="147" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>150</v>
+      </c>
+      <c r="I146" s="90"/>
+    </row>
+    <row r="147" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C147" s="13"/>
-      <c r="D147" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="E147" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F147" s="66" t="s">
-        <v>169</v>
+      <c r="D147" s="79" t="s">
+        <v>151</v>
+      </c>
+      <c r="E147" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F147" s="85" t="s">
+        <v>152</v>
       </c>
       <c r="G147" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H147" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="I147" s="68" t="s">
+        <v>153</v>
+      </c>
+      <c r="I147" s="88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C148" s="13"/>
-      <c r="D148" s="63"/>
-      <c r="E148" s="65"/>
-      <c r="F148" s="67"/>
+      <c r="D148" s="80"/>
+      <c r="E148" s="83"/>
+      <c r="F148" s="86"/>
       <c r="G148" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H148" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I148" s="69"/>
-    </row>
-    <row r="149" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+      <c r="I148" s="89"/>
+    </row>
+    <row r="149" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C149" s="13"/>
-      <c r="D149" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="E149" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F149" s="66" t="s">
-        <v>173</v>
-      </c>
-      <c r="G149" s="18" t="s">
+      <c r="D149" s="80"/>
+      <c r="E149" s="83"/>
+      <c r="F149" s="86"/>
+      <c r="G149" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H149" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="I149" s="89"/>
+    </row>
+    <row r="150" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C150" s="13"/>
+      <c r="D150" s="81"/>
+      <c r="E150" s="84"/>
+      <c r="F150" s="87"/>
+      <c r="G150" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H150" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="I150" s="90"/>
+    </row>
+    <row r="151" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C151" s="13"/>
+      <c r="D151" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="E151" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F151" s="85" t="s">
+        <v>158</v>
+      </c>
+      <c r="G151" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H149" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="I149" s="68" t="s">
+      <c r="H151" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="I151" s="88" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="150" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C150" s="13"/>
-      <c r="D150" s="86"/>
-      <c r="E150" s="84"/>
-      <c r="F150" s="85"/>
-      <c r="G150" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="H150" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I150" s="144"/>
-    </row>
-    <row r="151" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C151" s="13"/>
-      <c r="D151" s="86"/>
-      <c r="E151" s="84"/>
-      <c r="F151" s="85"/>
-      <c r="G151" s="20" t="s">
+    <row r="152" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C152" s="13"/>
+      <c r="D152" s="80"/>
+      <c r="E152" s="83"/>
+      <c r="F152" s="86"/>
+      <c r="G152" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H151" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I151" s="144"/>
-    </row>
-    <row r="152" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C152" s="13"/>
-      <c r="D152" s="63"/>
-      <c r="E152" s="65"/>
-      <c r="F152" s="67"/>
-      <c r="G152" s="20" t="s">
+      <c r="H152" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I152" s="89"/>
+    </row>
+    <row r="153" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C153" s="13"/>
+      <c r="D153" s="80"/>
+      <c r="E153" s="83"/>
+      <c r="F153" s="86"/>
+      <c r="G153" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H152" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I152" s="69"/>
-    </row>
-    <row r="153" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C153" s="13"/>
-      <c r="D153" s="62" t="s">
-        <v>175</v>
-      </c>
-      <c r="E153" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F153" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G153" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H153" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="I153" s="68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="154" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C154" s="146"/>
-      <c r="D154" s="63"/>
-      <c r="E154" s="65"/>
-      <c r="F154" s="67"/>
-      <c r="G154" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="H154" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I154" s="69"/>
-    </row>
-    <row r="155" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C155" s="146"/>
-      <c r="D155" s="147" t="s">
-        <v>197</v>
-      </c>
-      <c r="E155" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F155" s="66" t="s">
-        <v>198</v>
+      <c r="H153" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I153" s="89"/>
+    </row>
+    <row r="154" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C154" s="13"/>
+      <c r="D154" s="81"/>
+      <c r="E154" s="84"/>
+      <c r="F154" s="87"/>
+      <c r="G154" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H154" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="I154" s="90"/>
+    </row>
+    <row r="155" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C155" s="13"/>
+      <c r="D155" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="E155" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F155" s="85" t="s">
+        <v>161</v>
       </c>
       <c r="G155" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H155" s="23" t="s">
+      <c r="H155" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="I155" s="88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C156" s="13"/>
+      <c r="D156" s="80"/>
+      <c r="E156" s="83"/>
+      <c r="F156" s="86"/>
+      <c r="G156" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H156" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="I156" s="89"/>
+    </row>
+    <row r="157" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C157" s="14"/>
+      <c r="D157" s="81"/>
+      <c r="E157" s="84"/>
+      <c r="F157" s="87"/>
+      <c r="G157" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H157" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="I157" s="90"/>
+    </row>
+    <row r="158" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C158" s="14"/>
+      <c r="D158" s="79" t="s">
+        <v>164</v>
+      </c>
+      <c r="E158" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F158" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="G158" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H158" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="I158" s="88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C159" s="13"/>
+      <c r="D159" s="81"/>
+      <c r="E159" s="84"/>
+      <c r="F159" s="87"/>
+      <c r="G159" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H159" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="I159" s="90"/>
+    </row>
+    <row r="160" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C160" s="13"/>
+      <c r="D160" s="79" t="s">
+        <v>168</v>
+      </c>
+      <c r="E160" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F160" s="85" t="s">
+        <v>169</v>
+      </c>
+      <c r="G160" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H160" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="I155" s="68" t="s">
+      <c r="I160" s="88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="3:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C156" s="15"/>
-      <c r="D156" s="63"/>
-      <c r="E156" s="65"/>
-      <c r="F156" s="67"/>
-      <c r="G156" s="24" t="s">
+    <row r="161" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C161" s="13"/>
+      <c r="D161" s="81"/>
+      <c r="E161" s="84"/>
+      <c r="F161" s="87"/>
+      <c r="G161" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H161" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I161" s="90"/>
+    </row>
+    <row r="162" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C162" s="13"/>
+      <c r="D162" s="79" t="s">
+        <v>172</v>
+      </c>
+      <c r="E162" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F162" s="85" t="s">
+        <v>173</v>
+      </c>
+      <c r="G162" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H162" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="I162" s="88" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="163" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C163" s="13"/>
+      <c r="D163" s="80"/>
+      <c r="E163" s="83"/>
+      <c r="F163" s="86"/>
+      <c r="G163" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H163" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I163" s="89"/>
+    </row>
+    <row r="164" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C164" s="13"/>
+      <c r="D164" s="80"/>
+      <c r="E164" s="83"/>
+      <c r="F164" s="86"/>
+      <c r="G164" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H164" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I164" s="89"/>
+    </row>
+    <row r="165" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C165" s="13"/>
+      <c r="D165" s="81"/>
+      <c r="E165" s="84"/>
+      <c r="F165" s="87"/>
+      <c r="G165" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H156" s="25" t="s">
+      <c r="H165" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I165" s="90"/>
+    </row>
+    <row r="166" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C166" s="13"/>
+      <c r="D166" s="79" t="s">
+        <v>175</v>
+      </c>
+      <c r="E166" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F166" s="85" t="s">
+        <v>176</v>
+      </c>
+      <c r="G166" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H166" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I166" s="88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="167" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C167" s="62"/>
+      <c r="D167" s="81"/>
+      <c r="E167" s="84"/>
+      <c r="F167" s="87"/>
+      <c r="G167" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H167" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I167" s="90"/>
+    </row>
+    <row r="168" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C168" s="62"/>
+      <c r="D168" s="91" t="s">
+        <v>197</v>
+      </c>
+      <c r="E168" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F168" s="85" t="s">
+        <v>198</v>
+      </c>
+      <c r="G168" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H168" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="I168" s="88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="169" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C169" s="15"/>
+      <c r="D169" s="81"/>
+      <c r="E169" s="84"/>
+      <c r="F169" s="87"/>
+      <c r="G169" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H169" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="I156" s="69"/>
+      <c r="I169" s="90"/>
     </row>
   </sheetData>
-  <mergeCells count="181">
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="D149:D152"/>
-    <mergeCell ref="E149:E152"/>
-    <mergeCell ref="F149:F152"/>
-    <mergeCell ref="I149:I152"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="E153:E154"/>
-    <mergeCell ref="F153:F154"/>
-    <mergeCell ref="I153:I154"/>
-    <mergeCell ref="D155:D156"/>
-    <mergeCell ref="E155:E156"/>
-    <mergeCell ref="F155:F156"/>
-    <mergeCell ref="I155:I156"/>
-    <mergeCell ref="D142:D144"/>
-    <mergeCell ref="E142:E144"/>
-    <mergeCell ref="F142:F144"/>
-    <mergeCell ref="I142:I144"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="F145:F146"/>
-    <mergeCell ref="I145:I146"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="D130:D133"/>
-    <mergeCell ref="E130:E133"/>
-    <mergeCell ref="F130:F133"/>
-    <mergeCell ref="I130:I133"/>
-    <mergeCell ref="D134:D137"/>
-    <mergeCell ref="E134:E137"/>
-    <mergeCell ref="F134:F137"/>
-    <mergeCell ref="I134:I137"/>
-    <mergeCell ref="D138:D141"/>
-    <mergeCell ref="E138:E141"/>
-    <mergeCell ref="F138:F141"/>
-    <mergeCell ref="I138:I141"/>
-    <mergeCell ref="I126:I127"/>
-    <mergeCell ref="I85:I87"/>
-    <mergeCell ref="I97:I99"/>
-    <mergeCell ref="I103:I106"/>
-    <mergeCell ref="I107:I110"/>
-    <mergeCell ref="I111:I114"/>
-    <mergeCell ref="I88:I90"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="I75:I78"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I60"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="I115:I117"/>
-    <mergeCell ref="I118:I119"/>
-    <mergeCell ref="I120:I121"/>
-    <mergeCell ref="I122:I125"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="I82:I84"/>
-    <mergeCell ref="I79:I81"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="F122:F125"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="E122:E125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="D111:D114"/>
-    <mergeCell ref="F111:F114"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="F115:F117"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E111:E114"/>
-    <mergeCell ref="E115:E117"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="D122:D125"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="F65:F70"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="D61:D64"/>
+  <mergeCells count="193">
+    <mergeCell ref="D79:D83"/>
+    <mergeCell ref="E79:E83"/>
+    <mergeCell ref="D84:D88"/>
+    <mergeCell ref="E84:E88"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="E89:E91"/>
+    <mergeCell ref="F79:F83"/>
+    <mergeCell ref="F84:F88"/>
+    <mergeCell ref="F89:F91"/>
+    <mergeCell ref="I79:I83"/>
+    <mergeCell ref="I84:I88"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="E141:E142"/>
+    <mergeCell ref="F141:F142"/>
+    <mergeCell ref="I141:I142"/>
+    <mergeCell ref="D101:D103"/>
+    <mergeCell ref="D104:D106"/>
+    <mergeCell ref="E104:E106"/>
+    <mergeCell ref="F104:F106"/>
+    <mergeCell ref="C99:C109"/>
+    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="E107:E109"/>
+    <mergeCell ref="F107:F109"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="E120:E123"/>
+    <mergeCell ref="E116:E119"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F120:F123"/>
+    <mergeCell ref="D120:D123"/>
+    <mergeCell ref="F116:F119"/>
+    <mergeCell ref="D116:D119"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="F101:F103"/>
+    <mergeCell ref="E101:E103"/>
+    <mergeCell ref="E95:E97"/>
+    <mergeCell ref="D98:D100"/>
+    <mergeCell ref="E98:E100"/>
+    <mergeCell ref="D92:D94"/>
+    <mergeCell ref="E92:E94"/>
+    <mergeCell ref="F92:F94"/>
+    <mergeCell ref="F95:F97"/>
+    <mergeCell ref="D95:D97"/>
+    <mergeCell ref="F98:F100"/>
     <mergeCell ref="C70:C74"/>
     <mergeCell ref="D71:D74"/>
     <mergeCell ref="E71:E74"/>
@@ -4718,39 +4951,131 @@
     <mergeCell ref="D49:D51"/>
     <mergeCell ref="E49:E51"/>
     <mergeCell ref="I65:I70"/>
-    <mergeCell ref="E82:E84"/>
-    <mergeCell ref="D85:D87"/>
-    <mergeCell ref="E85:E87"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="E79:E81"/>
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="D82:D84"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="D88:D90"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="E91:E93"/>
-    <mergeCell ref="F91:F93"/>
-    <mergeCell ref="C86:C96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="I91:I93"/>
-    <mergeCell ref="E107:E110"/>
-    <mergeCell ref="E103:E106"/>
-    <mergeCell ref="E97:E99"/>
-    <mergeCell ref="F107:F110"/>
-    <mergeCell ref="D107:D110"/>
-    <mergeCell ref="F103:F106"/>
-    <mergeCell ref="D103:D106"/>
-    <mergeCell ref="F97:F99"/>
-    <mergeCell ref="D97:D99"/>
-    <mergeCell ref="F88:F90"/>
-    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="F135:F138"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="F139:F140"/>
+    <mergeCell ref="E135:E138"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="E133:E134"/>
+    <mergeCell ref="D124:D127"/>
+    <mergeCell ref="F124:F127"/>
+    <mergeCell ref="D128:D130"/>
+    <mergeCell ref="F128:F130"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="F131:F132"/>
+    <mergeCell ref="E124:E127"/>
+    <mergeCell ref="E128:E130"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="F133:F134"/>
+    <mergeCell ref="D133:D134"/>
+    <mergeCell ref="D135:D138"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="I131:I132"/>
+    <mergeCell ref="I133:I134"/>
+    <mergeCell ref="I135:I138"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="I95:I97"/>
+    <mergeCell ref="I92:I94"/>
+    <mergeCell ref="I89:I91"/>
+    <mergeCell ref="I98:I100"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="I116:I119"/>
+    <mergeCell ref="I120:I123"/>
+    <mergeCell ref="I124:I127"/>
+    <mergeCell ref="I101:I103"/>
+    <mergeCell ref="I107:I109"/>
+    <mergeCell ref="I75:I78"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="D168:D169"/>
+    <mergeCell ref="E168:E169"/>
+    <mergeCell ref="F168:F169"/>
+    <mergeCell ref="I168:I169"/>
+    <mergeCell ref="D155:D157"/>
+    <mergeCell ref="E155:E157"/>
+    <mergeCell ref="F155:F157"/>
+    <mergeCell ref="I155:I157"/>
+    <mergeCell ref="D158:D159"/>
+    <mergeCell ref="E158:E159"/>
+    <mergeCell ref="F158:F159"/>
+    <mergeCell ref="I158:I159"/>
+    <mergeCell ref="D160:D161"/>
+    <mergeCell ref="E160:E161"/>
+    <mergeCell ref="F160:F161"/>
+    <mergeCell ref="I160:I161"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="D162:D165"/>
+    <mergeCell ref="E162:E165"/>
+    <mergeCell ref="F162:F165"/>
+    <mergeCell ref="I162:I165"/>
+    <mergeCell ref="D166:D167"/>
+    <mergeCell ref="E166:E167"/>
+    <mergeCell ref="F166:F167"/>
+    <mergeCell ref="I166:I167"/>
+    <mergeCell ref="D143:D146"/>
+    <mergeCell ref="E143:E146"/>
+    <mergeCell ref="F143:F146"/>
+    <mergeCell ref="I143:I146"/>
+    <mergeCell ref="D147:D150"/>
+    <mergeCell ref="E147:E150"/>
+    <mergeCell ref="F147:F150"/>
+    <mergeCell ref="I147:I150"/>
+    <mergeCell ref="D151:D154"/>
+    <mergeCell ref="E151:E154"/>
+    <mergeCell ref="F151:F154"/>
+    <mergeCell ref="I151:I154"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="I128:I130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Añadidos endpoints update account al excel
</commit_message>
<xml_diff>
--- a/.readmeFiles/Endpoints.xlsx
+++ b/.readmeFiles/Endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmanzanm\Git\back-end-framework\.readmeFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C36E7FD-A3C3-4604-A151-440F1B00E1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07362125-9F5F-4B60-A38B-CA543767B8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{0E9BAC8A-EC6D-48F4-987C-BCB17744126F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="236">
   <si>
     <t>HTTP Method</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>List&lt;Customer&gt;</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
   <si>
     <t>/api/account/{id}</t>
@@ -1584,23 +1581,128 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1608,80 +1710,137 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1704,191 +1863,29 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2239,10 +2236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA3F6E-09E5-46A7-9DF8-4B95ED8D48E7}">
-  <dimension ref="B2:I169"/>
+  <dimension ref="C2:I169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,8 +2253,8 @@
     <col min="9" max="9" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2280,7 +2277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -2301,7 +2298,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="5"/>
       <c r="D5" s="34" t="s">
         <v>13</v>
@@ -2320,7 +2317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="5"/>
       <c r="D6" s="34" t="s">
         <v>16</v>
@@ -2339,174 +2336,171 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
+    <row r="7" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="5"/>
       <c r="D7" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="34" t="s">
         <v>20</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="34" t="s">
-        <v>21</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="5"/>
       <c r="D8" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="34" t="s">
         <v>23</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>24</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" s="45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="5"/>
-      <c r="D9" s="100" t="s">
+      <c r="D9" s="152" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="153" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="152" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="116" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="100" t="s">
+      <c r="G9" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="H9" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="158" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="98" t="s">
+    </row>
+    <row r="10" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="5"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="153"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="39" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="5"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="39" t="s">
+      <c r="H10" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="158"/>
+    </row>
+    <row r="11" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="5"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="153"/>
+      <c r="F11" s="152"/>
+      <c r="G11" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="98"/>
-    </row>
-    <row r="11" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="5"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="39" t="s">
+      <c r="H11" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="158"/>
+    </row>
+    <row r="12" spans="3:9" ht="28.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="5"/>
+      <c r="D12" s="152" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="98"/>
-    </row>
-    <row r="12" spans="2:9" ht="28.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="5"/>
-      <c r="D12" s="100" t="s">
+      <c r="E12" s="153" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="152" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="116" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="100" t="s">
+      <c r="G12" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="H12" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="98" t="s">
+      <c r="I12" s="158" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="5"/>
+      <c r="D13" s="152"/>
+      <c r="E13" s="153"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="39" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="5"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="39" t="s">
+      <c r="H13" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="158"/>
+    </row>
+    <row r="14" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="5"/>
+      <c r="D14" s="152"/>
+      <c r="E14" s="153"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="98"/>
-    </row>
-    <row r="14" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="5"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="116"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="39" t="s">
-        <v>31</v>
-      </c>
       <c r="H14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="98"/>
-    </row>
-    <row r="15" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="158"/>
+    </row>
+    <row r="15" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="5"/>
       <c r="D15" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="34" t="s">
         <v>36</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>37</v>
       </c>
       <c r="G15" s="41"/>
       <c r="H15" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" s="45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="5"/>
       <c r="D16" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="34" t="s">
         <v>38</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>39</v>
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I16" s="45" t="s">
         <v>12</v>
@@ -2515,17 +2509,17 @@
     <row r="17" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="5"/>
       <c r="D17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="34" t="s">
         <v>41</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>42</v>
       </c>
       <c r="G17" s="41"/>
       <c r="H17" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I17" s="45" t="s">
         <v>12</v>
@@ -2534,17 +2528,17 @@
     <row r="18" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="5"/>
       <c r="D18" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="34" t="s">
         <v>44</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>45</v>
       </c>
       <c r="G18" s="41"/>
       <c r="H18" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="45" t="s">
         <v>12</v>
@@ -2553,545 +2547,545 @@
     <row r="19" spans="3:9" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="5"/>
       <c r="D19" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="34" t="s">
         <v>46</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>47</v>
       </c>
       <c r="G19" s="34"/>
       <c r="H19" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="3:9" ht="40.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="5"/>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="152" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="153" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="152" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="116" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="100" t="s">
+      <c r="G20" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" s="98" t="s">
-        <v>29</v>
+      <c r="I20" s="158" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="40.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="5"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="116"/>
-      <c r="F21" s="100"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="153"/>
+      <c r="F21" s="152"/>
       <c r="G21" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H21" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="I21" s="98"/>
+        <v>51</v>
+      </c>
+      <c r="I21" s="158"/>
     </row>
     <row r="22" spans="3:9" ht="40.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="5"/>
-      <c r="D22" s="100"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="100"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="153"/>
+      <c r="F22" s="152"/>
       <c r="G22" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="98"/>
+      <c r="I22" s="158"/>
     </row>
     <row r="23" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="5"/>
-      <c r="D23" s="100"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="100"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="153"/>
+      <c r="F23" s="152"/>
       <c r="G23" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="I23" s="98"/>
+        <v>54</v>
+      </c>
+      <c r="I23" s="158"/>
     </row>
     <row r="24" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="5"/>
-      <c r="D24" s="100" t="s">
+      <c r="D24" s="152" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="153" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="152" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="116" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="100" t="s">
-        <v>57</v>
-      </c>
       <c r="G24" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H24" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="I24" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="158" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="66" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="5"/>
-      <c r="D25" s="100"/>
-      <c r="E25" s="116"/>
-      <c r="F25" s="100"/>
+      <c r="D25" s="152"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="152"/>
       <c r="G25" s="42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H25" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="I25" s="98"/>
+        <v>57</v>
+      </c>
+      <c r="I25" s="158"/>
     </row>
     <row r="26" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="5"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="116"/>
-      <c r="F26" s="100"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="153"/>
+      <c r="F26" s="152"/>
       <c r="G26" s="42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H26" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="I26" s="98"/>
+        <v>58</v>
+      </c>
+      <c r="I26" s="158"/>
     </row>
     <row r="27" spans="3:9" ht="58.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
-      <c r="D27" s="100" t="s">
+      <c r="D27" s="152" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="157" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="120" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="102" t="s">
+      <c r="G27" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="I27" s="98" t="s">
+      <c r="I27" s="158" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="5"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="122"/>
-      <c r="F28" s="102"/>
+      <c r="D28" s="152"/>
+      <c r="E28" s="135"/>
+      <c r="F28" s="157"/>
       <c r="G28" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H28" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="98"/>
+      <c r="I28" s="158"/>
     </row>
     <row r="29" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="5"/>
-      <c r="D29" s="117" t="s">
-        <v>180</v>
-      </c>
-      <c r="E29" s="120" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="103" t="s">
+      <c r="D29" s="154" t="s">
+        <v>179</v>
+      </c>
+      <c r="E29" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="136" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="160" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="106" t="s">
-        <v>65</v>
-      </c>
-      <c r="H29" s="108" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="113" t="s">
-        <v>29</v>
+      <c r="H29" s="162" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="139" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="5"/>
-      <c r="D30" s="118"/>
-      <c r="E30" s="121"/>
-      <c r="F30" s="104"/>
-      <c r="G30" s="107"/>
-      <c r="H30" s="108"/>
-      <c r="I30" s="114"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="137"/>
+      <c r="G30" s="161"/>
+      <c r="H30" s="162"/>
+      <c r="I30" s="140"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="5"/>
-      <c r="D31" s="118"/>
-      <c r="E31" s="121"/>
-      <c r="F31" s="104"/>
-      <c r="G31" s="109" t="s">
-        <v>53</v>
-      </c>
-      <c r="H31" s="111" t="s">
-        <v>66</v>
-      </c>
-      <c r="I31" s="114"/>
+      <c r="D31" s="155"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="137"/>
+      <c r="G31" s="163" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" s="165" t="s">
+        <v>65</v>
+      </c>
+      <c r="I31" s="140"/>
     </row>
     <row r="32" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="5"/>
-      <c r="D32" s="119"/>
-      <c r="E32" s="122"/>
-      <c r="F32" s="105"/>
-      <c r="G32" s="110"/>
-      <c r="H32" s="112"/>
-      <c r="I32" s="115"/>
+      <c r="D32" s="156"/>
+      <c r="E32" s="135"/>
+      <c r="F32" s="138"/>
+      <c r="G32" s="164"/>
+      <c r="H32" s="166"/>
+      <c r="I32" s="141"/>
     </row>
     <row r="33" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="5"/>
-      <c r="D33" s="102" t="s">
+      <c r="D33" s="157" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="153" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="157" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="116" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="102" t="s">
+      <c r="G33" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G33" s="54" t="s">
+      <c r="I33" s="158" t="s">
         <v>28</v>
-      </c>
-      <c r="H33" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="I33" s="98" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="5"/>
-      <c r="D34" s="102"/>
-      <c r="E34" s="116"/>
-      <c r="F34" s="102"/>
+      <c r="D34" s="157"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="157"/>
       <c r="G34" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="H34" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="H34" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="I34" s="98"/>
+      <c r="I34" s="158"/>
     </row>
     <row r="35" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="5"/>
-      <c r="D35" s="102"/>
-      <c r="E35" s="116"/>
-      <c r="F35" s="102"/>
+      <c r="D35" s="157"/>
+      <c r="E35" s="153"/>
+      <c r="F35" s="157"/>
       <c r="G35" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="H35" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="H35" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" s="98"/>
+      <c r="I35" s="158"/>
     </row>
     <row r="36" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="5"/>
-      <c r="D36" s="102"/>
-      <c r="E36" s="116"/>
-      <c r="F36" s="102"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="153"/>
+      <c r="F36" s="157"/>
       <c r="G36" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H36" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I36" s="98"/>
+        <v>73</v>
+      </c>
+      <c r="I36" s="158"/>
     </row>
     <row r="37" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="5"/>
-      <c r="D37" s="146" t="s">
+      <c r="D37" s="130" t="s">
+        <v>180</v>
+      </c>
+      <c r="E37" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="136" t="s">
         <v>181</v>
       </c>
-      <c r="E37" s="120" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="103" t="s">
+      <c r="G37" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="I37" s="139" t="s">
         <v>182</v>
-      </c>
-      <c r="G37" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="61" t="s">
-        <v>184</v>
-      </c>
-      <c r="I37" s="113" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="5"/>
-      <c r="D38" s="147"/>
-      <c r="E38" s="121"/>
-      <c r="F38" s="104"/>
+      <c r="D38" s="131"/>
+      <c r="E38" s="134"/>
+      <c r="F38" s="137"/>
       <c r="G38" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H38" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="I38" s="140"/>
+    </row>
+    <row r="39" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="142"/>
+      <c r="D39" s="132"/>
+      <c r="E39" s="135"/>
+      <c r="F39" s="138"/>
+      <c r="G39" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="114"/>
-    </row>
-    <row r="39" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="149"/>
-      <c r="D39" s="148"/>
-      <c r="E39" s="122"/>
-      <c r="F39" s="105"/>
-      <c r="G39" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="H39" s="55" t="s">
-        <v>99</v>
-      </c>
-      <c r="I39" s="115"/>
+      <c r="I39" s="141"/>
     </row>
     <row r="40" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="149"/>
-      <c r="D40" s="146" t="s">
+      <c r="C40" s="142"/>
+      <c r="D40" s="130" t="s">
+        <v>184</v>
+      </c>
+      <c r="E40" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="136" t="s">
         <v>185</v>
       </c>
-      <c r="E40" s="120" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="103" t="s">
+      <c r="G40" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="H40" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="I40" s="139" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="142"/>
+      <c r="D41" s="131"/>
+      <c r="E41" s="134"/>
+      <c r="F41" s="137"/>
+      <c r="G41" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="H41" s="55" t="s">
+        <v>198</v>
+      </c>
+      <c r="I41" s="140"/>
+    </row>
+    <row r="42" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="142"/>
+      <c r="D42" s="132"/>
+      <c r="E42" s="135"/>
+      <c r="F42" s="138"/>
+      <c r="G42" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="55" t="s">
+        <v>201</v>
+      </c>
+      <c r="I42" s="141"/>
+    </row>
+    <row r="43" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="142"/>
+      <c r="D43" s="130" t="s">
         <v>186</v>
       </c>
-      <c r="G40" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="H40" s="61" t="s">
-        <v>184</v>
-      </c>
-      <c r="I40" s="113" t="s">
+      <c r="E43" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="136" t="s">
+        <v>187</v>
+      </c>
+      <c r="G43" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="H43" s="61" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="41" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="149"/>
-      <c r="D41" s="147"/>
-      <c r="E41" s="121"/>
-      <c r="F41" s="104"/>
-      <c r="G41" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="H41" s="55" t="s">
-        <v>199</v>
-      </c>
-      <c r="I41" s="114"/>
-    </row>
-    <row r="42" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="149"/>
-      <c r="D42" s="148"/>
-      <c r="E42" s="122"/>
-      <c r="F42" s="105"/>
-      <c r="G42" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="H42" s="55" t="s">
+      <c r="I43" s="139" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="142"/>
+      <c r="D44" s="131"/>
+      <c r="E44" s="134"/>
+      <c r="F44" s="137"/>
+      <c r="G44" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="H44" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="I42" s="115"/>
-    </row>
-    <row r="43" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="149"/>
-      <c r="D43" s="146" t="s">
-        <v>187</v>
-      </c>
-      <c r="E43" s="120" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="103" t="s">
-        <v>188</v>
-      </c>
-      <c r="G43" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="H43" s="61" t="s">
-        <v>184</v>
-      </c>
-      <c r="I43" s="113" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="44" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="149"/>
-      <c r="D44" s="147"/>
-      <c r="E44" s="121"/>
-      <c r="F44" s="104"/>
-      <c r="G44" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="H44" s="55" t="s">
+      <c r="I44" s="140"/>
+    </row>
+    <row r="45" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="143"/>
+      <c r="D45" s="132"/>
+      <c r="E45" s="135"/>
+      <c r="F45" s="138"/>
+      <c r="G45" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="I44" s="114"/>
-    </row>
-    <row r="45" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="150"/>
-      <c r="D45" s="148"/>
-      <c r="E45" s="122"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="H45" s="55" t="s">
-        <v>204</v>
-      </c>
-      <c r="I45" s="115"/>
+      <c r="I45" s="141"/>
     </row>
     <row r="46" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="144" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="151" t="s">
+      <c r="E46" s="145" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="152" t="s">
+      <c r="F46" s="159" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="101" t="s">
+      <c r="G46" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="G46" s="30" t="s">
+      <c r="H46" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="H46" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="I46" s="99" t="s">
+      <c r="I46" s="168" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="16"/>
-      <c r="D47" s="151"/>
-      <c r="E47" s="152"/>
-      <c r="F47" s="101"/>
+      <c r="D47" s="144"/>
+      <c r="E47" s="145"/>
+      <c r="F47" s="159"/>
       <c r="G47" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H47" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="I47" s="99"/>
+        <v>80</v>
+      </c>
+      <c r="I47" s="168"/>
     </row>
     <row r="48" spans="3:9" ht="31.35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="7"/>
-      <c r="D48" s="151"/>
-      <c r="E48" s="152"/>
-      <c r="F48" s="101"/>
+      <c r="D48" s="144"/>
+      <c r="E48" s="145"/>
+      <c r="F48" s="159"/>
       <c r="G48" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H48" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="I48" s="99"/>
+        <v>81</v>
+      </c>
+      <c r="I48" s="168"/>
     </row>
     <row r="49" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="7"/>
-      <c r="D49" s="138" t="s">
+      <c r="D49" s="146" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="123" t="s">
+      <c r="F49" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="129" t="s">
+      <c r="G49" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H49" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="G49" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H49" s="31" t="s">
+      <c r="I49" s="127" t="s">
         <v>86</v>
-      </c>
-      <c r="I49" s="95" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="50" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="7"/>
-      <c r="D50" s="140"/>
-      <c r="E50" s="124"/>
-      <c r="F50" s="130"/>
+      <c r="D50" s="147"/>
+      <c r="E50" s="122"/>
+      <c r="F50" s="125"/>
       <c r="G50" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H50" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="I50" s="96"/>
+        <v>87</v>
+      </c>
+      <c r="I50" s="128"/>
     </row>
     <row r="51" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="7"/>
-      <c r="D51" s="139"/>
-      <c r="E51" s="125"/>
-      <c r="F51" s="131"/>
+      <c r="D51" s="148"/>
+      <c r="E51" s="123"/>
+      <c r="F51" s="126"/>
       <c r="G51" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H51" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="I51" s="97"/>
+        <v>88</v>
+      </c>
+      <c r="I51" s="129"/>
     </row>
     <row r="52" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="7"/>
-      <c r="D52" s="138" t="s">
+      <c r="D52" s="146" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="121" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="124" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="123" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="129" t="s">
+      <c r="G52" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H52" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="G52" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H52" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="I52" s="95" t="s">
-        <v>87</v>
+      <c r="I52" s="127" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="7"/>
-      <c r="D53" s="139"/>
-      <c r="E53" s="125"/>
-      <c r="F53" s="131"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="123"/>
+      <c r="F53" s="126"/>
       <c r="G53" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H53" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="I53" s="97"/>
+        <v>92</v>
+      </c>
+      <c r="I53" s="129"/>
     </row>
     <row r="54" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="7"/>
@@ -3099,29 +3093,29 @@
       <c r="E54" s="49"/>
       <c r="F54" s="48"/>
       <c r="G54" s="32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H54" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I54" s="51"/>
     </row>
     <row r="55" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="7"/>
       <c r="D55" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="E55" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="F55" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="E55" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="F55" s="48" t="s">
-        <v>179</v>
-      </c>
       <c r="G55" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H55" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I55" s="51"/>
     </row>
@@ -3131,892 +3125,892 @@
       <c r="E56" s="49"/>
       <c r="F56" s="48"/>
       <c r="G56" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H56" s="52"/>
       <c r="I56" s="51"/>
     </row>
     <row r="57" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="7"/>
-      <c r="D57" s="138" t="s">
+      <c r="D57" s="146" t="s">
+        <v>93</v>
+      </c>
+      <c r="E57" s="121" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="123" t="s">
+      <c r="F57" s="124" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="129" t="s">
+      <c r="G57" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="H57" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="G57" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="H57" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="I57" s="95" t="s">
-        <v>29</v>
+      <c r="I57" s="127" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="7"/>
-      <c r="D58" s="140"/>
-      <c r="E58" s="124"/>
-      <c r="F58" s="130"/>
+      <c r="D58" s="147"/>
+      <c r="E58" s="122"/>
+      <c r="F58" s="125"/>
       <c r="G58" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H58" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="I58" s="96"/>
+        <v>97</v>
+      </c>
+      <c r="I58" s="128"/>
     </row>
     <row r="59" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="7"/>
-      <c r="D59" s="140"/>
-      <c r="E59" s="124"/>
-      <c r="F59" s="130"/>
+      <c r="D59" s="147"/>
+      <c r="E59" s="122"/>
+      <c r="F59" s="125"/>
       <c r="G59" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H59" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="I59" s="96"/>
+        <v>98</v>
+      </c>
+      <c r="I59" s="128"/>
     </row>
     <row r="60" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="7"/>
-      <c r="D60" s="139"/>
-      <c r="E60" s="125"/>
-      <c r="F60" s="131"/>
+      <c r="D60" s="148"/>
+      <c r="E60" s="123"/>
+      <c r="F60" s="126"/>
       <c r="G60" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H60" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="H60" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="I60" s="97"/>
+      <c r="I60" s="129"/>
     </row>
     <row r="61" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="7"/>
-      <c r="D61" s="138" t="s">
+      <c r="D61" s="146" t="s">
+        <v>101</v>
+      </c>
+      <c r="E61" s="121" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="123" t="s">
+      <c r="F61" s="124" t="s">
         <v>103</v>
       </c>
-      <c r="F61" s="129" t="s">
+      <c r="G61" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H61" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="30" t="s">
+      <c r="I61" s="127" t="s">
         <v>28</v>
-      </c>
-      <c r="H61" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="I61" s="95" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="62" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="7"/>
-      <c r="D62" s="140"/>
-      <c r="E62" s="124"/>
-      <c r="F62" s="130"/>
+      <c r="D62" s="147"/>
+      <c r="E62" s="122"/>
+      <c r="F62" s="125"/>
       <c r="G62" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H62" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="I62" s="96"/>
+        <v>105</v>
+      </c>
+      <c r="I62" s="128"/>
     </row>
     <row r="63" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C63" s="7"/>
-      <c r="D63" s="140"/>
-      <c r="E63" s="124"/>
-      <c r="F63" s="130"/>
+      <c r="D63" s="147"/>
+      <c r="E63" s="122"/>
+      <c r="F63" s="125"/>
       <c r="G63" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H63" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="I63" s="96"/>
+        <v>106</v>
+      </c>
+      <c r="I63" s="128"/>
     </row>
     <row r="64" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="7"/>
-      <c r="D64" s="139"/>
-      <c r="E64" s="125"/>
-      <c r="F64" s="131"/>
+      <c r="D64" s="148"/>
+      <c r="E64" s="123"/>
+      <c r="F64" s="126"/>
       <c r="G64" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H64" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="I64" s="97"/>
+        <v>107</v>
+      </c>
+      <c r="I64" s="129"/>
     </row>
     <row r="65" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="7"/>
-      <c r="D65" s="138" t="s">
+      <c r="D65" s="146" t="s">
+        <v>108</v>
+      </c>
+      <c r="E65" s="121" t="s">
         <v>109</v>
       </c>
-      <c r="E65" s="123" t="s">
+      <c r="F65" s="124" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="129" t="s">
+      <c r="G65" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H65" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G65" s="30" t="s">
+      <c r="I65" s="127" t="s">
         <v>28</v>
-      </c>
-      <c r="H65" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="I65" s="95" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="66" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="7"/>
-      <c r="D66" s="140"/>
-      <c r="E66" s="124"/>
-      <c r="F66" s="130"/>
+      <c r="D66" s="147"/>
+      <c r="E66" s="122"/>
+      <c r="F66" s="125"/>
       <c r="G66" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H66" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="I66" s="96"/>
+        <v>112</v>
+      </c>
+      <c r="I66" s="128"/>
     </row>
     <row r="67" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="7"/>
-      <c r="D67" s="140"/>
-      <c r="E67" s="124"/>
-      <c r="F67" s="130"/>
+      <c r="D67" s="147"/>
+      <c r="E67" s="122"/>
+      <c r="F67" s="125"/>
       <c r="G67" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H67" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="I67" s="96"/>
+        <v>113</v>
+      </c>
+      <c r="I67" s="128"/>
     </row>
     <row r="68" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="7"/>
-      <c r="D68" s="140"/>
-      <c r="E68" s="124"/>
-      <c r="F68" s="130"/>
+      <c r="D68" s="147"/>
+      <c r="E68" s="122"/>
+      <c r="F68" s="125"/>
       <c r="G68" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H68" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="I68" s="96"/>
+        <v>114</v>
+      </c>
+      <c r="I68" s="128"/>
     </row>
     <row r="69" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="7"/>
-      <c r="D69" s="140"/>
-      <c r="E69" s="124"/>
-      <c r="F69" s="130"/>
+      <c r="D69" s="147"/>
+      <c r="E69" s="122"/>
+      <c r="F69" s="125"/>
       <c r="G69" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H69" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="I69" s="128"/>
+    </row>
+    <row r="70" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="116"/>
+      <c r="D70" s="148"/>
+      <c r="E70" s="123"/>
+      <c r="F70" s="126"/>
+      <c r="G70" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="H70" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I69" s="96"/>
-    </row>
-    <row r="70" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C70" s="141"/>
-      <c r="D70" s="139"/>
-      <c r="E70" s="125"/>
-      <c r="F70" s="131"/>
-      <c r="G70" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="H70" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="I70" s="97"/>
+      <c r="I70" s="129"/>
     </row>
     <row r="71" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C71" s="141"/>
-      <c r="D71" s="143" t="s">
+      <c r="C71" s="116"/>
+      <c r="D71" s="118" t="s">
+        <v>188</v>
+      </c>
+      <c r="E71" s="121" t="s">
         <v>189</v>
       </c>
-      <c r="E71" s="123" t="s">
+      <c r="F71" s="124" t="s">
         <v>190</v>
       </c>
-      <c r="F71" s="129" t="s">
-        <v>191</v>
-      </c>
       <c r="G71" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H71" s="58" t="s">
-        <v>201</v>
-      </c>
-      <c r="I71" s="95" t="s">
-        <v>183</v>
+        <v>200</v>
+      </c>
+      <c r="I71" s="127" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="72" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="141"/>
-      <c r="D72" s="144"/>
-      <c r="E72" s="124"/>
-      <c r="F72" s="130"/>
+      <c r="C72" s="116"/>
+      <c r="D72" s="119"/>
+      <c r="E72" s="122"/>
+      <c r="F72" s="125"/>
       <c r="G72" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H72" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="I72" s="96"/>
+        <v>97</v>
+      </c>
+      <c r="I72" s="128"/>
     </row>
     <row r="73" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C73" s="141"/>
-      <c r="D73" s="144"/>
-      <c r="E73" s="124"/>
-      <c r="F73" s="130"/>
+      <c r="C73" s="116"/>
+      <c r="D73" s="119"/>
+      <c r="E73" s="122"/>
+      <c r="F73" s="125"/>
       <c r="G73" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H73" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="I73" s="128"/>
+    </row>
+    <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="117"/>
+      <c r="D74" s="120"/>
+      <c r="E74" s="123"/>
+      <c r="F74" s="126"/>
+      <c r="G74" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="I73" s="96"/>
-    </row>
-    <row r="74" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C74" s="142"/>
-      <c r="D74" s="145"/>
-      <c r="E74" s="125"/>
-      <c r="F74" s="131"/>
-      <c r="G74" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="H74" s="52" t="s">
-        <v>200</v>
-      </c>
-      <c r="I74" s="97"/>
+      <c r="I74" s="129"/>
     </row>
     <row r="75" spans="3:9" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="D75" s="135" t="s">
+      <c r="E75" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="132" t="s">
+      <c r="F75" s="149" t="s">
         <v>120</v>
       </c>
-      <c r="F75" s="126" t="s">
+      <c r="G75" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H75" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="G75" s="26" t="s">
+      <c r="I75" s="93" t="s">
         <v>28</v>
-      </c>
-      <c r="H75" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="I75" s="92" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="76" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C76" s="9"/>
-      <c r="D76" s="136"/>
-      <c r="E76" s="133"/>
-      <c r="F76" s="127"/>
+      <c r="D76" s="85"/>
+      <c r="E76" s="88"/>
+      <c r="F76" s="150"/>
       <c r="G76" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="I76" s="93"/>
+        <v>122</v>
+      </c>
+      <c r="I76" s="94"/>
     </row>
     <row r="77" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C77" s="10"/>
-      <c r="D77" s="136"/>
-      <c r="E77" s="133"/>
-      <c r="F77" s="127"/>
+      <c r="D77" s="85"/>
+      <c r="E77" s="88"/>
+      <c r="F77" s="150"/>
       <c r="G77" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="I77" s="93"/>
+        <v>123</v>
+      </c>
+      <c r="I77" s="94"/>
     </row>
     <row r="78" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C78" s="10"/>
-      <c r="D78" s="137"/>
-      <c r="E78" s="134"/>
-      <c r="F78" s="128"/>
+      <c r="D78" s="86"/>
+      <c r="E78" s="89"/>
+      <c r="F78" s="151"/>
       <c r="G78" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H78" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="I78" s="94"/>
+        <v>124</v>
+      </c>
+      <c r="I78" s="95"/>
     </row>
     <row r="79" spans="3:9" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="10"/>
-      <c r="D79" s="135" t="s">
+      <c r="D79" s="84" t="s">
+        <v>220</v>
+      </c>
+      <c r="E79" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F79" s="90" t="s">
         <v>221</v>
       </c>
-      <c r="E79" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="F79" s="153" t="s">
+      <c r="G79" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="H79" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="G79" s="166" t="s">
+      <c r="I79" s="93" t="s">
         <v>28</v>
-      </c>
-      <c r="H79" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="I79" s="92" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="80" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C80" s="10"/>
-      <c r="D80" s="136"/>
-      <c r="E80" s="133"/>
-      <c r="F80" s="154"/>
-      <c r="G80" s="167" t="s">
-        <v>65</v>
-      </c>
-      <c r="H80" s="164" t="s">
-        <v>234</v>
-      </c>
-      <c r="I80" s="93"/>
+      <c r="D80" s="85"/>
+      <c r="E80" s="88"/>
+      <c r="F80" s="91"/>
+      <c r="G80" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="H80" s="73" t="s">
+        <v>233</v>
+      </c>
+      <c r="I80" s="94"/>
     </row>
     <row r="81" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="10"/>
-      <c r="D81" s="136"/>
-      <c r="E81" s="133"/>
-      <c r="F81" s="154"/>
-      <c r="G81" s="165" t="s">
-        <v>53</v>
-      </c>
-      <c r="H81" s="164" t="s">
-        <v>233</v>
-      </c>
-      <c r="I81" s="93"/>
+      <c r="D81" s="85"/>
+      <c r="E81" s="88"/>
+      <c r="F81" s="91"/>
+      <c r="G81" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="H81" s="73" t="s">
+        <v>232</v>
+      </c>
+      <c r="I81" s="94"/>
     </row>
     <row r="82" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C82" s="10"/>
-      <c r="D82" s="136"/>
-      <c r="E82" s="133"/>
-      <c r="F82" s="154"/>
+      <c r="D82" s="85"/>
+      <c r="E82" s="88"/>
+      <c r="F82" s="91"/>
       <c r="G82" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H82" s="29" t="s">
-        <v>224</v>
-      </c>
-      <c r="I82" s="93"/>
+        <v>223</v>
+      </c>
+      <c r="I82" s="94"/>
     </row>
     <row r="83" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C83" s="10"/>
-      <c r="D83" s="137"/>
-      <c r="E83" s="134"/>
-      <c r="F83" s="155"/>
+      <c r="D83" s="86"/>
+      <c r="E83" s="89"/>
+      <c r="F83" s="92"/>
       <c r="G83" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="I83" s="94"/>
+        <v>129</v>
+      </c>
+      <c r="I83" s="95"/>
     </row>
     <row r="84" spans="3:9" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C84" s="10"/>
-      <c r="D84" s="135" t="s">
+      <c r="D84" s="84" t="s">
+        <v>224</v>
+      </c>
+      <c r="E84" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F84" s="90" t="s">
         <v>225</v>
       </c>
-      <c r="E84" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="F84" s="153" t="s">
+      <c r="G84" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="H84" s="79" t="s">
         <v>226</v>
       </c>
-      <c r="G84" s="168" t="s">
-        <v>28</v>
-      </c>
-      <c r="H84" s="170" t="s">
-        <v>227</v>
-      </c>
-      <c r="I84" s="92" t="s">
+      <c r="I84" s="93" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="85" spans="3:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="10"/>
-      <c r="D85" s="136"/>
-      <c r="E85" s="133"/>
-      <c r="F85" s="154"/>
-      <c r="G85" s="169" t="s">
-        <v>28</v>
-      </c>
-      <c r="H85" s="171" t="s">
-        <v>236</v>
-      </c>
-      <c r="I85" s="93"/>
+      <c r="D85" s="85"/>
+      <c r="E85" s="88"/>
+      <c r="F85" s="91"/>
+      <c r="G85" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="H85" s="80" t="s">
+        <v>235</v>
+      </c>
+      <c r="I85" s="94"/>
     </row>
     <row r="86" spans="3:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="10"/>
-      <c r="D86" s="136"/>
-      <c r="E86" s="133"/>
-      <c r="F86" s="154"/>
-      <c r="G86" s="169" t="s">
-        <v>53</v>
-      </c>
-      <c r="H86" s="171" t="s">
-        <v>235</v>
-      </c>
-      <c r="I86" s="93"/>
+      <c r="D86" s="85"/>
+      <c r="E86" s="88"/>
+      <c r="F86" s="91"/>
+      <c r="G86" s="78" t="s">
+        <v>52</v>
+      </c>
+      <c r="H86" s="80" t="s">
+        <v>234</v>
+      </c>
+      <c r="I86" s="94"/>
     </row>
     <row r="87" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C87" s="10"/>
-      <c r="D87" s="136"/>
-      <c r="E87" s="133"/>
-      <c r="F87" s="154"/>
-      <c r="G87" s="173" t="s">
-        <v>53</v>
-      </c>
-      <c r="H87" s="174" t="s">
-        <v>228</v>
-      </c>
-      <c r="I87" s="93"/>
+      <c r="D87" s="85"/>
+      <c r="E87" s="88"/>
+      <c r="F87" s="91"/>
+      <c r="G87" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="H87" s="83" t="s">
+        <v>227</v>
+      </c>
+      <c r="I87" s="94"/>
     </row>
     <row r="88" spans="3:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C88" s="10"/>
-      <c r="D88" s="137"/>
-      <c r="E88" s="134"/>
-      <c r="F88" s="155"/>
-      <c r="G88" s="172" t="s">
-        <v>70</v>
+      <c r="D88" s="86"/>
+      <c r="E88" s="89"/>
+      <c r="F88" s="92"/>
+      <c r="G88" s="81" t="s">
+        <v>69</v>
       </c>
       <c r="H88" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="I88" s="94"/>
+        <v>129</v>
+      </c>
+      <c r="I88" s="95"/>
     </row>
     <row r="89" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C89" s="10"/>
-      <c r="D89" s="135" t="s">
+      <c r="D89" s="84" t="s">
+        <v>228</v>
+      </c>
+      <c r="E89" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F89" s="90" t="s">
         <v>229</v>
       </c>
-      <c r="E89" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="F89" s="153" t="s">
+      <c r="G89" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H89" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="G89" s="26" t="s">
+      <c r="I89" s="93" t="s">
         <v>28</v>
-      </c>
-      <c r="H89" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="I89" s="92" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="90" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="10"/>
-      <c r="D90" s="136"/>
-      <c r="E90" s="133"/>
-      <c r="F90" s="154"/>
+      <c r="D90" s="85"/>
+      <c r="E90" s="88"/>
+      <c r="F90" s="91"/>
       <c r="G90" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H90" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="I90" s="93"/>
+        <v>231</v>
+      </c>
+      <c r="I90" s="94"/>
     </row>
     <row r="91" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C91" s="10"/>
-      <c r="D91" s="137"/>
-      <c r="E91" s="134"/>
-      <c r="F91" s="155"/>
+      <c r="D91" s="86"/>
+      <c r="E91" s="89"/>
+      <c r="F91" s="92"/>
       <c r="G91" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H91" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="I91" s="94"/>
+        <v>129</v>
+      </c>
+      <c r="I91" s="95"/>
     </row>
     <row r="92" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C92" s="10"/>
-      <c r="D92" s="135" t="s">
+      <c r="D92" s="84" t="s">
+        <v>125</v>
+      </c>
+      <c r="E92" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F92" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="E92" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="F92" s="153" t="s">
+      <c r="G92" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H92" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G92" s="26" t="s">
+      <c r="I92" s="93" t="s">
         <v>28</v>
-      </c>
-      <c r="H92" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="I92" s="92" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="93" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C93" s="10"/>
-      <c r="D93" s="136"/>
-      <c r="E93" s="133"/>
-      <c r="F93" s="154"/>
+      <c r="D93" s="85"/>
+      <c r="E93" s="88"/>
+      <c r="F93" s="91"/>
       <c r="G93" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H93" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="I93" s="93"/>
+        <v>128</v>
+      </c>
+      <c r="I93" s="94"/>
     </row>
     <row r="94" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C94" s="10"/>
-      <c r="D94" s="137"/>
-      <c r="E94" s="134"/>
-      <c r="F94" s="155"/>
+      <c r="D94" s="86"/>
+      <c r="E94" s="89"/>
+      <c r="F94" s="92"/>
       <c r="G94" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H94" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="I94" s="94"/>
+        <v>129</v>
+      </c>
+      <c r="I94" s="95"/>
     </row>
     <row r="95" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C95" s="10"/>
-      <c r="D95" s="135" t="s">
+      <c r="D95" s="84" t="s">
+        <v>130</v>
+      </c>
+      <c r="E95" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F95" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="E95" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="F95" s="153" t="s">
+      <c r="G95" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H95" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="G95" s="26" t="s">
+      <c r="I95" s="93" t="s">
         <v>28</v>
-      </c>
-      <c r="H95" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="I95" s="92" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="96" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C96" s="10"/>
-      <c r="D96" s="136"/>
-      <c r="E96" s="133"/>
-      <c r="F96" s="154"/>
+      <c r="D96" s="85"/>
+      <c r="E96" s="88"/>
+      <c r="F96" s="91"/>
       <c r="G96" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H96" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="I96" s="93"/>
+        <v>133</v>
+      </c>
+      <c r="I96" s="94"/>
     </row>
     <row r="97" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C97" s="10"/>
-      <c r="D97" s="137"/>
-      <c r="E97" s="134"/>
-      <c r="F97" s="155"/>
+      <c r="D97" s="86"/>
+      <c r="E97" s="89"/>
+      <c r="F97" s="92"/>
       <c r="G97" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H97" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="I97" s="94"/>
+        <v>129</v>
+      </c>
+      <c r="I97" s="95"/>
     </row>
     <row r="98" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C98" s="10"/>
-      <c r="D98" s="135" t="s">
+      <c r="D98" s="84" t="s">
+        <v>134</v>
+      </c>
+      <c r="E98" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F98" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="E98" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="F98" s="153" t="s">
+      <c r="G98" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H98" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="G98" s="26" t="s">
+      <c r="I98" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="H98" s="27" t="s">
+    </row>
+    <row r="99" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C99" s="110"/>
+      <c r="D99" s="85"/>
+      <c r="E99" s="88"/>
+      <c r="F99" s="91"/>
+      <c r="G99" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H99" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="I98" s="92" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="99" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C99" s="162"/>
-      <c r="D99" s="136"/>
-      <c r="E99" s="133"/>
-      <c r="F99" s="154"/>
-      <c r="G99" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="H99" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="I99" s="93"/>
+      <c r="I99" s="94"/>
     </row>
     <row r="100" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C100" s="162"/>
-      <c r="D100" s="137"/>
-      <c r="E100" s="134"/>
-      <c r="F100" s="155"/>
+      <c r="C100" s="110"/>
+      <c r="D100" s="86"/>
+      <c r="E100" s="89"/>
+      <c r="F100" s="92"/>
       <c r="G100" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H100" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="I100" s="94"/>
+        <v>129</v>
+      </c>
+      <c r="I100" s="95"/>
     </row>
     <row r="101" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C101" s="162"/>
-      <c r="D101" s="156" t="s">
+      <c r="C101" s="110"/>
+      <c r="D101" s="104" t="s">
+        <v>191</v>
+      </c>
+      <c r="E101" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F101" s="107" t="s">
+        <v>194</v>
+      </c>
+      <c r="G101" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H101" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="I101" s="93" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="102" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="110"/>
+      <c r="D102" s="105"/>
+      <c r="E102" s="88"/>
+      <c r="F102" s="108"/>
+      <c r="G102" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="H102" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="I102" s="94"/>
+    </row>
+    <row r="103" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C103" s="110"/>
+      <c r="D103" s="106"/>
+      <c r="E103" s="89"/>
+      <c r="F103" s="109"/>
+      <c r="G103" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="H103" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="I103" s="95"/>
+    </row>
+    <row r="104" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C104" s="110"/>
+      <c r="D104" s="104" t="s">
         <v>192</v>
       </c>
-      <c r="E101" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="F101" s="159" t="s">
+      <c r="E104" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F104" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="G101" s="26" t="s">
+      <c r="G104" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="H104" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="I104" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="H101" s="59" t="s">
+    </row>
+    <row r="105" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C105" s="110"/>
+      <c r="D105" s="105"/>
+      <c r="E105" s="88"/>
+      <c r="F105" s="108"/>
+      <c r="G105" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="H105" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="I105" s="94"/>
+    </row>
+    <row r="106" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C106" s="110"/>
+      <c r="D106" s="106"/>
+      <c r="E106" s="89"/>
+      <c r="F106" s="109"/>
+      <c r="G106" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H106" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="I106" s="95"/>
+    </row>
+    <row r="107" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="110"/>
+      <c r="D107" s="104" t="s">
+        <v>193</v>
+      </c>
+      <c r="E107" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="F107" s="107" t="s">
+        <v>195</v>
+      </c>
+      <c r="G107" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="I101" s="92" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="102" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C102" s="162"/>
-      <c r="D102" s="157"/>
-      <c r="E102" s="133"/>
-      <c r="F102" s="160"/>
-      <c r="G102" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="H102" s="56" t="s">
-        <v>207</v>
-      </c>
-      <c r="I102" s="93"/>
-    </row>
-    <row r="103" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C103" s="162"/>
-      <c r="D103" s="158"/>
-      <c r="E103" s="134"/>
-      <c r="F103" s="161"/>
-      <c r="G103" s="28" t="s">
+      <c r="H107" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="I107" s="93" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="108" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C108" s="110"/>
+      <c r="D108" s="105"/>
+      <c r="E108" s="88"/>
+      <c r="F108" s="108"/>
+      <c r="G108" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="H108" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="I108" s="94"/>
+    </row>
+    <row r="109" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C109" s="111"/>
+      <c r="D109" s="106"/>
+      <c r="E109" s="89"/>
+      <c r="F109" s="109"/>
+      <c r="G109" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H109" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="H103" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="I103" s="94"/>
-    </row>
-    <row r="104" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C104" s="162"/>
-      <c r="D104" s="156" t="s">
-        <v>193</v>
-      </c>
-      <c r="E104" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="F104" s="159" t="s">
-        <v>196</v>
-      </c>
-      <c r="G104" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="H104" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="I104" s="92" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="105" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C105" s="162"/>
-      <c r="D105" s="157"/>
-      <c r="E105" s="133"/>
-      <c r="F105" s="160"/>
-      <c r="G105" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="H105" s="56" t="s">
-        <v>213</v>
-      </c>
-      <c r="I105" s="93"/>
-    </row>
-    <row r="106" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C106" s="162"/>
-      <c r="D106" s="158"/>
-      <c r="E106" s="134"/>
-      <c r="F106" s="161"/>
-      <c r="G106" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="H106" s="56" t="s">
-        <v>207</v>
-      </c>
-      <c r="I106" s="94"/>
-    </row>
-    <row r="107" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C107" s="162"/>
-      <c r="D107" s="156" t="s">
-        <v>194</v>
-      </c>
-      <c r="E107" s="132" t="s">
-        <v>120</v>
-      </c>
-      <c r="F107" s="159" t="s">
-        <v>196</v>
-      </c>
-      <c r="G107" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="H107" s="59" t="s">
-        <v>214</v>
-      </c>
-      <c r="I107" s="92" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="108" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C108" s="162"/>
-      <c r="D108" s="157"/>
-      <c r="E108" s="133"/>
-      <c r="F108" s="160"/>
-      <c r="G108" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="H108" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="I108" s="93"/>
-    </row>
-    <row r="109" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C109" s="163"/>
-      <c r="D109" s="158"/>
-      <c r="E109" s="134"/>
-      <c r="F109" s="161"/>
-      <c r="G109" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="H109" s="56" t="s">
-        <v>207</v>
-      </c>
-      <c r="I109" s="94"/>
+      <c r="I109" s="95"/>
     </row>
     <row r="110" spans="3:9" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C110" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D110" s="114" t="s">
         <v>139</v>
       </c>
-      <c r="D110" s="79" t="s">
+      <c r="E110" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="E110" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F110" s="85" t="s">
-        <v>141</v>
-      </c>
       <c r="G110" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H110" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="I110" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="I110" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="111" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="12"/>
-      <c r="D111" s="80"/>
-      <c r="E111" s="83"/>
-      <c r="F111" s="86"/>
+      <c r="D111" s="115"/>
+      <c r="E111" s="112"/>
+      <c r="F111" s="113"/>
       <c r="G111" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H111" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="I111" s="89"/>
+        <v>153</v>
+      </c>
+      <c r="I111" s="167"/>
     </row>
     <row r="112" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C112" s="13"/>
-      <c r="D112" s="81"/>
-      <c r="E112" s="84"/>
-      <c r="F112" s="87"/>
+      <c r="D112" s="97"/>
+      <c r="E112" s="99"/>
+      <c r="F112" s="101"/>
       <c r="G112" s="69" t="s">
+        <v>142</v>
+      </c>
+      <c r="H112" s="70" t="s">
         <v>143</v>
       </c>
-      <c r="H112" s="70" t="s">
-        <v>144</v>
-      </c>
-      <c r="I112" s="90"/>
+      <c r="I112" s="103"/>
     </row>
     <row r="113" spans="3:9" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C113" s="13"/>
       <c r="D113" s="67"/>
-      <c r="E113" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F113" s="76" t="s">
+      <c r="E113" s="169" t="s">
+        <v>9</v>
+      </c>
+      <c r="F113" s="172" t="s">
+        <v>216</v>
+      </c>
+      <c r="G113" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="H113" s="72" t="s">
         <v>217</v>
-      </c>
-      <c r="G113" s="71" t="s">
-        <v>28</v>
-      </c>
-      <c r="H113" s="72" t="s">
-        <v>218</v>
       </c>
       <c r="I113" s="65"/>
     </row>
     <row r="114" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C114" s="13"/>
       <c r="D114" s="67" t="s">
-        <v>216</v>
-      </c>
-      <c r="E114" s="74"/>
-      <c r="F114" s="77"/>
+        <v>215</v>
+      </c>
+      <c r="E114" s="170"/>
+      <c r="F114" s="173"/>
       <c r="G114" s="66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H114" s="64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I114" s="65" t="s">
         <v>12</v>
@@ -4025,908 +4019,981 @@
     <row r="115" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C115" s="13"/>
       <c r="D115" s="68"/>
-      <c r="E115" s="75"/>
-      <c r="F115" s="78"/>
+      <c r="E115" s="171"/>
+      <c r="F115" s="174"/>
       <c r="G115" s="63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H115" s="64" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I115" s="65"/>
     </row>
     <row r="116" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C116" s="13"/>
-      <c r="D116" s="79" t="s">
+      <c r="D116" s="114" t="s">
+        <v>144</v>
+      </c>
+      <c r="E116" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F116" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="E116" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F116" s="85" t="s">
+      <c r="G116" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H116" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="G116" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H116" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I116" s="88" t="s">
+      <c r="I116" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="117" spans="3:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C117" s="13"/>
-      <c r="D117" s="80"/>
-      <c r="E117" s="83"/>
-      <c r="F117" s="86"/>
+      <c r="D117" s="115"/>
+      <c r="E117" s="112"/>
+      <c r="F117" s="113"/>
       <c r="G117" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H117" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="I117" s="89"/>
+        <v>147</v>
+      </c>
+      <c r="I117" s="167"/>
     </row>
     <row r="118" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C118" s="13"/>
-      <c r="D118" s="80"/>
-      <c r="E118" s="83"/>
-      <c r="F118" s="86"/>
+      <c r="D118" s="115"/>
+      <c r="E118" s="112"/>
+      <c r="F118" s="113"/>
       <c r="G118" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H118" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="I118" s="89"/>
+        <v>148</v>
+      </c>
+      <c r="I118" s="167"/>
     </row>
     <row r="119" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C119" s="13"/>
-      <c r="D119" s="81"/>
-      <c r="E119" s="84"/>
-      <c r="F119" s="87"/>
+      <c r="D119" s="97"/>
+      <c r="E119" s="99"/>
+      <c r="F119" s="101"/>
       <c r="G119" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H119" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I119" s="90"/>
+        <v>149</v>
+      </c>
+      <c r="I119" s="103"/>
     </row>
     <row r="120" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C120" s="13"/>
-      <c r="D120" s="79" t="s">
+      <c r="D120" s="114" t="s">
+        <v>150</v>
+      </c>
+      <c r="E120" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120" s="100" t="s">
         <v>151</v>
       </c>
-      <c r="E120" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F120" s="85" t="s">
+      <c r="G120" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H120" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="G120" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H120" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="I120" s="88" t="s">
+      <c r="I120" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="121" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C121" s="13"/>
-      <c r="D121" s="80"/>
-      <c r="E121" s="83"/>
-      <c r="F121" s="86"/>
+      <c r="D121" s="115"/>
+      <c r="E121" s="112"/>
+      <c r="F121" s="113"/>
       <c r="G121" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H121" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="I121" s="89"/>
+        <v>153</v>
+      </c>
+      <c r="I121" s="167"/>
     </row>
     <row r="122" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C122" s="13"/>
-      <c r="D122" s="80"/>
-      <c r="E122" s="83"/>
-      <c r="F122" s="86"/>
+      <c r="D122" s="115"/>
+      <c r="E122" s="112"/>
+      <c r="F122" s="113"/>
       <c r="G122" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H122" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I122" s="89"/>
+        <v>154</v>
+      </c>
+      <c r="I122" s="167"/>
     </row>
     <row r="123" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C123" s="13"/>
-      <c r="D123" s="81"/>
-      <c r="E123" s="84"/>
-      <c r="F123" s="87"/>
+      <c r="D123" s="97"/>
+      <c r="E123" s="99"/>
+      <c r="F123" s="101"/>
       <c r="G123" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H123" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I123" s="90"/>
+        <v>155</v>
+      </c>
+      <c r="I123" s="103"/>
     </row>
     <row r="124" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C124" s="13"/>
-      <c r="D124" s="79" t="s">
+      <c r="D124" s="114" t="s">
+        <v>156</v>
+      </c>
+      <c r="E124" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F124" s="100" t="s">
         <v>157</v>
       </c>
-      <c r="E124" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F124" s="85" t="s">
+      <c r="G124" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H124" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="G124" s="18" t="s">
+      <c r="I124" s="102" t="s">
         <v>28</v>
-      </c>
-      <c r="H124" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="I124" s="88" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="125" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C125" s="13"/>
-      <c r="D125" s="80"/>
-      <c r="E125" s="83"/>
-      <c r="F125" s="86"/>
+      <c r="D125" s="115"/>
+      <c r="E125" s="112"/>
+      <c r="F125" s="113"/>
       <c r="G125" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H125" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I125" s="89"/>
+      <c r="I125" s="167"/>
     </row>
     <row r="126" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C126" s="13"/>
-      <c r="D126" s="80"/>
-      <c r="E126" s="83"/>
-      <c r="F126" s="86"/>
+      <c r="D126" s="115"/>
+      <c r="E126" s="112"/>
+      <c r="F126" s="113"/>
       <c r="G126" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H126" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I126" s="89"/>
+      <c r="I126" s="167"/>
     </row>
     <row r="127" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C127" s="13"/>
-      <c r="D127" s="81"/>
-      <c r="E127" s="84"/>
-      <c r="F127" s="87"/>
+      <c r="D127" s="97"/>
+      <c r="E127" s="99"/>
+      <c r="F127" s="101"/>
       <c r="G127" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H127" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I127" s="90"/>
+        <v>155</v>
+      </c>
+      <c r="I127" s="103"/>
     </row>
     <row r="128" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C128" s="13"/>
-      <c r="D128" s="79" t="s">
+      <c r="D128" s="114" t="s">
+        <v>159</v>
+      </c>
+      <c r="E128" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F128" s="100" t="s">
         <v>160</v>
       </c>
-      <c r="E128" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F128" s="85" t="s">
+      <c r="G128" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H128" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="G128" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H128" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="I128" s="88" t="s">
+      <c r="I128" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="129" spans="3:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C129" s="13"/>
-      <c r="D129" s="80"/>
-      <c r="E129" s="83"/>
-      <c r="F129" s="86"/>
+      <c r="D129" s="115"/>
+      <c r="E129" s="112"/>
+      <c r="F129" s="113"/>
       <c r="G129" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H129" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="I129" s="89"/>
+        <v>162</v>
+      </c>
+      <c r="I129" s="167"/>
     </row>
     <row r="130" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C130" s="14"/>
-      <c r="D130" s="81"/>
-      <c r="E130" s="84"/>
-      <c r="F130" s="87"/>
+      <c r="D130" s="97"/>
+      <c r="E130" s="99"/>
+      <c r="F130" s="101"/>
       <c r="G130" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H130" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="I130" s="90"/>
+        <v>147</v>
+      </c>
+      <c r="I130" s="103"/>
     </row>
     <row r="131" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C131" s="14"/>
-      <c r="D131" s="79" t="s">
+      <c r="D131" s="114" t="s">
+        <v>163</v>
+      </c>
+      <c r="E131" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F131" s="100" t="s">
         <v>164</v>
       </c>
-      <c r="E131" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F131" s="85" t="s">
+      <c r="G131" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H131" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="G131" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H131" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="I131" s="88" t="s">
+      <c r="I131" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="132" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C132" s="13"/>
-      <c r="D132" s="81"/>
-      <c r="E132" s="84"/>
-      <c r="F132" s="87"/>
+      <c r="D132" s="97"/>
+      <c r="E132" s="99"/>
+      <c r="F132" s="101"/>
       <c r="G132" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H132" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="I132" s="90"/>
+        <v>166</v>
+      </c>
+      <c r="I132" s="103"/>
     </row>
     <row r="133" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C133" s="13"/>
-      <c r="D133" s="79" t="s">
+      <c r="D133" s="114" t="s">
+        <v>167</v>
+      </c>
+      <c r="E133" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F133" s="100" t="s">
         <v>168</v>
       </c>
-      <c r="E133" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F133" s="85" t="s">
+      <c r="G133" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H133" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="G133" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H133" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="I133" s="88" t="s">
+      <c r="I133" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="134" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C134" s="13"/>
-      <c r="D134" s="81"/>
-      <c r="E134" s="84"/>
-      <c r="F134" s="87"/>
+      <c r="D134" s="97"/>
+      <c r="E134" s="99"/>
+      <c r="F134" s="101"/>
       <c r="G134" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H134" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I134" s="90"/>
+        <v>170</v>
+      </c>
+      <c r="I134" s="103"/>
     </row>
     <row r="135" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C135" s="13"/>
-      <c r="D135" s="79" t="s">
+      <c r="D135" s="114" t="s">
+        <v>171</v>
+      </c>
+      <c r="E135" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="E135" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F135" s="85" t="s">
+      <c r="G135" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H135" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="G135" s="18" t="s">
+      <c r="I135" s="102" t="s">
         <v>28</v>
-      </c>
-      <c r="H135" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="I135" s="88" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="136" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C136" s="13"/>
-      <c r="D136" s="80"/>
-      <c r="E136" s="83"/>
-      <c r="F136" s="86"/>
+      <c r="D136" s="115"/>
+      <c r="E136" s="112"/>
+      <c r="F136" s="113"/>
       <c r="G136" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H136" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I136" s="89"/>
+        <v>170</v>
+      </c>
+      <c r="I136" s="167"/>
     </row>
     <row r="137" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C137" s="13"/>
-      <c r="D137" s="80"/>
-      <c r="E137" s="83"/>
-      <c r="F137" s="86"/>
+      <c r="D137" s="115"/>
+      <c r="E137" s="112"/>
+      <c r="F137" s="113"/>
       <c r="G137" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H137" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I137" s="89"/>
+      <c r="I137" s="167"/>
     </row>
     <row r="138" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C138" s="13"/>
-      <c r="D138" s="81"/>
-      <c r="E138" s="84"/>
-      <c r="F138" s="87"/>
+      <c r="D138" s="97"/>
+      <c r="E138" s="99"/>
+      <c r="F138" s="101"/>
       <c r="G138" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H138" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I138" s="90"/>
+      <c r="I138" s="103"/>
     </row>
     <row r="139" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C139" s="13"/>
-      <c r="D139" s="79" t="s">
+      <c r="D139" s="114" t="s">
+        <v>174</v>
+      </c>
+      <c r="E139" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F139" s="100" t="s">
         <v>175</v>
       </c>
-      <c r="E139" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F139" s="85" t="s">
-        <v>176</v>
-      </c>
       <c r="G139" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H139" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I139" s="88" t="s">
+      <c r="I139" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="140" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C140" s="62"/>
-      <c r="D140" s="81"/>
-      <c r="E140" s="84"/>
-      <c r="F140" s="87"/>
+      <c r="D140" s="97"/>
+      <c r="E140" s="99"/>
+      <c r="F140" s="101"/>
       <c r="G140" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H140" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I140" s="90"/>
+      <c r="I140" s="103"/>
     </row>
     <row r="141" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C141" s="62"/>
-      <c r="D141" s="91" t="s">
+      <c r="D141" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="E141" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F141" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="E141" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F141" s="85" t="s">
-        <v>198</v>
-      </c>
       <c r="G141" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H141" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="I141" s="88" t="s">
+        <v>169</v>
+      </c>
+      <c r="I141" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="142" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C142" s="13"/>
-      <c r="D142" s="81"/>
-      <c r="E142" s="84"/>
-      <c r="F142" s="87"/>
+      <c r="D142" s="97"/>
+      <c r="E142" s="99"/>
+      <c r="F142" s="101"/>
       <c r="G142" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H142" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="I142" s="90"/>
+        <v>170</v>
+      </c>
+      <c r="I142" s="103"/>
     </row>
     <row r="143" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C143" s="13"/>
-      <c r="D143" s="79" t="s">
+      <c r="D143" s="114" t="s">
+        <v>144</v>
+      </c>
+      <c r="E143" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="100" t="s">
         <v>145</v>
       </c>
-      <c r="E143" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F143" s="85" t="s">
+      <c r="G143" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H143" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="G143" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H143" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I143" s="88" t="s">
+      <c r="I143" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="144" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C144" s="13"/>
-      <c r="D144" s="80"/>
-      <c r="E144" s="83"/>
-      <c r="F144" s="86"/>
+      <c r="D144" s="115"/>
+      <c r="E144" s="112"/>
+      <c r="F144" s="113"/>
       <c r="G144" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H144" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="I144" s="89"/>
+        <v>147</v>
+      </c>
+      <c r="I144" s="167"/>
     </row>
     <row r="145" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C145" s="13"/>
-      <c r="D145" s="80"/>
-      <c r="E145" s="83"/>
-      <c r="F145" s="86"/>
+      <c r="D145" s="115"/>
+      <c r="E145" s="112"/>
+      <c r="F145" s="113"/>
       <c r="G145" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H145" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="I145" s="89"/>
+        <v>148</v>
+      </c>
+      <c r="I145" s="167"/>
     </row>
     <row r="146" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C146" s="13"/>
-      <c r="D146" s="81"/>
-      <c r="E146" s="84"/>
-      <c r="F146" s="87"/>
+      <c r="D146" s="97"/>
+      <c r="E146" s="99"/>
+      <c r="F146" s="101"/>
       <c r="G146" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H146" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I146" s="90"/>
+        <v>149</v>
+      </c>
+      <c r="I146" s="103"/>
     </row>
     <row r="147" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C147" s="13"/>
-      <c r="D147" s="79" t="s">
+      <c r="D147" s="114" t="s">
+        <v>150</v>
+      </c>
+      <c r="E147" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F147" s="100" t="s">
         <v>151</v>
       </c>
-      <c r="E147" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F147" s="85" t="s">
+      <c r="G147" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H147" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="G147" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H147" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="I147" s="88" t="s">
+      <c r="I147" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="148" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C148" s="13"/>
-      <c r="D148" s="80"/>
-      <c r="E148" s="83"/>
-      <c r="F148" s="86"/>
+      <c r="D148" s="115"/>
+      <c r="E148" s="112"/>
+      <c r="F148" s="113"/>
       <c r="G148" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H148" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="I148" s="89"/>
+        <v>153</v>
+      </c>
+      <c r="I148" s="167"/>
     </row>
     <row r="149" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C149" s="13"/>
-      <c r="D149" s="80"/>
-      <c r="E149" s="83"/>
-      <c r="F149" s="86"/>
+      <c r="D149" s="115"/>
+      <c r="E149" s="112"/>
+      <c r="F149" s="113"/>
       <c r="G149" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H149" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I149" s="89"/>
+        <v>154</v>
+      </c>
+      <c r="I149" s="167"/>
     </row>
     <row r="150" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C150" s="13"/>
-      <c r="D150" s="81"/>
-      <c r="E150" s="84"/>
-      <c r="F150" s="87"/>
+      <c r="D150" s="97"/>
+      <c r="E150" s="99"/>
+      <c r="F150" s="101"/>
       <c r="G150" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H150" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I150" s="90"/>
+        <v>155</v>
+      </c>
+      <c r="I150" s="103"/>
     </row>
     <row r="151" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C151" s="13"/>
-      <c r="D151" s="79" t="s">
+      <c r="D151" s="114" t="s">
+        <v>156</v>
+      </c>
+      <c r="E151" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F151" s="100" t="s">
         <v>157</v>
       </c>
-      <c r="E151" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F151" s="85" t="s">
+      <c r="G151" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H151" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="G151" s="18" t="s">
+      <c r="I151" s="102" t="s">
         <v>28</v>
-      </c>
-      <c r="H151" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="I151" s="88" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="152" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C152" s="13"/>
-      <c r="D152" s="80"/>
-      <c r="E152" s="83"/>
-      <c r="F152" s="86"/>
+      <c r="D152" s="115"/>
+      <c r="E152" s="112"/>
+      <c r="F152" s="113"/>
       <c r="G152" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H152" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I152" s="89"/>
+      <c r="I152" s="167"/>
     </row>
     <row r="153" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C153" s="13"/>
-      <c r="D153" s="80"/>
-      <c r="E153" s="83"/>
-      <c r="F153" s="86"/>
+      <c r="D153" s="115"/>
+      <c r="E153" s="112"/>
+      <c r="F153" s="113"/>
       <c r="G153" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H153" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I153" s="89"/>
+      <c r="I153" s="167"/>
     </row>
     <row r="154" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C154" s="13"/>
-      <c r="D154" s="81"/>
-      <c r="E154" s="84"/>
-      <c r="F154" s="87"/>
+      <c r="D154" s="97"/>
+      <c r="E154" s="99"/>
+      <c r="F154" s="101"/>
       <c r="G154" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H154" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I154" s="90"/>
+        <v>155</v>
+      </c>
+      <c r="I154" s="103"/>
     </row>
     <row r="155" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C155" s="13"/>
-      <c r="D155" s="79" t="s">
+      <c r="D155" s="114" t="s">
+        <v>159</v>
+      </c>
+      <c r="E155" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F155" s="100" t="s">
         <v>160</v>
       </c>
-      <c r="E155" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F155" s="85" t="s">
+      <c r="G155" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H155" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="G155" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H155" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="I155" s="88" t="s">
+      <c r="I155" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="156" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C156" s="13"/>
-      <c r="D156" s="80"/>
-      <c r="E156" s="83"/>
-      <c r="F156" s="86"/>
+      <c r="D156" s="115"/>
+      <c r="E156" s="112"/>
+      <c r="F156" s="113"/>
       <c r="G156" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H156" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="I156" s="89"/>
+        <v>162</v>
+      </c>
+      <c r="I156" s="167"/>
     </row>
     <row r="157" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C157" s="14"/>
-      <c r="D157" s="81"/>
-      <c r="E157" s="84"/>
-      <c r="F157" s="87"/>
+      <c r="D157" s="97"/>
+      <c r="E157" s="99"/>
+      <c r="F157" s="101"/>
       <c r="G157" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H157" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="I157" s="90"/>
+        <v>147</v>
+      </c>
+      <c r="I157" s="103"/>
     </row>
     <row r="158" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C158" s="14"/>
-      <c r="D158" s="79" t="s">
+      <c r="D158" s="114" t="s">
+        <v>163</v>
+      </c>
+      <c r="E158" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F158" s="100" t="s">
         <v>164</v>
       </c>
-      <c r="E158" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F158" s="85" t="s">
+      <c r="G158" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H158" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="G158" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H158" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="I158" s="88" t="s">
+      <c r="I158" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="159" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C159" s="13"/>
-      <c r="D159" s="81"/>
-      <c r="E159" s="84"/>
-      <c r="F159" s="87"/>
+      <c r="D159" s="97"/>
+      <c r="E159" s="99"/>
+      <c r="F159" s="101"/>
       <c r="G159" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H159" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="I159" s="90"/>
+        <v>166</v>
+      </c>
+      <c r="I159" s="103"/>
     </row>
     <row r="160" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C160" s="13"/>
-      <c r="D160" s="79" t="s">
+      <c r="D160" s="114" t="s">
+        <v>167</v>
+      </c>
+      <c r="E160" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F160" s="100" t="s">
         <v>168</v>
       </c>
-      <c r="E160" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F160" s="85" t="s">
+      <c r="G160" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H160" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="G160" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H160" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="I160" s="88" t="s">
+      <c r="I160" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="161" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C161" s="13"/>
-      <c r="D161" s="81"/>
-      <c r="E161" s="84"/>
-      <c r="F161" s="87"/>
+      <c r="D161" s="97"/>
+      <c r="E161" s="99"/>
+      <c r="F161" s="101"/>
       <c r="G161" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H161" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I161" s="90"/>
+        <v>170</v>
+      </c>
+      <c r="I161" s="103"/>
     </row>
     <row r="162" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C162" s="13"/>
-      <c r="D162" s="79" t="s">
+      <c r="D162" s="114" t="s">
+        <v>171</v>
+      </c>
+      <c r="E162" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F162" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="E162" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F162" s="85" t="s">
+      <c r="G162" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H162" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="G162" s="18" t="s">
+      <c r="I162" s="102" t="s">
         <v>28</v>
-      </c>
-      <c r="H162" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="I162" s="88" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="163" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C163" s="13"/>
-      <c r="D163" s="80"/>
-      <c r="E163" s="83"/>
-      <c r="F163" s="86"/>
+      <c r="D163" s="115"/>
+      <c r="E163" s="112"/>
+      <c r="F163" s="113"/>
       <c r="G163" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H163" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I163" s="89"/>
+        <v>170</v>
+      </c>
+      <c r="I163" s="167"/>
     </row>
     <row r="164" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C164" s="13"/>
-      <c r="D164" s="80"/>
-      <c r="E164" s="83"/>
-      <c r="F164" s="86"/>
+      <c r="D164" s="115"/>
+      <c r="E164" s="112"/>
+      <c r="F164" s="113"/>
       <c r="G164" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H164" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I164" s="89"/>
+      <c r="I164" s="167"/>
     </row>
     <row r="165" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C165" s="13"/>
-      <c r="D165" s="81"/>
-      <c r="E165" s="84"/>
-      <c r="F165" s="87"/>
+      <c r="D165" s="97"/>
+      <c r="E165" s="99"/>
+      <c r="F165" s="101"/>
       <c r="G165" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H165" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I165" s="90"/>
+      <c r="I165" s="103"/>
     </row>
     <row r="166" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C166" s="13"/>
-      <c r="D166" s="79" t="s">
+      <c r="D166" s="114" t="s">
+        <v>174</v>
+      </c>
+      <c r="E166" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F166" s="100" t="s">
         <v>175</v>
       </c>
-      <c r="E166" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F166" s="85" t="s">
-        <v>176</v>
-      </c>
       <c r="G166" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H166" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I166" s="88" t="s">
+      <c r="I166" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="167" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C167" s="62"/>
-      <c r="D167" s="81"/>
-      <c r="E167" s="84"/>
-      <c r="F167" s="87"/>
+      <c r="D167" s="97"/>
+      <c r="E167" s="99"/>
+      <c r="F167" s="101"/>
       <c r="G167" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H167" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I167" s="90"/>
+      <c r="I167" s="103"/>
     </row>
     <row r="168" spans="3:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C168" s="62"/>
-      <c r="D168" s="91" t="s">
+      <c r="D168" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="E168" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F168" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="E168" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="F168" s="85" t="s">
-        <v>198</v>
-      </c>
       <c r="G168" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H168" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="I168" s="88" t="s">
+        <v>169</v>
+      </c>
+      <c r="I168" s="102" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="169" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C169" s="15"/>
-      <c r="D169" s="81"/>
-      <c r="E169" s="84"/>
-      <c r="F169" s="87"/>
+      <c r="D169" s="97"/>
+      <c r="E169" s="99"/>
+      <c r="F169" s="101"/>
       <c r="G169" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H169" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="I169" s="90"/>
+        <v>170</v>
+      </c>
+      <c r="I169" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="193">
-    <mergeCell ref="D79:D83"/>
-    <mergeCell ref="E79:E83"/>
-    <mergeCell ref="D84:D88"/>
-    <mergeCell ref="E84:E88"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="E89:E91"/>
-    <mergeCell ref="F79:F83"/>
-    <mergeCell ref="F84:F88"/>
-    <mergeCell ref="F89:F91"/>
-    <mergeCell ref="I79:I83"/>
-    <mergeCell ref="I84:I88"/>
-    <mergeCell ref="D141:D142"/>
-    <mergeCell ref="E141:E142"/>
-    <mergeCell ref="F141:F142"/>
-    <mergeCell ref="I141:I142"/>
-    <mergeCell ref="D101:D103"/>
-    <mergeCell ref="D104:D106"/>
-    <mergeCell ref="E104:E106"/>
-    <mergeCell ref="F104:F106"/>
-    <mergeCell ref="C99:C109"/>
-    <mergeCell ref="D107:D109"/>
-    <mergeCell ref="E107:E109"/>
-    <mergeCell ref="F107:F109"/>
-    <mergeCell ref="I104:I106"/>
-    <mergeCell ref="E120:E123"/>
-    <mergeCell ref="E116:E119"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F120:F123"/>
-    <mergeCell ref="D120:D123"/>
-    <mergeCell ref="F116:F119"/>
-    <mergeCell ref="D116:D119"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="F101:F103"/>
-    <mergeCell ref="E101:E103"/>
-    <mergeCell ref="E95:E97"/>
-    <mergeCell ref="D98:D100"/>
-    <mergeCell ref="E98:E100"/>
-    <mergeCell ref="D92:D94"/>
-    <mergeCell ref="E92:E94"/>
-    <mergeCell ref="F92:F94"/>
-    <mergeCell ref="F95:F97"/>
-    <mergeCell ref="D95:D97"/>
-    <mergeCell ref="F98:F100"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="I128:I130"/>
+    <mergeCell ref="E162:E165"/>
+    <mergeCell ref="F162:F165"/>
+    <mergeCell ref="I162:I165"/>
+    <mergeCell ref="D166:D167"/>
+    <mergeCell ref="E166:E167"/>
+    <mergeCell ref="F166:F167"/>
+    <mergeCell ref="I166:I167"/>
+    <mergeCell ref="D143:D146"/>
+    <mergeCell ref="E143:E146"/>
+    <mergeCell ref="F143:F146"/>
+    <mergeCell ref="I143:I146"/>
+    <mergeCell ref="D147:D150"/>
+    <mergeCell ref="E147:E150"/>
+    <mergeCell ref="F147:F150"/>
+    <mergeCell ref="I147:I150"/>
+    <mergeCell ref="D151:D154"/>
+    <mergeCell ref="E151:E154"/>
+    <mergeCell ref="F151:F154"/>
+    <mergeCell ref="I151:I154"/>
+    <mergeCell ref="I75:I78"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="D168:D169"/>
+    <mergeCell ref="E168:E169"/>
+    <mergeCell ref="F168:F169"/>
+    <mergeCell ref="I168:I169"/>
+    <mergeCell ref="D155:D157"/>
+    <mergeCell ref="E155:E157"/>
+    <mergeCell ref="F155:F157"/>
+    <mergeCell ref="I155:I157"/>
+    <mergeCell ref="D158:D159"/>
+    <mergeCell ref="E158:E159"/>
+    <mergeCell ref="F158:F159"/>
+    <mergeCell ref="I158:I159"/>
+    <mergeCell ref="D160:D161"/>
+    <mergeCell ref="E160:E161"/>
+    <mergeCell ref="F160:F161"/>
+    <mergeCell ref="I160:I161"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="D162:D165"/>
+    <mergeCell ref="I95:I97"/>
+    <mergeCell ref="I92:I94"/>
+    <mergeCell ref="I89:I91"/>
+    <mergeCell ref="I98:I100"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="I116:I119"/>
+    <mergeCell ref="I120:I123"/>
+    <mergeCell ref="I124:I127"/>
+    <mergeCell ref="I101:I103"/>
+    <mergeCell ref="I107:I109"/>
+    <mergeCell ref="D135:D138"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="I131:I132"/>
+    <mergeCell ref="I133:I134"/>
+    <mergeCell ref="I135:I138"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="D128:D130"/>
+    <mergeCell ref="F128:F130"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="F131:F132"/>
+    <mergeCell ref="E124:E127"/>
+    <mergeCell ref="E128:E130"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="F133:F134"/>
+    <mergeCell ref="D133:D134"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="F65:F70"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="D61:D64"/>
     <mergeCell ref="C70:C74"/>
     <mergeCell ref="D71:D74"/>
     <mergeCell ref="E71:E74"/>
@@ -4951,35 +5018,41 @@
     <mergeCell ref="D49:D51"/>
     <mergeCell ref="E49:E51"/>
     <mergeCell ref="I65:I70"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="F65:F70"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="D61:D64"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="C99:C109"/>
+    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="E107:E109"/>
+    <mergeCell ref="F107:F109"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="E120:E123"/>
+    <mergeCell ref="E116:E119"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F120:F123"/>
+    <mergeCell ref="D120:D123"/>
+    <mergeCell ref="F116:F119"/>
+    <mergeCell ref="D116:D119"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="F101:F103"/>
+    <mergeCell ref="E101:E103"/>
+    <mergeCell ref="D98:D100"/>
+    <mergeCell ref="E98:E100"/>
+    <mergeCell ref="F98:F100"/>
+    <mergeCell ref="I79:I83"/>
+    <mergeCell ref="I84:I88"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="E141:E142"/>
+    <mergeCell ref="F141:F142"/>
+    <mergeCell ref="I141:I142"/>
+    <mergeCell ref="D101:D103"/>
+    <mergeCell ref="D104:D106"/>
+    <mergeCell ref="E104:E106"/>
+    <mergeCell ref="F104:F106"/>
+    <mergeCell ref="E95:E97"/>
+    <mergeCell ref="D92:D94"/>
+    <mergeCell ref="E92:E94"/>
+    <mergeCell ref="F92:F94"/>
+    <mergeCell ref="F95:F97"/>
+    <mergeCell ref="D95:D97"/>
     <mergeCell ref="F135:F138"/>
     <mergeCell ref="D139:D140"/>
     <mergeCell ref="F139:F140"/>
@@ -4988,94 +5061,15 @@
     <mergeCell ref="E133:E134"/>
     <mergeCell ref="D124:D127"/>
     <mergeCell ref="F124:F127"/>
-    <mergeCell ref="D128:D130"/>
-    <mergeCell ref="F128:F130"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="F131:F132"/>
-    <mergeCell ref="E124:E127"/>
-    <mergeCell ref="E128:E130"/>
-    <mergeCell ref="E131:E132"/>
-    <mergeCell ref="F133:F134"/>
-    <mergeCell ref="D133:D134"/>
-    <mergeCell ref="D135:D138"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="I131:I132"/>
-    <mergeCell ref="I133:I134"/>
-    <mergeCell ref="I135:I138"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="I95:I97"/>
-    <mergeCell ref="I92:I94"/>
-    <mergeCell ref="I89:I91"/>
-    <mergeCell ref="I98:I100"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="I116:I119"/>
-    <mergeCell ref="I120:I123"/>
-    <mergeCell ref="I124:I127"/>
-    <mergeCell ref="I101:I103"/>
-    <mergeCell ref="I107:I109"/>
-    <mergeCell ref="I75:I78"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I57:I60"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="D168:D169"/>
-    <mergeCell ref="E168:E169"/>
-    <mergeCell ref="F168:F169"/>
-    <mergeCell ref="I168:I169"/>
-    <mergeCell ref="D155:D157"/>
-    <mergeCell ref="E155:E157"/>
-    <mergeCell ref="F155:F157"/>
-    <mergeCell ref="I155:I157"/>
-    <mergeCell ref="D158:D159"/>
-    <mergeCell ref="E158:E159"/>
-    <mergeCell ref="F158:F159"/>
-    <mergeCell ref="I158:I159"/>
-    <mergeCell ref="D160:D161"/>
-    <mergeCell ref="E160:E161"/>
-    <mergeCell ref="F160:F161"/>
-    <mergeCell ref="I160:I161"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="D162:D165"/>
-    <mergeCell ref="E162:E165"/>
-    <mergeCell ref="F162:F165"/>
-    <mergeCell ref="I162:I165"/>
-    <mergeCell ref="D166:D167"/>
-    <mergeCell ref="E166:E167"/>
-    <mergeCell ref="F166:F167"/>
-    <mergeCell ref="I166:I167"/>
-    <mergeCell ref="D143:D146"/>
-    <mergeCell ref="E143:E146"/>
-    <mergeCell ref="F143:F146"/>
-    <mergeCell ref="I143:I146"/>
-    <mergeCell ref="D147:D150"/>
-    <mergeCell ref="E147:E150"/>
-    <mergeCell ref="F147:F150"/>
-    <mergeCell ref="I147:I150"/>
-    <mergeCell ref="D151:D154"/>
-    <mergeCell ref="E151:E154"/>
-    <mergeCell ref="F151:F154"/>
-    <mergeCell ref="I151:I154"/>
-    <mergeCell ref="I139:I140"/>
-    <mergeCell ref="I128:I130"/>
+    <mergeCell ref="D79:D83"/>
+    <mergeCell ref="E79:E83"/>
+    <mergeCell ref="D84:D88"/>
+    <mergeCell ref="E84:E88"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="E89:E91"/>
+    <mergeCell ref="F79:F83"/>
+    <mergeCell ref="F84:F88"/>
+    <mergeCell ref="F89:F91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>